<commit_message>
new hashes and some regex changes
added:
hMailServer
MediaWiki

changed regex:
vBulletin ≥ v3.8.5
Cisco-ASA(MD5)

renamed:
BCrypt(SHA256) to BCrypt(SHA-256)
</commit_message>
<xml_diff>
--- a/hashinfo.xlsx
+++ b/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="557">
   <si>
     <t>Hash</t>
   </si>
@@ -101,7 +101,7 @@
     <t>http://pythonhosted.org/passlib/lib/passlib.hash.apr_md5_crypt.html</t>
   </si>
   <si>
-    <t>BCrypt(SHA256)</t>
+    <t>BCrypt(SHA-256)</t>
   </si>
   <si>
     <t>^\$bcrypt-sha256\$.{5}\$[a-z0-9\/\.]{22}\$[a-z0-9\/\.]{31}$/i</t>
@@ -170,10 +170,13 @@
     <t>Cisco-ASA(MD5)</t>
   </si>
   <si>
-    <t>^[a-z0-9\/\.]{16}(:[0-9]{2})?$/i</t>
-  </si>
-  <si>
-    <t>02dMBMYkTdC5Ziyp:36</t>
+    <t>^[a-z0-9\/\.]{16}(:.{1,})?$/i</t>
+  </si>
+  <si>
+    <t>.ewJz0Du3XKnFk/d:hashid</t>
+  </si>
+  <si>
+    <t>https://github.com/stekershaw/asa-password-encrypt</t>
   </si>
   <si>
     <t>Cisco-IOS(MD5)</t>
@@ -203,7 +206,7 @@
     <t>Itn9sO/yhumXJ7Jv</t>
   </si>
   <si>
-    <t>http://wiki.insidepro.com/index.php/MD5%28Cisco_PIX%29</t>
+    <t>https://pythonhosted.org/passlib/lib/passlib.hash.cisco_pix.html</t>
   </si>
   <si>
     <t>Citrix Netscaler</t>
@@ -224,7 +227,7 @@
     <t>^crypt1:[a-z0-9\+\=]{12}:[a-z0-9\+\=]{12}$/i</t>
   </si>
   <si>
-    <t>crypt1:fnd+8xl+U1E=:Wc30H8MPgAc= </t>
+    <t>crypt1:fnd+8xl+U1E=:Wc30H8MPgAc=</t>
   </si>
   <si>
     <t>CRC-16</t>
@@ -635,6 +638,18 @@
     <t>4f6938531f0bc8991f62da7bbd6f7de3fad44562b8c6f4ebf146d5b4e46f7c17</t>
   </si>
   <si>
+    <t>hMailServer</t>
+  </si>
+  <si>
+    <t>^[a-f0-9]{70}$/i</t>
+  </si>
+  <si>
+    <t>cc06fa688a64cdeea43d3c0fb761fede7e3ccf00a9daea9c79f7d458e06f88327f16dd </t>
+  </si>
+  <si>
+    <t>http://www.hmailserver.com/forum/viewtopic.php?f=7&amp;t=16658&amp;start=0</t>
+  </si>
+  <si>
     <t>IP.Board ≥ v2</t>
   </si>
   <si>
@@ -833,6 +848,18 @@
     <t>MD5(Chap)</t>
   </si>
   <si>
+    <t>MediaWiki</t>
+  </si>
+  <si>
+    <t>^[:\$][AB][:\$]([a-f0-9]{1,8}[:\$])?[a-f0-9]{32}$/i</t>
+  </si>
+  <si>
+    <t>$B$113$de2874e33da25313d808d2a8cbf31485</t>
+  </si>
+  <si>
+    <t>https://www.mediawiki.org/wiki/Manual_talk%3aUser_table</t>
+  </si>
+  <si>
     <t>Microsoft MSTSC(RDP-File)</t>
   </si>
   <si>
@@ -857,10 +884,10 @@
     <t>^0x0100[a-f0-9]{88}$/i</t>
   </si>
   <si>
-    <t>0x010011223344fc9def6a4f847576458241bf11c2a906140b1db2fc9def6a4f847576458241bf11c2a906140b1db2</t>
-  </si>
-  <si>
-    <t>http://wiki.insidepro.com/index.php/MSSQL%282000%29</t>
+    <t>0x0100200420C4988140FD3920894C3EDC188E94F428D57DAD5905F6CC1CBAF950CAD4C63F272B2C91E4DEEB5E6444</t>
+  </si>
+  <si>
+    <t>https://pythonhosted.org/passlib/lib/passlib.hash.mssql2000.html</t>
   </si>
   <si>
     <t>MSSQL(2005)</t>
@@ -869,10 +896,10 @@
     <t>^0x0100[a-f0-9]{48}$/i</t>
   </si>
   <si>
-    <t>0x0100112233445810a72b6c3ee34a0a811d5bb7d9261fce9db2e0</t>
-  </si>
-  <si>
-    <t>http://wiki.insidepro.com/index.php/MSSQL%282005%29</t>
+    <t>0x01006ACDF9FF5D2E211B392EEF1175EFFE13B3A368CE2F94038B</t>
+  </si>
+  <si>
+    <t>https://pythonhosted.org/passlib/lib/passlib.hash.mssql2005.html</t>
   </si>
   <si>
     <t>MSSQL(2008)</t>
@@ -905,6 +932,9 @@
     <t>77374c3b35d41755</t>
   </si>
   <si>
+    <t>https://pythonhosted.org/passlib/lib/passlib.hash.mysql323.html</t>
+  </si>
+  <si>
     <t>MySQL4.1</t>
   </si>
   <si>
@@ -914,6 +944,9 @@
     <t>*85ADE5DDF71E348162894C71D73324C043838751</t>
   </si>
   <si>
+    <t>https://pythonhosted.org/passlib/lib/passlib.hash.mysql41.html</t>
+  </si>
+  <si>
     <t>MySQL5.x</t>
   </si>
   <si>
@@ -1232,7 +1265,7 @@
     <t>^\$sha1\$[0-9]+\$[a-z0-9\/\.]{0,64}\$[a-z0-9\/\.]{28}$/i</t>
   </si>
   <si>
-    <t>$sha1$40000$jtNX3nZ2$hBNaIXkt4wBI2o5rsi8KejSjNqIq </t>
+    <t>$sha1$40000$jtNX3nZ2$hBNaIXkt4wBI2o5rsi8KejSjNqIq</t>
   </si>
   <si>
     <t>https://pythonhosted.org/passlib/lib/passlib.hash.sha1_crypt.html</t>
@@ -1493,7 +1526,7 @@
     <t>SSHA-512(Base64)</t>
   </si>
   <si>
-    <t>{SSHA512}ALtwKGBdRgD+U0fPAy31C28RyKYx7+a8kmfksccsOeLknLHv2DBXYI7TDnTolQMBuPkWDISgZr2cHfnNPFjGZTEyNDU4OTkw </t>
+    <t>{SSHA512}ALtwKGBdRgD+U0fPAy31C28RyKYx7+a8kmfksccsOeLknLHv2DBXYI7TDnTolQMBuPkWDISgZr2cHfnNPFjGZTEyNDU4OTkw</t>
   </si>
   <si>
     <t>Sun MD5 Crypt</t>
@@ -1562,10 +1595,10 @@
     <t>16780ba78d2d5f02f3202901c1b6d975:568</t>
   </si>
   <si>
-    <t>VBulletin ≥ v3.8.5</t>
-  </si>
-  <si>
-    <t>^[a-f0-9]{32}:[a-z0-9]{30}$/i</t>
+    <t>vBulletin ≥ v3.8.5</t>
+  </si>
+  <si>
+    <t>^[a-f0-9]{32}:.{30}$/i</t>
   </si>
   <si>
     <t>bf366348c53ddcfbd16e63edfdd1eee6:181264250056774603641874043270</t>
@@ -1608,6 +1641,9 @@
   </si>
   <si>
     <t>19fa61d75522a4669b44e39c1d2e1726c530232130d407f89afee0964997f7a73e83be698b288febcf88e3e03c4f0757ea8964e59b63d93708b138cc42a66eb3</t>
+  </si>
+  <si>
+    <t>http://wiki.insidepro.com/index.php/Whirlpool</t>
   </si>
   <si>
     <t>Wordpress ≥ v2.6.2</t>
@@ -1819,10 +1855,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F170"/>
+  <dimension ref="A1:F172"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A52" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="B65" activeCellId="0" pane="topLeft" sqref="B65"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A144" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="A175" activeCellId="0" pane="topLeft" sqref="A175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.85"/>
@@ -2038,7 +2074,7 @@
         <v>47</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="13">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="13" s="4">
       <c r="A13" s="1" t="s">
         <v>48</v>
       </c>
@@ -2061,2402 +2097,2443 @@
       <c r="D14" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="15">
+      <c r="E14" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="15" s="4">
       <c r="A15" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C15" s="11" t="n">
         <v>500</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="16">
+        <v>56</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="16" s="4">
       <c r="A16" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C16" s="11" t="n">
         <v>5700</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="17">
       <c r="A17" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C17" s="11" t="n">
         <v>2400</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="18">
       <c r="A18" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C18" s="11" t="n">
         <v>8100</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="19">
+        <v>67</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="19" s="4">
       <c r="A19" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="3" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="20">
       <c r="A20" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="21">
       <c r="A21" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="22">
       <c r="A22" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="23">
       <c r="A23" s="1" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="24">
       <c r="A24" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="25">
       <c r="A25" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="26">
       <c r="A26" s="1" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="27">
       <c r="A27" s="1" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="2" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="28">
       <c r="A28" s="1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="29">
       <c r="A29" s="1" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C29" s="11" t="n">
         <v>3100</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="30">
       <c r="A30" s="13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C30" s="11" t="n">
         <v>1500</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="31">
       <c r="A31" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C31" s="11" t="n">
         <v>800</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="32">
       <c r="A32" s="4" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="11" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="33">
       <c r="A33" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="11" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="34">
       <c r="A34" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C34" s="9" t="n">
         <v>8300</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="35">
       <c r="A35" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C35" s="11" t="n">
         <v>1100</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="36">
       <c r="A36" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C36" s="11" t="n">
         <v>2100</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="37">
+        <v>133</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="37" s="4">
       <c r="A37" s="4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C37" s="9" t="n">
         <v>2600</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="38">
+        <v>136</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="38" s="4">
       <c r="A38" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C38" s="9" t="n">
         <v>4500</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="39">
       <c r="A39" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C39" s="11" t="n">
         <v>7900</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="40">
       <c r="A40" s="1" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="2" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="41">
+        <v>146</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="41" s="4">
       <c r="A41" s="1" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="C41" s="11" t="n">
         <v>123</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="42">
+        <v>149</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="42" s="4">
       <c r="A42" s="1" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C42" s="11" t="n">
         <v>141</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="43">
+        <v>152</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="43" s="4">
       <c r="A43" s="1" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C43" s="11" t="n">
         <v>1441</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="44">
       <c r="A44" s="1" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C44" s="9"/>
       <c r="D44" s="2" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="45">
       <c r="A45" s="1" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C45" s="9"/>
       <c r="D45" s="2" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="46">
       <c r="A46" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C46" s="9"/>
       <c r="D46" s="2" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="47">
       <c r="A47" s="1" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C47" s="9"/>
       <c r="D47" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="48">
       <c r="A48" s="1" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C48" s="9"/>
       <c r="D48" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="49">
+        <v>170</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="49" s="4">
       <c r="A49" s="1" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="C49" s="11" t="n">
         <v>7000</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="50">
+        <v>173</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="50" s="4">
       <c r="A50" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C50" s="11" t="n">
         <v>500</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="51">
       <c r="A51" s="1" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C51" s="9"/>
       <c r="D51" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="52">
       <c r="A52" s="1" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C52" s="9"/>
       <c r="D52" s="11" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="53">
       <c r="A53" s="1" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C53" s="11" t="n">
         <v>6900</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="54">
+        <v>185</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="54" s="4">
       <c r="A54" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C54" s="11" t="n">
         <v>7200</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F54" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="55">
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="55" s="4">
       <c r="A55" s="1" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C55" s="11" t="n">
         <v>5100</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="56">
       <c r="A56" s="1" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C56" s="9"/>
       <c r="D56" s="11" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="57">
       <c r="A57" s="1" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C57" s="9"/>
       <c r="D57" s="2" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="58">
       <c r="A58" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C58" s="9"/>
       <c r="D58" s="2" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="59">
       <c r="A59" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="C59" s="9"/>
       <c r="D59" s="2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="60">
       <c r="A60" s="1" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="C60" s="9"/>
       <c r="D60" s="2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="61">
       <c r="A61" s="1" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C61" s="9"/>
       <c r="D61" s="2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="62">
-      <c r="A62" s="13" t="s">
-        <v>206</v>
+      <c r="A62" s="4" t="s">
+        <v>207</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C62" s="11" t="n">
+        <v>208</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="63" s="4">
+      <c r="A63" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C63" s="11" t="n">
         <v>2811</v>
       </c>
-      <c r="D62" s="3" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="63">
-      <c r="A63" s="4" t="s">
-        <v>209</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="C63" s="9"/>
       <c r="D63" s="3" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="64">
-      <c r="A64" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B64" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C64" s="11" t="n">
-        <v>4800</v>
-      </c>
-      <c r="D64" s="11" t="s">
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="64" s="4">
+      <c r="A64" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="B64" s="4" t="s">
         <v>215</v>
+      </c>
+      <c r="C64" s="9" t="n">
+        <v>7300</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>216</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="65">
       <c r="A65" s="1" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C65" s="11" t="n">
+        <v>4800</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="66" s="4">
+      <c r="A66" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="B66" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C65" s="9"/>
-      <c r="D65" s="11" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="66">
-      <c r="A66" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="C66" s="11" t="n">
-        <v>11</v>
-      </c>
+      <c r="C66" s="9"/>
       <c r="D66" s="11" t="s">
-        <v>220</v>
-      </c>
-      <c r="E66" s="3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="67">
       <c r="A67" s="1" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C67" s="11" t="n">
+        <v>11</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="68" s="4">
+      <c r="A68" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C68" s="11" t="n">
         <v>22</v>
       </c>
-      <c r="D67" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="68">
-      <c r="A68" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="C68" s="11" t="n">
+      <c r="D68" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="69" s="4">
+      <c r="A69" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C69" s="11" t="n">
         <v>7500</v>
       </c>
-      <c r="D68" s="11" t="s">
-        <v>227</v>
-      </c>
-      <c r="F68" s="4" t="s">
+      <c r="D69" s="11" t="s">
+        <v>232</v>
+      </c>
+      <c r="F69" s="4" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="69">
-      <c r="A69" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="C69" s="11" t="n">
-        <v>6800</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>231</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="70">
       <c r="A70" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B70" s="2" t="s">
         <v>233</v>
       </c>
+      <c r="B70" s="4" t="s">
+        <v>234</v>
+      </c>
       <c r="C70" s="11" t="n">
-        <v>1711</v>
-      </c>
-      <c r="D70" s="11" t="s">
-        <v>234</v>
+        <v>6800</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>235</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="71">
       <c r="A71" s="1" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="C71" s="9"/>
-      <c r="D71" s="2" t="s">
         <v>238</v>
       </c>
+      <c r="C71" s="11" t="n">
+        <v>1711</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>239</v>
+      </c>
       <c r="E71" s="3" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="72">
       <c r="A72" s="1" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C72" s="11" t="n">
-        <v>190</v>
-      </c>
-      <c r="D72" s="11" t="s">
-        <v>241</v>
+        <v>242</v>
+      </c>
+      <c r="C72" s="9"/>
+      <c r="D72" s="2" t="s">
+        <v>243</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="73">
       <c r="A73" s="1" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C73" s="11" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>244</v>
+        <v>190</v>
+      </c>
+      <c r="D73" s="11" t="s">
+        <v>246</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="74">
       <c r="A74" s="1" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C74" s="9"/>
-      <c r="D74" s="11" t="s">
-        <v>248</v>
+        <v>135</v>
+      </c>
+      <c r="C74" s="11" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>249</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="75">
       <c r="A75" s="1" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>137</v>
+        <v>252</v>
       </c>
       <c r="C75" s="9"/>
       <c r="D75" s="11" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="76">
-      <c r="A76" s="4" t="s">
-        <v>253</v>
+      <c r="A76" s="1" t="s">
+        <v>255</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C76" s="9"/>
       <c r="D76" s="11" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="77">
-      <c r="A77" s="1" t="s">
-        <v>256</v>
+      <c r="A77" s="4" t="s">
+        <v>258</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C77" s="9"/>
-      <c r="D77" s="2" t="s">
-        <v>257</v>
+      <c r="D77" s="11" t="s">
+        <v>259</v>
       </c>
       <c r="E77" s="3" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="78">
       <c r="A78" s="1" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C78" s="11" t="n">
-        <v>900</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="C78" s="9"/>
       <c r="D78" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="79">
       <c r="A79" s="1" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>263</v>
+        <v>135</v>
+      </c>
+      <c r="C79" s="11" t="n">
+        <v>900</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="80">
       <c r="A80" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C80" s="11" t="n">
-        <v>500</v>
+        <v>135</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>268</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="81">
       <c r="A81" s="1" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>270</v>
+        <v>55</v>
       </c>
       <c r="C81" s="11" t="n">
-        <v>1600</v>
+        <v>500</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>26</v>
+        <v>272</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>27</v>
+        <v>273</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="82">
       <c r="A82" s="1" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>213</v>
+        <v>275</v>
       </c>
       <c r="C82" s="11" t="n">
-        <v>4800</v>
-      </c>
-      <c r="D82" s="11" t="s">
-        <v>214</v>
+        <v>1600</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>215</v>
+        <v>27</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="83">
       <c r="A83" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="B83" s="9" t="s">
-        <v>273</v>
-      </c>
-      <c r="C83" s="9"/>
-      <c r="D83" s="11"/>
+        <v>276</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C83" s="11" t="n">
+        <v>4800</v>
+      </c>
+      <c r="D83" s="11" t="s">
+        <v>219</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="84">
       <c r="A84" s="1" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="C84" s="9"/>
+        <v>278</v>
+      </c>
       <c r="D84" s="2" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="85">
+        <v>280</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="85" s="4">
       <c r="A85" s="1" t="s">
-        <v>278</v>
-      </c>
-      <c r="B85" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="C85" s="11" t="n">
-        <v>131</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="E85" s="3" t="s">
         <v>281</v>
       </c>
+      <c r="B85" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="C85" s="9"/>
+      <c r="D85" s="11"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="86">
       <c r="A86" s="1" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="C86" s="11" t="n">
-        <v>132</v>
-      </c>
+        <v>284</v>
+      </c>
+      <c r="C86" s="9"/>
       <c r="D86" s="2" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="87">
       <c r="A87" s="1" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="C87" s="9"/>
-      <c r="D87" s="11"/>
+        <v>288</v>
+      </c>
+      <c r="C87" s="11" t="n">
+        <v>131</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>290</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="88">
       <c r="A88" s="1" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="C88" s="11" t="n">
+        <v>132</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="89" s="4">
+      <c r="A89" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="C89" s="9"/>
+      <c r="D89" s="11"/>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="90" s="4">
+      <c r="A90" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="C90" s="11" t="n">
         <v>1731</v>
       </c>
-      <c r="D88" s="11" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="89">
-      <c r="A89" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="B89" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="C89" s="11" t="n">
+      <c r="D90" s="11" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="91">
+      <c r="A91" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="C91" s="11" t="n">
         <v>2811</v>
       </c>
-      <c r="D89" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="90">
-      <c r="A90" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C90" s="11" t="n">
-        <v>200</v>
-      </c>
-      <c r="D90" s="2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="91">
-      <c r="A91" s="13" t="s">
-        <v>296</v>
-      </c>
-      <c r="B91" s="2" t="s">
-        <v>297</v>
-      </c>
-      <c r="C91" s="11" t="n">
-        <v>300</v>
-      </c>
-      <c r="D91" s="11" t="s">
-        <v>298</v>
+      <c r="D91" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>302</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="92">
       <c r="A92" s="1" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>297</v>
+        <v>85</v>
       </c>
       <c r="C92" s="11" t="n">
+        <v>200</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="93">
+      <c r="A93" s="13" t="s">
+        <v>306</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C93" s="11" t="n">
         <v>300</v>
       </c>
-      <c r="D92" s="2" t="s">
-        <v>300</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="93">
-      <c r="A93" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="B93" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="C93" s="11" t="n">
-        <v>5500</v>
-      </c>
       <c r="D93" s="11" t="s">
-        <v>304</v>
+        <v>308</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>309</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="94">
       <c r="A94" s="1" t="s">
-        <v>305</v>
+        <v>310</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="C94" s="11" t="n">
+        <v>300</v>
+      </c>
+      <c r="D94" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="95" s="4">
+      <c r="A95" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="B95" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="C95" s="11" t="n">
+        <v>5500</v>
+      </c>
+      <c r="D95" s="11" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="96" s="4">
+      <c r="A96" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>317</v>
+      </c>
+      <c r="C96" s="11" t="n">
         <v>5600</v>
       </c>
-      <c r="D94" s="11" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="95">
-      <c r="A95" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C95" s="11" t="n">
-        <v>101</v>
-      </c>
-      <c r="D95" s="11" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="96">
-      <c r="A96" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="C96" s="11" t="n">
-        <v>111</v>
-      </c>
       <c r="D96" s="11" t="s">
-        <v>313</v>
+        <v>318</v>
       </c>
     </row>
     <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="97" s="4">
       <c r="A97" s="1" t="s">
-        <v>314</v>
+        <v>319</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="E97" s="3" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="98">
+        <v>320</v>
+      </c>
+      <c r="C97" s="11" t="n">
+        <v>101</v>
+      </c>
+      <c r="D97" s="11" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="98" s="4">
       <c r="A98" s="1" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>134</v>
+        <v>323</v>
       </c>
       <c r="C98" s="11" t="n">
+        <v>111</v>
+      </c>
+      <c r="D98" s="11" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="99" s="4">
+      <c r="A99" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="B99" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="100" s="4">
+      <c r="A100" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="B100" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C100" s="11" t="n">
         <v>1000</v>
       </c>
-      <c r="D98" s="2" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="99">
-      <c r="A99" s="1" t="s">
-        <v>319</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="C99" s="11" t="n">
-        <v>112</v>
-      </c>
-      <c r="D99" s="11" t="s">
-        <v>321</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="100">
-      <c r="A100" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C100" s="11" t="n">
-        <v>3100</v>
-      </c>
-      <c r="D100" s="11" t="s">
-        <v>324</v>
-      </c>
-      <c r="E100" s="3" t="s">
-        <v>325</v>
+      <c r="D100" s="2" t="s">
+        <v>265</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="101">
       <c r="A101" s="1" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="C101" s="11" t="n">
-        <v>21</v>
+        <v>112</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="E101" s="3" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="102">
       <c r="A102" s="1" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>199</v>
+        <v>85</v>
       </c>
       <c r="C102" s="11" t="n">
-        <v>122</v>
+        <v>3100</v>
       </c>
       <c r="D102" s="11" t="s">
-        <v>331</v>
+        <v>335</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>336</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="103">
       <c r="A103" s="1" t="s">
-        <v>332</v>
+        <v>337</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>333</v>
+        <v>338</v>
       </c>
       <c r="C103" s="11" t="n">
+        <v>21</v>
+      </c>
+      <c r="D103" s="11" t="s">
+        <v>339</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="104" s="4">
+      <c r="A104" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B104" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C104" s="11" t="n">
+        <v>122</v>
+      </c>
+      <c r="D104" s="11" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="105" s="4">
+      <c r="A105" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="C105" s="11" t="n">
         <v>1722</v>
       </c>
-      <c r="D103" s="11" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="104">
-      <c r="A104" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="C104" s="11" t="n">
+      <c r="D105" s="11" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="106" s="4">
+      <c r="A106" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="C106" s="11" t="n">
         <v>7100</v>
       </c>
-      <c r="D104" s="11" t="s">
-        <v>337</v>
-      </c>
-      <c r="F104" s="4" t="s">
+      <c r="D106" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="F106" s="4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="105">
-      <c r="A105" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="C105" s="9"/>
-      <c r="D105" s="2" t="s">
-        <v>340</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="106">
-      <c r="A106" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="C106" s="11" t="n">
-        <v>400</v>
-      </c>
-      <c r="D106" s="2" t="s">
-        <v>344</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>345</v>
-      </c>
-    </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="107">
-      <c r="A107" s="4" t="s">
-        <v>346</v>
+      <c r="A107" s="1" t="s">
+        <v>349</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="C107" s="11" t="n">
-        <v>400</v>
-      </c>
+        <v>350</v>
+      </c>
+      <c r="C107" s="9"/>
       <c r="D107" s="2" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="108">
       <c r="A108" s="1" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="C108" s="2" t="s">
-        <v>351</v>
+        <v>354</v>
+      </c>
+      <c r="C108" s="11" t="n">
+        <v>400</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="E108" s="3" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="109">
-      <c r="A109" s="1" t="s">
+      <c r="A109" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="B109" s="2" t="s">
         <v>354</v>
       </c>
-      <c r="B109" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C109" s="9"/>
+      <c r="C109" s="11" t="n">
+        <v>400</v>
+      </c>
       <c r="D109" s="2" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="110">
       <c r="A110" s="1" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>358</v>
-      </c>
-      <c r="C110" s="11" t="n">
-        <v>7600</v>
-      </c>
-      <c r="D110" s="3" t="s">
-        <v>359</v>
+        <v>361</v>
+      </c>
+      <c r="C110" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="D110" s="2" t="s">
+        <v>363</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="111">
       <c r="A111" s="1" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C111" s="9"/>
       <c r="D111" s="2" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="E111" s="3" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="112">
       <c r="A112" s="1" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>137</v>
+        <v>369</v>
       </c>
       <c r="C112" s="11" t="n">
-        <v>6000</v>
-      </c>
-      <c r="D112" s="2" t="s">
-        <v>365</v>
+        <v>7600</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>370</v>
       </c>
       <c r="E112" s="3" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="113">
       <c r="A113" s="1" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>182</v>
+        <v>135</v>
       </c>
       <c r="C113" s="9"/>
       <c r="D113" s="2" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="E113" s="3" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="114">
       <c r="A114" s="1" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="C114" s="9"/>
+        <v>138</v>
+      </c>
+      <c r="C114" s="11" t="n">
+        <v>6000</v>
+      </c>
       <c r="D114" s="2" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="E114" s="3" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="115">
       <c r="A115" s="1" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>375</v>
+        <v>183</v>
       </c>
       <c r="C115" s="9"/>
-      <c r="D115" s="11" t="s">
-        <v>376</v>
+      <c r="D115" s="2" t="s">
+        <v>379</v>
       </c>
       <c r="E115" s="3" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="116">
       <c r="A116" s="1" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="C116" s="9"/>
-      <c r="D116" s="11" t="s">
-        <v>379</v>
+      <c r="D116" s="2" t="s">
+        <v>383</v>
       </c>
       <c r="E116" s="3" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="117">
       <c r="A117" s="1" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="C117" s="9"/>
-      <c r="D117" s="2" t="s">
-        <v>383</v>
+      <c r="D117" s="11" t="s">
+        <v>387</v>
       </c>
       <c r="E117" s="3" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="118">
       <c r="A118" s="1" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="B118" s="2" t="s">
         <v>386</v>
       </c>
-      <c r="C118" s="11" t="n">
-        <v>5800</v>
-      </c>
+      <c r="C118" s="9"/>
       <c r="D118" s="11" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="E118" s="3" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="119">
       <c r="A119" s="1" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>390</v>
-      </c>
-      <c r="C119" s="11" t="n">
-        <v>7700</v>
-      </c>
-      <c r="D119" s="3" t="s">
-        <v>391</v>
+        <v>393</v>
+      </c>
+      <c r="C119" s="9"/>
+      <c r="D119" s="2" t="s">
+        <v>394</v>
       </c>
       <c r="E119" s="3" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="120">
       <c r="A120" s="1" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="C120" s="11" t="n">
-        <v>7800</v>
-      </c>
-      <c r="D120" s="3" t="s">
-        <v>395</v>
+        <v>5800</v>
+      </c>
+      <c r="D120" s="11" t="s">
+        <v>398</v>
       </c>
       <c r="E120" s="3" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="121">
       <c r="A121" s="1" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="C121" s="9"/>
-      <c r="D121" s="11" t="s">
-        <v>398</v>
+        <v>401</v>
+      </c>
+      <c r="C121" s="11" t="n">
+        <v>7700</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>402</v>
       </c>
       <c r="E121" s="3" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="122">
       <c r="A122" s="1" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C122" s="9" t="n">
-        <v>100</v>
-      </c>
-      <c r="D122" s="11" t="s">
-        <v>401</v>
+        <v>405</v>
+      </c>
+      <c r="C122" s="11" t="n">
+        <v>7800</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>406</v>
       </c>
       <c r="E122" s="3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="123">
       <c r="A123" s="1" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>404</v>
-      </c>
-      <c r="D123" s="3" t="s">
-        <v>405</v>
+        <v>408</v>
+      </c>
+      <c r="C123" s="9"/>
+      <c r="D123" s="11" t="s">
+        <v>409</v>
       </c>
       <c r="E123" s="3" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="124">
       <c r="A124" s="1" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>309</v>
-      </c>
-      <c r="C124" s="11" t="n">
+        <v>138</v>
+      </c>
+      <c r="C124" s="9" t="n">
+        <v>100</v>
+      </c>
+      <c r="D124" s="11" t="s">
+        <v>412</v>
+      </c>
+      <c r="E124" s="3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="125" s="4">
+      <c r="A125" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="E125" s="3" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="126" s="4">
+      <c r="A126" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="C126" s="11" t="n">
         <v>101</v>
       </c>
-      <c r="D124" s="11" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="125">
-      <c r="A125" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="B125" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="C125" s="9"/>
-      <c r="D125" s="2" t="s">
-        <v>409</v>
-      </c>
-      <c r="E125" s="3" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="126">
-      <c r="A126" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="B126" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="C126" s="9"/>
       <c r="D126" s="11" t="s">
-        <v>412</v>
-      </c>
-      <c r="E126" s="3" t="s">
-        <v>413</v>
+        <v>321</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="127">
       <c r="A127" s="1" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C127" s="11" t="n">
-        <v>1400</v>
-      </c>
-      <c r="D127" s="11" t="s">
-        <v>415</v>
+        <v>200</v>
+      </c>
+      <c r="C127" s="9"/>
+      <c r="D127" s="2" t="s">
+        <v>420</v>
       </c>
       <c r="E127" s="3" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="128">
-      <c r="A128" s="4" t="s">
-        <v>417</v>
+      <c r="A128" s="1" t="s">
+        <v>422</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="C128" s="11" t="n">
-        <v>7400</v>
-      </c>
+        <v>203</v>
+      </c>
+      <c r="C128" s="9"/>
       <c r="D128" s="11" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="129">
       <c r="A129" s="1" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="C129" s="9"/>
-      <c r="D129" s="2" t="s">
-        <v>423</v>
+        <v>183</v>
+      </c>
+      <c r="C129" s="11" t="n">
+        <v>1400</v>
+      </c>
+      <c r="D129" s="11" t="s">
+        <v>426</v>
       </c>
       <c r="E129" s="3" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="130">
-      <c r="A130" s="1" t="s">
-        <v>425</v>
+      <c r="A130" s="4" t="s">
+        <v>428</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>375</v>
+        <v>429</v>
       </c>
       <c r="C130" s="11" t="n">
-        <v>1700</v>
-      </c>
-      <c r="D130" s="2" t="s">
-        <v>426</v>
+        <v>7400</v>
+      </c>
+      <c r="D130" s="11" t="s">
+        <v>430</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="131">
       <c r="A131" s="1" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="C131" s="11" t="n">
-        <v>1800</v>
-      </c>
-      <c r="D131" s="11" t="s">
-        <v>430</v>
+        <v>433</v>
+      </c>
+      <c r="C131" s="9"/>
+      <c r="D131" s="2" t="s">
+        <v>434</v>
       </c>
       <c r="E131" s="3" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="132">
       <c r="A132" s="1" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>202</v>
+        <v>386</v>
       </c>
       <c r="C132" s="11" t="n">
-        <v>5000</v>
-      </c>
-      <c r="D132" s="11" t="s">
-        <v>433</v>
+        <v>1700</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>437</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="133">
       <c r="A133" s="1" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C133" s="9"/>
+        <v>440</v>
+      </c>
+      <c r="C133" s="11" t="n">
+        <v>1800</v>
+      </c>
       <c r="D133" s="11" t="s">
-        <v>436</v>
+        <v>441</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>434</v>
+        <v>442</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="134">
       <c r="A134" s="1" t="s">
-        <v>437</v>
+        <v>443</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="C134" s="9"/>
+        <v>203</v>
+      </c>
+      <c r="C134" s="11" t="n">
+        <v>5000</v>
+      </c>
       <c r="D134" s="11" t="s">
-        <v>438</v>
+        <v>444</v>
       </c>
       <c r="E134" s="3" t="s">
-        <v>434</v>
+        <v>445</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="135">
       <c r="A135" s="1" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>375</v>
+        <v>183</v>
       </c>
       <c r="C135" s="9"/>
       <c r="D135" s="11" t="s">
-        <v>440</v>
+        <v>447</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>434</v>
+        <v>445</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="136">
       <c r="A136" s="1" t="s">
-        <v>441</v>
+        <v>448</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>442</v>
+        <v>433</v>
       </c>
       <c r="C136" s="9"/>
       <c r="D136" s="11" t="s">
-        <v>443</v>
+        <v>449</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="137">
       <c r="A137" s="1" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>422</v>
+        <v>386</v>
       </c>
       <c r="C137" s="9"/>
       <c r="D137" s="11" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="138">
       <c r="A138" s="1" t="s">
-        <v>448</v>
+        <v>452</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>375</v>
+        <v>453</v>
       </c>
       <c r="C138" s="9"/>
       <c r="D138" s="11" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>450</v>
+        <v>455</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="139">
       <c r="A139" s="1" t="s">
-        <v>451</v>
+        <v>456</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>182</v>
+        <v>433</v>
       </c>
       <c r="C139" s="9"/>
       <c r="D139" s="11" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="E139" s="3" t="s">
-        <v>453</v>
+        <v>458</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="140">
       <c r="A140" s="1" t="s">
-        <v>454</v>
+        <v>459</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>134</v>
+        <v>386</v>
       </c>
       <c r="C140" s="9"/>
       <c r="D140" s="11" t="s">
-        <v>455</v>
+        <v>460</v>
       </c>
       <c r="E140" s="3" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="141">
       <c r="A141" s="1" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>137</v>
+        <v>183</v>
       </c>
       <c r="C141" s="9"/>
       <c r="D141" s="11" t="s">
-        <v>458</v>
+        <v>463</v>
       </c>
       <c r="E141" s="3" t="s">
-        <v>459</v>
+        <v>464</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="142">
       <c r="A142" s="1" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>202</v>
+        <v>135</v>
       </c>
       <c r="C142" s="9"/>
       <c r="D142" s="11" t="s">
-        <v>461</v>
+        <v>466</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="143">
       <c r="A143" s="1" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>375</v>
+        <v>138</v>
       </c>
       <c r="C143" s="9"/>
       <c r="D143" s="11" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="E143" s="3" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="144">
       <c r="A144" s="1" t="s">
-        <v>466</v>
+        <v>471</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>134</v>
+        <v>203</v>
       </c>
       <c r="C144" s="9"/>
       <c r="D144" s="11" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="E144" s="3" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="145">
       <c r="A145" s="1" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>137</v>
+        <v>386</v>
       </c>
       <c r="C145" s="9"/>
       <c r="D145" s="11" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="146">
       <c r="A146" s="1" t="s">
-        <v>472</v>
+        <v>477</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>202</v>
+        <v>135</v>
       </c>
       <c r="C146" s="9"/>
       <c r="D146" s="11" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="147">
       <c r="A147" s="1" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>182</v>
+        <v>138</v>
       </c>
       <c r="C147" s="9"/>
       <c r="D147" s="11" t="s">
-        <v>476</v>
+        <v>481</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="148">
       <c r="A148" s="1" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>422</v>
+        <v>203</v>
       </c>
       <c r="C148" s="9"/>
       <c r="D148" s="11" t="s">
-        <v>479</v>
+        <v>484</v>
       </c>
       <c r="E148" s="3" t="s">
-        <v>480</v>
+        <v>485</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="149">
       <c r="A149" s="1" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="C149" s="11" t="n">
-        <v>121</v>
-      </c>
-      <c r="D149" s="3" t="s">
-        <v>483</v>
+        <v>183</v>
+      </c>
+      <c r="C149" s="9"/>
+      <c r="D149" s="11" t="s">
+        <v>487</v>
+      </c>
+      <c r="E149" s="3" t="s">
+        <v>488</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="150">
       <c r="A150" s="1" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>134</v>
+        <v>433</v>
       </c>
       <c r="C150" s="9"/>
       <c r="D150" s="11" t="s">
-        <v>485</v>
+        <v>490</v>
       </c>
       <c r="E150" s="3" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="151">
+        <v>491</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="151" s="4">
       <c r="A151" s="1" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C151" s="9"/>
-      <c r="D151" s="11" t="s">
-        <v>488</v>
-      </c>
-      <c r="E151" s="3" t="s">
-        <v>489</v>
+        <v>493</v>
+      </c>
+      <c r="C151" s="11" t="n">
+        <v>121</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>494</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="152">
       <c r="A152" s="1" t="s">
-        <v>490</v>
+        <v>495</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="C152" s="11" t="n">
-        <v>111</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="C152" s="9"/>
       <c r="D152" s="11" t="s">
-        <v>313</v>
+        <v>496</v>
+      </c>
+      <c r="E152" s="3" t="s">
+        <v>497</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="153">
       <c r="A153" s="1" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="C153" s="11" t="n">
-        <v>1711</v>
-      </c>
-      <c r="D153" s="3" t="s">
-        <v>492</v>
+        <v>183</v>
+      </c>
+      <c r="C153" s="9"/>
+      <c r="D153" s="11" t="s">
+        <v>499</v>
       </c>
       <c r="E153" s="3" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="154">
-      <c r="A154" s="4" t="s">
-        <v>493</v>
+        <v>500</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="154" s="4">
+      <c r="A154" s="1" t="s">
+        <v>501</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>494</v>
+        <v>323</v>
       </c>
       <c r="C154" s="11" t="n">
-        <v>3300</v>
+        <v>111</v>
       </c>
       <c r="D154" s="11" t="s">
-        <v>495</v>
-      </c>
-      <c r="E154" s="3" t="s">
-        <v>496</v>
+        <v>324</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="155">
       <c r="A155" s="1" t="s">
-        <v>497</v>
+        <v>502</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>498</v>
+        <v>238</v>
       </c>
       <c r="C155" s="11" t="n">
-        <v>8000</v>
-      </c>
-      <c r="D155" s="11" t="s">
-        <v>499</v>
+        <v>1711</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>503</v>
       </c>
       <c r="E155" s="3" t="s">
-        <v>500</v>
+        <v>240</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="156">
-      <c r="A156" s="1" t="s">
-        <v>501</v>
+      <c r="A156" s="4" t="s">
+        <v>504</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="C156" s="9"/>
+        <v>505</v>
+      </c>
+      <c r="C156" s="11" t="n">
+        <v>3300</v>
+      </c>
       <c r="D156" s="11" t="s">
-        <v>502</v>
+        <v>506</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>503</v>
+        <v>507</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="157">
       <c r="A157" s="1" t="s">
-        <v>504</v>
+        <v>508</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C157" s="9"/>
+        <v>509</v>
+      </c>
+      <c r="C157" s="11" t="n">
+        <v>8000</v>
+      </c>
       <c r="D157" s="11" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="E157" s="3" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="158">
       <c r="A158" s="1" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>199</v>
+        <v>135</v>
       </c>
       <c r="C158" s="9"/>
       <c r="D158" s="11" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="E158" s="3" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="159">
       <c r="A159" s="1" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C159" s="11" t="n">
-        <v>1500</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="C159" s="9"/>
       <c r="D159" s="11" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
       <c r="E159" s="3" t="s">
-        <v>108</v>
+        <v>517</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="160">
       <c r="A160" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="B160" s="9" t="s">
-        <v>513</v>
-      </c>
-      <c r="C160" s="11" t="n">
-        <v>2611</v>
-      </c>
+        <v>518</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C160" s="9"/>
       <c r="D160" s="11" t="s">
-        <v>514</v>
+        <v>519</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>520</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="161">
       <c r="A161" s="1" t="s">
-        <v>515</v>
+        <v>521</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>516</v>
+        <v>107</v>
       </c>
       <c r="C161" s="11" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D161" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="162" s="4">
+      <c r="A162" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="B162" s="9" t="s">
+        <v>524</v>
+      </c>
+      <c r="C162" s="11" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D162" s="11" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="163" s="4">
+      <c r="A163" s="1" t="s">
+        <v>526</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>527</v>
+      </c>
+      <c r="C163" s="11" t="n">
         <v>2711</v>
       </c>
-      <c r="D161" s="11" t="s">
-        <v>517</v>
-      </c>
-      <c r="F161" s="4" t="s">
+      <c r="D163" s="11" t="s">
+        <v>528</v>
+      </c>
+      <c r="F163" s="4" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="162">
-      <c r="A162" s="1" t="s">
-        <v>518</v>
-      </c>
-      <c r="B162" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C162" s="9"/>
-      <c r="D162" s="11" t="s">
-        <v>519</v>
-      </c>
-      <c r="E162" s="3" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="163">
-      <c r="A163" s="1" t="s">
-        <v>521</v>
-      </c>
-      <c r="B163" s="2" t="s">
-        <v>522</v>
-      </c>
-      <c r="C163" s="9"/>
-      <c r="D163" s="3" t="s">
-        <v>523</v>
-      </c>
-      <c r="E163" s="3" t="s">
-        <v>524</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="164">
       <c r="A164" s="1" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>526</v>
-      </c>
-      <c r="C164" s="11" t="n">
-        <v>3721</v>
-      </c>
-      <c r="D164" s="3" t="s">
-        <v>527</v>
+        <v>183</v>
+      </c>
+      <c r="C164" s="9"/>
+      <c r="D164" s="11" t="s">
+        <v>530</v>
       </c>
       <c r="E164" s="3" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="165">
       <c r="A165" s="1" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>375</v>
-      </c>
-      <c r="C165" s="11" t="n">
+        <v>533</v>
+      </c>
+      <c r="C165" s="9"/>
+      <c r="D165" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="166">
+      <c r="A166" s="1" t="s">
+        <v>536</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>537</v>
+      </c>
+      <c r="C166" s="11" t="n">
+        <v>3721</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="167">
+      <c r="A167" s="1" t="s">
+        <v>540</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C167" s="11" t="n">
         <v>6100</v>
       </c>
-      <c r="D165" s="2" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="166">
-      <c r="A166" s="4" t="s">
-        <v>531</v>
-      </c>
-      <c r="B166" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="C166" s="11" t="n">
+      <c r="D167" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="168">
+      <c r="A168" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="C168" s="11" t="n">
         <v>400</v>
       </c>
-      <c r="D166" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="E166" s="3" t="s">
-        <v>534</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="167">
-      <c r="A167" s="4" t="s">
-        <v>535</v>
-      </c>
-      <c r="B167" s="2" t="s">
-        <v>343</v>
-      </c>
-      <c r="C167" s="11"/>
-      <c r="D167" s="3" t="s">
-        <v>536</v>
-      </c>
-      <c r="E167" s="3" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="168">
-      <c r="A168" s="1" t="s">
-        <v>537</v>
-      </c>
-      <c r="B168" s="2" t="s">
+      <c r="D168" s="2" t="s">
+        <v>545</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="169">
+      <c r="A169" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="C169" s="11" t="n">
+        <v>400</v>
+      </c>
+      <c r="D169" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="170">
+      <c r="A170" s="1" t="s">
+        <v>549</v>
+      </c>
+      <c r="B170" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C168" s="9"/>
-      <c r="D168" s="2" t="s">
-        <v>538</v>
-      </c>
-      <c r="E168" s="3" t="s">
-        <v>539</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="169">
-      <c r="A169" s="1" t="s">
-        <v>540</v>
-      </c>
-      <c r="B169" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="C169" s="11" t="n">
+      <c r="C170" s="9"/>
+      <c r="D170" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="true" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="171" s="4">
+      <c r="A171" s="1" t="s">
+        <v>552</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C171" s="11" t="n">
         <v>21</v>
       </c>
-      <c r="D169" s="11" t="s">
-        <v>541</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="170">
-      <c r="A170" s="4" t="s">
-        <v>542</v>
-      </c>
-      <c r="B170" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D170" s="11" t="s">
-        <v>543</v>
-      </c>
-      <c r="E170" s="3" t="s">
-        <v>544</v>
+      <c r="D171" s="11" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.85" outlineLevel="0" r="172">
+      <c r="A172" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D172" s="11" t="s">
+        <v>555</v>
+      </c>
+      <c r="E172" s="3" t="s">
+        <v>556</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Lotus Notes/Domino 5 & 6
added:
- Lotus Notes/Domino 5
hashcatmode added:
- Lotus Notes/Domino 5
- Lotus Notes/Domino 6
renamed:
Lotus Domino to Lotus Notes/Domino 6
regex changed:
- DNSSEC(NSEC3)
</commit_message>
<xml_diff>
--- a/hashinfo.xlsx
+++ b/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="760" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="636">
   <si>
     <t>Hash</t>
   </si>
@@ -386,7 +386,7 @@
     <t>DNSSEC(NSEC3)</t>
   </si>
   <si>
-    <t>^[a-z0-9]{32}(:([a-z0-9-]+\.)?[a-z0-9-]+\.[a-z]{2,7}:.+:[0-9]+)?$/i</t>
+    <t>^[a-z0-9]{32}(:([a-z0-9-]+\.)?[a-z0-9-.]+\.[a-z]{2,7}:.+:[0-9]+)?$/i</t>
   </si>
   <si>
     <t>2rpoiv7tgpg21jm3qb3ifdj6kajk0g29:test.example.com:33164473:10</t>
@@ -419,7 +419,7 @@
     <t>mscach2</t>
   </si>
   <si>
-    <t>4c253e4b65c007a8cd683ea57bc43c76</t>
+    <t>$DCC2$10240#hashid#4c253e4b65c007a8cd683ea57bc43c76</t>
   </si>
   <si>
     <t>http://pythonhosted.org/passlib/lib/passlib.hash.msdcc2.html</t>
@@ -833,21 +833,33 @@
     <t>http://pythonhosted.org/passlib/lib/passlib.hash.lmhash.html</t>
   </si>
   <si>
-    <t>Lotus Domino</t>
+    <t>Lotus Notes/Domino 5</t>
+  </si>
+  <si>
+    <t>8600</t>
+  </si>
+  <si>
+    <t>lotus5</t>
+  </si>
+  <si>
+    <t>3dd2e1e5ac03e230243d58b8c5ada076</t>
+  </si>
+  <si>
+    <t>Lotus Notes/Domino 6</t>
   </si>
   <si>
     <t>^\([a-z0-9\+\/]{20}\)$/i</t>
   </si>
   <si>
+    <t>8700</t>
+  </si>
+  <si>
     <t>dominosec</t>
   </si>
   <si>
     <t>(Gv0GtxzT8DYnLKAKDNsB)</t>
   </si>
   <si>
-    <t>https://en.wikipedia.org/wiki/IBM_Lotus_Domino</t>
-  </si>
-  <si>
     <t>MaNGOS CMS</t>
   </si>
   <si>
@@ -1248,6 +1260,18 @@
   </si>
   <si>
     <t>http://wiki.insidepro.com/index.php/MD5%28phpBB3%29</t>
+  </si>
+  <si>
+    <t>PHPS</t>
+  </si>
+  <si>
+    <t>^\$PHPS\$[0-9]{14}\$[a-f0-9]{32}$/i</t>
+  </si>
+  <si>
+    <t>phps</t>
+  </si>
+  <si>
+    <t>$PHPS$34323438373734$5b07e065b9d78d69603e71201c6cf29f</t>
   </si>
   <si>
     <t>RACF</t>
@@ -1994,7 +2018,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2055,6 +2079,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -2073,10 +2101,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G181"/>
+  <dimension ref="A1:G183"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D28" activeCellId="0" sqref="D28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3404,43 +3432,49 @@
         <v>271</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="8" t="s">
         <v>272</v>
       </c>
       <c r="B77" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C77" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="C77" s="10"/>
-      <c r="D77" s="10" t="s">
+      <c r="D77" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="E77" s="9" t="s">
+      <c r="E77" s="15" t="s">
         <v>275</v>
       </c>
-      <c r="F77" s="3" t="s">
+      <c r="G77" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="8" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="8" t="s">
+      <c r="B78" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="B78" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
+      <c r="C78" s="10" t="s">
+        <v>278</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>279</v>
+      </c>
       <c r="E78" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="F78" s="3" t="s">
-        <v>279</v>
+        <v>280</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="1" t="s">
-        <v>280</v>
+      <c r="A79" s="8" t="s">
+        <v>281</v>
       </c>
       <c r="B79" s="9" t="s">
         <v>140</v>
@@ -3448,41 +3482,37 @@
       <c r="C79" s="10"/>
       <c r="D79" s="10"/>
       <c r="E79" s="9" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="8" t="s">
-        <v>283</v>
+      <c r="A80" s="1" t="s">
+        <v>284</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="C80" s="10"/>
       <c r="D80" s="10"/>
       <c r="E80" s="9" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="8" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B81" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C81" s="9" t="n">
-        <v>900</v>
-      </c>
-      <c r="D81" s="9" t="s">
-        <v>287</v>
-      </c>
+      <c r="C81" s="10"/>
+      <c r="D81" s="10"/>
       <c r="E81" s="9" t="s">
         <v>288</v>
       </c>
@@ -3497,116 +3527,120 @@
       <c r="B82" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="C82" s="9" t="s">
+      <c r="C82" s="9" t="n">
+        <v>900</v>
+      </c>
+      <c r="D82" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="D82" s="9" t="s">
+      <c r="E82" s="9" t="s">
         <v>292</v>
       </c>
-      <c r="E82" s="9" t="s">
+      <c r="F82" s="3" t="s">
         <v>293</v>
-      </c>
-      <c r="F82" s="3" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="B83" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C83" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="B83" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C83" s="9" t="n">
-        <v>500</v>
-      </c>
-      <c r="D83" s="9"/>
+      <c r="D83" s="9" t="s">
+        <v>296</v>
+      </c>
       <c r="E83" s="9" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="8" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>299</v>
+        <v>50</v>
       </c>
       <c r="C84" s="9" t="n">
-        <v>1600</v>
+        <v>500</v>
       </c>
       <c r="D84" s="9"/>
       <c r="E84" s="9" t="s">
-        <v>27</v>
+        <v>300</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>28</v>
+        <v>301</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="8" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>231</v>
+        <v>303</v>
       </c>
       <c r="C85" s="9" t="n">
-        <v>4800</v>
+        <v>1600</v>
       </c>
       <c r="D85" s="9"/>
       <c r="E85" s="9" t="s">
-        <v>232</v>
+        <v>27</v>
       </c>
       <c r="F85" s="3" t="s">
-        <v>233</v>
+        <v>28</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="8" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10" t="s">
-        <v>303</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="C86" s="9" t="n">
+        <v>4800</v>
+      </c>
+      <c r="D86" s="9"/>
       <c r="E86" s="9" t="s">
-        <v>304</v>
+        <v>232</v>
       </c>
       <c r="F86" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="8" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="87" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="8" t="s">
+      <c r="B87" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="B87" s="13" t="s">
+      <c r="C87" s="10"/>
+      <c r="D87" s="10" t="s">
         <v>307</v>
       </c>
-      <c r="C87" s="10"/>
-      <c r="D87" s="10"/>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E87" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="88" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="8" t="s">
-        <v>308</v>
-      </c>
-      <c r="B88" s="9" t="s">
-        <v>309</v>
+        <v>310</v>
+      </c>
+      <c r="B88" s="13" t="s">
+        <v>311</v>
       </c>
       <c r="C88" s="10"/>
       <c r="D88" s="10"/>
-      <c r="E88" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>311</v>
-      </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="8" t="s">
@@ -3615,105 +3649,103 @@
       <c r="B89" s="9" t="s">
         <v>313</v>
       </c>
-      <c r="C89" s="9" t="n">
-        <v>131</v>
-      </c>
-      <c r="D89" s="9" t="s">
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
+      <c r="E89" s="9" t="s">
         <v>314</v>
       </c>
-      <c r="E89" s="11" t="s">
+      <c r="F89" s="3" t="s">
         <v>315</v>
-      </c>
-      <c r="F89" s="3" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="B90" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="B90" s="9" t="s">
+      <c r="C90" s="9" t="n">
+        <v>131</v>
+      </c>
+      <c r="D90" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="C90" s="9" t="n">
+      <c r="E90" s="11" t="s">
+        <v>319</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="C91" s="9" t="n">
         <v>132</v>
       </c>
-      <c r="D90" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="E90" s="11" t="s">
-        <v>320</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="91" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="8" t="s">
-        <v>322</v>
-      </c>
-      <c r="B91" s="9" t="s">
-        <v>318</v>
-      </c>
-      <c r="C91" s="10" t="n">
-        <v>132</v>
-      </c>
-      <c r="D91" s="10"/>
-      <c r="G91" s="1" t="s">
-        <v>15</v>
+      <c r="D91" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="E91" s="11" t="s">
+        <v>324</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="92" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="8" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="C92" s="9" t="n">
-        <v>1731</v>
-      </c>
-      <c r="D92" s="9"/>
-      <c r="E92" s="9" t="s">
-        <v>325</v>
-      </c>
+        <v>322</v>
+      </c>
+      <c r="C92" s="10" t="n">
+        <v>132</v>
+      </c>
+      <c r="D92" s="10"/>
       <c r="G92" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="93" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="8" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="C93" s="9" t="n">
         <v>1731</v>
       </c>
       <c r="D93" s="9"/>
-      <c r="F93" s="3" t="s">
-        <v>327</v>
+      <c r="E93" s="9" t="s">
+        <v>329</v>
       </c>
       <c r="G93" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="B94" s="9" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="8" t="s">
-        <v>329</v>
-      </c>
-      <c r="B94" s="9" t="s">
-        <v>330</v>
-      </c>
       <c r="C94" s="9" t="n">
-        <v>2811</v>
+        <v>1731</v>
       </c>
       <c r="D94" s="9"/>
-      <c r="E94" s="11" t="s">
+      <c r="F94" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="F94" s="3" t="s">
+      <c r="G94" s="1" t="s">
         <v>332</v>
       </c>
     </row>
@@ -3722,15 +3754,13 @@
         <v>333</v>
       </c>
       <c r="B95" s="9" t="s">
-        <v>84</v>
+        <v>334</v>
       </c>
       <c r="C95" s="9" t="n">
-        <v>200</v>
-      </c>
-      <c r="D95" s="9" t="s">
-        <v>334</v>
-      </c>
-      <c r="E95" s="9" t="s">
+        <v>2811</v>
+      </c>
+      <c r="D95" s="9"/>
+      <c r="E95" s="11" t="s">
         <v>335</v>
       </c>
       <c r="F95" s="3" t="s">
@@ -3738,76 +3768,78 @@
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="14" t="s">
+      <c r="A96" s="8" t="s">
         <v>337</v>
       </c>
       <c r="B96" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C96" s="9" t="n">
+        <v>200</v>
+      </c>
+      <c r="D96" s="9" t="s">
         <v>338</v>
       </c>
-      <c r="C96" s="9" t="n">
-        <v>300</v>
-      </c>
-      <c r="D96" s="9" t="s">
+      <c r="E96" s="9" t="s">
         <v>339</v>
       </c>
-      <c r="E96" s="9" t="s">
+      <c r="F96" s="3" t="s">
         <v>340</v>
       </c>
-      <c r="F96" s="3" t="s">
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="14" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="8" t="s">
+      <c r="B97" s="9" t="s">
         <v>342</v>
-      </c>
-      <c r="B97" s="9" t="s">
-        <v>338</v>
       </c>
       <c r="C97" s="9" t="n">
         <v>300</v>
       </c>
       <c r="D97" s="9" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="E97" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="8" t="s">
+        <v>346</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="C98" s="9" t="n">
+        <v>300</v>
+      </c>
+      <c r="D98" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="F97" s="3" t="s">
-        <v>344</v>
-      </c>
-    </row>
-    <row r="98" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="8" t="s">
-        <v>345</v>
-      </c>
-      <c r="B98" s="9" t="s">
-        <v>346</v>
-      </c>
-      <c r="C98" s="9" t="n">
-        <v>5500</v>
-      </c>
-      <c r="D98" s="9"/>
       <c r="E98" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="G98" s="1" t="s">
-        <v>15</v>
+      <c r="F98" s="3" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="99" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="8" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C99" s="9" t="n">
-        <v>5600</v>
+        <v>5500</v>
       </c>
       <c r="D99" s="9"/>
       <c r="E99" s="9" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="G99" s="1" t="s">
         <v>15</v>
@@ -3815,17 +3847,15 @@
     </row>
     <row r="100" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="8" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="C100" s="9" t="n">
-        <v>101</v>
-      </c>
-      <c r="D100" s="9" t="s">
-        <v>353</v>
-      </c>
+        <v>5600</v>
+      </c>
+      <c r="D100" s="9"/>
       <c r="E100" s="9" t="s">
         <v>354</v>
       </c>
@@ -3841,7 +3871,7 @@
         <v>356</v>
       </c>
       <c r="C101" s="9" t="n">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D101" s="9" t="s">
         <v>357</v>
@@ -3853,86 +3883,88 @@
         <v>15</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="8" t="s">
         <v>359</v>
       </c>
       <c r="B102" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="C102" s="10"/>
-      <c r="D102" s="10"/>
-      <c r="E102" s="11" t="s">
+      <c r="C102" s="9" t="n">
+        <v>111</v>
+      </c>
+      <c r="D102" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="F102" s="3" t="s">
+      <c r="E102" s="9" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="103" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G102" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="8" t="s">
         <v>363</v>
       </c>
       <c r="B103" s="9" t="s">
         <v>364</v>
       </c>
-      <c r="C103" s="9" t="n">
+      <c r="C103" s="10"/>
+      <c r="D103" s="10"/>
+      <c r="E103" s="11" t="s">
+        <v>365</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="104" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="8" t="s">
+        <v>367</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="C104" s="9" t="n">
         <v>1000</v>
       </c>
-      <c r="D103" s="9" t="s">
-        <v>365</v>
-      </c>
-      <c r="E103" s="9" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="8" t="s">
-        <v>366</v>
-      </c>
-      <c r="B104" s="9" t="s">
-        <v>367</v>
-      </c>
-      <c r="C104" s="9" t="n">
-        <v>112</v>
-      </c>
       <c r="D104" s="9" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="E104" s="9" t="s">
-        <v>369</v>
-      </c>
-      <c r="F104" s="3" t="s">
-        <v>370</v>
+        <v>292</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="B105" s="9" t="s">
         <v>371</v>
       </c>
-      <c r="B105" s="9" t="s">
-        <v>84</v>
-      </c>
       <c r="C105" s="9" t="n">
-        <v>3100</v>
-      </c>
-      <c r="D105" s="9"/>
+        <v>112</v>
+      </c>
+      <c r="D105" s="9" t="s">
+        <v>372</v>
+      </c>
       <c r="E105" s="9" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="8" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>375</v>
+        <v>84</v>
       </c>
       <c r="C106" s="9" t="n">
-        <v>21</v>
+        <v>3100</v>
       </c>
       <c r="D106" s="9"/>
       <c r="E106" s="9" t="s">
@@ -3942,39 +3974,39 @@
         <v>377</v>
       </c>
     </row>
-    <row r="107" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="8" t="s">
         <v>378</v>
       </c>
       <c r="B107" s="9" t="s">
-        <v>212</v>
+        <v>379</v>
       </c>
       <c r="C107" s="9" t="n">
-        <v>122</v>
-      </c>
-      <c r="D107" s="9" t="s">
-        <v>379</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D107" s="9"/>
       <c r="E107" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="G107" s="1" t="s">
-        <v>15</v>
+      <c r="F107" s="3" t="s">
+        <v>381</v>
       </c>
     </row>
     <row r="108" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="8" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>382</v>
+        <v>212</v>
       </c>
       <c r="C108" s="9" t="n">
-        <v>1722</v>
-      </c>
-      <c r="D108" s="9"/>
+        <v>122</v>
+      </c>
+      <c r="D108" s="9" t="s">
+        <v>383</v>
+      </c>
       <c r="E108" s="9" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>15</v>
@@ -3982,36 +4014,38 @@
     </row>
     <row r="109" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="8" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C109" s="9" t="n">
-        <v>7100</v>
+        <v>1722</v>
       </c>
       <c r="D109" s="9"/>
       <c r="E109" s="9" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="110" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="8" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>388</v>
-      </c>
-      <c r="C110" s="10"/>
-      <c r="D110" s="10"/>
+        <v>389</v>
+      </c>
+      <c r="C110" s="9" t="n">
+        <v>7100</v>
+      </c>
+      <c r="D110" s="9"/>
       <c r="E110" s="9" t="s">
-        <v>389</v>
-      </c>
-      <c r="F110" s="3" t="s">
         <v>390</v>
+      </c>
+      <c r="G110" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4023,14 +4057,11 @@
       </c>
       <c r="C111" s="10"/>
       <c r="D111" s="10"/>
-      <c r="E111" s="11" t="s">
+      <c r="E111" s="9" t="s">
         <v>393</v>
       </c>
       <c r="F111" s="3" t="s">
         <v>394</v>
-      </c>
-      <c r="G111" s="1" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4053,7 +4084,7 @@
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="1" t="s">
+      <c r="A113" s="8" t="s">
         <v>399</v>
       </c>
       <c r="B113" s="9" t="s">
@@ -4072,37 +4103,38 @@
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="8" t="s">
+      <c r="A114" s="1" t="s">
         <v>403</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="C114" s="9" t="n">
-        <v>400</v>
-      </c>
-      <c r="D114" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="E114" s="9" t="s">
+      <c r="C114" s="10"/>
+      <c r="D114" s="10"/>
+      <c r="E114" s="11" t="s">
         <v>405</v>
       </c>
       <c r="F114" s="3" t="s">
         <v>406</v>
       </c>
+      <c r="G114" s="1" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="1" t="s">
+      <c r="A115" s="8" t="s">
         <v>407</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>408</v>
+        <v>241</v>
       </c>
       <c r="C115" s="9" t="n">
         <v>400</v>
       </c>
-      <c r="D115" s="9"/>
-      <c r="E115" s="8" t="s">
+      <c r="D115" s="9" t="s">
+        <v>408</v>
+      </c>
+      <c r="E115" s="9" t="s">
         <v>409</v>
       </c>
       <c r="F115" s="3" t="s">
@@ -4110,37 +4142,41 @@
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="8" t="s">
+      <c r="A116" s="1" t="s">
         <v>411</v>
       </c>
       <c r="B116" s="9" t="s">
         <v>412</v>
       </c>
-      <c r="C116" s="9" t="s">
+      <c r="C116" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="D116" s="9"/>
+      <c r="E116" s="8" t="s">
         <v>413</v>
       </c>
-      <c r="D116" s="9"/>
-      <c r="E116" s="9" t="s">
+      <c r="F116" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="F116" s="3" t="s">
+    </row>
+    <row r="117" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A117" s="1" t="s">
         <v>415</v>
       </c>
-    </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A117" s="8" t="s">
+      <c r="B117" s="2" t="s">
         <v>416</v>
       </c>
-      <c r="B117" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C117" s="10"/>
-      <c r="D117" s="10"/>
-      <c r="E117" s="9" t="s">
+      <c r="C117" s="2" t="n">
+        <v>2612</v>
+      </c>
+      <c r="D117" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="F117" s="3" t="s">
+      <c r="E117" s="15" t="s">
         <v>418</v>
+      </c>
+      <c r="G117" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4150,20 +4186,20 @@
       <c r="B118" s="9" t="s">
         <v>420</v>
       </c>
-      <c r="C118" s="9" t="n">
-        <v>7600</v>
+      <c r="C118" s="9" t="s">
+        <v>421</v>
       </c>
       <c r="D118" s="9"/>
-      <c r="E118" s="11" t="s">
-        <v>421</v>
+      <c r="E118" s="9" t="s">
+        <v>422</v>
       </c>
       <c r="F118" s="3" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B119" s="9" t="s">
         <v>137</v>
@@ -4171,68 +4207,70 @@
       <c r="C119" s="10"/>
       <c r="D119" s="10"/>
       <c r="E119" s="9" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="F119" s="3" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="8" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>140</v>
+        <v>428</v>
       </c>
       <c r="C120" s="9" t="n">
-        <v>6000</v>
+        <v>7600</v>
       </c>
       <c r="D120" s="9"/>
-      <c r="E120" s="9" t="s">
-        <v>427</v>
+      <c r="E120" s="11" t="s">
+        <v>429</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="8" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B121" s="9" t="s">
-        <v>195</v>
+        <v>137</v>
       </c>
       <c r="C121" s="10"/>
       <c r="D121" s="10"/>
       <c r="E121" s="9" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="F121" s="3" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="8" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="B122" s="9" t="s">
-        <v>433</v>
-      </c>
-      <c r="C122" s="10"/>
-      <c r="D122" s="10"/>
+        <v>140</v>
+      </c>
+      <c r="C122" s="9" t="n">
+        <v>6000</v>
+      </c>
+      <c r="D122" s="9"/>
       <c r="E122" s="9" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="8" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>437</v>
+        <v>195</v>
       </c>
       <c r="C123" s="10"/>
       <c r="D123" s="10"/>
@@ -4248,44 +4286,42 @@
         <v>440</v>
       </c>
       <c r="B124" s="9" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="C124" s="10"/>
       <c r="D124" s="10"/>
       <c r="E124" s="9" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="F124" s="3" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="8" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="B125" s="9" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C125" s="10"/>
       <c r="D125" s="10"/>
       <c r="E125" s="9" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F125" s="3" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="8" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>448</v>
-      </c>
-      <c r="C126" s="9" t="n">
-        <v>5800</v>
-      </c>
-      <c r="D126" s="9"/>
+        <v>445</v>
+      </c>
+      <c r="C126" s="10"/>
+      <c r="D126" s="10"/>
       <c r="E126" s="9" t="s">
         <v>449</v>
       </c>
@@ -4300,49 +4336,47 @@
       <c r="B127" s="9" t="s">
         <v>452</v>
       </c>
-      <c r="C127" s="9" t="n">
-        <v>7700</v>
-      </c>
-      <c r="D127" s="9" t="s">
+      <c r="C127" s="10"/>
+      <c r="D127" s="10"/>
+      <c r="E127" s="9" t="s">
         <v>453</v>
       </c>
-      <c r="E127" s="11" t="s">
+      <c r="F127" s="3" t="s">
         <v>454</v>
-      </c>
-      <c r="F127" s="3" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="B128" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="B128" s="9" t="s">
+      <c r="C128" s="9" t="n">
+        <v>5800</v>
+      </c>
+      <c r="D128" s="9"/>
+      <c r="E128" s="9" t="s">
         <v>457</v>
       </c>
-      <c r="C128" s="9" t="n">
-        <v>7800</v>
-      </c>
-      <c r="D128" s="9" t="s">
+      <c r="F128" s="3" t="s">
         <v>458</v>
-      </c>
-      <c r="E128" s="11" t="s">
-        <v>459</v>
-      </c>
-      <c r="F128" s="3" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="B129" s="9" t="s">
         <v>460</v>
       </c>
-      <c r="B129" s="9" t="s">
+      <c r="C129" s="9" t="n">
+        <v>7700</v>
+      </c>
+      <c r="D129" s="9" t="s">
         <v>461</v>
       </c>
-      <c r="C129" s="10"/>
-      <c r="D129" s="10"/>
-      <c r="E129" s="9" t="s">
+      <c r="E129" s="11" t="s">
         <v>462</v>
       </c>
       <c r="F129" s="3" t="s">
@@ -4354,19 +4388,19 @@
         <v>464</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="C130" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="D130" s="10" t="s">
         <v>465</v>
       </c>
-      <c r="E130" s="9" t="s">
+      <c r="C130" s="9" t="n">
+        <v>7800</v>
+      </c>
+      <c r="D130" s="9" t="s">
         <v>466</v>
       </c>
+      <c r="E130" s="11" t="s">
+        <v>467</v>
+      </c>
       <c r="F130" s="3" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4378,78 +4412,76 @@
       </c>
       <c r="C131" s="10"/>
       <c r="D131" s="10"/>
-      <c r="E131" s="11" t="s">
+      <c r="E131" s="9" t="s">
         <v>470</v>
       </c>
       <c r="F131" s="3" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="132" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="8" t="s">
         <v>472</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="C132" s="9" t="n">
-        <v>101</v>
-      </c>
-      <c r="D132" s="9"/>
+        <v>140</v>
+      </c>
+      <c r="C132" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="D132" s="10" t="s">
+        <v>473</v>
+      </c>
       <c r="E132" s="9" t="s">
-        <v>354</v>
-      </c>
-      <c r="G132" s="1" t="s">
-        <v>15</v>
+        <v>474</v>
+      </c>
+      <c r="F132" s="3" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="8" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>212</v>
+        <v>477</v>
       </c>
       <c r="C133" s="10"/>
       <c r="D133" s="10"/>
-      <c r="E133" s="9" t="s">
-        <v>474</v>
+      <c r="E133" s="11" t="s">
+        <v>478</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="134" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="8" t="s">
-        <v>476</v>
+        <v>480</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>215</v>
-      </c>
-      <c r="C134" s="10"/>
-      <c r="D134" s="10" t="s">
-        <v>477</v>
-      </c>
+        <v>356</v>
+      </c>
+      <c r="C134" s="9" t="n">
+        <v>101</v>
+      </c>
+      <c r="D134" s="9"/>
       <c r="E134" s="9" t="s">
-        <v>478</v>
-      </c>
-      <c r="F134" s="3" t="s">
-        <v>479</v>
+        <v>358</v>
+      </c>
+      <c r="G134" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="8" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="B135" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="C135" s="9" t="n">
-        <v>1400</v>
-      </c>
-      <c r="D135" s="9" t="s">
-        <v>481</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="C135" s="10"/>
+      <c r="D135" s="10"/>
       <c r="E135" s="9" t="s">
         <v>482</v>
       </c>
@@ -4458,17 +4490,15 @@
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="1" t="s">
+      <c r="A136" s="8" t="s">
         <v>484</v>
       </c>
       <c r="B136" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C136" s="10"/>
+      <c r="D136" s="10" t="s">
         <v>485</v>
-      </c>
-      <c r="C136" s="9" t="n">
-        <v>7400</v>
-      </c>
-      <c r="D136" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="E136" s="9" t="s">
         <v>486</v>
@@ -4482,51 +4512,51 @@
         <v>488</v>
       </c>
       <c r="B137" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="C137" s="9" t="n">
+        <v>1400</v>
+      </c>
+      <c r="D137" s="9" t="s">
         <v>489</v>
       </c>
-      <c r="C137" s="10"/>
-      <c r="D137" s="10" t="s">
+      <c r="E137" s="9" t="s">
         <v>490</v>
       </c>
-      <c r="E137" s="9" t="s">
+      <c r="F137" s="3" t="s">
         <v>491</v>
       </c>
-      <c r="F137" s="3" t="s">
+    </row>
+    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="s">
         <v>492</v>
       </c>
-    </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="8" t="s">
+      <c r="B138" s="9" t="s">
         <v>493</v>
       </c>
-      <c r="B138" s="9" t="s">
-        <v>437</v>
-      </c>
       <c r="C138" s="9" t="n">
-        <v>1700</v>
+        <v>7400</v>
       </c>
       <c r="D138" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E138" s="9" t="s">
         <v>494</v>
       </c>
-      <c r="E138" s="9" t="s">
+      <c r="F138" s="3" t="s">
         <v>495</v>
-      </c>
-      <c r="F138" s="3" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="B139" s="9" t="s">
         <v>497</v>
       </c>
-      <c r="B139" s="9" t="s">
+      <c r="C139" s="10"/>
+      <c r="D139" s="10" t="s">
         <v>498</v>
-      </c>
-      <c r="C139" s="9" t="n">
-        <v>1800</v>
-      </c>
-      <c r="D139" s="9" t="s">
-        <v>107</v>
       </c>
       <c r="E139" s="9" t="s">
         <v>499</v>
@@ -4535,411 +4565,415 @@
         <v>500</v>
       </c>
     </row>
-    <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="8" t="s">
         <v>501</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>215</v>
+        <v>445</v>
+      </c>
+      <c r="C140" s="9" t="n">
+        <v>1700</v>
+      </c>
+      <c r="D140" s="9" t="s">
+        <v>502</v>
       </c>
       <c r="E140" s="9" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="8" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="C141" s="10" t="s">
-        <v>505</v>
-      </c>
-      <c r="D141" s="10"/>
+        <v>506</v>
+      </c>
+      <c r="C141" s="9" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D141" s="9" t="s">
+        <v>107</v>
+      </c>
       <c r="E141" s="9" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="8" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>489</v>
-      </c>
-      <c r="C142" s="10"/>
-      <c r="D142" s="10"/>
+        <v>215</v>
+      </c>
       <c r="E142" s="9" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="F142" s="3" t="s">
-        <v>503</v>
+        <v>511</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="8" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>437</v>
-      </c>
-      <c r="C143" s="10"/>
+        <v>195</v>
+      </c>
+      <c r="C143" s="10" t="s">
+        <v>513</v>
+      </c>
       <c r="D143" s="10"/>
       <c r="E143" s="9" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="F143" s="3" t="s">
-        <v>503</v>
+        <v>511</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="8" t="s">
-        <v>511</v>
+        <v>515</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>512</v>
+        <v>497</v>
       </c>
       <c r="C144" s="10"/>
       <c r="D144" s="10"/>
       <c r="E144" s="9" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="F144" s="3" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="8" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>489</v>
+        <v>445</v>
       </c>
       <c r="C145" s="10"/>
       <c r="D145" s="10"/>
       <c r="E145" s="9" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="F145" s="3" t="s">
-        <v>517</v>
+        <v>511</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="8" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="B146" s="9" t="s">
-        <v>437</v>
+        <v>520</v>
       </c>
       <c r="C146" s="10"/>
       <c r="D146" s="10"/>
       <c r="E146" s="9" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="8" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="B147" s="9" t="s">
-        <v>195</v>
+        <v>497</v>
       </c>
       <c r="C147" s="10"/>
       <c r="D147" s="10"/>
       <c r="E147" s="9" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="F147" s="3" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="8" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>137</v>
+        <v>445</v>
       </c>
       <c r="C148" s="10"/>
       <c r="D148" s="10"/>
       <c r="E148" s="9" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="F148" s="3" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="8" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>140</v>
+        <v>195</v>
       </c>
       <c r="C149" s="10"/>
       <c r="D149" s="10"/>
       <c r="E149" s="9" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="8" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>215</v>
+        <v>137</v>
       </c>
       <c r="C150" s="10"/>
       <c r="D150" s="10"/>
       <c r="E150" s="9" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="8" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="B151" s="9" t="s">
-        <v>437</v>
+        <v>140</v>
       </c>
       <c r="C151" s="10"/>
       <c r="D151" s="10"/>
       <c r="E151" s="9" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="F151" s="3" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="8" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>137</v>
+        <v>215</v>
       </c>
       <c r="C152" s="10"/>
       <c r="D152" s="10"/>
       <c r="E152" s="9" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="F152" s="3" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="8" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>140</v>
+        <v>445</v>
       </c>
       <c r="C153" s="10"/>
       <c r="D153" s="10"/>
       <c r="E153" s="9" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="F153" s="3" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="8" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="B154" s="9" t="s">
-        <v>215</v>
+        <v>137</v>
       </c>
       <c r="C154" s="10"/>
       <c r="D154" s="10"/>
       <c r="E154" s="9" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="8" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="B155" s="9" t="s">
-        <v>195</v>
+        <v>140</v>
       </c>
       <c r="C155" s="10"/>
       <c r="D155" s="10"/>
       <c r="E155" s="9" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="F155" s="3" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="8" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>489</v>
+        <v>215</v>
       </c>
       <c r="C156" s="10"/>
       <c r="D156" s="10"/>
       <c r="E156" s="9" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="F156" s="3" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="8" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="B157" s="9" t="s">
-        <v>552</v>
-      </c>
-      <c r="C157" s="9" t="n">
-        <v>121</v>
-      </c>
-      <c r="D157" s="9"/>
-      <c r="E157" s="11" t="s">
-        <v>553</v>
+        <v>195</v>
+      </c>
+      <c r="C157" s="10"/>
+      <c r="D157" s="10"/>
+      <c r="E157" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>555</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="8" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="B158" s="9" t="s">
-        <v>137</v>
+        <v>497</v>
       </c>
       <c r="C158" s="10"/>
       <c r="D158" s="10"/>
       <c r="E158" s="9" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="F158" s="3" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="159" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="8" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="B159" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="C159" s="10"/>
-      <c r="D159" s="10"/>
-      <c r="E159" s="9" t="s">
-        <v>558</v>
-      </c>
-      <c r="F159" s="3" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>560</v>
+      </c>
+      <c r="C159" s="9" t="n">
+        <v>121</v>
+      </c>
+      <c r="D159" s="9"/>
+      <c r="E159" s="11" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="8" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B160" s="9" t="s">
-        <v>356</v>
-      </c>
-      <c r="C160" s="9" t="n">
-        <v>111</v>
-      </c>
-      <c r="D160" s="9"/>
+        <v>137</v>
+      </c>
+      <c r="C160" s="10"/>
+      <c r="D160" s="10"/>
       <c r="E160" s="9" t="s">
-        <v>358</v>
-      </c>
-      <c r="G160" s="1" t="s">
-        <v>15</v>
+        <v>563</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="8" t="s">
-        <v>561</v>
+        <v>565</v>
       </c>
       <c r="B161" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="C161" s="9" t="n">
-        <v>1711</v>
-      </c>
-      <c r="D161" s="9"/>
-      <c r="E161" s="11" t="s">
-        <v>562</v>
+        <v>195</v>
+      </c>
+      <c r="C161" s="10"/>
+      <c r="D161" s="10"/>
+      <c r="E161" s="9" t="s">
+        <v>566</v>
       </c>
       <c r="F161" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="G161" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A162" s="1" t="s">
-        <v>563</v>
+        <v>567</v>
+      </c>
+    </row>
+    <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A162" s="8" t="s">
+        <v>568</v>
       </c>
       <c r="B162" s="9" t="s">
-        <v>564</v>
+        <v>360</v>
       </c>
       <c r="C162" s="9" t="n">
-        <v>3300</v>
+        <v>111</v>
       </c>
       <c r="D162" s="9"/>
       <c r="E162" s="9" t="s">
-        <v>565</v>
-      </c>
-      <c r="F162" s="3" t="s">
-        <v>566</v>
+        <v>362</v>
+      </c>
+      <c r="G162" s="1" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="8" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>568</v>
+        <v>257</v>
       </c>
       <c r="C163" s="9" t="n">
-        <v>8000</v>
-      </c>
-      <c r="D163" s="9" t="s">
-        <v>569</v>
-      </c>
-      <c r="E163" s="9" t="s">
+        <v>1711</v>
+      </c>
+      <c r="D163" s="9"/>
+      <c r="E163" s="11" t="s">
         <v>570</v>
       </c>
       <c r="F163" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="G163" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="1" t="s">
         <v>571</v>
       </c>
-    </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="8" t="s">
+      <c r="B164" s="9" t="s">
         <v>572</v>
       </c>
-      <c r="B164" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C164" s="10"/>
-      <c r="D164" s="10"/>
+      <c r="C164" s="9" t="n">
+        <v>3300</v>
+      </c>
+      <c r="D164" s="9"/>
       <c r="E164" s="9" t="s">
         <v>573</v>
       </c>
@@ -4952,127 +4986,129 @@
         <v>575</v>
       </c>
       <c r="B165" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="C165" s="10"/>
-      <c r="D165" s="10"/>
+        <v>576</v>
+      </c>
+      <c r="C165" s="9" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D165" s="9" t="s">
+        <v>577</v>
+      </c>
       <c r="E165" s="9" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="F165" s="3" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="8" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="B166" s="9" t="s">
-        <v>212</v>
+        <v>137</v>
       </c>
       <c r="C166" s="10"/>
       <c r="D166" s="10"/>
       <c r="E166" s="9" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="F166" s="3" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="8" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="B167" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="C167" s="10"/>
+      <c r="D167" s="10"/>
+      <c r="E167" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="F167" s="3" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A168" s="8" t="s">
+        <v>586</v>
+      </c>
+      <c r="B168" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="C168" s="10"/>
+      <c r="D168" s="10"/>
+      <c r="E168" s="9" t="s">
+        <v>587</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="8" t="s">
+        <v>589</v>
+      </c>
+      <c r="B169" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="C167" s="9" t="n">
+      <c r="C169" s="9" t="n">
         <v>1500</v>
       </c>
-      <c r="D167" s="9" t="s">
-        <v>582</v>
-      </c>
-      <c r="E167" s="9" t="s">
-        <v>583</v>
-      </c>
-      <c r="F167" s="3" t="s">
+      <c r="D169" s="9" t="s">
+        <v>590</v>
+      </c>
+      <c r="E169" s="9" t="s">
+        <v>591</v>
+      </c>
+      <c r="F169" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="8" t="s">
-        <v>584</v>
-      </c>
-      <c r="B168" s="13" t="s">
-        <v>585</v>
-      </c>
-      <c r="C168" s="9" t="n">
+    <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="8" t="s">
+        <v>592</v>
+      </c>
+      <c r="B170" s="13" t="s">
+        <v>593</v>
+      </c>
+      <c r="C170" s="9" t="n">
         <v>2611</v>
       </c>
-      <c r="D168" s="9"/>
-      <c r="E168" s="9" t="s">
-        <v>586</v>
-      </c>
-    </row>
-    <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="8" t="s">
-        <v>587</v>
-      </c>
-      <c r="B169" s="9" t="s">
-        <v>588</v>
-      </c>
-      <c r="C169" s="9" t="n">
+      <c r="D170" s="9"/>
+      <c r="E170" s="9" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="8" t="s">
+        <v>595</v>
+      </c>
+      <c r="B171" s="9" t="s">
+        <v>596</v>
+      </c>
+      <c r="C171" s="9" t="n">
         <v>2711</v>
       </c>
-      <c r="D169" s="9"/>
-      <c r="E169" s="9" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="8" t="s">
-        <v>590</v>
-      </c>
-      <c r="B170" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="C170" s="10"/>
-      <c r="D170" s="10"/>
-      <c r="E170" s="9" t="s">
-        <v>591</v>
-      </c>
-      <c r="F170" s="3" t="s">
-        <v>592</v>
-      </c>
-    </row>
-    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="8" t="s">
-        <v>593</v>
-      </c>
-      <c r="B171" s="9" t="s">
-        <v>594</v>
-      </c>
-      <c r="C171" s="10"/>
-      <c r="D171" s="10"/>
-      <c r="E171" s="11" t="s">
-        <v>595</v>
-      </c>
-      <c r="F171" s="3" t="s">
-        <v>596</v>
+      <c r="D171" s="9"/>
+      <c r="E171" s="9" t="s">
+        <v>597</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="8" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>598</v>
-      </c>
-      <c r="C172" s="9" t="n">
-        <v>3721</v>
-      </c>
-      <c r="D172" s="9"/>
-      <c r="E172" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C172" s="10"/>
+      <c r="D172" s="10"/>
+      <c r="E172" s="9" t="s">
         <v>599</v>
       </c>
       <c r="F172" s="3" t="s">
@@ -5084,146 +5120,180 @@
         <v>601</v>
       </c>
       <c r="B173" s="9" t="s">
-        <v>437</v>
-      </c>
-      <c r="C173" s="9" t="n">
-        <v>6100</v>
-      </c>
-      <c r="D173" s="9"/>
-      <c r="E173" s="9" t="s">
         <v>602</v>
       </c>
+      <c r="C173" s="10"/>
+      <c r="D173" s="10"/>
+      <c r="E173" s="11" t="s">
+        <v>603</v>
+      </c>
       <c r="F173" s="3" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="8" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>605</v>
-      </c>
-      <c r="C174" s="10" t="n">
+        <v>606</v>
+      </c>
+      <c r="C174" s="9" t="n">
+        <v>3721</v>
+      </c>
+      <c r="D174" s="9"/>
+      <c r="E174" s="11" t="s">
+        <v>607</v>
+      </c>
+      <c r="F174" s="3" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="8" t="s">
+        <v>609</v>
+      </c>
+      <c r="B175" s="9" t="s">
+        <v>445</v>
+      </c>
+      <c r="C175" s="9" t="n">
+        <v>6100</v>
+      </c>
+      <c r="D175" s="9"/>
+      <c r="E175" s="9" t="s">
+        <v>610</v>
+      </c>
+      <c r="F175" s="3" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A176" s="8" t="s">
+        <v>612</v>
+      </c>
+      <c r="B176" s="9" t="s">
+        <v>613</v>
+      </c>
+      <c r="C176" s="10" t="n">
         <v>8400</v>
       </c>
-      <c r="D174" s="10"/>
-      <c r="E174" s="9" t="s">
-        <v>606</v>
-      </c>
-      <c r="F174" s="3" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="8" t="s">
-        <v>608</v>
-      </c>
-      <c r="B175" s="9" t="s">
+      <c r="D176" s="10"/>
+      <c r="E176" s="9" t="s">
+        <v>614</v>
+      </c>
+      <c r="F176" s="3" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="8" t="s">
+        <v>616</v>
+      </c>
+      <c r="B177" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E175" s="9" t="s">
-        <v>609</v>
-      </c>
-      <c r="F175" s="3" t="s">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A176" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="B176" s="9" t="s">
+      <c r="E177" s="9" t="s">
+        <v>617</v>
+      </c>
+      <c r="F177" s="3" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A178" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="B178" s="9" t="s">
         <v>241</v>
       </c>
-      <c r="C176" s="9" t="n">
+      <c r="C178" s="9" t="n">
         <v>400</v>
       </c>
-      <c r="D176" s="9"/>
-      <c r="E176" s="9" t="s">
-        <v>612</v>
-      </c>
-      <c r="F176" s="3" t="s">
-        <v>613</v>
-      </c>
-    </row>
-    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="1" t="s">
-        <v>614</v>
-      </c>
-      <c r="B177" s="9" t="s">
-        <v>408</v>
-      </c>
-      <c r="C177" s="9" t="n">
+      <c r="D178" s="9"/>
+      <c r="E178" s="9" t="s">
+        <v>620</v>
+      </c>
+      <c r="F178" s="3" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="1" t="s">
+        <v>622</v>
+      </c>
+      <c r="B179" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="C179" s="9" t="n">
         <v>400</v>
       </c>
-      <c r="D177" s="9"/>
-      <c r="E177" s="11" t="s">
-        <v>615</v>
-      </c>
-      <c r="F177" s="3" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="8" t="s">
-        <v>616</v>
-      </c>
-      <c r="B178" s="9" t="s">
-        <v>617</v>
-      </c>
-      <c r="C178" s="10"/>
-      <c r="D178" s="10"/>
-      <c r="E178" s="11" t="s">
-        <v>618</v>
-      </c>
-      <c r="F178" s="3" t="s">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="8" t="s">
-        <v>620</v>
-      </c>
-      <c r="B179" s="9" t="s">
+      <c r="D179" s="9"/>
+      <c r="E179" s="11" t="s">
+        <v>623</v>
+      </c>
+      <c r="F179" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A180" s="8" t="s">
+        <v>624</v>
+      </c>
+      <c r="B180" s="9" t="s">
+        <v>625</v>
+      </c>
+      <c r="C180" s="10"/>
+      <c r="D180" s="10"/>
+      <c r="E180" s="11" t="s">
+        <v>626</v>
+      </c>
+      <c r="F180" s="3" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="8" t="s">
+        <v>628</v>
+      </c>
+      <c r="B181" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C179" s="10"/>
-      <c r="D179" s="10"/>
-      <c r="E179" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F179" s="3" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A180" s="8" t="s">
-        <v>623</v>
-      </c>
-      <c r="B180" s="9" t="s">
-        <v>375</v>
-      </c>
-      <c r="C180" s="9" t="n">
+      <c r="C181" s="10"/>
+      <c r="D181" s="10"/>
+      <c r="E181" s="9" t="s">
+        <v>629</v>
+      </c>
+      <c r="F181" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="8" t="s">
+        <v>631</v>
+      </c>
+      <c r="B182" s="9" t="s">
+        <v>379</v>
+      </c>
+      <c r="C182" s="9" t="n">
         <v>21</v>
       </c>
-      <c r="D180" s="9"/>
-      <c r="E180" s="9" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="B181" s="9" t="s">
+      <c r="D182" s="9"/>
+      <c r="E182" s="9" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="B183" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="E181" s="9" t="s">
-        <v>626</v>
-      </c>
-      <c r="F181" s="3" t="s">
-        <v>627</v>
+      <c r="E183" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="F183" s="3" t="s">
+        <v>635</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renamed xAuth to Minecraft(xAuth)
</commit_message>
<xml_diff>
--- a/hashinfo.xlsx
+++ b/hashinfo.xlsx
@@ -1034,6 +1034,18 @@
     <t>http://dev.bukkit.org/bukkit-plugins/authme-reloaded/</t>
   </si>
   <si>
+    <t>Minecraft(xAuth)</t>
+  </si>
+  <si>
+    <t>^[a-f0-9]{140}$/i</t>
+  </si>
+  <si>
+    <t>cb5ef15b400cef07addb37e00e2cdd6d1b508a2a26f0befcb0f9d8fd03c1d67be1690eba2287c4f76a590f2feae654ce5aee9943a23babb8e56381fe3214a48ad8754a1fd9eb</t>
+  </si>
+  <si>
+    <t>https://github.com/CypherX/xAuth/wiki/Password-Hashing</t>
+  </si>
+  <si>
     <t>MSSQL(2000)</t>
   </si>
   <si>
@@ -1959,18 +1971,6 @@
   </si>
   <si>
     <t>$H$91234567894GGuEJpikxPnFVUioh9e.</t>
-  </si>
-  <si>
-    <t>xAuth</t>
-  </si>
-  <si>
-    <t>^[a-f0-9]{140}$/i</t>
-  </si>
-  <si>
-    <t>cb5ef15b400cef07addb37e00e2cdd6d1b508a2a26f0befcb0f9d8fd03c1d67be1690eba2287c4f76a590f2feae654ce5aee9943a23babb8e56381fe3214a48ad8754a1fd9eb</t>
-  </si>
-  <si>
-    <t>https://github.com/CypherX/xAuth/wiki/Password-Hashing</t>
   </si>
   <si>
     <t>XOR-32</t>
@@ -2171,8 +2171,8 @@
   </sheetPr>
   <dimension ref="A1:G187"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A91" activeCellId="0" sqref="A91"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A83" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B101" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2252,7 +2252,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
@@ -2267,7 +2267,6 @@
       <c r="F4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
@@ -2353,7 +2352,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
         <v>32</v>
       </c>
@@ -2370,9 +2369,8 @@
       <c r="F9" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G9" s="0"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="10" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
         <v>36</v>
       </c>
@@ -2387,9 +2385,8 @@
       <c r="F10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="G10" s="0"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="11" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
         <v>40</v>
       </c>
@@ -2408,9 +2405,8 @@
       <c r="F11" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="12" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="11" t="s">
         <v>45</v>
       </c>
@@ -2427,9 +2423,8 @@
       <c r="F12" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="0"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="13" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
         <v>50</v>
       </c>
@@ -2444,9 +2439,8 @@
       <c r="F13" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="0"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="14" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
         <v>54</v>
       </c>
@@ -2463,9 +2457,8 @@
       <c r="F14" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="G14" s="0"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="15" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
         <v>58</v>
       </c>
@@ -2479,12 +2472,11 @@
       <c r="E15" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="0"/>
       <c r="G15" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
         <v>62</v>
       </c>
@@ -2498,12 +2490,11 @@
       <c r="E16" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F16" s="0"/>
       <c r="G16" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
         <v>65</v>
       </c>
@@ -2522,9 +2513,8 @@
       <c r="F17" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="G17" s="0"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="18" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
         <v>70</v>
       </c>
@@ -2541,9 +2531,8 @@
       <c r="F18" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="G18" s="0"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="19" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
         <v>74</v>
       </c>
@@ -2555,12 +2544,11 @@
       <c r="E19" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F19" s="0"/>
       <c r="G19" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
         <v>77</v>
       </c>
@@ -2575,9 +2563,8 @@
       <c r="F20" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G20" s="0"/>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="21" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
         <v>81</v>
       </c>
@@ -2592,9 +2579,8 @@
       <c r="F21" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="G21" s="0"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="22" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>84</v>
       </c>
@@ -2606,12 +2592,11 @@
       <c r="E22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F22" s="0"/>
       <c r="G22" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="8" t="s">
         <v>87</v>
       </c>
@@ -2626,9 +2611,8 @@
       <c r="F23" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="G23" s="0"/>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="24" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
         <v>90</v>
       </c>
@@ -2643,9 +2627,8 @@
       <c r="F24" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="G24" s="0"/>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="25" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="8" t="s">
         <v>93</v>
       </c>
@@ -2660,9 +2643,8 @@
       <c r="F25" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="G25" s="0"/>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="26" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="8" t="s">
         <v>97</v>
       </c>
@@ -2677,9 +2659,8 @@
       <c r="F26" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="G26" s="0"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="27" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="8" t="s">
         <v>101</v>
       </c>
@@ -2694,9 +2675,8 @@
       <c r="F27" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="G27" s="0"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="28" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="8" t="s">
         <v>105</v>
       </c>
@@ -2711,9 +2691,8 @@
       <c r="F28" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="G28" s="0"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="29" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="8" t="s">
         <v>109</v>
       </c>
@@ -2728,9 +2707,8 @@
       <c r="F29" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="G29" s="0"/>
-    </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="30" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="8" t="s">
         <v>112</v>
       </c>
@@ -2747,9 +2725,8 @@
       <c r="F30" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="G30" s="0"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="31" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="12" t="s">
         <v>115</v>
       </c>
@@ -2768,9 +2745,8 @@
       <c r="F31" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="G31" s="0"/>
-    </row>
-    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="32" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>120</v>
       </c>
@@ -2787,9 +2763,8 @@
       <c r="F32" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="G32" s="0"/>
-    </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="33" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>124</v>
       </c>
@@ -2804,9 +2779,8 @@
       <c r="F33" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="G33" s="0"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="34" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>128</v>
       </c>
@@ -2821,9 +2795,8 @@
       <c r="F34" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="G34" s="0"/>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="35" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>132</v>
       </c>
@@ -2840,9 +2813,8 @@
       <c r="F35" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="G35" s="0"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="36" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="8" t="s">
         <v>136</v>
       </c>
@@ -2861,9 +2833,8 @@
       <c r="F36" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="G36" s="0"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="37" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
         <v>141</v>
       </c>
@@ -2882,9 +2853,8 @@
       <c r="F37" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="G37" s="0"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="38" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>146</v>
       </c>
@@ -2898,12 +2868,11 @@
       <c r="E38" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="F38" s="0"/>
       <c r="G38" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>149</v>
       </c>
@@ -2917,12 +2886,11 @@
       <c r="E39" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="F39" s="0"/>
       <c r="G39" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
         <v>152</v>
       </c>
@@ -2939,9 +2907,8 @@
       <c r="F40" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="G40" s="0"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="41" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
         <v>156</v>
       </c>
@@ -2958,9 +2925,8 @@
       <c r="F41" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="G41" s="0"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="42" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="s">
         <v>161</v>
       </c>
@@ -2975,9 +2941,8 @@
       <c r="F42" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="G42" s="0"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="43" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
         <v>164</v>
       </c>
@@ -2991,12 +2956,11 @@
       <c r="E43" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="F43" s="0"/>
       <c r="G43" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8" t="s">
         <v>167</v>
       </c>
@@ -3010,12 +2974,11 @@
       <c r="E44" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="F44" s="0"/>
       <c r="G44" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="s">
         <v>170</v>
       </c>
@@ -3029,12 +2992,11 @@
       <c r="E45" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="F45" s="0"/>
       <c r="G45" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>173</v>
       </c>
@@ -3049,9 +3011,8 @@
       <c r="F46" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="G46" s="0"/>
-    </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="47" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
         <v>177</v>
       </c>
@@ -3066,9 +3027,8 @@
       <c r="F47" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="G47" s="0"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="48" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="s">
         <v>180</v>
       </c>
@@ -3083,9 +3043,8 @@
       <c r="F48" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="G48" s="0"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="49" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="8" t="s">
         <v>183</v>
       </c>
@@ -3100,9 +3059,8 @@
       <c r="F49" s="9" t="s">
         <v>185</v>
       </c>
-      <c r="G49" s="0"/>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="50" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="8" t="s">
         <v>186</v>
       </c>
@@ -3117,9 +3075,8 @@
       <c r="F50" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="G50" s="0"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="51" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="8" t="s">
         <v>189</v>
       </c>
@@ -3134,9 +3091,8 @@
       <c r="F51" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="G51" s="0"/>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="52" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="8" t="s">
         <v>192</v>
       </c>
@@ -3150,12 +3106,11 @@
       <c r="E52" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="F52" s="0"/>
       <c r="G52" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="8" t="s">
         <v>195</v>
       </c>
@@ -3171,12 +3126,11 @@
       <c r="E53" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="F53" s="0"/>
       <c r="G53" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="8" t="s">
         <v>198</v>
       </c>
@@ -3191,9 +3145,8 @@
       <c r="F54" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="G54" s="0"/>
-    </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="55" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="8" t="s">
         <v>201</v>
       </c>
@@ -3208,9 +3161,8 @@
       <c r="F55" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="G55" s="0"/>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="56" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="8" t="s">
         <v>204</v>
       </c>
@@ -3227,9 +3179,8 @@
       <c r="F56" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="G56" s="0"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="57" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="8" t="s">
         <v>208</v>
       </c>
@@ -3246,9 +3197,8 @@
       <c r="F57" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="G57" s="0"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="58" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="8" t="s">
         <v>212</v>
       </c>
@@ -3265,9 +3215,8 @@
       <c r="F58" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="G58" s="0"/>
-    </row>
-    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="59" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="8" t="s">
         <v>215</v>
       </c>
@@ -3282,9 +3231,8 @@
       <c r="F59" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="G59" s="0"/>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="60" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="8" t="s">
         <v>218</v>
       </c>
@@ -3299,9 +3247,8 @@
       <c r="F60" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="G60" s="0"/>
-    </row>
-    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="61" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="8" t="s">
         <v>221</v>
       </c>
@@ -3316,9 +3263,8 @@
       <c r="F61" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="G61" s="0"/>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="62" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="8" t="s">
         <v>223</v>
       </c>
@@ -3333,9 +3279,8 @@
       <c r="F62" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="G62" s="0"/>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="63" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="8" t="s">
         <v>226</v>
       </c>
@@ -3350,9 +3295,8 @@
       <c r="F63" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="G63" s="0"/>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="64" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="8" t="s">
         <v>229</v>
       </c>
@@ -3367,9 +3311,8 @@
       <c r="F64" s="9" t="s">
         <v>220</v>
       </c>
-      <c r="G64" s="0"/>
-    </row>
-    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="65" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
         <v>231</v>
       </c>
@@ -3388,7 +3331,6 @@
       <c r="F65" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="G65" s="0"/>
     </row>
     <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="13" t="s">
@@ -3432,7 +3374,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="68" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="12" t="s">
         <v>243</v>
       </c>
@@ -3446,12 +3388,11 @@
       <c r="E68" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="F68" s="0"/>
       <c r="G68" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
         <v>246</v>
       </c>
@@ -3465,12 +3406,11 @@
       <c r="E69" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="F69" s="0"/>
       <c r="G69" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="8" t="s">
         <v>249</v>
       </c>
@@ -3487,9 +3427,8 @@
       <c r="F70" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="G70" s="0"/>
-    </row>
-    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="71" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="8" t="s">
         <v>253</v>
       </c>
@@ -3501,12 +3440,11 @@
       <c r="E71" s="9" t="s">
         <v>254</v>
       </c>
-      <c r="F71" s="0"/>
       <c r="G71" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="8" t="s">
         <v>255</v>
       </c>
@@ -3523,9 +3461,8 @@
       <c r="F72" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="G72" s="0"/>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="73" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="8" t="s">
         <v>259</v>
       </c>
@@ -3542,9 +3479,8 @@
       <c r="F73" s="9" t="s">
         <v>263</v>
       </c>
-      <c r="G73" s="0"/>
-    </row>
-    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="74" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="8" t="s">
         <v>264</v>
       </c>
@@ -3563,7 +3499,6 @@
       <c r="F74" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="G74" s="0"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="8" t="s">
@@ -3586,7 +3521,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="76" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="8" t="s">
         <v>273</v>
       </c>
@@ -3603,7 +3538,6 @@
       <c r="F76" s="9" t="s">
         <v>276</v>
       </c>
-      <c r="G76" s="0"/>
     </row>
     <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="8" t="s">
@@ -3626,7 +3560,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="8" t="s">
         <v>281</v>
       </c>
@@ -3641,9 +3575,8 @@
       <c r="F78" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="G78" s="0"/>
-    </row>
-    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="79" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="8" t="s">
         <v>285</v>
       </c>
@@ -3660,9 +3593,8 @@
       <c r="F79" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="G79" s="0"/>
-    </row>
-    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="80" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="8" t="s">
         <v>288</v>
       </c>
@@ -3681,9 +3613,8 @@
       <c r="F80" s="9" t="s">
         <v>291</v>
       </c>
-      <c r="G80" s="0"/>
-    </row>
-    <row r="81" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="81" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="8" t="s">
         <v>292</v>
       </c>
@@ -3699,12 +3630,11 @@
       <c r="E81" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="F81" s="0"/>
       <c r="G81" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="8" t="s">
         <v>296</v>
       </c>
@@ -3720,12 +3650,11 @@
       <c r="E82" s="9" t="s">
         <v>300</v>
       </c>
-      <c r="F82" s="0"/>
       <c r="G82" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="8" t="s">
         <v>301</v>
       </c>
@@ -3740,9 +3669,8 @@
       <c r="F83" s="9" t="s">
         <v>303</v>
       </c>
-      <c r="G83" s="0"/>
-    </row>
-    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="84" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="1" t="s">
         <v>304</v>
       </c>
@@ -3757,9 +3685,8 @@
       <c r="F84" s="9" t="s">
         <v>306</v>
       </c>
-      <c r="G84" s="0"/>
-    </row>
-    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="85" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="8" t="s">
         <v>307</v>
       </c>
@@ -3774,9 +3701,8 @@
       <c r="F85" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="G85" s="0"/>
-    </row>
-    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="86" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="8" t="s">
         <v>310</v>
       </c>
@@ -3795,9 +3721,8 @@
       <c r="F86" s="9" t="s">
         <v>313</v>
       </c>
-      <c r="G86" s="0"/>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="87" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="8" t="s">
         <v>314</v>
       </c>
@@ -3816,9 +3741,8 @@
       <c r="F87" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="G87" s="0"/>
-    </row>
-    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="88" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="8" t="s">
         <v>319</v>
       </c>
@@ -3835,9 +3759,8 @@
       <c r="F88" s="9" t="s">
         <v>321</v>
       </c>
-      <c r="G88" s="0"/>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="89" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="8" t="s">
         <v>322</v>
       </c>
@@ -3854,9 +3777,8 @@
       <c r="F89" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="G89" s="0"/>
-    </row>
-    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="90" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="8" t="s">
         <v>324</v>
       </c>
@@ -3873,9 +3795,8 @@
       <c r="F90" s="9" t="s">
         <v>252</v>
       </c>
-      <c r="G90" s="0"/>
-    </row>
-    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="91" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="8" t="s">
         <v>325</v>
       </c>
@@ -3894,9 +3815,8 @@
       <c r="F91" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="G91" s="0"/>
-    </row>
-    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="92" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="8" t="s">
         <v>331</v>
       </c>
@@ -3911,9 +3831,8 @@
       <c r="F92" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="G92" s="0"/>
-    </row>
-    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="93" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="8" t="s">
         <v>335</v>
       </c>
@@ -3928,247 +3847,229 @@
       <c r="F93" s="9" t="s">
         <v>338</v>
       </c>
-      <c r="G93" s="0"/>
-    </row>
-    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="94" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="8" t="s">
         <v>339</v>
       </c>
       <c r="B94" s="9" t="s">
         <v>340</v>
       </c>
-      <c r="C94" s="9" t="n">
+      <c r="C94" s="10"/>
+      <c r="D94" s="10"/>
+      <c r="E94" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="F94" s="9" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="95" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="8" t="s">
+        <v>343</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="C95" s="9" t="n">
         <v>131</v>
       </c>
-      <c r="D94" s="9" t="s">
-        <v>341</v>
-      </c>
-      <c r="E94" s="9" t="s">
-        <v>342</v>
-      </c>
-      <c r="F94" s="9" t="s">
-        <v>343</v>
-      </c>
-      <c r="G94" s="0"/>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="8" t="s">
-        <v>344</v>
-      </c>
-      <c r="B95" s="9" t="s">
+      <c r="D95" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="C95" s="9" t="n">
+      <c r="E95" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="F95" s="9" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="96" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="C96" s="9" t="n">
         <v>132</v>
       </c>
-      <c r="D95" s="9" t="s">
-        <v>346</v>
-      </c>
-      <c r="E95" s="9" t="s">
-        <v>347</v>
-      </c>
-      <c r="F95" s="9" t="s">
-        <v>348</v>
-      </c>
-      <c r="G95" s="0"/>
-    </row>
-    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="8" t="s">
+      <c r="D96" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="F96" s="9" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="97" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="B97" s="9" t="s">
         <v>349</v>
       </c>
-      <c r="B96" s="9" t="s">
-        <v>345</v>
-      </c>
-      <c r="C96" s="10" t="n">
+      <c r="C97" s="10" t="n">
         <v>132</v>
       </c>
-      <c r="D96" s="10"/>
-      <c r="E96" s="0"/>
-      <c r="F96" s="0"/>
-      <c r="G96" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="8" t="s">
-        <v>350</v>
-      </c>
-      <c r="B97" s="9" t="s">
-        <v>351</v>
-      </c>
-      <c r="C97" s="9" t="n">
-        <v>1731</v>
-      </c>
-      <c r="D97" s="9"/>
-      <c r="E97" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="F97" s="0"/>
+      <c r="D97" s="10"/>
       <c r="G97" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="8" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="C98" s="9" t="n">
         <v>1731</v>
       </c>
       <c r="D98" s="9"/>
-      <c r="E98" s="0"/>
-      <c r="F98" s="9" t="s">
-        <v>354</v>
+      <c r="E98" s="9" t="s">
+        <v>356</v>
       </c>
       <c r="G98" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="99" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="B99" s="9" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="B99" s="9" t="s">
-        <v>357</v>
-      </c>
       <c r="C99" s="9" t="n">
-        <v>2811</v>
+        <v>1731</v>
       </c>
       <c r="D99" s="9"/>
-      <c r="E99" s="9" t="s">
+      <c r="F99" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="F99" s="9" t="s">
+      <c r="G99" s="3" t="s">
         <v>359</v>
       </c>
-      <c r="G99" s="0"/>
-    </row>
-    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="100" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="8" t="s">
         <v>360</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>94</v>
+        <v>361</v>
       </c>
       <c r="C100" s="9" t="n">
-        <v>200</v>
-      </c>
-      <c r="D100" s="9" t="s">
-        <v>361</v>
-      </c>
+        <v>2811</v>
+      </c>
+      <c r="D100" s="9"/>
       <c r="E100" s="9" t="s">
         <v>362</v>
       </c>
       <c r="F100" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="G100" s="0"/>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="12" t="s">
+    </row>
+    <row r="101" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="8" t="s">
         <v>364</v>
       </c>
       <c r="B101" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C101" s="9" t="n">
+        <v>200</v>
+      </c>
+      <c r="D101" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="C101" s="9" t="n">
-        <v>300</v>
-      </c>
-      <c r="D101" s="9" t="s">
+      <c r="E101" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="E101" s="9" t="s">
+      <c r="F101" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="F101" s="9" t="s">
+    </row>
+    <row r="102" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="12" t="s">
         <v>368</v>
       </c>
-      <c r="G101" s="0"/>
-    </row>
-    <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="8" t="s">
+      <c r="B102" s="9" t="s">
         <v>369</v>
-      </c>
-      <c r="B102" s="9" t="s">
-        <v>365</v>
       </c>
       <c r="C102" s="9" t="n">
         <v>300</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="E102" s="9" t="s">
+        <v>371</v>
+      </c>
+      <c r="F102" s="9" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="103" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="8" t="s">
+        <v>373</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="C103" s="9" t="n">
+        <v>300</v>
+      </c>
+      <c r="D103" s="9" t="s">
         <v>370</v>
       </c>
-      <c r="F102" s="9" t="s">
-        <v>371</v>
-      </c>
-      <c r="G102" s="0"/>
-    </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="8" t="s">
-        <v>372</v>
-      </c>
-      <c r="B103" s="9" t="s">
-        <v>373</v>
-      </c>
-      <c r="C103" s="9" t="n">
-        <v>5500</v>
-      </c>
-      <c r="D103" s="9"/>
       <c r="E103" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="F103" s="0"/>
-      <c r="G103" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F103" s="9" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="104" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="8" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C104" s="9" t="n">
-        <v>5600</v>
+        <v>5500</v>
       </c>
       <c r="D104" s="9"/>
       <c r="E104" s="9" t="s">
-        <v>377</v>
-      </c>
-      <c r="F104" s="0"/>
+        <v>378</v>
+      </c>
       <c r="G104" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="105" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="8" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="C105" s="9" t="n">
-        <v>101</v>
-      </c>
-      <c r="D105" s="9" t="s">
-        <v>380</v>
-      </c>
+        <v>5600</v>
+      </c>
+      <c r="D105" s="9"/>
       <c r="E105" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="F105" s="0"/>
       <c r="G105" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="106" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="8" t="s">
         <v>382</v>
       </c>
@@ -4176,7 +4077,7 @@
         <v>383</v>
       </c>
       <c r="C106" s="9" t="n">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D106" s="9" t="s">
         <v>384</v>
@@ -4184,98 +4085,95 @@
       <c r="E106" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="F106" s="0"/>
       <c r="G106" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="107" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="8" t="s">
         <v>386</v>
       </c>
       <c r="B107" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
+      <c r="C107" s="9" t="n">
+        <v>111</v>
+      </c>
+      <c r="D107" s="9" t="s">
+        <v>388</v>
+      </c>
       <c r="E107" s="9" t="s">
-        <v>388</v>
-      </c>
-      <c r="F107" s="9" t="s">
         <v>389</v>
       </c>
-      <c r="G107" s="0"/>
-    </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G107" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="108" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="8" t="s">
         <v>390</v>
       </c>
       <c r="B108" s="9" t="s">
         <v>391</v>
       </c>
-      <c r="C108" s="9" t="n">
+      <c r="C108" s="10"/>
+      <c r="D108" s="10"/>
+      <c r="E108" s="9" t="s">
+        <v>392</v>
+      </c>
+      <c r="F108" s="9" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="109" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>395</v>
+      </c>
+      <c r="C109" s="9" t="n">
         <v>1000</v>
       </c>
-      <c r="D108" s="9" t="s">
-        <v>392</v>
-      </c>
-      <c r="E108" s="9" t="s">
+      <c r="D109" s="9" t="s">
+        <v>396</v>
+      </c>
+      <c r="E109" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="F108" s="0"/>
-      <c r="G108" s="3" t="s">
+      <c r="G109" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="8" t="s">
-        <v>393</v>
-      </c>
-      <c r="B109" s="9" t="s">
-        <v>394</v>
-      </c>
-      <c r="C109" s="9" t="n">
+    <row r="110" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="8" t="s">
+        <v>397</v>
+      </c>
+      <c r="B110" s="9" t="s">
+        <v>398</v>
+      </c>
+      <c r="C110" s="9" t="n">
         <v>112</v>
       </c>
-      <c r="D109" s="9" t="s">
-        <v>395</v>
-      </c>
-      <c r="E109" s="9" t="s">
-        <v>396</v>
-      </c>
-      <c r="F109" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="G109" s="0"/>
-    </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="8" t="s">
-        <v>398</v>
-      </c>
-      <c r="B110" s="9" t="s">
+      <c r="D110" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="E110" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="F110" s="9" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="111" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="B111" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C110" s="9" t="n">
+      <c r="C111" s="9" t="n">
         <v>3100</v>
-      </c>
-      <c r="D110" s="9"/>
-      <c r="E110" s="9" t="s">
-        <v>399</v>
-      </c>
-      <c r="F110" s="9" t="s">
-        <v>400</v>
-      </c>
-      <c r="G110" s="0"/>
-    </row>
-    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="B111" s="9" t="s">
-        <v>402</v>
-      </c>
-      <c r="C111" s="9" t="n">
-        <v>21</v>
       </c>
       <c r="D111" s="9"/>
       <c r="E111" s="9" t="s">
@@ -4284,85 +4182,82 @@
       <c r="F111" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="G111" s="0"/>
-    </row>
-    <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="112" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="8" t="s">
         <v>405</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>224</v>
+        <v>406</v>
       </c>
       <c r="C112" s="9" t="n">
-        <v>122</v>
-      </c>
-      <c r="D112" s="9" t="s">
-        <v>406</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D112" s="9"/>
       <c r="E112" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="F112" s="0"/>
-      <c r="G112" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F112" s="9" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="8" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>409</v>
+        <v>224</v>
       </c>
       <c r="C113" s="9" t="n">
-        <v>1722</v>
-      </c>
-      <c r="D113" s="9"/>
+        <v>122</v>
+      </c>
+      <c r="D113" s="9" t="s">
+        <v>410</v>
+      </c>
       <c r="E113" s="9" t="s">
-        <v>410</v>
-      </c>
-      <c r="F113" s="0"/>
+        <v>411</v>
+      </c>
       <c r="G113" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="8" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C114" s="9" t="n">
-        <v>7100</v>
+        <v>1722</v>
       </c>
       <c r="D114" s="9"/>
       <c r="E114" s="9" t="s">
-        <v>413</v>
-      </c>
-      <c r="F114" s="0"/>
+        <v>414</v>
+      </c>
       <c r="G114" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="8" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>415</v>
-      </c>
-      <c r="C115" s="10"/>
-      <c r="D115" s="10"/>
+        <v>416</v>
+      </c>
+      <c r="C115" s="9" t="n">
+        <v>7100</v>
+      </c>
+      <c r="D115" s="9"/>
       <c r="E115" s="9" t="s">
-        <v>416</v>
-      </c>
-      <c r="F115" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="G115" s="0"/>
-    </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G115" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="116" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="8" t="s">
         <v>418</v>
       </c>
@@ -4377,9 +4272,6 @@
       <c r="F116" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="G116" s="3" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="8" t="s">
@@ -4401,7 +4293,7 @@
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="1" t="s">
+      <c r="A118" s="8" t="s">
         <v>426</v>
       </c>
       <c r="B118" s="9" t="s">
@@ -4420,180 +4312,174 @@
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="8" t="s">
+      <c r="A119" s="1" t="s">
         <v>430</v>
       </c>
       <c r="B119" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C119" s="9" t="n">
-        <v>400</v>
-      </c>
-      <c r="D119" s="9" t="s">
         <v>431</v>
       </c>
+      <c r="C119" s="10"/>
+      <c r="D119" s="10"/>
       <c r="E119" s="9" t="s">
         <v>432</v>
       </c>
       <c r="F119" s="9" t="s">
         <v>433</v>
       </c>
-      <c r="G119" s="0"/>
-    </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="1" t="s">
+      <c r="G119" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="120" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="8" t="s">
         <v>434</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>435</v>
+        <v>260</v>
       </c>
       <c r="C120" s="9" t="n">
         <v>400</v>
       </c>
-      <c r="D120" s="9"/>
+      <c r="D120" s="9" t="s">
+        <v>435</v>
+      </c>
       <c r="E120" s="9" t="s">
         <v>436</v>
       </c>
       <c r="F120" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="G120" s="0"/>
-    </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="121" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B121" s="9" t="s">
         <v>439</v>
       </c>
-      <c r="C121" s="2" t="n">
+      <c r="C121" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="D121" s="9"/>
+      <c r="E121" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="F121" s="9" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="122" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="1" t="s">
+        <v>442</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="C122" s="2" t="n">
         <v>2612</v>
       </c>
-      <c r="D121" s="2" t="s">
-        <v>440</v>
-      </c>
-      <c r="E121" s="2" t="s">
-        <v>441</v>
-      </c>
-      <c r="F121" s="9" t="s">
-        <v>442</v>
-      </c>
-      <c r="G121" s="0"/>
-    </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="8" t="s">
-        <v>443</v>
-      </c>
-      <c r="B122" s="9" t="s">
+      <c r="D122" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="C122" s="9" t="s">
+      <c r="E122" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="D122" s="9"/>
-      <c r="E122" s="9" t="s">
+      <c r="F122" s="9" t="s">
         <v>446</v>
       </c>
-      <c r="F122" s="9" t="s">
+    </row>
+    <row r="123" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="8" t="s">
         <v>447</v>
       </c>
-      <c r="G122" s="0"/>
-    </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="8" t="s">
+      <c r="B123" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="B123" s="9" t="s">
+      <c r="C123" s="9" t="s">
+        <v>449</v>
+      </c>
+      <c r="D123" s="9"/>
+      <c r="E123" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="F123" s="9" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="124" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="8" t="s">
+        <v>452</v>
+      </c>
+      <c r="B124" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C123" s="10"/>
-      <c r="D123" s="10"/>
-      <c r="E123" s="9" t="s">
-        <v>449</v>
-      </c>
-      <c r="F123" s="9" t="s">
-        <v>450</v>
-      </c>
-      <c r="G123" s="0"/>
-    </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="8" t="s">
-        <v>451</v>
-      </c>
-      <c r="B124" s="9" t="s">
-        <v>452</v>
-      </c>
-      <c r="C124" s="9" t="n">
-        <v>7600</v>
-      </c>
-      <c r="D124" s="9"/>
+      <c r="C124" s="10"/>
+      <c r="D124" s="10"/>
       <c r="E124" s="9" t="s">
         <v>453</v>
       </c>
       <c r="F124" s="9" t="s">
         <v>454</v>
       </c>
-      <c r="G124" s="0"/>
-    </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="125" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="8" t="s">
         <v>455</v>
       </c>
       <c r="B125" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="C125" s="9" t="n">
+        <v>7600</v>
+      </c>
+      <c r="D125" s="9"/>
+      <c r="E125" s="9" t="s">
+        <v>457</v>
+      </c>
+      <c r="F125" s="9" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="B126" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C125" s="10"/>
-      <c r="D125" s="10"/>
-      <c r="E125" s="9" t="s">
-        <v>456</v>
-      </c>
-      <c r="F125" s="9" t="s">
-        <v>457</v>
-      </c>
-      <c r="G125" s="0"/>
-    </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="8" t="s">
-        <v>458</v>
-      </c>
-      <c r="B126" s="9" t="s">
+      <c r="C126" s="10"/>
+      <c r="D126" s="10"/>
+      <c r="E126" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="F126" s="9" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="B127" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="C126" s="9" t="n">
+      <c r="C127" s="9" t="n">
         <v>6000</v>
       </c>
-      <c r="D126" s="9"/>
-      <c r="E126" s="9" t="s">
-        <v>459</v>
-      </c>
-      <c r="F126" s="9" t="s">
-        <v>460</v>
-      </c>
-      <c r="G126" s="0"/>
-    </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="8" t="s">
-        <v>461</v>
-      </c>
-      <c r="B127" s="9" t="s">
+      <c r="D127" s="9"/>
+      <c r="E127" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="F127" s="9" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="128" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A128" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="B128" s="9" t="s">
         <v>205</v>
-      </c>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
-      <c r="E127" s="9" t="s">
-        <v>462</v>
-      </c>
-      <c r="F127" s="9" t="s">
-        <v>463</v>
-      </c>
-      <c r="G127" s="0"/>
-    </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="8" t="s">
-        <v>464</v>
-      </c>
-      <c r="B128" s="9" t="s">
-        <v>465</v>
       </c>
       <c r="C128" s="10"/>
       <c r="D128" s="10"/>
@@ -4603,9 +4489,8 @@
       <c r="F128" s="9" t="s">
         <v>467</v>
       </c>
-      <c r="G128" s="0"/>
-    </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="8" t="s">
         <v>468</v>
       </c>
@@ -4620,31 +4505,29 @@
       <c r="F129" s="9" t="s">
         <v>471</v>
       </c>
-      <c r="G129" s="0"/>
-    </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="130" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="8" t="s">
         <v>472</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="C130" s="10"/>
       <c r="D130" s="10"/>
       <c r="E130" s="9" t="s">
+        <v>474</v>
+      </c>
+      <c r="F130" s="9" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="131" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="B131" s="9" t="s">
         <v>473</v>
-      </c>
-      <c r="F130" s="9" t="s">
-        <v>474</v>
-      </c>
-      <c r="G130" s="0"/>
-    </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="8" t="s">
-        <v>475</v>
-      </c>
-      <c r="B131" s="9" t="s">
-        <v>476</v>
       </c>
       <c r="C131" s="10"/>
       <c r="D131" s="10"/>
@@ -4654,28 +4537,24 @@
       <c r="F131" s="9" t="s">
         <v>478</v>
       </c>
-      <c r="G131" s="0"/>
-    </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="132" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="8" t="s">
         <v>479</v>
       </c>
       <c r="B132" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="C132" s="9" t="n">
-        <v>5800</v>
-      </c>
-      <c r="D132" s="9"/>
+      <c r="C132" s="10"/>
+      <c r="D132" s="10"/>
       <c r="E132" s="9" t="s">
         <v>481</v>
       </c>
       <c r="F132" s="9" t="s">
         <v>482</v>
       </c>
-      <c r="G132" s="0"/>
-    </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="133" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="8" t="s">
         <v>483</v>
       </c>
@@ -4683,161 +4562,151 @@
         <v>484</v>
       </c>
       <c r="C133" s="9" t="n">
+        <v>5800</v>
+      </c>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9" t="s">
+        <v>485</v>
+      </c>
+      <c r="F133" s="9" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="134" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="8" t="s">
+        <v>487</v>
+      </c>
+      <c r="B134" s="9" t="s">
+        <v>488</v>
+      </c>
+      <c r="C134" s="9" t="n">
         <v>7700</v>
       </c>
-      <c r="D133" s="9" t="s">
-        <v>485</v>
-      </c>
-      <c r="E133" s="9" t="s">
-        <v>486</v>
-      </c>
-      <c r="F133" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="G133" s="0"/>
-    </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="8" t="s">
-        <v>488</v>
-      </c>
-      <c r="B134" s="9" t="s">
+      <c r="D134" s="9" t="s">
         <v>489</v>
       </c>
-      <c r="C134" s="9" t="n">
-        <v>7800</v>
-      </c>
-      <c r="D134" s="9" t="s">
+      <c r="E134" s="9" t="s">
         <v>490</v>
       </c>
-      <c r="E134" s="9" t="s">
+      <c r="F134" s="9" t="s">
         <v>491</v>
       </c>
-      <c r="F134" s="9" t="s">
-        <v>487</v>
-      </c>
-      <c r="G134" s="0"/>
-    </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="135" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="8" t="s">
         <v>492</v>
       </c>
       <c r="B135" s="9" t="s">
         <v>493</v>
       </c>
-      <c r="C135" s="10"/>
-      <c r="D135" s="10"/>
+      <c r="C135" s="9" t="n">
+        <v>7800</v>
+      </c>
+      <c r="D135" s="9" t="s">
+        <v>494</v>
+      </c>
       <c r="E135" s="9" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="F135" s="9" t="s">
-        <v>495</v>
-      </c>
-      <c r="G135" s="0"/>
-    </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="8" t="s">
         <v>496</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C136" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="D136" s="10" t="s">
         <v>497</v>
       </c>
+      <c r="C136" s="10"/>
+      <c r="D136" s="10"/>
       <c r="E136" s="9" t="s">
         <v>498</v>
       </c>
       <c r="F136" s="9" t="s">
         <v>499</v>
       </c>
-      <c r="G136" s="0"/>
-    </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="8" t="s">
         <v>500</v>
       </c>
       <c r="B137" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C137" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="D137" s="10" t="s">
         <v>501</v>
       </c>
-      <c r="C137" s="10"/>
-      <c r="D137" s="10"/>
       <c r="E137" s="9" t="s">
         <v>502</v>
       </c>
       <c r="F137" s="9" t="s">
         <v>503</v>
       </c>
-      <c r="G137" s="0"/>
-    </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="8" t="s">
         <v>504</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>379</v>
-      </c>
-      <c r="C138" s="9" t="n">
+        <v>505</v>
+      </c>
+      <c r="C138" s="10"/>
+      <c r="D138" s="10"/>
+      <c r="E138" s="9" t="s">
+        <v>506</v>
+      </c>
+      <c r="F138" s="9" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="B139" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="C139" s="9" t="n">
         <v>101</v>
       </c>
-      <c r="D138" s="9"/>
-      <c r="E138" s="9" t="s">
-        <v>381</v>
-      </c>
-      <c r="F138" s="0"/>
-      <c r="G138" s="3" t="s">
+      <c r="D139" s="9"/>
+      <c r="E139" s="9" t="s">
+        <v>385</v>
+      </c>
+      <c r="G139" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="8" t="s">
-        <v>505</v>
-      </c>
-      <c r="B139" s="9" t="s">
+    <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="8" t="s">
+        <v>509</v>
+      </c>
+      <c r="B140" s="9" t="s">
         <v>224</v>
       </c>
-      <c r="C139" s="10"/>
-      <c r="D139" s="10"/>
-      <c r="E139" s="9" t="s">
-        <v>506</v>
-      </c>
-      <c r="F139" s="9" t="s">
-        <v>507</v>
-      </c>
-      <c r="G139" s="0"/>
-    </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A140" s="8" t="s">
-        <v>508</v>
-      </c>
-      <c r="B140" s="9" t="s">
-        <v>227</v>
-      </c>
       <c r="C140" s="10"/>
-      <c r="D140" s="10" t="s">
-        <v>509</v>
-      </c>
+      <c r="D140" s="10"/>
       <c r="E140" s="9" t="s">
         <v>510</v>
       </c>
       <c r="F140" s="9" t="s">
         <v>511</v>
       </c>
-      <c r="G140" s="0"/>
-    </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="8" t="s">
         <v>512</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C141" s="9" t="n">
-        <v>1400</v>
-      </c>
-      <c r="D141" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="C141" s="10"/>
+      <c r="D141" s="10" t="s">
         <v>513</v>
       </c>
       <c r="E141" s="9" t="s">
@@ -4846,20 +4715,19 @@
       <c r="F141" s="9" t="s">
         <v>515</v>
       </c>
-      <c r="G141" s="0"/>
-    </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A142" s="1" t="s">
+    </row>
+    <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A142" s="8" t="s">
         <v>516</v>
       </c>
       <c r="B142" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="C142" s="9" t="n">
+        <v>1400</v>
+      </c>
+      <c r="D142" s="9" t="s">
         <v>517</v>
-      </c>
-      <c r="C142" s="9" t="n">
-        <v>7400</v>
-      </c>
-      <c r="D142" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="E142" s="9" t="s">
         <v>518</v>
@@ -4867,38 +4735,36 @@
       <c r="F142" s="9" t="s">
         <v>519</v>
       </c>
-      <c r="G142" s="0"/>
-    </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="8" t="s">
+    </row>
+    <row r="143" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="1" t="s">
         <v>520</v>
       </c>
       <c r="B143" s="9" t="s">
         <v>521</v>
       </c>
-      <c r="C143" s="10"/>
-      <c r="D143" s="10" t="s">
+      <c r="C143" s="9" t="n">
+        <v>7400</v>
+      </c>
+      <c r="D143" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E143" s="9" t="s">
         <v>522</v>
       </c>
-      <c r="E143" s="9" t="s">
+      <c r="F143" s="9" t="s">
         <v>523</v>
       </c>
-      <c r="F143" s="9" t="s">
+    </row>
+    <row r="144" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A144" s="8" t="s">
         <v>524</v>
       </c>
-      <c r="G143" s="0"/>
-    </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A144" s="8" t="s">
+      <c r="B144" s="9" t="s">
         <v>525</v>
       </c>
-      <c r="B144" s="9" t="s">
-        <v>469</v>
-      </c>
-      <c r="C144" s="9" t="n">
-        <v>1700</v>
-      </c>
-      <c r="D144" s="9" t="s">
+      <c r="C144" s="10"/>
+      <c r="D144" s="10" t="s">
         <v>526</v>
       </c>
       <c r="E144" s="9" t="s">
@@ -4907,20 +4773,19 @@
       <c r="F144" s="9" t="s">
         <v>528</v>
       </c>
-      <c r="G144" s="0"/>
-    </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="8" t="s">
         <v>529</v>
       </c>
       <c r="B145" s="9" t="s">
+        <v>473</v>
+      </c>
+      <c r="C145" s="9" t="n">
+        <v>1700</v>
+      </c>
+      <c r="D145" s="9" t="s">
         <v>530</v>
-      </c>
-      <c r="C145" s="9" t="n">
-        <v>1800</v>
-      </c>
-      <c r="D145" s="9" t="s">
-        <v>117</v>
       </c>
       <c r="E145" s="9" t="s">
         <v>531</v>
@@ -4928,565 +4793,538 @@
       <c r="F145" s="9" t="s">
         <v>532</v>
       </c>
-      <c r="G145" s="0"/>
-    </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="146" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="8" t="s">
         <v>533</v>
       </c>
       <c r="B146" s="9" t="s">
+        <v>534</v>
+      </c>
+      <c r="C146" s="9" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D146" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E146" s="9" t="s">
+        <v>535</v>
+      </c>
+      <c r="F146" s="9" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A147" s="8" t="s">
+        <v>537</v>
+      </c>
+      <c r="B147" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="C146" s="7"/>
-      <c r="D146" s="7"/>
-      <c r="E146" s="9" t="s">
-        <v>534</v>
-      </c>
-      <c r="F146" s="9" t="s">
-        <v>535</v>
-      </c>
-      <c r="G146" s="0"/>
-    </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="8" t="s">
-        <v>536</v>
-      </c>
-      <c r="B147" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C147" s="10" t="s">
-        <v>537</v>
-      </c>
-      <c r="D147" s="10"/>
+      <c r="C147" s="7"/>
+      <c r="D147" s="7"/>
       <c r="E147" s="9" t="s">
         <v>538</v>
       </c>
       <c r="F147" s="9" t="s">
-        <v>535</v>
-      </c>
-      <c r="G147" s="0"/>
-    </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="8" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>521</v>
-      </c>
-      <c r="C148" s="10"/>
+        <v>205</v>
+      </c>
+      <c r="C148" s="10" t="s">
+        <v>541</v>
+      </c>
       <c r="D148" s="10"/>
       <c r="E148" s="9" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="F148" s="9" t="s">
-        <v>535</v>
-      </c>
-      <c r="G148" s="0"/>
-    </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="8" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>469</v>
+        <v>525</v>
       </c>
       <c r="C149" s="10"/>
       <c r="D149" s="10"/>
       <c r="E149" s="9" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="F149" s="9" t="s">
-        <v>535</v>
-      </c>
-      <c r="G149" s="0"/>
-    </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="8" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>544</v>
+        <v>473</v>
       </c>
       <c r="C150" s="10"/>
       <c r="D150" s="10"/>
       <c r="E150" s="9" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="F150" s="9" t="s">
-        <v>546</v>
-      </c>
-      <c r="G150" s="0"/>
-    </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="8" t="s">
         <v>547</v>
       </c>
       <c r="B151" s="9" t="s">
-        <v>521</v>
+        <v>548</v>
       </c>
       <c r="C151" s="10"/>
       <c r="D151" s="10"/>
       <c r="E151" s="9" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F151" s="9" t="s">
-        <v>549</v>
-      </c>
-      <c r="G151" s="0"/>
-    </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="8" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>469</v>
+        <v>525</v>
       </c>
       <c r="C152" s="10"/>
       <c r="D152" s="10"/>
       <c r="E152" s="9" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="F152" s="9" t="s">
-        <v>552</v>
-      </c>
-      <c r="G152" s="0"/>
-    </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="8" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>205</v>
+        <v>473</v>
       </c>
       <c r="C153" s="10"/>
       <c r="D153" s="10"/>
       <c r="E153" s="9" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="F153" s="9" t="s">
-        <v>555</v>
-      </c>
-      <c r="G153" s="0"/>
-    </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="8" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B154" s="9" t="s">
-        <v>147</v>
+        <v>205</v>
       </c>
       <c r="C154" s="10"/>
       <c r="D154" s="10"/>
       <c r="E154" s="9" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="F154" s="9" t="s">
-        <v>558</v>
-      </c>
-      <c r="G154" s="0"/>
-    </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="8" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B155" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C155" s="10"/>
       <c r="D155" s="10"/>
       <c r="E155" s="9" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="F155" s="9" t="s">
-        <v>561</v>
-      </c>
-      <c r="G155" s="0"/>
-    </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="8" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>227</v>
+        <v>150</v>
       </c>
       <c r="C156" s="10"/>
       <c r="D156" s="10"/>
       <c r="E156" s="9" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="F156" s="9" t="s">
-        <v>564</v>
-      </c>
-      <c r="G156" s="0"/>
-    </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="8" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="B157" s="9" t="s">
-        <v>469</v>
+        <v>227</v>
       </c>
       <c r="C157" s="10"/>
       <c r="D157" s="10"/>
       <c r="E157" s="9" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="F157" s="9" t="s">
-        <v>567</v>
-      </c>
-      <c r="G157" s="0"/>
-    </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="8" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B158" s="9" t="s">
-        <v>147</v>
+        <v>473</v>
       </c>
       <c r="C158" s="10"/>
       <c r="D158" s="10"/>
       <c r="E158" s="9" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="F158" s="9" t="s">
-        <v>570</v>
-      </c>
-      <c r="G158" s="0"/>
-    </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="159" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="8" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B159" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C159" s="10"/>
       <c r="D159" s="10"/>
       <c r="E159" s="9" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="F159" s="9" t="s">
-        <v>573</v>
-      </c>
-      <c r="G159" s="0"/>
-    </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="8" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B160" s="9" t="s">
-        <v>227</v>
+        <v>150</v>
       </c>
       <c r="C160" s="10"/>
       <c r="D160" s="10"/>
       <c r="E160" s="9" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="F160" s="9" t="s">
-        <v>576</v>
-      </c>
-      <c r="G160" s="0"/>
-    </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="8" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B161" s="9" t="s">
-        <v>205</v>
+        <v>227</v>
       </c>
       <c r="C161" s="10"/>
       <c r="D161" s="10"/>
       <c r="E161" s="9" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="F161" s="9" t="s">
-        <v>579</v>
-      </c>
-      <c r="G161" s="0"/>
-    </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="8" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B162" s="9" t="s">
-        <v>521</v>
+        <v>205</v>
       </c>
       <c r="C162" s="10"/>
       <c r="D162" s="10"/>
       <c r="E162" s="9" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="F162" s="9" t="s">
-        <v>582</v>
-      </c>
-      <c r="G162" s="0"/>
-    </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="8" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>584</v>
-      </c>
-      <c r="C163" s="9" t="n">
-        <v>121</v>
-      </c>
-      <c r="D163" s="9"/>
+        <v>525</v>
+      </c>
+      <c r="C163" s="10"/>
+      <c r="D163" s="10"/>
       <c r="E163" s="9" t="s">
         <v>585</v>
       </c>
-      <c r="F163" s="0"/>
-      <c r="G163" s="3" t="s">
+      <c r="F163" s="9" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="164" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A164" s="8" t="s">
+        <v>587</v>
+      </c>
+      <c r="B164" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="C164" s="9" t="n">
+        <v>121</v>
+      </c>
+      <c r="D164" s="9"/>
+      <c r="E164" s="9" t="s">
+        <v>589</v>
+      </c>
+      <c r="G164" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A164" s="8" t="s">
-        <v>586</v>
-      </c>
-      <c r="B164" s="9" t="s">
+    <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A165" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="B165" s="9" t="s">
         <v>147</v>
-      </c>
-      <c r="C164" s="10"/>
-      <c r="D164" s="10"/>
-      <c r="E164" s="9" t="s">
-        <v>587</v>
-      </c>
-      <c r="F164" s="9" t="s">
-        <v>588</v>
-      </c>
-      <c r="G164" s="0"/>
-    </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A165" s="8" t="s">
-        <v>589</v>
-      </c>
-      <c r="B165" s="9" t="s">
-        <v>205</v>
       </c>
       <c r="C165" s="10"/>
       <c r="D165" s="10"/>
       <c r="E165" s="9" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="F165" s="9" t="s">
-        <v>591</v>
-      </c>
-      <c r="G165" s="0"/>
-    </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="166" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="8" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="B166" s="9" t="s">
-        <v>383</v>
-      </c>
-      <c r="C166" s="9" t="n">
+        <v>205</v>
+      </c>
+      <c r="C166" s="10"/>
+      <c r="D166" s="10"/>
+      <c r="E166" s="9" t="s">
+        <v>594</v>
+      </c>
+      <c r="F166" s="9" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A167" s="8" t="s">
+        <v>596</v>
+      </c>
+      <c r="B167" s="9" t="s">
+        <v>387</v>
+      </c>
+      <c r="C167" s="9" t="n">
         <v>111</v>
-      </c>
-      <c r="D166" s="9"/>
-      <c r="E166" s="9" t="s">
-        <v>385</v>
-      </c>
-      <c r="F166" s="0"/>
-      <c r="G166" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A167" s="8" t="s">
-        <v>593</v>
-      </c>
-      <c r="B167" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="C167" s="9" t="n">
-        <v>1711</v>
       </c>
       <c r="D167" s="9"/>
       <c r="E167" s="9" t="s">
-        <v>594</v>
-      </c>
-      <c r="F167" s="9" t="s">
-        <v>280</v>
+        <v>389</v>
       </c>
       <c r="G167" s="3" t="s">
-        <v>11</v>
+        <v>61</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A168" s="1" t="s">
-        <v>595</v>
+      <c r="A168" s="8" t="s">
+        <v>597</v>
       </c>
       <c r="B168" s="9" t="s">
-        <v>596</v>
+        <v>278</v>
       </c>
       <c r="C168" s="9" t="n">
-        <v>3300</v>
+        <v>1711</v>
       </c>
       <c r="D168" s="9"/>
       <c r="E168" s="9" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="F168" s="9" t="s">
-        <v>598</v>
-      </c>
-      <c r="G168" s="0"/>
-    </row>
-    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="G168" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A169" s="1" t="s">
         <v>599</v>
       </c>
       <c r="B169" s="9" t="s">
         <v>600</v>
       </c>
       <c r="C169" s="9" t="n">
+        <v>3300</v>
+      </c>
+      <c r="D169" s="9"/>
+      <c r="E169" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="F169" s="9" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A170" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="B170" s="9" t="s">
+        <v>604</v>
+      </c>
+      <c r="C170" s="9" t="n">
         <v>8000</v>
       </c>
-      <c r="D169" s="9" t="s">
-        <v>601</v>
-      </c>
-      <c r="E169" s="9" t="s">
-        <v>602</v>
-      </c>
-      <c r="F169" s="9" t="s">
-        <v>603</v>
-      </c>
-      <c r="G169" s="0"/>
-    </row>
-    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A170" s="8" t="s">
-        <v>604</v>
-      </c>
-      <c r="B170" s="9" t="s">
+      <c r="D170" s="9" t="s">
+        <v>605</v>
+      </c>
+      <c r="E170" s="9" t="s">
+        <v>606</v>
+      </c>
+      <c r="F170" s="9" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A171" s="8" t="s">
+        <v>608</v>
+      </c>
+      <c r="B171" s="9" t="s">
         <v>147</v>
-      </c>
-      <c r="C170" s="10"/>
-      <c r="D170" s="10"/>
-      <c r="E170" s="9" t="s">
-        <v>605</v>
-      </c>
-      <c r="F170" s="9" t="s">
-        <v>606</v>
-      </c>
-      <c r="G170" s="0"/>
-    </row>
-    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A171" s="8" t="s">
-        <v>607</v>
-      </c>
-      <c r="B171" s="9" t="s">
-        <v>150</v>
       </c>
       <c r="C171" s="10"/>
       <c r="D171" s="10"/>
       <c r="E171" s="9" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="F171" s="9" t="s">
-        <v>609</v>
-      </c>
-      <c r="G171" s="0"/>
-    </row>
-    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="8" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>224</v>
+        <v>150</v>
       </c>
       <c r="C172" s="10"/>
       <c r="D172" s="10"/>
       <c r="E172" s="9" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="F172" s="9" t="s">
-        <v>612</v>
-      </c>
-      <c r="G172" s="0"/>
-    </row>
-    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="8" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B173" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C173" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D173" s="9" t="s">
-        <v>614</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="C173" s="10"/>
+      <c r="D173" s="10"/>
       <c r="E173" s="9" t="s">
         <v>615</v>
       </c>
       <c r="F173" s="9" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A174" s="8" t="s">
+        <v>617</v>
+      </c>
+      <c r="B174" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C174" s="9" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D174" s="9" t="s">
+        <v>618</v>
+      </c>
+      <c r="E174" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="F174" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="G173" s="0"/>
-    </row>
-    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="8" t="s">
-        <v>616</v>
-      </c>
-      <c r="B174" s="7" t="s">
-        <v>617</v>
-      </c>
-      <c r="C174" s="9" t="n">
+    </row>
+    <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A175" s="8" t="s">
+        <v>620</v>
+      </c>
+      <c r="B175" s="7" t="s">
+        <v>621</v>
+      </c>
+      <c r="C175" s="9" t="n">
         <v>2611</v>
-      </c>
-      <c r="D174" s="9"/>
-      <c r="E174" s="9" t="s">
-        <v>618</v>
-      </c>
-      <c r="F174" s="0"/>
-      <c r="G174" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A175" s="8" t="s">
-        <v>619</v>
-      </c>
-      <c r="B175" s="9" t="s">
-        <v>620</v>
-      </c>
-      <c r="C175" s="9" t="n">
-        <v>2711</v>
       </c>
       <c r="D175" s="9"/>
       <c r="E175" s="9" t="s">
-        <v>621</v>
-      </c>
-      <c r="F175" s="0"/>
+        <v>622</v>
+      </c>
       <c r="G175" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="176" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="8" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B176" s="9" t="s">
+        <v>624</v>
+      </c>
+      <c r="C176" s="9" t="n">
+        <v>2711</v>
+      </c>
+      <c r="D176" s="9"/>
+      <c r="E176" s="9" t="s">
+        <v>625</v>
+      </c>
+      <c r="G176" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A177" s="8" t="s">
+        <v>626</v>
+      </c>
+      <c r="B177" s="9" t="s">
         <v>205</v>
-      </c>
-      <c r="C176" s="10"/>
-      <c r="D176" s="10"/>
-      <c r="E176" s="9" t="s">
-        <v>623</v>
-      </c>
-      <c r="F176" s="9" t="s">
-        <v>624</v>
-      </c>
-      <c r="G176" s="0"/>
-    </row>
-    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A177" s="8" t="s">
-        <v>625</v>
-      </c>
-      <c r="B177" s="9" t="s">
-        <v>626</v>
       </c>
       <c r="C177" s="10"/>
       <c r="D177" s="10"/>
@@ -5496,138 +5334,130 @@
       <c r="F177" s="9" t="s">
         <v>628</v>
       </c>
-      <c r="G177" s="0"/>
-    </row>
-    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="8" t="s">
         <v>629</v>
       </c>
       <c r="B178" s="9" t="s">
         <v>630</v>
       </c>
-      <c r="C178" s="9" t="n">
-        <v>3721</v>
-      </c>
-      <c r="D178" s="9"/>
+      <c r="C178" s="10"/>
+      <c r="D178" s="10"/>
       <c r="E178" s="9" t="s">
         <v>631</v>
       </c>
       <c r="F178" s="9" t="s">
         <v>632</v>
       </c>
-      <c r="G178" s="0"/>
-    </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="8" t="s">
         <v>633</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>469</v>
+        <v>634</v>
       </c>
       <c r="C179" s="9" t="n">
-        <v>6100</v>
+        <v>3721</v>
       </c>
       <c r="D179" s="9"/>
       <c r="E179" s="9" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="F179" s="9" t="s">
-        <v>635</v>
-      </c>
-      <c r="G179" s="0"/>
-    </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="8" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="B180" s="9" t="s">
-        <v>637</v>
-      </c>
-      <c r="C180" s="10" t="n">
-        <v>8400</v>
-      </c>
-      <c r="D180" s="10"/>
+        <v>473</v>
+      </c>
+      <c r="C180" s="9" t="n">
+        <v>6100</v>
+      </c>
+      <c r="D180" s="9"/>
       <c r="E180" s="9" t="s">
         <v>638</v>
       </c>
       <c r="F180" s="9" t="s">
         <v>639</v>
       </c>
-      <c r="G180" s="0"/>
-    </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="8" t="s">
         <v>640</v>
       </c>
       <c r="B181" s="9" t="s">
+        <v>641</v>
+      </c>
+      <c r="C181" s="10" t="n">
+        <v>8400</v>
+      </c>
+      <c r="D181" s="10"/>
+      <c r="E181" s="9" t="s">
+        <v>642</v>
+      </c>
+      <c r="F181" s="9" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A182" s="8" t="s">
+        <v>644</v>
+      </c>
+      <c r="B182" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C181" s="7"/>
-      <c r="D181" s="7"/>
-      <c r="E181" s="9" t="s">
-        <v>641</v>
-      </c>
-      <c r="F181" s="9" t="s">
-        <v>642</v>
-      </c>
-      <c r="G181" s="0"/>
-    </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A182" s="1" t="s">
-        <v>643</v>
-      </c>
-      <c r="B182" s="9" t="s">
+      <c r="C182" s="7"/>
+      <c r="D182" s="7"/>
+      <c r="E182" s="9" t="s">
+        <v>645</v>
+      </c>
+      <c r="F182" s="9" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A183" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="B183" s="9" t="s">
         <v>260</v>
-      </c>
-      <c r="C182" s="9" t="n">
-        <v>400</v>
-      </c>
-      <c r="D182" s="9"/>
-      <c r="E182" s="9" t="s">
-        <v>644</v>
-      </c>
-      <c r="F182" s="9" t="s">
-        <v>645</v>
-      </c>
-      <c r="G182" s="0"/>
-    </row>
-    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="1" t="s">
-        <v>646</v>
-      </c>
-      <c r="B183" s="9" t="s">
-        <v>435</v>
       </c>
       <c r="C183" s="9" t="n">
         <v>400</v>
       </c>
       <c r="D183" s="9"/>
       <c r="E183" s="9" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="F183" s="9" t="s">
-        <v>437</v>
-      </c>
-      <c r="G183" s="0"/>
-    </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="8" t="s">
-        <v>648</v>
+        <v>649</v>
+      </c>
+    </row>
+    <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A184" s="1" t="s">
+        <v>650</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>649</v>
-      </c>
-      <c r="C184" s="10"/>
-      <c r="D184" s="10"/>
+        <v>439</v>
+      </c>
+      <c r="C184" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="D184" s="9"/>
       <c r="E184" s="9" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="F184" s="9" t="s">
-        <v>651</v>
-      </c>
-      <c r="G184" s="0"/>
-    </row>
-    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="8" t="s">
         <v>652</v>
       </c>
@@ -5642,14 +5472,13 @@
       <c r="F185" s="9" t="s">
         <v>654</v>
       </c>
-      <c r="G185" s="0"/>
-    </row>
-    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="8" t="s">
         <v>655</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="C186" s="9" t="n">
         <v>21</v>
@@ -5658,7 +5487,6 @@
       <c r="E186" s="9" t="s">
         <v>656</v>
       </c>
-      <c r="F186" s="0"/>
       <c r="G186" s="3" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
new hashes added and some name changes
added:
Django(DES Crypt Wrapper)
Django(PBKDF2-HMAC-SHA256)
Django(PBKDF2-HMAC-SHA1)
Django(BCrypt)
Django(MD5)

renamed:
Django CMS(SHA-1) to Django(SHA-1)
Django CMS(SHA-256) to Django(SHA-256)
Django CMS(SHA-384) to Django(SHA-384)
</commit_message>
<xml_diff>
--- a/hashinfo.xlsx
+++ b/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="681">
   <si>
     <t>Hash</t>
   </si>
@@ -377,22 +377,82 @@
     <t>http://pythonhosted.org/passlib/lib/passlib.hash.des_crypt.html</t>
   </si>
   <si>
-    <t>Django CMS(SHA-1)</t>
-  </si>
-  <si>
-    <t>^sha1\$[a-z0-9\/\.]{1,12}\$[a-f0-9]{40}$/i</t>
+    <t>Django(BCrypt)</t>
+  </si>
+  <si>
+    <t>^bcrypt(\$2[axy]|\$2)\$[0-9]{0,2}?\$[a-z0-9\/\.]{53}$/i</t>
+  </si>
+  <si>
+    <t>bcrypt$2a$05$LhayLxezLhK1LhWvKxCyLOj0j1u.Kj0jZ0pEmm134uzrQlFvQJLF6</t>
+  </si>
+  <si>
+    <t>https://pythonhosted.org/passlib/lib/passlib.hash.django_std.html#passlib.hash.django_bcrypt</t>
+  </si>
+  <si>
+    <t>Django(DES Crypt Wrapper)</t>
+  </si>
+  <si>
+    <t>^crypt\$[a-f0-9]{5}\$[a-z0-9.\/]{13}$/i</t>
+  </si>
+  <si>
+    <t>crypt$cd1a4$cdlRbNJGImptk </t>
+  </si>
+  <si>
+    <t>https://pythonhosted.org/passlib/lib/passlib.hash.django_std.html#des-crypt-wrapper</t>
+  </si>
+  <si>
+    <t>Django(MD5)</t>
+  </si>
+  <si>
+    <t>^md5\$[a-f0-9]{1,}\$[a-f0-9]{32}$/i</t>
+  </si>
+  <si>
+    <t>md5$be7b1$4e9c5b51bd070727b0ed21956cb68de7</t>
+  </si>
+  <si>
+    <t>https://pythonhosted.org/passlib/lib/passlib.hash.django_std.html#passlib.hash.django_salted_md5</t>
+  </si>
+  <si>
+    <t>Django(PBKDF2-HMAC-SHA1)</t>
+  </si>
+  <si>
+    <t>^pbkdf2_sha1\$[0-9]+\$[a-z0-9]{1,}\$[a-z0-9+\/]{27}=$/i</t>
+  </si>
+  <si>
+    <t>pbkdf2_sha1$10000$s1w0UXDd00XB$zTsOichpYtEkA2Gj50dM0twCn4c=</t>
+  </si>
+  <si>
+    <t>https://pythonhosted.org/passlib/lib/passlib.hash.django_std.html#passlib.hash.django_pbkdf2_sha1</t>
+  </si>
+  <si>
+    <t>Django(PBKDF2-HMAC-SHA256)</t>
+  </si>
+  <si>
+    <t>^pbkdf2_sha256\$[0-9]+\$[a-z0-9]{1,}\$[a-z0-9+\/]{43}=$/i</t>
+  </si>
+  <si>
+    <t>pbkdf2_sha256$10000$s1w0UXDd00XB$+4ORmyvVWAQvoAEWlDgN34vlaJx1ZTZpa1pCSRey2Yk= </t>
+  </si>
+  <si>
+    <t>https://pythonhosted.org/passlib/lib/passlib.hash.django_std.html#passlib.hash.django_pbkdf2_sha256</t>
+  </si>
+  <si>
+    <t>Django(SHA-1)</t>
+  </si>
+  <si>
+    <t>^sha1\$[a-f0-9]{1,}\$[a-f0-9]{40}$/i</t>
   </si>
   <si>
     <t>sha1$12345678$6214c0c5e54360fc3986741f8d68b062808ab348</t>
   </si>
   <si>
-    <t>http://wiki.insidepro.com/index.php/SHA-1%28Django%29</t>
-  </si>
-  <si>
-    <t>Django CMS(SHA-256)</t>
-  </si>
-  <si>
-    <t>^sha256\$[a-z0-9\/\.]{1,12}\$[a-f0-9]{64}$/i</t>
+    <t>https://pythonhosted.org/passlib/lib/passlib.hash.django_std.html#passlib.hash.django_salted_sha1</t>
+  </si>
+  <si>
+    <t>Django(SHA-256)</t>
+  </si>
+  <si>
+    <t>^sha256\$[a-f0-9]{1,}\$[a-f0-9]{64}$/i</t>
   </si>
   <si>
     <t>sha256$12345678$9171fc5e7cd440fac61adc27cbebb78ff028a19a1abeaa041807a5ea936fbd94</t>
@@ -401,10 +461,10 @@
     <t>http://wiki.insidepro.com/index.php/SHA-256%28Django%29</t>
   </si>
   <si>
-    <t>Django CMS(SHA-384)</t>
-  </si>
-  <si>
-    <t>^sha384\$[a-z0-9\/\.]{1,12}\$[a-f0-9]{96}$/i</t>
+    <t>Django(SHA-384)</t>
+  </si>
+  <si>
+    <t>^sha384\$[a-f0-9]{1,}\$[a-f0-9]{96}$/i</t>
   </si>
   <si>
     <t>sha384$12345678$fe014d8b5dc1733a9727330fb8b4695f82c7e833382a27c513b258f46f29ababb9d9963ddaa13db306b2bbd1459b95e6</t>
@@ -2172,10 +2232,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G187"/>
+  <dimension ref="A1:G192"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E119" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A1:G192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2749,161 +2809,137 @@
         <v>119</v>
       </c>
     </row>
-    <row r="32" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C32" s="9" t="n">
-        <v>800</v>
-      </c>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9" t="s">
+      <c r="E32" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="F32" s="9" t="s">
+      <c r="F32" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="33" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="F33" s="9" t="s">
+      <c r="F33" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="34" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F34" s="9" t="s">
+      <c r="F34" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="35" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C35" s="10" t="n">
-        <v>8300</v>
-      </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="F35" s="9" t="s">
+      <c r="F35" s="2" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="36" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="8" t="s">
+    <row r="36" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B36" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C36" s="9" t="n">
-        <v>1100</v>
-      </c>
-      <c r="D36" s="9" t="s">
+      <c r="E36" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="F36" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="F36" s="9" t="s">
+    </row>
+    <row r="37" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="37" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="8" t="s">
+      <c r="B37" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B37" s="9" t="s">
+      <c r="C37" s="9" t="n">
+        <v>800</v>
+      </c>
+      <c r="D37" s="9"/>
+      <c r="E37" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="C37" s="9" t="n">
-        <v>2100</v>
-      </c>
-      <c r="D37" s="9" t="s">
+      <c r="F37" s="9" t="s">
         <v>143</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="38" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B38" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="C38" s="10" t="n">
-        <v>2600</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="C38" s="10"/>
       <c r="D38" s="10"/>
       <c r="E38" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="G38" s="3" t="s">
-        <v>61</v>
+        <v>146</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="39" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B39" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="B39" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C39" s="10" t="n">
-        <v>4500</v>
-      </c>
+      <c r="C39" s="10"/>
       <c r="D39" s="10"/>
       <c r="E39" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F39" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="G39" s="3" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="40" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="1" t="s">
         <v>152</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="C40" s="9" t="n">
-        <v>7900</v>
-      </c>
-      <c r="D40" s="9"/>
+      <c r="C40" s="10" t="n">
+        <v>8300</v>
+      </c>
+      <c r="D40" s="10"/>
       <c r="E40" s="9" t="s">
         <v>154</v>
       </c>
@@ -2918,8 +2954,10 @@
       <c r="B41" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10" t="s">
+      <c r="C41" s="9" t="n">
+        <v>1100</v>
+      </c>
+      <c r="D41" s="9" t="s">
         <v>158</v>
       </c>
       <c r="E41" s="9" t="s">
@@ -2934,48 +2972,52 @@
         <v>161</v>
       </c>
       <c r="B42" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" s="10"/>
-      <c r="D42" s="10"/>
+        <v>162</v>
+      </c>
+      <c r="C42" s="9" t="n">
+        <v>2100</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>163</v>
+      </c>
       <c r="E42" s="9" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="F42" s="9" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="43" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="B43" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="C43" s="9" t="n">
-        <v>123</v>
-      </c>
-      <c r="D43" s="9"/>
+      <c r="A43" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" s="10" t="n">
+        <v>2600</v>
+      </c>
+      <c r="D43" s="10"/>
       <c r="E43" s="9" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="G43" s="3" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="44" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="8" t="s">
-        <v>167</v>
+      <c r="A44" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="C44" s="9" t="n">
-        <v>141</v>
-      </c>
-      <c r="D44" s="9"/>
+        <v>170</v>
+      </c>
+      <c r="C44" s="10" t="n">
+        <v>4500</v>
+      </c>
+      <c r="D44" s="10"/>
       <c r="E44" s="9" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G44" s="3" t="s">
         <v>61</v>
@@ -2983,159 +3025,161 @@
     </row>
     <row r="45" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="C45" s="9" t="n">
-        <v>1441</v>
+        <v>7900</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>61</v>
+        <v>174</v>
+      </c>
+      <c r="F45" s="9" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
-        <v>173</v>
+      <c r="A46" s="8" t="s">
+        <v>176</v>
       </c>
       <c r="B46" s="9" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C46" s="10"/>
-      <c r="D46" s="10"/>
+      <c r="D46" s="10" t="s">
+        <v>178</v>
+      </c>
       <c r="E46" s="9" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>78</v>
+        <v>16</v>
       </c>
       <c r="C47" s="10"/>
       <c r="D47" s="10"/>
       <c r="E47" s="9" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="48" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
+        <v>184</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="C48" s="9" t="n">
+        <v>123</v>
+      </c>
+      <c r="D48" s="9"/>
       <c r="E48" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="F48" s="9" t="s">
-        <v>182</v>
+        <v>186</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="49" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="8" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10"/>
+        <v>188</v>
+      </c>
+      <c r="C49" s="9" t="n">
+        <v>141</v>
+      </c>
+      <c r="D49" s="9"/>
       <c r="E49" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="F49" s="9" t="s">
-        <v>185</v>
+        <v>189</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="8" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="B50" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
+        <v>191</v>
+      </c>
+      <c r="C50" s="9" t="n">
+        <v>1441</v>
+      </c>
+      <c r="D50" s="9"/>
       <c r="E50" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F50" s="9" t="s">
-        <v>188</v>
+        <v>192</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="51" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="8" t="s">
-        <v>189</v>
+      <c r="A51" s="1" t="s">
+        <v>193</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>94</v>
+        <v>194</v>
       </c>
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
       <c r="E51" s="9" t="s">
-        <v>190</v>
+        <v>195</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
     </row>
     <row r="52" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="8" t="s">
-        <v>192</v>
+        <v>197</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C52" s="9" t="n">
-        <v>7000</v>
-      </c>
-      <c r="D52" s="9"/>
+        <v>78</v>
+      </c>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
       <c r="E52" s="9" t="s">
-        <v>194</v>
-      </c>
-      <c r="G52" s="3" t="s">
-        <v>61</v>
+        <v>198</v>
+      </c>
+      <c r="F52" s="9" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="53" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="8" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="B53" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C53" s="9" t="n">
-        <v>500</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>196</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
       <c r="E53" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="G53" s="3" t="s">
-        <v>61</v>
+        <v>201</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="54" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="8" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="B54" s="9" t="s">
         <v>16</v>
@@ -3143,15 +3187,15 @@
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
       <c r="E54" s="9" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
     </row>
     <row r="55" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="8" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
       <c r="B55" s="9" t="s">
         <v>16</v>
@@ -3159,351 +3203,347 @@
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
       <c r="E55" s="9" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="F55" s="9" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
     </row>
     <row r="56" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="8" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="B56" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C56" s="9" t="n">
-        <v>6900</v>
-      </c>
-      <c r="D56" s="9"/>
+        <v>94</v>
+      </c>
+      <c r="C56" s="10"/>
+      <c r="D56" s="10"/>
       <c r="E56" s="9" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="8" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="B57" s="9" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C57" s="9" t="n">
-        <v>7200</v>
+        <v>7000</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>211</v>
+        <v>214</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="58" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="8" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="B58" s="9" t="s">
-        <v>94</v>
+        <v>59</v>
       </c>
       <c r="C58" s="9" t="n">
-        <v>5100</v>
-      </c>
-      <c r="D58" s="9"/>
+        <v>500</v>
+      </c>
+      <c r="D58" s="9" t="s">
+        <v>216</v>
+      </c>
       <c r="E58" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="F58" s="2" t="s">
-        <v>214</v>
+        <v>217</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="59" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="8" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>150</v>
+        <v>16</v>
       </c>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
       <c r="E59" s="9" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="F59" s="9" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
     <row r="60" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="8" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>147</v>
+        <v>16</v>
       </c>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
       <c r="E60" s="9" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="F60" s="9" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="61" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="8" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C61" s="10"/>
-      <c r="D61" s="10"/>
+        <v>225</v>
+      </c>
+      <c r="C61" s="9" t="n">
+        <v>6900</v>
+      </c>
+      <c r="D61" s="9"/>
       <c r="E61" s="9" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="F61" s="9" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="8" t="s">
-        <v>223</v>
+        <v>228</v>
       </c>
       <c r="B62" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
+        <v>229</v>
+      </c>
+      <c r="C62" s="9" t="n">
+        <v>7200</v>
+      </c>
+      <c r="D62" s="9"/>
       <c r="E62" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="F62" s="9" t="s">
-        <v>220</v>
+        <v>230</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="63" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="8" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="C63" s="10"/>
-      <c r="D63" s="10"/>
+        <v>94</v>
+      </c>
+      <c r="C63" s="9" t="n">
+        <v>5100</v>
+      </c>
+      <c r="D63" s="9"/>
       <c r="E63" s="9" t="s">
-        <v>228</v>
-      </c>
-      <c r="F63" s="9" t="s">
-        <v>220</v>
+        <v>233</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="64" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="8" t="s">
-        <v>229</v>
+        <v>235</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>205</v>
+        <v>170</v>
       </c>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
       <c r="E64" s="9" t="s">
-        <v>230</v>
+        <v>236</v>
       </c>
       <c r="F64" s="9" t="s">
-        <v>220</v>
+        <v>237</v>
       </c>
     </row>
     <row r="65" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="1" t="s">
-        <v>231</v>
+      <c r="A65" s="8" t="s">
+        <v>238</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>232</v>
-      </c>
-      <c r="C65" s="10" t="n">
-        <v>1421</v>
-      </c>
-      <c r="D65" s="10" t="s">
-        <v>233</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="C65" s="10"/>
+      <c r="D65" s="10"/>
       <c r="E65" s="9" t="s">
-        <v>234</v>
+        <v>239</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="13" t="s">
-        <v>236</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="C66" s="2" t="n">
-        <v>5300</v>
-      </c>
-      <c r="D66" s="7"/>
-      <c r="E66" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="G66" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="13" t="s">
         <v>240</v>
       </c>
-      <c r="B67" s="2" t="s">
+    </row>
+    <row r="66" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="C67" s="2" t="n">
-        <v>5400</v>
-      </c>
-      <c r="D67" s="7"/>
-      <c r="E67" s="2" t="s">
+      <c r="B66" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="C66" s="10"/>
+      <c r="D66" s="10"/>
+      <c r="E66" s="9" t="s">
         <v>242</v>
       </c>
-      <c r="F67" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="G67" s="3" t="s">
-        <v>11</v>
+      <c r="F66" s="9" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="67" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="B67" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C67" s="10"/>
+      <c r="D67" s="10"/>
+      <c r="E67" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="F67" s="9" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="68" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="12" t="s">
-        <v>243</v>
+      <c r="A68" s="8" t="s">
+        <v>246</v>
       </c>
       <c r="B68" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="C68" s="9" t="n">
-        <v>2811</v>
-      </c>
-      <c r="D68" s="9"/>
+        <v>247</v>
+      </c>
+      <c r="C68" s="10"/>
+      <c r="D68" s="10"/>
       <c r="E68" s="9" t="s">
-        <v>245</v>
-      </c>
-      <c r="G68" s="3" t="s">
-        <v>61</v>
+        <v>248</v>
+      </c>
+      <c r="F68" s="9" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="69" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>247</v>
-      </c>
-      <c r="C69" s="10" t="n">
-        <v>7300</v>
-      </c>
+      <c r="A69" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B69" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C69" s="10"/>
       <c r="D69" s="10"/>
       <c r="E69" s="9" t="s">
-        <v>248</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>61</v>
+        <v>250</v>
+      </c>
+      <c r="F69" s="9" t="s">
+        <v>240</v>
       </c>
     </row>
     <row r="70" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="8" t="s">
-        <v>249</v>
+      <c r="A70" s="1" t="s">
+        <v>251</v>
       </c>
       <c r="B70" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="C70" s="9" t="n">
-        <v>4800</v>
-      </c>
-      <c r="D70" s="9"/>
+        <v>252</v>
+      </c>
+      <c r="C70" s="10" t="n">
+        <v>1421</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>253</v>
+      </c>
       <c r="E70" s="9" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="F70" s="9" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="71" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="B71" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C71" s="10"/>
-      <c r="D71" s="10"/>
-      <c r="E71" s="9" t="s">
-        <v>254</v>
+        <v>255</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C71" s="2" t="n">
+        <v>5300</v>
+      </c>
+      <c r="D71" s="7"/>
+      <c r="E71" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>259</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="72" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="8" t="s">
-        <v>255</v>
-      </c>
-      <c r="B72" s="9" t="s">
-        <v>256</v>
-      </c>
-      <c r="C72" s="9" t="n">
         <v>11</v>
       </c>
-      <c r="D72" s="9"/>
-      <c r="E72" s="9" t="s">
-        <v>257</v>
-      </c>
-      <c r="F72" s="9" t="s">
-        <v>258</v>
+    </row>
+    <row r="72" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="13" t="s">
+        <v>260</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="C72" s="2" t="n">
+        <v>5400</v>
+      </c>
+      <c r="D72" s="7"/>
+      <c r="E72" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="73" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="8" t="s">
-        <v>259</v>
+      <c r="A73" s="12" t="s">
+        <v>263</v>
       </c>
       <c r="B73" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>261</v>
+        <v>264</v>
+      </c>
+      <c r="C73" s="9" t="n">
+        <v>2811</v>
       </c>
       <c r="D73" s="9"/>
       <c r="E73" s="9" t="s">
-        <v>262</v>
-      </c>
-      <c r="F73" s="9" t="s">
-        <v>263</v>
+        <v>265</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="74" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="B74" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="C74" s="9" t="n">
-        <v>22</v>
-      </c>
-      <c r="D74" s="9" t="s">
+      <c r="A74" s="1" t="s">
         <v>266</v>
       </c>
+      <c r="B74" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="C74" s="10" t="n">
+        <v>7300</v>
+      </c>
+      <c r="D74" s="10"/>
       <c r="E74" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="F74" s="2" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G74" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="75" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="8" t="s">
         <v>269</v>
       </c>
@@ -3511,222 +3551,220 @@
         <v>270</v>
       </c>
       <c r="C75" s="9" t="n">
-        <v>7500</v>
+        <v>4800</v>
       </c>
       <c r="D75" s="9"/>
       <c r="E75" s="9" t="s">
         <v>271</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="F75" s="9" t="s">
         <v>272</v>
-      </c>
-      <c r="G75" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="76" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="8" t="s">
         <v>273</v>
       </c>
-      <c r="B76" s="7" t="s">
+      <c r="B76" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10"/>
+      <c r="E76" s="9" t="s">
         <v>274</v>
       </c>
-      <c r="C76" s="9" t="n">
-        <v>6800</v>
-      </c>
-      <c r="D76" s="9"/>
-      <c r="E76" s="9" t="s">
+      <c r="G76" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="77" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="F76" s="9" t="s">
+      <c r="B77" s="9" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="8" t="s">
-        <v>277</v>
-      </c>
-      <c r="B77" s="9" t="s">
-        <v>278</v>
-      </c>
       <c r="C77" s="9" t="n">
-        <v>1711</v>
+        <v>11</v>
       </c>
       <c r="D77" s="9"/>
       <c r="E77" s="9" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="F77" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="G77" s="3" t="s">
-        <v>11</v>
+        <v>278</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="B78" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C78" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="D78" s="9"/>
+      <c r="E78" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="C78" s="10"/>
-      <c r="D78" s="10"/>
-      <c r="E78" s="9" t="s">
+      <c r="F78" s="9" t="s">
         <v>283</v>
-      </c>
-      <c r="F78" s="9" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="79" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="B79" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="B79" s="9" t="s">
-        <v>150</v>
-      </c>
       <c r="C79" s="9" t="n">
-        <v>190</v>
-      </c>
-      <c r="D79" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>286</v>
+      </c>
       <c r="E79" s="9" t="s">
-        <v>286</v>
-      </c>
-      <c r="F79" s="9" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="80" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F79" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="8" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>147</v>
+        <v>290</v>
       </c>
       <c r="C80" s="9" t="n">
-        <v>3000</v>
-      </c>
-      <c r="D80" s="9" t="s">
-        <v>289</v>
-      </c>
+        <v>7500</v>
+      </c>
+      <c r="D80" s="9"/>
       <c r="E80" s="9" t="s">
-        <v>290</v>
-      </c>
-      <c r="F80" s="9" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="81" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F80" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="81" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="8" t="s">
-        <v>292</v>
-      </c>
-      <c r="B81" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="C81" s="10" t="s">
         <v>293</v>
       </c>
-      <c r="D81" s="14" t="s">
+      <c r="B81" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="C81" s="9" t="n">
+        <v>6800</v>
+      </c>
+      <c r="D81" s="9"/>
+      <c r="E81" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="G81" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="82" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F81" s="9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="8" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B82" s="9" t="s">
-        <v>297</v>
-      </c>
-      <c r="C82" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="D82" s="10" t="s">
+      <c r="C82" s="9" t="n">
+        <v>1711</v>
+      </c>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9" t="s">
         <v>299</v>
       </c>
-      <c r="E82" s="9" t="s">
+      <c r="F82" s="9" t="s">
         <v>300</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="83" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="83" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="8" t="s">
         <v>301</v>
       </c>
       <c r="B83" s="9" t="s">
-        <v>150</v>
+        <v>302</v>
       </c>
       <c r="C83" s="10"/>
       <c r="D83" s="10"/>
-      <c r="E83" s="13" t="s">
-        <v>302</v>
+      <c r="E83" s="9" t="s">
+        <v>303</v>
       </c>
       <c r="F83" s="9" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="84" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="8" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B84" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="C84" s="10"/>
-      <c r="D84" s="10"/>
+        <v>170</v>
+      </c>
+      <c r="C84" s="9" t="n">
+        <v>190</v>
+      </c>
+      <c r="D84" s="9"/>
       <c r="E84" s="9" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F84" s="9" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="8" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="C85" s="9" t="n">
-        <v>900</v>
+        <v>3000</v>
       </c>
       <c r="D85" s="9" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="E85" s="9" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="F85" s="9" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="86" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="86" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="8" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B86" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="C86" s="9" t="s">
-        <v>312</v>
-      </c>
-      <c r="D86" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C86" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="E86" s="9" t="s">
+      <c r="D86" s="14" t="s">
         <v>314</v>
       </c>
-      <c r="F86" s="9" t="s">
+      <c r="E86" s="2" t="s">
         <v>315</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="87" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3734,399 +3772,397 @@
         <v>316</v>
       </c>
       <c r="B87" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="C87" s="9" t="n">
-        <v>500</v>
-      </c>
-      <c r="D87" s="9"/>
+        <v>317</v>
+      </c>
+      <c r="C87" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="D87" s="10" t="s">
+        <v>319</v>
+      </c>
       <c r="E87" s="9" t="s">
-        <v>317</v>
-      </c>
-      <c r="F87" s="9" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="88" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>320</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="88" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="8" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="B88" s="9" t="s">
-        <v>320</v>
-      </c>
-      <c r="C88" s="9" t="n">
-        <v>1600</v>
-      </c>
-      <c r="D88" s="9"/>
-      <c r="E88" s="9" t="s">
-        <v>34</v>
+        <v>170</v>
+      </c>
+      <c r="C88" s="10"/>
+      <c r="D88" s="10"/>
+      <c r="E88" s="13" t="s">
+        <v>322</v>
       </c>
       <c r="F88" s="9" t="s">
-        <v>35</v>
+        <v>323</v>
       </c>
     </row>
     <row r="89" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="8" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="B89" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="C89" s="9" t="n">
-        <v>4800</v>
-      </c>
-      <c r="D89" s="9"/>
+        <v>167</v>
+      </c>
+      <c r="C89" s="10"/>
+      <c r="D89" s="10"/>
       <c r="E89" s="9" t="s">
-        <v>251</v>
+        <v>325</v>
       </c>
       <c r="F89" s="9" t="s">
-        <v>252</v>
+        <v>326</v>
       </c>
     </row>
     <row r="90" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="8" t="s">
-        <v>322</v>
+        <v>327</v>
       </c>
       <c r="B90" s="9" t="s">
-        <v>323</v>
-      </c>
-      <c r="C90" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="D90" s="10" t="s">
-        <v>325</v>
+        <v>167</v>
+      </c>
+      <c r="C90" s="9" t="n">
+        <v>900</v>
+      </c>
+      <c r="D90" s="9" t="s">
+        <v>328</v>
       </c>
       <c r="E90" s="9" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="91" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="8" t="s">
-        <v>328</v>
-      </c>
-      <c r="B91" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="C91" s="10"/>
-      <c r="D91" s="10"/>
-      <c r="E91" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="F91" s="2" t="s">
         <v>331</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="F91" s="9" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="92" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="8" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="B92" s="9" t="s">
-        <v>333</v>
-      </c>
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
+        <v>59</v>
+      </c>
+      <c r="C92" s="9" t="n">
+        <v>500</v>
+      </c>
+      <c r="D92" s="9"/>
       <c r="E92" s="9" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="F92" s="9" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
     </row>
     <row r="93" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="8" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="B93" s="9" t="s">
-        <v>337</v>
-      </c>
-      <c r="C93" s="10"/>
-      <c r="D93" s="10"/>
+        <v>340</v>
+      </c>
+      <c r="C93" s="9" t="n">
+        <v>1600</v>
+      </c>
+      <c r="D93" s="9"/>
       <c r="E93" s="9" t="s">
-        <v>338</v>
+        <v>34</v>
       </c>
       <c r="F93" s="9" t="s">
-        <v>339</v>
+        <v>35</v>
       </c>
     </row>
     <row r="94" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="8" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B94" s="9" t="s">
-        <v>341</v>
+        <v>270</v>
       </c>
       <c r="C94" s="9" t="n">
-        <v>131</v>
-      </c>
-      <c r="D94" s="9" t="s">
-        <v>342</v>
-      </c>
+        <v>4800</v>
+      </c>
+      <c r="D94" s="9"/>
       <c r="E94" s="9" t="s">
-        <v>343</v>
+        <v>271</v>
       </c>
       <c r="F94" s="9" t="s">
-        <v>344</v>
+        <v>272</v>
       </c>
     </row>
     <row r="95" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="8" t="s">
+        <v>342</v>
+      </c>
+      <c r="B95" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="C95" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="D95" s="10" t="s">
         <v>345</v>
       </c>
-      <c r="B95" s="9" t="s">
+      <c r="E95" s="9" t="s">
         <v>346</v>
       </c>
-      <c r="C95" s="9" t="n">
-        <v>132</v>
-      </c>
-      <c r="D95" s="9" t="s">
+      <c r="F95" s="9" t="s">
         <v>347</v>
-      </c>
-      <c r="E95" s="9" t="s">
-        <v>348</v>
-      </c>
-      <c r="F95" s="9" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="96" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="8" t="s">
+        <v>348</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="C96" s="10"/>
+      <c r="D96" s="10"/>
+      <c r="E96" s="2" t="s">
         <v>350</v>
       </c>
-      <c r="B96" s="9" t="s">
-        <v>346</v>
-      </c>
-      <c r="C96" s="10" t="n">
-        <v>132</v>
-      </c>
-      <c r="D96" s="10"/>
-      <c r="G96" s="3" t="s">
-        <v>61</v>
+      <c r="F96" s="2" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="97" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="8" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B97" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="C97" s="9" t="n">
-        <v>1731</v>
-      </c>
-      <c r="D97" s="9"/>
+        <v>353</v>
+      </c>
+      <c r="C97" s="10"/>
+      <c r="D97" s="10"/>
       <c r="E97" s="9" t="s">
-        <v>353</v>
-      </c>
-      <c r="G97" s="3" t="s">
-        <v>61</v>
+        <v>354</v>
+      </c>
+      <c r="F97" s="9" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="98" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="8" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B98" s="9" t="s">
-        <v>352</v>
-      </c>
-      <c r="C98" s="9" t="n">
-        <v>1731</v>
-      </c>
-      <c r="D98" s="9"/>
+        <v>357</v>
+      </c>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
+      <c r="E98" s="9" t="s">
+        <v>358</v>
+      </c>
       <c r="F98" s="9" t="s">
-        <v>355</v>
-      </c>
-      <c r="G98" s="3" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="99" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="8" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="B99" s="9" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="C99" s="9" t="n">
-        <v>2811</v>
-      </c>
-      <c r="D99" s="9"/>
+        <v>131</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>362</v>
+      </c>
       <c r="E99" s="9" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="F99" s="9" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
     </row>
     <row r="100" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="8" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="B100" s="9" t="s">
-        <v>94</v>
+        <v>366</v>
       </c>
       <c r="C100" s="9" t="n">
-        <v>200</v>
+        <v>132</v>
       </c>
       <c r="D100" s="9" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
       <c r="E100" s="9" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="F100" s="9" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
     </row>
     <row r="101" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="12" t="s">
-        <v>365</v>
+      <c r="A101" s="8" t="s">
+        <v>370</v>
       </c>
       <c r="B101" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="C101" s="9" t="n">
-        <v>300</v>
-      </c>
-      <c r="D101" s="9" t="s">
-        <v>367</v>
-      </c>
-      <c r="E101" s="9" t="s">
-        <v>368</v>
-      </c>
-      <c r="F101" s="9" t="s">
-        <v>369</v>
+      <c r="C101" s="10" t="n">
+        <v>132</v>
+      </c>
+      <c r="D101" s="10"/>
+      <c r="G101" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="102" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="8" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B102" s="9" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="C102" s="9" t="n">
-        <v>300</v>
-      </c>
-      <c r="D102" s="9" t="s">
-        <v>367</v>
-      </c>
+        <v>1731</v>
+      </c>
+      <c r="D102" s="9"/>
       <c r="E102" s="9" t="s">
-        <v>371</v>
-      </c>
-      <c r="F102" s="9" t="s">
-        <v>372</v>
+        <v>373</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="103" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="8" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B103" s="9" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="C103" s="9" t="n">
-        <v>5500</v>
+        <v>1731</v>
       </c>
       <c r="D103" s="9"/>
-      <c r="E103" s="9" t="s">
+      <c r="F103" s="9" t="s">
         <v>375</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>61</v>
+        <v>376</v>
       </c>
     </row>
     <row r="104" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="8" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B104" s="9" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C104" s="9" t="n">
-        <v>5600</v>
+        <v>2811</v>
       </c>
       <c r="D104" s="9"/>
       <c r="E104" s="9" t="s">
-        <v>378</v>
-      </c>
-      <c r="G104" s="3" t="s">
-        <v>61</v>
+        <v>379</v>
+      </c>
+      <c r="F104" s="9" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="105" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="8" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B105" s="9" t="s">
-        <v>380</v>
+        <v>94</v>
       </c>
       <c r="C105" s="9" t="n">
-        <v>101</v>
+        <v>200</v>
       </c>
       <c r="D105" s="9" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="E105" s="9" t="s">
-        <v>382</v>
-      </c>
-      <c r="G105" s="3" t="s">
-        <v>61</v>
+        <v>383</v>
+      </c>
+      <c r="F105" s="9" t="s">
+        <v>384</v>
       </c>
     </row>
     <row r="106" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="8" t="s">
-        <v>383</v>
+      <c r="A106" s="12" t="s">
+        <v>385</v>
       </c>
       <c r="B106" s="9" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="C106" s="9" t="n">
-        <v>111</v>
+        <v>300</v>
       </c>
       <c r="D106" s="9" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="E106" s="9" t="s">
-        <v>386</v>
-      </c>
-      <c r="G106" s="3" t="s">
-        <v>61</v>
+        <v>388</v>
+      </c>
+      <c r="F106" s="9" t="s">
+        <v>389</v>
       </c>
     </row>
     <row r="107" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>386</v>
+      </c>
+      <c r="C107" s="9" t="n">
+        <v>300</v>
+      </c>
+      <c r="D107" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="B107" s="9" t="s">
-        <v>388</v>
-      </c>
-      <c r="C107" s="10"/>
-      <c r="D107" s="10"/>
       <c r="E107" s="9" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="F107" s="9" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="108" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="8" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B108" s="9" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C108" s="9" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D108" s="9" t="s">
-        <v>393</v>
-      </c>
+        <v>5500</v>
+      </c>
+      <c r="D108" s="9"/>
       <c r="E108" s="9" t="s">
-        <v>309</v>
+        <v>395</v>
       </c>
       <c r="G108" s="3" t="s">
         <v>61</v>
@@ -4134,22 +4170,20 @@
     </row>
     <row r="109" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="8" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="B109" s="9" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="C109" s="9" t="n">
-        <v>112</v>
-      </c>
-      <c r="D109" s="9" t="s">
-        <v>396</v>
-      </c>
+        <v>5600</v>
+      </c>
+      <c r="D109" s="9"/>
       <c r="E109" s="9" t="s">
-        <v>397</v>
-      </c>
-      <c r="F109" s="9" t="s">
         <v>398</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4157,70 +4191,72 @@
         <v>399</v>
       </c>
       <c r="B110" s="9" t="s">
-        <v>94</v>
+        <v>400</v>
       </c>
       <c r="C110" s="9" t="n">
-        <v>3100</v>
-      </c>
-      <c r="D110" s="9"/>
+        <v>101</v>
+      </c>
+      <c r="D110" s="9" t="s">
+        <v>401</v>
+      </c>
       <c r="E110" s="9" t="s">
-        <v>400</v>
-      </c>
-      <c r="F110" s="9" t="s">
-        <v>401</v>
+        <v>402</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="111" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="8" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B111" s="9" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C111" s="9" t="n">
-        <v>21</v>
-      </c>
-      <c r="D111" s="9"/>
+        <v>111</v>
+      </c>
+      <c r="D111" s="9" t="s">
+        <v>405</v>
+      </c>
       <c r="E111" s="9" t="s">
-        <v>404</v>
-      </c>
-      <c r="F111" s="9" t="s">
-        <v>405</v>
+        <v>406</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="112" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="8" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B112" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="C112" s="9" t="n">
-        <v>122</v>
-      </c>
-      <c r="D112" s="9" t="s">
-        <v>407</v>
-      </c>
+        <v>408</v>
+      </c>
+      <c r="C112" s="10"/>
+      <c r="D112" s="10"/>
       <c r="E112" s="9" t="s">
-        <v>408</v>
-      </c>
-      <c r="G112" s="3" t="s">
-        <v>61</v>
+        <v>409</v>
+      </c>
+      <c r="F112" s="9" t="s">
+        <v>410</v>
       </c>
     </row>
     <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="8" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B113" s="9" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C113" s="9" t="n">
-        <v>1722</v>
-      </c>
-      <c r="D113" s="9"/>
+        <v>1000</v>
+      </c>
+      <c r="D113" s="9" t="s">
+        <v>413</v>
+      </c>
       <c r="E113" s="9" t="s">
-        <v>411</v>
+        <v>329</v>
       </c>
       <c r="G113" s="3" t="s">
         <v>61</v>
@@ -4228,110 +4264,114 @@
     </row>
     <row r="114" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="8" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="B114" s="9" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="C114" s="9" t="n">
-        <v>7100</v>
-      </c>
-      <c r="D114" s="9"/>
+        <v>112</v>
+      </c>
+      <c r="D114" s="9" t="s">
+        <v>416</v>
+      </c>
       <c r="E114" s="9" t="s">
-        <v>414</v>
-      </c>
-      <c r="G114" s="3" t="s">
-        <v>61</v>
+        <v>417</v>
+      </c>
+      <c r="F114" s="9" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="115" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="8" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="B115" s="9" t="s">
-        <v>416</v>
-      </c>
-      <c r="C115" s="10"/>
-      <c r="D115" s="10"/>
+        <v>94</v>
+      </c>
+      <c r="C115" s="9" t="n">
+        <v>3100</v>
+      </c>
+      <c r="D115" s="9"/>
       <c r="E115" s="9" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="F115" s="9" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="116" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="8" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="B116" s="9" t="s">
-        <v>420</v>
-      </c>
-      <c r="C116" s="10"/>
-      <c r="D116" s="10"/>
+        <v>423</v>
+      </c>
+      <c r="C116" s="9" t="n">
+        <v>21</v>
+      </c>
+      <c r="D116" s="9"/>
       <c r="E116" s="9" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="F116" s="9" t="s">
-        <v>422</v>
-      </c>
-      <c r="G116" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="117" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="8" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="B117" s="9" t="s">
-        <v>424</v>
-      </c>
-      <c r="C117" s="10"/>
-      <c r="D117" s="10"/>
+        <v>244</v>
+      </c>
+      <c r="C117" s="9" t="n">
+        <v>122</v>
+      </c>
+      <c r="D117" s="9" t="s">
+        <v>427</v>
+      </c>
       <c r="E117" s="9" t="s">
-        <v>425</v>
-      </c>
-      <c r="F117" s="9" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="1" t="s">
-        <v>427</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="118" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="8" t="s">
+        <v>429</v>
       </c>
       <c r="B118" s="9" t="s">
-        <v>428</v>
-      </c>
-      <c r="C118" s="10"/>
-      <c r="D118" s="10"/>
+        <v>430</v>
+      </c>
+      <c r="C118" s="9" t="n">
+        <v>1722</v>
+      </c>
+      <c r="D118" s="9"/>
       <c r="E118" s="9" t="s">
-        <v>429</v>
-      </c>
-      <c r="F118" s="9" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="B119" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="119" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="8" t="s">
         <v>432</v>
       </c>
-      <c r="C119" s="2" t="n">
-        <v>133</v>
-      </c>
-      <c r="E119" s="2" t="s">
+      <c r="B119" s="9" t="s">
         <v>433</v>
       </c>
-      <c r="F119" s="2" t="s">
+      <c r="C119" s="9" t="n">
+        <v>7100</v>
+      </c>
+      <c r="D119" s="9"/>
+      <c r="E119" s="9" t="s">
         <v>434</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="120" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4339,14 +4379,10 @@
         <v>435</v>
       </c>
       <c r="B120" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C120" s="9" t="n">
-        <v>400</v>
-      </c>
-      <c r="D120" s="9" t="s">
         <v>436</v>
       </c>
+      <c r="C120" s="10"/>
+      <c r="D120" s="10"/>
       <c r="E120" s="9" t="s">
         <v>437</v>
       </c>
@@ -4354,105 +4390,111 @@
         <v>438</v>
       </c>
     </row>
-    <row r="121" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="1" t="s">
+    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="8" t="s">
         <v>439</v>
       </c>
       <c r="B121" s="9" t="s">
         <v>440</v>
       </c>
-      <c r="C121" s="9" t="n">
-        <v>400</v>
-      </c>
-      <c r="D121" s="9"/>
+      <c r="C121" s="10"/>
+      <c r="D121" s="10"/>
       <c r="E121" s="9" t="s">
         <v>441</v>
       </c>
       <c r="F121" s="9" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="122" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="1" t="s">
+      <c r="G121" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A122" s="8" t="s">
         <v>443</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B122" s="9" t="s">
         <v>444</v>
       </c>
-      <c r="C122" s="2" t="n">
-        <v>2612</v>
-      </c>
-      <c r="D122" s="2" t="s">
+      <c r="C122" s="10"/>
+      <c r="D122" s="10"/>
+      <c r="E122" s="9" t="s">
         <v>445</v>
       </c>
-      <c r="E122" s="2" t="s">
+      <c r="F122" s="9" t="s">
         <v>446</v>
       </c>
-      <c r="F122" s="9" t="s">
+      <c r="G122" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="s">
         <v>447</v>
       </c>
-    </row>
-    <row r="123" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="8" t="s">
+      <c r="B123" s="9" t="s">
         <v>448</v>
       </c>
-      <c r="B123" s="9" t="s">
+      <c r="C123" s="10"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="9" t="s">
         <v>449</v>
       </c>
-      <c r="C123" s="9" t="s">
+      <c r="F123" s="9" t="s">
         <v>450</v>
       </c>
-      <c r="D123" s="9"/>
-      <c r="E123" s="9" t="s">
+      <c r="G123" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="124" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A124" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="F123" s="9" t="s">
+      <c r="B124" s="2" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="124" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A124" s="8" t="s">
+      <c r="C124" s="2" t="n">
+        <v>133</v>
+      </c>
+      <c r="E124" s="2" t="s">
         <v>453</v>
       </c>
-      <c r="B124" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="C124" s="10"/>
-      <c r="D124" s="10"/>
-      <c r="E124" s="9" t="s">
+      <c r="F124" s="2" t="s">
         <v>454</v>
-      </c>
-      <c r="F124" s="9" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="125" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="B125" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C125" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="D125" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="B125" s="9" t="s">
+      <c r="E125" s="9" t="s">
         <v>457</v>
       </c>
-      <c r="C125" s="9" t="n">
-        <v>7600</v>
-      </c>
-      <c r="D125" s="9"/>
-      <c r="E125" s="9" t="s">
+      <c r="F125" s="9" t="s">
         <v>458</v>
       </c>
-      <c r="F125" s="9" t="s">
+    </row>
+    <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A126" s="1" t="s">
         <v>459</v>
       </c>
-    </row>
-    <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="8" t="s">
+      <c r="B126" s="9" t="s">
         <v>460</v>
       </c>
-      <c r="B126" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="C126" s="10"/>
-      <c r="D126" s="10"/>
+      <c r="C126" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="D126" s="9"/>
       <c r="E126" s="9" t="s">
         <v>461</v>
       </c>
@@ -4461,134 +4503,136 @@
       </c>
     </row>
     <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="8" t="s">
+      <c r="A127" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="B127" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C127" s="9" t="n">
-        <v>6000</v>
-      </c>
-      <c r="D127" s="9"/>
-      <c r="E127" s="9" t="s">
+      <c r="B127" s="2" t="s">
         <v>464</v>
       </c>
+      <c r="C127" s="2" t="n">
+        <v>2612</v>
+      </c>
+      <c r="D127" s="2" t="s">
+        <v>465</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>466</v>
+      </c>
       <c r="F127" s="9" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="128" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="8" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C128" s="10"/>
-      <c r="D128" s="10"/>
+        <v>469</v>
+      </c>
+      <c r="C128" s="9" t="s">
+        <v>470</v>
+      </c>
+      <c r="D128" s="9"/>
       <c r="E128" s="9" t="s">
-        <v>467</v>
+        <v>471</v>
       </c>
       <c r="F128" s="9" t="s">
-        <v>468</v>
+        <v>472</v>
       </c>
     </row>
     <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="8" t="s">
-        <v>469</v>
+        <v>473</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>470</v>
+        <v>167</v>
       </c>
       <c r="C129" s="10"/>
       <c r="D129" s="10"/>
       <c r="E129" s="9" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="F129" s="9" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="130" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="8" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>474</v>
-      </c>
-      <c r="C130" s="10"/>
-      <c r="D130" s="10"/>
+        <v>477</v>
+      </c>
+      <c r="C130" s="9" t="n">
+        <v>7600</v>
+      </c>
+      <c r="D130" s="9"/>
       <c r="E130" s="9" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="F130" s="9" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
     </row>
     <row r="131" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="8" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>474</v>
+        <v>167</v>
       </c>
       <c r="C131" s="10"/>
       <c r="D131" s="10"/>
       <c r="E131" s="9" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="F131" s="9" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
     </row>
     <row r="132" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="8" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>481</v>
-      </c>
-      <c r="C132" s="10"/>
-      <c r="D132" s="10"/>
+        <v>170</v>
+      </c>
+      <c r="C132" s="9" t="n">
+        <v>6000</v>
+      </c>
+      <c r="D132" s="9"/>
       <c r="E132" s="9" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="F132" s="9" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
     </row>
     <row r="133" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="8" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>485</v>
-      </c>
-      <c r="C133" s="9" t="n">
-        <v>5800</v>
-      </c>
-      <c r="D133" s="9"/>
+        <v>225</v>
+      </c>
+      <c r="C133" s="10"/>
+      <c r="D133" s="10"/>
       <c r="E133" s="9" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="F133" s="9" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="134" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="8" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>489</v>
-      </c>
-      <c r="C134" s="9" t="n">
-        <v>7700</v>
-      </c>
-      <c r="D134" s="9" t="s">
         <v>490</v>
       </c>
+      <c r="C134" s="10"/>
+      <c r="D134" s="10"/>
       <c r="E134" s="9" t="s">
         <v>491</v>
       </c>
@@ -4603,17 +4647,13 @@
       <c r="B135" s="9" t="s">
         <v>494</v>
       </c>
-      <c r="C135" s="9" t="n">
-        <v>7800</v>
-      </c>
-      <c r="D135" s="9" t="s">
+      <c r="C135" s="10"/>
+      <c r="D135" s="10"/>
+      <c r="E135" s="9" t="s">
         <v>495</v>
       </c>
-      <c r="E135" s="9" t="s">
+      <c r="F135" s="9" t="s">
         <v>496</v>
-      </c>
-      <c r="F135" s="9" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4621,82 +4661,86 @@
         <v>497</v>
       </c>
       <c r="B136" s="9" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C136" s="10"/>
       <c r="D136" s="10"/>
       <c r="E136" s="9" t="s">
+        <v>498</v>
+      </c>
+      <c r="F136" s="9" t="s">
         <v>499</v>
-      </c>
-      <c r="F136" s="9" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="8" t="s">
+        <v>500</v>
+      </c>
+      <c r="B137" s="9" t="s">
         <v>501</v>
       </c>
-      <c r="B137" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C137" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="D137" s="10" t="s">
+      <c r="C137" s="10"/>
+      <c r="D137" s="10"/>
+      <c r="E137" s="9" t="s">
         <v>502</v>
       </c>
-      <c r="E137" s="9" t="s">
+      <c r="F137" s="9" t="s">
         <v>503</v>
-      </c>
-      <c r="F137" s="9" t="s">
-        <v>504</v>
       </c>
     </row>
     <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="8" t="s">
+        <v>504</v>
+      </c>
+      <c r="B138" s="9" t="s">
         <v>505</v>
       </c>
-      <c r="B138" s="9" t="s">
+      <c r="C138" s="9" t="n">
+        <v>5800</v>
+      </c>
+      <c r="D138" s="9"/>
+      <c r="E138" s="9" t="s">
         <v>506</v>
       </c>
-      <c r="C138" s="10"/>
-      <c r="D138" s="10"/>
-      <c r="E138" s="9" t="s">
+      <c r="F138" s="9" t="s">
         <v>507</v>
-      </c>
-      <c r="F138" s="9" t="s">
-        <v>508</v>
       </c>
     </row>
     <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="B139" s="9" t="s">
         <v>509</v>
       </c>
-      <c r="B139" s="9" t="s">
-        <v>380</v>
-      </c>
       <c r="C139" s="9" t="n">
-        <v>101</v>
-      </c>
-      <c r="D139" s="9"/>
+        <v>7700</v>
+      </c>
+      <c r="D139" s="9" t="s">
+        <v>510</v>
+      </c>
       <c r="E139" s="9" t="s">
-        <v>382</v>
-      </c>
-      <c r="G139" s="3" t="s">
-        <v>61</v>
+        <v>511</v>
+      </c>
+      <c r="F139" s="9" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="8" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="B140" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="C140" s="10"/>
-      <c r="D140" s="10"/>
+        <v>514</v>
+      </c>
+      <c r="C140" s="9" t="n">
+        <v>7800</v>
+      </c>
+      <c r="D140" s="9" t="s">
+        <v>515</v>
+      </c>
       <c r="E140" s="9" t="s">
-        <v>511</v>
+        <v>516</v>
       </c>
       <c r="F140" s="9" t="s">
         <v>512</v>
@@ -4704,78 +4748,72 @@
     </row>
     <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="8" t="s">
-        <v>513</v>
+        <v>517</v>
       </c>
       <c r="B141" s="9" t="s">
-        <v>227</v>
+        <v>518</v>
       </c>
       <c r="C141" s="10"/>
-      <c r="D141" s="10" t="s">
-        <v>514</v>
-      </c>
+      <c r="D141" s="10"/>
       <c r="E141" s="9" t="s">
-        <v>515</v>
+        <v>519</v>
       </c>
       <c r="F141" s="9" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
     </row>
     <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="8" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="B142" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C142" s="9" t="n">
-        <v>1400</v>
-      </c>
-      <c r="D142" s="9" t="s">
-        <v>518</v>
+        <v>170</v>
+      </c>
+      <c r="C142" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="D142" s="10" t="s">
+        <v>522</v>
       </c>
       <c r="E142" s="9" t="s">
-        <v>519</v>
+        <v>523</v>
       </c>
       <c r="F142" s="9" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
     </row>
     <row r="143" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A143" s="1" t="s">
-        <v>521</v>
+      <c r="A143" s="8" t="s">
+        <v>525</v>
       </c>
       <c r="B143" s="9" t="s">
-        <v>522</v>
-      </c>
-      <c r="C143" s="9" t="n">
-        <v>7400</v>
-      </c>
-      <c r="D143" s="9" t="s">
-        <v>117</v>
-      </c>
+        <v>526</v>
+      </c>
+      <c r="C143" s="10"/>
+      <c r="D143" s="10"/>
       <c r="E143" s="9" t="s">
-        <v>523</v>
+        <v>527</v>
       </c>
       <c r="F143" s="9" t="s">
-        <v>524</v>
+        <v>528</v>
       </c>
     </row>
     <row r="144" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="8" t="s">
-        <v>525</v>
+        <v>529</v>
       </c>
       <c r="B144" s="9" t="s">
-        <v>526</v>
-      </c>
-      <c r="C144" s="10"/>
-      <c r="D144" s="10" t="s">
-        <v>527</v>
-      </c>
+        <v>400</v>
+      </c>
+      <c r="C144" s="9" t="n">
+        <v>101</v>
+      </c>
+      <c r="D144" s="9"/>
       <c r="E144" s="9" t="s">
-        <v>528</v>
-      </c>
-      <c r="F144" s="9" t="s">
-        <v>529</v>
+        <v>402</v>
+      </c>
+      <c r="G144" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4783,50 +4821,48 @@
         <v>530</v>
       </c>
       <c r="B145" s="9" t="s">
-        <v>474</v>
-      </c>
-      <c r="C145" s="9" t="n">
-        <v>1700</v>
-      </c>
-      <c r="D145" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="C145" s="10"/>
+      <c r="D145" s="10"/>
+      <c r="E145" s="9" t="s">
         <v>531</v>
       </c>
-      <c r="E145" s="9" t="s">
+      <c r="F145" s="9" t="s">
         <v>532</v>
-      </c>
-      <c r="F145" s="9" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="146" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="8" t="s">
+        <v>533</v>
+      </c>
+      <c r="B146" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="C146" s="10"/>
+      <c r="D146" s="10" t="s">
         <v>534</v>
       </c>
-      <c r="B146" s="9" t="s">
+      <c r="E146" s="9" t="s">
         <v>535</v>
       </c>
-      <c r="C146" s="9" t="n">
-        <v>1800</v>
-      </c>
-      <c r="D146" s="9" t="s">
-        <v>117</v>
-      </c>
-      <c r="E146" s="9" t="s">
+      <c r="F146" s="9" t="s">
         <v>536</v>
-      </c>
-      <c r="F146" s="9" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="8" t="s">
+        <v>537</v>
+      </c>
+      <c r="B147" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C147" s="9" t="n">
+        <v>1400</v>
+      </c>
+      <c r="D147" s="9" t="s">
         <v>538</v>
       </c>
-      <c r="B147" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="C147" s="7"/>
-      <c r="D147" s="7"/>
       <c r="E147" s="9" t="s">
         <v>539</v>
       </c>
@@ -4835,114 +4871,128 @@
       </c>
     </row>
     <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A148" s="8" t="s">
+      <c r="A148" s="1" t="s">
         <v>541</v>
       </c>
       <c r="B148" s="9" t="s">
-        <v>205</v>
-      </c>
-      <c r="C148" s="10" t="s">
         <v>542</v>
       </c>
-      <c r="D148" s="10"/>
+      <c r="C148" s="9" t="n">
+        <v>7400</v>
+      </c>
+      <c r="D148" s="9" t="s">
+        <v>117</v>
+      </c>
       <c r="E148" s="9" t="s">
         <v>543</v>
       </c>
       <c r="F148" s="9" t="s">
-        <v>540</v>
+        <v>544</v>
       </c>
     </row>
     <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="8" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B149" s="9" t="s">
-        <v>526</v>
+        <v>546</v>
       </c>
       <c r="C149" s="10"/>
-      <c r="D149" s="10"/>
+      <c r="D149" s="10" t="s">
+        <v>547</v>
+      </c>
       <c r="E149" s="9" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="F149" s="9" t="s">
-        <v>540</v>
+        <v>549</v>
       </c>
     </row>
     <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="8" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="B150" s="9" t="s">
-        <v>474</v>
-      </c>
-      <c r="C150" s="10"/>
-      <c r="D150" s="10"/>
+        <v>494</v>
+      </c>
+      <c r="C150" s="9" t="n">
+        <v>1700</v>
+      </c>
+      <c r="D150" s="9" t="s">
+        <v>551</v>
+      </c>
       <c r="E150" s="9" t="s">
-        <v>547</v>
+        <v>552</v>
       </c>
       <c r="F150" s="9" t="s">
-        <v>540</v>
+        <v>553</v>
       </c>
     </row>
     <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="8" t="s">
-        <v>548</v>
+        <v>554</v>
       </c>
       <c r="B151" s="9" t="s">
-        <v>549</v>
-      </c>
-      <c r="C151" s="10"/>
-      <c r="D151" s="10"/>
+        <v>555</v>
+      </c>
+      <c r="C151" s="9" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D151" s="9" t="s">
+        <v>117</v>
+      </c>
       <c r="E151" s="9" t="s">
-        <v>550</v>
+        <v>556</v>
       </c>
       <c r="F151" s="9" t="s">
-        <v>551</v>
+        <v>557</v>
       </c>
     </row>
     <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="8" t="s">
-        <v>552</v>
+        <v>558</v>
       </c>
       <c r="B152" s="9" t="s">
-        <v>526</v>
-      </c>
-      <c r="C152" s="10"/>
-      <c r="D152" s="10"/>
+        <v>247</v>
+      </c>
+      <c r="C152" s="7"/>
+      <c r="D152" s="7"/>
       <c r="E152" s="9" t="s">
-        <v>553</v>
+        <v>559</v>
       </c>
       <c r="F152" s="9" t="s">
-        <v>554</v>
+        <v>560</v>
       </c>
     </row>
     <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="8" t="s">
-        <v>555</v>
+        <v>561</v>
       </c>
       <c r="B153" s="9" t="s">
-        <v>474</v>
-      </c>
-      <c r="C153" s="10"/>
+        <v>225</v>
+      </c>
+      <c r="C153" s="10" t="s">
+        <v>562</v>
+      </c>
       <c r="D153" s="10"/>
       <c r="E153" s="9" t="s">
-        <v>556</v>
+        <v>563</v>
       </c>
       <c r="F153" s="9" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
     </row>
     <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="8" t="s">
-        <v>558</v>
+        <v>564</v>
       </c>
       <c r="B154" s="9" t="s">
-        <v>205</v>
+        <v>546</v>
       </c>
       <c r="C154" s="10"/>
       <c r="D154" s="10"/>
       <c r="E154" s="9" t="s">
-        <v>559</v>
+        <v>565</v>
       </c>
       <c r="F154" s="9" t="s">
         <v>560</v>
@@ -4950,563 +5000,643 @@
     </row>
     <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="8" t="s">
-        <v>561</v>
+        <v>566</v>
       </c>
       <c r="B155" s="9" t="s">
-        <v>147</v>
+        <v>494</v>
       </c>
       <c r="C155" s="10"/>
       <c r="D155" s="10"/>
       <c r="E155" s="9" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
       <c r="F155" s="9" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="8" t="s">
-        <v>564</v>
+        <v>568</v>
       </c>
       <c r="B156" s="9" t="s">
-        <v>150</v>
+        <v>569</v>
       </c>
       <c r="C156" s="10"/>
       <c r="D156" s="10"/>
       <c r="E156" s="9" t="s">
-        <v>565</v>
+        <v>570</v>
       </c>
       <c r="F156" s="9" t="s">
-        <v>566</v>
+        <v>571</v>
       </c>
     </row>
     <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="8" t="s">
-        <v>567</v>
+        <v>572</v>
       </c>
       <c r="B157" s="9" t="s">
-        <v>227</v>
+        <v>546</v>
       </c>
       <c r="C157" s="10"/>
       <c r="D157" s="10"/>
       <c r="E157" s="9" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
       <c r="F157" s="9" t="s">
-        <v>569</v>
+        <v>574</v>
       </c>
     </row>
     <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="8" t="s">
-        <v>570</v>
+        <v>575</v>
       </c>
       <c r="B158" s="9" t="s">
-        <v>474</v>
+        <v>494</v>
       </c>
       <c r="C158" s="10"/>
       <c r="D158" s="10"/>
       <c r="E158" s="9" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="F158" s="9" t="s">
-        <v>572</v>
+        <v>577</v>
       </c>
     </row>
     <row r="159" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="8" t="s">
-        <v>573</v>
+        <v>578</v>
       </c>
       <c r="B159" s="9" t="s">
-        <v>147</v>
+        <v>225</v>
       </c>
       <c r="C159" s="10"/>
       <c r="D159" s="10"/>
       <c r="E159" s="9" t="s">
-        <v>574</v>
+        <v>579</v>
       </c>
       <c r="F159" s="9" t="s">
-        <v>575</v>
+        <v>580</v>
       </c>
     </row>
     <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="8" t="s">
-        <v>576</v>
+        <v>581</v>
       </c>
       <c r="B160" s="9" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="C160" s="10"/>
       <c r="D160" s="10"/>
       <c r="E160" s="9" t="s">
-        <v>577</v>
+        <v>582</v>
       </c>
       <c r="F160" s="9" t="s">
-        <v>578</v>
+        <v>583</v>
       </c>
     </row>
     <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="8" t="s">
-        <v>579</v>
+        <v>584</v>
       </c>
       <c r="B161" s="9" t="s">
-        <v>227</v>
+        <v>170</v>
       </c>
       <c r="C161" s="10"/>
       <c r="D161" s="10"/>
       <c r="E161" s="9" t="s">
-        <v>580</v>
+        <v>585</v>
       </c>
       <c r="F161" s="9" t="s">
-        <v>581</v>
+        <v>586</v>
       </c>
     </row>
     <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="8" t="s">
-        <v>582</v>
+        <v>587</v>
       </c>
       <c r="B162" s="9" t="s">
-        <v>205</v>
+        <v>247</v>
       </c>
       <c r="C162" s="10"/>
       <c r="D162" s="10"/>
       <c r="E162" s="9" t="s">
-        <v>583</v>
+        <v>588</v>
       </c>
       <c r="F162" s="9" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
     </row>
     <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="8" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="B163" s="9" t="s">
-        <v>526</v>
+        <v>494</v>
       </c>
       <c r="C163" s="10"/>
       <c r="D163" s="10"/>
       <c r="E163" s="9" t="s">
-        <v>586</v>
+        <v>591</v>
       </c>
       <c r="F163" s="9" t="s">
-        <v>587</v>
+        <v>592</v>
       </c>
     </row>
     <row r="164" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="8" t="s">
-        <v>588</v>
+        <v>593</v>
       </c>
       <c r="B164" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="C164" s="9" t="n">
-        <v>121</v>
-      </c>
-      <c r="D164" s="9"/>
+        <v>167</v>
+      </c>
+      <c r="C164" s="10"/>
+      <c r="D164" s="10"/>
       <c r="E164" s="9" t="s">
-        <v>590</v>
-      </c>
-      <c r="G164" s="3" t="s">
-        <v>61</v>
+        <v>594</v>
+      </c>
+      <c r="F164" s="9" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="8" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="B165" s="9" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="C165" s="10"/>
       <c r="D165" s="10"/>
       <c r="E165" s="9" t="s">
-        <v>592</v>
+        <v>597</v>
       </c>
       <c r="F165" s="9" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
     </row>
     <row r="166" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="8" t="s">
-        <v>594</v>
+        <v>599</v>
       </c>
       <c r="B166" s="9" t="s">
-        <v>205</v>
+        <v>247</v>
       </c>
       <c r="C166" s="10"/>
       <c r="D166" s="10"/>
       <c r="E166" s="9" t="s">
-        <v>595</v>
+        <v>600</v>
       </c>
       <c r="F166" s="9" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
     </row>
     <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="8" t="s">
-        <v>597</v>
+        <v>602</v>
       </c>
       <c r="B167" s="9" t="s">
-        <v>384</v>
-      </c>
-      <c r="C167" s="9" t="n">
-        <v>111</v>
-      </c>
-      <c r="D167" s="9"/>
+        <v>225</v>
+      </c>
+      <c r="C167" s="10"/>
+      <c r="D167" s="10"/>
       <c r="E167" s="9" t="s">
-        <v>386</v>
-      </c>
-      <c r="G167" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>603</v>
+      </c>
+      <c r="F167" s="9" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="8" t="s">
-        <v>598</v>
+        <v>605</v>
       </c>
       <c r="B168" s="9" t="s">
-        <v>278</v>
-      </c>
-      <c r="C168" s="9" t="n">
-        <v>1711</v>
-      </c>
-      <c r="D168" s="9"/>
+        <v>546</v>
+      </c>
+      <c r="C168" s="10"/>
+      <c r="D168" s="10"/>
       <c r="E168" s="9" t="s">
-        <v>599</v>
+        <v>606</v>
       </c>
       <c r="F168" s="9" t="s">
-        <v>280</v>
-      </c>
-      <c r="G168" s="3" t="s">
-        <v>11</v>
+        <v>607</v>
       </c>
     </row>
     <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A169" s="1" t="s">
-        <v>600</v>
+      <c r="A169" s="8" t="s">
+        <v>608</v>
       </c>
       <c r="B169" s="9" t="s">
-        <v>601</v>
+        <v>609</v>
       </c>
       <c r="C169" s="9" t="n">
-        <v>3300</v>
+        <v>121</v>
       </c>
       <c r="D169" s="9"/>
       <c r="E169" s="9" t="s">
-        <v>602</v>
-      </c>
-      <c r="F169" s="9" t="s">
-        <v>603</v>
+        <v>610</v>
+      </c>
+      <c r="G169" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="8" t="s">
-        <v>604</v>
+        <v>611</v>
       </c>
       <c r="B170" s="9" t="s">
-        <v>605</v>
-      </c>
-      <c r="C170" s="9" t="n">
-        <v>8000</v>
-      </c>
-      <c r="D170" s="9" t="s">
-        <v>606</v>
-      </c>
+        <v>167</v>
+      </c>
+      <c r="C170" s="10"/>
+      <c r="D170" s="10"/>
       <c r="E170" s="9" t="s">
-        <v>607</v>
+        <v>612</v>
       </c>
       <c r="F170" s="9" t="s">
-        <v>608</v>
+        <v>613</v>
       </c>
     </row>
     <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="8" t="s">
-        <v>609</v>
+        <v>614</v>
       </c>
       <c r="B171" s="9" t="s">
-        <v>147</v>
+        <v>225</v>
       </c>
       <c r="C171" s="10"/>
       <c r="D171" s="10"/>
       <c r="E171" s="9" t="s">
-        <v>610</v>
+        <v>615</v>
       </c>
       <c r="F171" s="9" t="s">
-        <v>611</v>
+        <v>616</v>
       </c>
     </row>
     <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="8" t="s">
-        <v>612</v>
+        <v>617</v>
       </c>
       <c r="B172" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C172" s="10"/>
-      <c r="D172" s="10"/>
+        <v>404</v>
+      </c>
+      <c r="C172" s="9" t="n">
+        <v>111</v>
+      </c>
+      <c r="D172" s="9"/>
       <c r="E172" s="9" t="s">
-        <v>613</v>
-      </c>
-      <c r="F172" s="9" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>406</v>
+      </c>
+      <c r="G172" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="8" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="B173" s="9" t="s">
-        <v>224</v>
-      </c>
-      <c r="C173" s="10"/>
-      <c r="D173" s="10"/>
+        <v>298</v>
+      </c>
+      <c r="C173" s="9" t="n">
+        <v>1711</v>
+      </c>
+      <c r="D173" s="9"/>
       <c r="E173" s="9" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="F173" s="9" t="s">
-        <v>617</v>
+        <v>300</v>
+      </c>
+      <c r="G173" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A174" s="8" t="s">
-        <v>618</v>
+      <c r="A174" s="1" t="s">
+        <v>620</v>
       </c>
       <c r="B174" s="9" t="s">
-        <v>116</v>
+        <v>621</v>
       </c>
       <c r="C174" s="9" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D174" s="9" t="s">
-        <v>619</v>
-      </c>
+        <v>3300</v>
+      </c>
+      <c r="D174" s="9"/>
       <c r="E174" s="9" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
       <c r="F174" s="9" t="s">
-        <v>119</v>
+        <v>623</v>
       </c>
     </row>
     <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="8" t="s">
-        <v>621</v>
-      </c>
-      <c r="B175" s="7" t="s">
-        <v>622</v>
+        <v>624</v>
+      </c>
+      <c r="B175" s="9" t="s">
+        <v>625</v>
       </c>
       <c r="C175" s="9" t="n">
-        <v>2611</v>
-      </c>
-      <c r="D175" s="9"/>
+        <v>8000</v>
+      </c>
+      <c r="D175" s="9" t="s">
+        <v>626</v>
+      </c>
       <c r="E175" s="9" t="s">
-        <v>623</v>
-      </c>
-      <c r="G175" s="3" t="s">
-        <v>61</v>
+        <v>627</v>
+      </c>
+      <c r="F175" s="9" t="s">
+        <v>628</v>
       </c>
     </row>
     <row r="176" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="8" t="s">
-        <v>624</v>
+        <v>629</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>625</v>
-      </c>
-      <c r="C176" s="9" t="n">
-        <v>2711</v>
-      </c>
-      <c r="D176" s="9"/>
+        <v>167</v>
+      </c>
+      <c r="C176" s="10"/>
+      <c r="D176" s="10"/>
       <c r="E176" s="9" t="s">
-        <v>626</v>
-      </c>
-      <c r="G176" s="3" t="s">
-        <v>61</v>
+        <v>630</v>
+      </c>
+      <c r="F176" s="9" t="s">
+        <v>631</v>
       </c>
     </row>
     <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="8" t="s">
-        <v>627</v>
+        <v>632</v>
       </c>
       <c r="B177" s="9" t="s">
-        <v>205</v>
+        <v>170</v>
       </c>
       <c r="C177" s="10"/>
       <c r="D177" s="10"/>
       <c r="E177" s="9" t="s">
-        <v>628</v>
+        <v>633</v>
       </c>
       <c r="F177" s="9" t="s">
-        <v>629</v>
+        <v>634</v>
       </c>
     </row>
     <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="8" t="s">
-        <v>630</v>
+        <v>635</v>
       </c>
       <c r="B178" s="9" t="s">
-        <v>631</v>
+        <v>244</v>
       </c>
       <c r="C178" s="10"/>
       <c r="D178" s="10"/>
       <c r="E178" s="9" t="s">
-        <v>632</v>
+        <v>636</v>
       </c>
       <c r="F178" s="9" t="s">
-        <v>633</v>
+        <v>637</v>
       </c>
     </row>
     <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="8" t="s">
-        <v>634</v>
+        <v>638</v>
       </c>
       <c r="B179" s="9" t="s">
-        <v>635</v>
+        <v>116</v>
       </c>
       <c r="C179" s="9" t="n">
-        <v>3721</v>
-      </c>
-      <c r="D179" s="9"/>
+        <v>1500</v>
+      </c>
+      <c r="D179" s="9" t="s">
+        <v>639</v>
+      </c>
       <c r="E179" s="9" t="s">
-        <v>636</v>
+        <v>640</v>
       </c>
       <c r="F179" s="9" t="s">
-        <v>637</v>
+        <v>119</v>
       </c>
     </row>
     <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="8" t="s">
-        <v>638</v>
-      </c>
-      <c r="B180" s="9" t="s">
-        <v>474</v>
+        <v>641</v>
+      </c>
+      <c r="B180" s="7" t="s">
+        <v>642</v>
       </c>
       <c r="C180" s="9" t="n">
-        <v>6100</v>
+        <v>2611</v>
       </c>
       <c r="D180" s="9"/>
       <c r="E180" s="9" t="s">
-        <v>639</v>
-      </c>
-      <c r="F180" s="9" t="s">
-        <v>640</v>
+        <v>643</v>
+      </c>
+      <c r="G180" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="8" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="B181" s="9" t="s">
-        <v>642</v>
-      </c>
-      <c r="C181" s="10" t="n">
-        <v>8400</v>
-      </c>
-      <c r="D181" s="10"/>
+        <v>645</v>
+      </c>
+      <c r="C181" s="9" t="n">
+        <v>2711</v>
+      </c>
+      <c r="D181" s="9"/>
       <c r="E181" s="9" t="s">
-        <v>643</v>
-      </c>
-      <c r="F181" s="9" t="s">
-        <v>644</v>
+        <v>646</v>
+      </c>
+      <c r="G181" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="8" t="s">
-        <v>645</v>
+        <v>647</v>
       </c>
       <c r="B182" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C182" s="7"/>
-      <c r="D182" s="7"/>
+        <v>225</v>
+      </c>
+      <c r="C182" s="10"/>
+      <c r="D182" s="10"/>
       <c r="E182" s="9" t="s">
-        <v>646</v>
+        <v>648</v>
       </c>
       <c r="F182" s="9" t="s">
-        <v>647</v>
+        <v>649</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A183" s="1" t="s">
-        <v>648</v>
+      <c r="A183" s="8" t="s">
+        <v>650</v>
       </c>
       <c r="B183" s="9" t="s">
-        <v>260</v>
-      </c>
-      <c r="C183" s="9" t="n">
-        <v>400</v>
-      </c>
-      <c r="D183" s="9"/>
+        <v>651</v>
+      </c>
+      <c r="C183" s="10"/>
+      <c r="D183" s="10"/>
       <c r="E183" s="9" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="F183" s="9" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
     </row>
     <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="1" t="s">
-        <v>651</v>
+      <c r="A184" s="8" t="s">
+        <v>654</v>
       </c>
       <c r="B184" s="9" t="s">
-        <v>440</v>
+        <v>655</v>
       </c>
       <c r="C184" s="9" t="n">
-        <v>400</v>
+        <v>3721</v>
       </c>
       <c r="D184" s="9"/>
       <c r="E184" s="9" t="s">
-        <v>652</v>
+        <v>656</v>
       </c>
       <c r="F184" s="9" t="s">
-        <v>442</v>
+        <v>657</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="8" t="s">
-        <v>653</v>
+        <v>658</v>
       </c>
       <c r="B185" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C185" s="10"/>
-      <c r="D185" s="10"/>
+        <v>494</v>
+      </c>
+      <c r="C185" s="9" t="n">
+        <v>6100</v>
+      </c>
+      <c r="D185" s="9"/>
       <c r="E185" s="9" t="s">
-        <v>654</v>
+        <v>659</v>
       </c>
       <c r="F185" s="9" t="s">
-        <v>655</v>
+        <v>660</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="8" t="s">
-        <v>656</v>
+        <v>661</v>
       </c>
       <c r="B186" s="9" t="s">
-        <v>403</v>
-      </c>
-      <c r="C186" s="9" t="n">
+        <v>662</v>
+      </c>
+      <c r="C186" s="10" t="n">
+        <v>8400</v>
+      </c>
+      <c r="D186" s="10"/>
+      <c r="E186" s="9" t="s">
+        <v>663</v>
+      </c>
+      <c r="F186" s="9" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="8" t="s">
+        <v>665</v>
+      </c>
+      <c r="B187" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C187" s="7"/>
+      <c r="D187" s="7"/>
+      <c r="E187" s="9" t="s">
+        <v>666</v>
+      </c>
+      <c r="F187" s="9" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A188" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="B188" s="9" t="s">
+        <v>280</v>
+      </c>
+      <c r="C188" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="D188" s="9"/>
+      <c r="E188" s="9" t="s">
+        <v>669</v>
+      </c>
+      <c r="F188" s="9" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A189" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="B189" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="C189" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="D189" s="9"/>
+      <c r="E189" s="9" t="s">
+        <v>672</v>
+      </c>
+      <c r="F189" s="9" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A190" s="8" t="s">
+        <v>673</v>
+      </c>
+      <c r="B190" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C190" s="10"/>
+      <c r="D190" s="10"/>
+      <c r="E190" s="9" t="s">
+        <v>674</v>
+      </c>
+      <c r="F190" s="9" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A191" s="8" t="s">
+        <v>676</v>
+      </c>
+      <c r="B191" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="C191" s="9" t="n">
         <v>21</v>
       </c>
-      <c r="D186" s="9"/>
-      <c r="E186" s="9" t="s">
-        <v>657</v>
-      </c>
-      <c r="G186" s="3" t="s">
+      <c r="D191" s="9"/>
+      <c r="E191" s="9" t="s">
+        <v>677</v>
+      </c>
+      <c r="G191" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="B187" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="E187" s="9" t="s">
-        <v>659</v>
-      </c>
-      <c r="F187" s="9" t="s">
-        <v>660</v>
+    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A192" s="1" t="s">
+        <v>678</v>
+      </c>
+      <c r="B192" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E192" s="9" t="s">
+        <v>679</v>
+      </c>
+      <c r="F192" s="9" t="s">
+        <v>680</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hashcat mode for RAdmin v2.x
added hashcat mode for RAdmin v2.x and removed extended flag on it
</commit_message>
<xml_diff>
--- a/hashinfo.xlsx
+++ b/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="867" uniqueCount="714">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="715">
   <si>
     <t>Hash</t>
   </si>
@@ -1527,6 +1527,9 @@
   </si>
   <si>
     <t>RAdmin v2.x</t>
+  </si>
+  <si>
+    <t>9900</t>
   </si>
   <si>
     <t>6d0bb00954ceb7fbee436bb55a8397a9</t>
@@ -2337,8 +2340,8 @@
   </sheetPr>
   <dimension ref="A1:G202"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A152" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B120" activeCellId="0" sqref="B120"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A107" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C138" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4473,7 +4476,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="1" t="s">
         <v>433</v>
       </c>
@@ -4794,36 +4797,38 @@
       <c r="B138" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="C138" s="10"/>
+      <c r="C138" s="10" t="s">
+        <v>504</v>
+      </c>
       <c r="D138" s="10"/>
       <c r="E138" s="8" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="F138" s="8" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
     </row>
     <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="9" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="B139" s="8" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C139" s="8" t="n">
         <v>7600</v>
       </c>
       <c r="D139" s="8"/>
       <c r="E139" s="8" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="F139" s="8" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="9" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B140" s="8" t="s">
         <v>177</v>
@@ -4831,15 +4836,15 @@
       <c r="C140" s="10"/>
       <c r="D140" s="10"/>
       <c r="E140" s="8" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F140" s="8" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
     </row>
     <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="9" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="B141" s="8" t="s">
         <v>180</v>
@@ -4849,15 +4854,15 @@
       </c>
       <c r="D141" s="8"/>
       <c r="E141" s="8" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="F141" s="8" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="9" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B142" s="8" t="s">
         <v>235</v>
@@ -4865,144 +4870,144 @@
       <c r="C142" s="10"/>
       <c r="D142" s="10"/>
       <c r="E142" s="8" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="F142" s="8" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
     </row>
     <row r="143" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="9" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C143" s="10"/>
       <c r="D143" s="10"/>
       <c r="E143" s="8" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="F143" s="8" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="144" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="9" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C144" s="10"/>
       <c r="D144" s="10"/>
       <c r="E144" s="8" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="F144" s="8" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
     </row>
     <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="9" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C145" s="10"/>
       <c r="D145" s="10"/>
       <c r="E145" s="8" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="F145" s="8" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="146" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="9" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="C146" s="10"/>
       <c r="D146" s="10"/>
       <c r="E146" s="8" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="F146" s="8" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
     </row>
     <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="9" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C147" s="8" t="n">
         <v>7700</v>
       </c>
       <c r="D147" s="8" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="E147" s="8" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="F147" s="8" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="9" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B148" s="8" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C148" s="8" t="n">
         <v>7800</v>
       </c>
       <c r="D148" s="8" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="E148" s="8" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="F148" s="8" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="9" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="C149" s="10"/>
       <c r="D149" s="10"/>
       <c r="E149" s="8" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="F149" s="8" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
     </row>
     <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="1" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="C150" s="2" t="n">
         <v>8900</v>
       </c>
       <c r="E150" s="8" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="G150" s="3" t="s">
         <v>11</v>
@@ -5010,7 +5015,7 @@
     </row>
     <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="9" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B151" s="8" t="s">
         <v>180</v>
@@ -5019,34 +5024,34 @@
         <v>100</v>
       </c>
       <c r="D151" s="10" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E151" s="8" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="F151" s="8" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
     </row>
     <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="9" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C152" s="10"/>
       <c r="D152" s="10"/>
       <c r="E152" s="8" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="F152" s="8" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="9" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B153" s="8" t="s">
         <v>413</v>
@@ -5064,7 +5069,7 @@
     </row>
     <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="9" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="B154" s="8" t="s">
         <v>254</v>
@@ -5072,33 +5077,33 @@
       <c r="C154" s="10"/>
       <c r="D154" s="10"/>
       <c r="E154" s="8" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="F154" s="8" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="9" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="B155" s="8" t="s">
         <v>257</v>
       </c>
       <c r="C155" s="10"/>
       <c r="D155" s="10" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="E155" s="8" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="F155" s="8" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
     </row>
     <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="9" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="B156" s="8" t="s">
         <v>235</v>
@@ -5107,21 +5112,21 @@
         <v>1400</v>
       </c>
       <c r="D156" s="8" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="E156" s="8" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="F156" s="8" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="1" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C157" s="8" t="n">
         <v>7400</v>
@@ -5130,56 +5135,56 @@
         <v>127</v>
       </c>
       <c r="E157" s="8" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="F157" s="8" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="9" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C158" s="10"/>
       <c r="D158" s="10" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="E158" s="8" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="F158" s="8" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="159" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="9" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C159" s="8" t="n">
         <v>1700</v>
       </c>
       <c r="D159" s="8" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="E159" s="8" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="F159" s="8" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
     </row>
     <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="9" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="C160" s="8" t="n">
         <v>1800</v>
@@ -5188,15 +5193,15 @@
         <v>127</v>
       </c>
       <c r="E160" s="8" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="F160" s="8" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="9" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B161" s="8" t="s">
         <v>257</v>
@@ -5204,113 +5209,113 @@
       <c r="C161" s="7"/>
       <c r="D161" s="7"/>
       <c r="E161" s="8" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="F161" s="8" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="9" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B162" s="8" t="s">
         <v>235</v>
       </c>
       <c r="C162" s="10" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="D162" s="10"/>
       <c r="E162" s="8" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="F162" s="8" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="9" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C163" s="10"/>
       <c r="D163" s="10"/>
       <c r="E163" s="8" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="F163" s="8" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="164" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="9" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C164" s="10"/>
       <c r="D164" s="10"/>
       <c r="E164" s="8" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="F164" s="8" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="9" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C165" s="10"/>
       <c r="D165" s="10"/>
       <c r="E165" s="8" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="F165" s="8" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
     </row>
     <row r="166" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="9" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C166" s="10"/>
       <c r="D166" s="10"/>
       <c r="E166" s="8" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="F166" s="8" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
     </row>
     <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="9" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C167" s="10"/>
       <c r="D167" s="10"/>
       <c r="E167" s="8" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="F167" s="8" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="9" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="B168" s="8" t="s">
         <v>235</v>
@@ -5318,15 +5323,15 @@
       <c r="C168" s="10"/>
       <c r="D168" s="10"/>
       <c r="E168" s="8" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="F168" s="8" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="9" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="B169" s="8" t="s">
         <v>177</v>
@@ -5334,15 +5339,15 @@
       <c r="C169" s="10"/>
       <c r="D169" s="10"/>
       <c r="E169" s="8" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="F169" s="8" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="9" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="B170" s="8" t="s">
         <v>180</v>
@@ -5350,15 +5355,15 @@
       <c r="C170" s="10"/>
       <c r="D170" s="10"/>
       <c r="E170" s="8" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="F170" s="8" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
     </row>
     <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="9" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="B171" s="8" t="s">
         <v>257</v>
@@ -5366,31 +5371,31 @@
       <c r="C171" s="10"/>
       <c r="D171" s="10"/>
       <c r="E171" s="8" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="F171" s="8" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="9" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C172" s="10"/>
       <c r="D172" s="10"/>
       <c r="E172" s="8" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="F172" s="8" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="9" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="B173" s="8" t="s">
         <v>177</v>
@@ -5398,15 +5403,15 @@
       <c r="C173" s="10"/>
       <c r="D173" s="10"/>
       <c r="E173" s="8" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="F173" s="8" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
     </row>
     <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="9" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="B174" s="8" t="s">
         <v>180</v>
@@ -5414,15 +5419,15 @@
       <c r="C174" s="10"/>
       <c r="D174" s="10"/>
       <c r="E174" s="8" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="F174" s="8" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
     </row>
     <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="9" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="B175" s="8" t="s">
         <v>257</v>
@@ -5430,15 +5435,15 @@
       <c r="C175" s="10"/>
       <c r="D175" s="10"/>
       <c r="E175" s="8" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="F175" s="8" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
     </row>
     <row r="176" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="9" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="B176" s="8" t="s">
         <v>235</v>
@@ -5446,58 +5451,58 @@
       <c r="C176" s="10"/>
       <c r="D176" s="10"/>
       <c r="E176" s="8" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="F176" s="8" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="9" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C177" s="10"/>
       <c r="D177" s="10"/>
       <c r="E177" s="8" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="F177" s="8" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="1" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="C178" s="2" t="n">
         <v>23</v>
       </c>
       <c r="E178" s="8" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="F178" s="2" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
     </row>
     <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="9" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="C179" s="8" t="n">
         <v>121</v>
       </c>
       <c r="D179" s="8"/>
       <c r="E179" s="8" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="G179" s="3" t="s">
         <v>57</v>
@@ -5505,7 +5510,7 @@
     </row>
     <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="9" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="B180" s="8" t="s">
         <v>177</v>
@@ -5513,15 +5518,15 @@
       <c r="C180" s="10"/>
       <c r="D180" s="10"/>
       <c r="E180" s="8" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="F180" s="8" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="9" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="B181" s="8" t="s">
         <v>235</v>
@@ -5529,18 +5534,18 @@
       <c r="C181" s="10"/>
       <c r="D181" s="10"/>
       <c r="E181" s="8" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="F181" s="8" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="9" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="C182" s="8" t="n">
         <v>111</v>
@@ -5555,7 +5560,7 @@
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="9" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B183" s="8" t="s">
         <v>308</v>
@@ -5573,45 +5578,45 @@
     </row>
     <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="1" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="C184" s="8" t="n">
         <v>3300</v>
       </c>
       <c r="D184" s="8"/>
       <c r="E184" s="8" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="F184" s="8" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="9" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="C185" s="8" t="n">
         <v>8000</v>
       </c>
       <c r="D185" s="8" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="E185" s="8" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="F185" s="8" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="9" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="B186" s="8" t="s">
         <v>177</v>
@@ -5619,15 +5624,15 @@
       <c r="C186" s="10"/>
       <c r="D186" s="10"/>
       <c r="E186" s="8" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="F186" s="8" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
     </row>
     <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="9" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="B187" s="8" t="s">
         <v>180</v>
@@ -5635,15 +5640,15 @@
       <c r="C187" s="10"/>
       <c r="D187" s="10"/>
       <c r="E187" s="8" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="F187" s="8" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
     </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="9" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="B188" s="8" t="s">
         <v>254</v>
@@ -5651,15 +5656,15 @@
       <c r="C188" s="10"/>
       <c r="D188" s="10"/>
       <c r="E188" s="8" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="F188" s="8" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
     </row>
     <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="9" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="B189" s="8" t="s">
         <v>126</v>
@@ -5668,10 +5673,10 @@
         <v>1500</v>
       </c>
       <c r="D189" s="8" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="E189" s="8" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="F189" s="8" t="s">
         <v>129</v>
@@ -5679,17 +5684,17 @@
     </row>
     <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="9" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="C190" s="8" t="n">
         <v>2611</v>
       </c>
       <c r="D190" s="8"/>
       <c r="E190" s="8" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="G190" s="3" t="s">
         <v>57</v>
@@ -5697,17 +5702,17 @@
     </row>
     <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="9" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="C191" s="8" t="n">
         <v>2711</v>
       </c>
       <c r="D191" s="8"/>
       <c r="E191" s="8" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="G191" s="3" t="s">
         <v>57</v>
@@ -5715,7 +5720,7 @@
     </row>
     <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="9" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="B192" s="8" t="s">
         <v>235</v>
@@ -5723,85 +5728,85 @@
       <c r="C192" s="10"/>
       <c r="D192" s="10"/>
       <c r="E192" s="8" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="F192" s="8" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="9" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="C193" s="10"/>
       <c r="D193" s="10"/>
       <c r="E193" s="8" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="F193" s="8" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="9" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="C194" s="8" t="n">
         <v>3721</v>
       </c>
       <c r="D194" s="8"/>
       <c r="E194" s="8" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="F194" s="8" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
     </row>
     <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="9" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C195" s="8" t="n">
         <v>6100</v>
       </c>
       <c r="D195" s="8"/>
       <c r="E195" s="8" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="F195" s="8" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
     </row>
     <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="9" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="C196" s="10" t="n">
         <v>8400</v>
       </c>
       <c r="D196" s="10"/>
       <c r="E196" s="8" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="F196" s="8" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="9" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B197" s="8" t="s">
         <v>45</v>
@@ -5809,15 +5814,15 @@
       <c r="C197" s="7"/>
       <c r="D197" s="7"/>
       <c r="E197" s="8" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="F197" s="8" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
     </row>
     <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="1" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B198" s="8" t="s">
         <v>290</v>
@@ -5827,15 +5832,15 @@
       </c>
       <c r="D198" s="8"/>
       <c r="E198" s="8" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="F198" s="8" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
     </row>
     <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="1" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B199" s="8" t="s">
         <v>486</v>
@@ -5845,7 +5850,7 @@
       </c>
       <c r="D199" s="8"/>
       <c r="E199" s="8" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="F199" s="8" t="s">
         <v>488</v>
@@ -5853,7 +5858,7 @@
     </row>
     <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="9" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B200" s="8" t="s">
         <v>16</v>
@@ -5861,15 +5866,15 @@
       <c r="C200" s="10"/>
       <c r="D200" s="10"/>
       <c r="E200" s="8" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="F200" s="8" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
     </row>
     <row r="201" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="9" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B201" s="8" t="s">
         <v>445</v>
@@ -5879,7 +5884,7 @@
       </c>
       <c r="D201" s="8"/>
       <c r="E201" s="8" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="G201" s="3" t="s">
         <v>57</v>
@@ -5887,16 +5892,16 @@
     </row>
     <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B202" s="8" t="s">
         <v>177</v>
       </c>
       <c r="E202" s="8" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="F202" s="8" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Android FDE ≤ 4.3
added Android FDE ≤ 4.3 supported in the latest release version of
oclHashcat
</commit_message>
<xml_diff>
--- a/hashinfo.xlsx
+++ b/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="718">
   <si>
     <t>Hash</t>
   </si>
@@ -113,6 +113,18 @@
     <t>{ssha512}06$otYx2eSXx.OkEY4F$71vDkRp8S0GNO96tgcvKDz7y8YYEenW8/mltpQsHuiueaHxSEMl1LMzQZTGQt7w.NLWoyb0WKZZfLuVtFIK...</t>
   </si>
   <si>
+    <t>Android FDE ≤ 4.3</t>
+  </si>
+  <si>
+    <t>^\$fde\$[0-9]{2}\$[a-f0-9]{32}\$[0-9]{2}\$[a-f0-9]{32}\$[a-f0-9]{3072}$</t>
+  </si>
+  <si>
+    <t>$fde$16$ca56e82e7b5a9c2fc1e3b5a7d671c2f9$16$7c124af19ac913be0fc137b75a34b20d$eac806ae7277c8d48243d52a8644fa57a817317bd3457f94dca727964cbc27c88296954f289597a9de3314a4e9d9f28dce70cf9ce3e1c3c0c6fc041687a0ad3cb333d4449bc9da8fcc7d5f85948a7ac3bc6d34f505e9d0d91da4396e35840bde3465ad11c5086c89ee6db68d65e47a2e5413f272caa01e02224e5ff3dc3bed3953a702e85e964e562e62f5c97a2df6c47547bfb5aeeb329ff8f9c9666724d399043fe970c8b282b45e93d008333f3b4edd5eb147bd023ed18ac1f9f75a6cd33444b507694c64e1e98a964b48c0a77276e9930250d01801813c235169a7b1952891c63ce0d462abc688bd96c0337174695a957858b4c9fd277d04abe8a0c2c5def4b352ba29410f8dbec91bcb2ca2b8faf26d44f02340b3373bc94e7487ce014e6adfbf7edfdd2057225f8aeb324c9d1be877c6ae4211ae387e07bf2a056984d2ed2815149b3e9cf9fbfae852f7dd5906c2b86e7910c0d7755ef5bcc39f0e135bf546c839693dc4af3e50b8382c7c8c754d4ee218fa85d70ee0a5707a9f827209a7ddb6c2fb9431a61c9775112cc88aa2a34f97c2f53dfce082aa0758917269a5fc30049ceab67d3efd721fee021ffca979f839b4f052e27f5c382c0dd5c02fd39fbc9b26e04bf9e051d1923eff9a7cde3244902bb8538b1b9f11631def5aad7c21d2113bcdc989b771ff6bf220f94354034dd417510117b55a669e969fc3bc6c5dcd4741b8313bf7d999dc94d4949f27eec0cd06f906c17a80d09f583a5dd601854832673b78d125a2c5ad0352932be7b93c611fee8c6049670442d8c532674f3d21d45d3d009211d2a9e6568252ac4682982172cb43e7c6b05e85851787ad90e25b77cce3f7968d455f92653a1d3790bc50e5f6e1f743ac47275ffa8e81bbe832a8d7d78d5d5a7c73f95703aebb355849ae566492093bd9cb51070f39c69bb4e22b99cc0e60e96d048385bb69f1c44a3b79547fbc19a873a632f43f05fa2d8a6f9155e59d153e2851b739c42444018b8c4e09a93be43570834667d0b5a5d2a53b1572dab3e750b3f9e641e303559bace06612fbd451a5e822201442828e79168c567a85d8c024cd8ce32bf650105b1af98cc5428675f4f4bbede37a0ef98d1533a8a6dcb27d87a2b799f18706f4677edaa0411becac4c591ede83993aedba660d1dd67f6c4a5c141ad3e6e0c77730cb0ecbf4f4bd8ef6067e05ca3bc563d9e1554a893fea0050bdd1733c883f533f87eac39cceee0ccf817fc1f19bcfdd13e9f241b89bfb149b509e9a0747658438536b6705514cc6d6bb3c64c903e4710435d8bebc35297d1ebbdff8074b203f37d1910d8b4637e4d3dab997f4aa378a7a67c79e698a11e83d0d7e759d0e7969c4f5408168b282fe28d3279ec1d4cc6f85a0f8e5d01f21c7508a69773c44167ff8d467d0801f9ec54f9ee2496d4e7e470214abc1ca11355bb18cd23273aac6b05b47f9e301b42b137a2455758c24e2716dcd2e55bbeb780f592e664e7392bf6eccb80959f24c8800816c84f2575e82e1f3559c33a5be7a3a0c843c2989f486b113d5eeada007caf6b5a0f6d71e2f5c09a4def57c7057168051868317a9ec790d570d76a0d21a45ad951c475db5a66101475871147c5a5907ec4e6b14128ed6695bb73c1c97952e96826eeb6003aa13462093e4afc209627241f03b0247e110fbab983640423b7cdf112e01579fed68c80ac7df7449d9d2114b9ae5539c03c2037be45c5f74e7357b25c6a24b7bd503864437147e50d7ac4ccc4bbd0cabecdc6bac60a362285fe450e2c2d0a446578c8880dc957e6e8061e691b83eb8062d1aad476e0c7b25e4d5454f1288686eb525f37fe649637b235b7828366b0219a9c63d6ddbb696dc3585a2ebfbd5f5e4c170d6784ab9993e15142535e194d2bee3dc9477ef8b8e1b07605e0c04f49edf6d42be3a9dabbc592dde78ce8b7dd9684bfcf4ca2f5a44b1872abe18fb6fa67a79390f273a9d12f9269389629456d71b9e7ed3447462269a849ce83e1893f253c832537f850b1acce5b11d2ba6b7c2f99e8e7c8085f390c21f69e1ce4bbf85b4e1ad86c0d6706432766978076f4cada9ca6f28d395d9cc5e74b2a6b46eb9d1de79eeecff7dc97ec2a8d8870e3894e1e4e26ccb98dd2f88c0229bbd3152fa149f0cc132561f</t>
+  </si>
+  <si>
+    <t>resource needed</t>
+  </si>
+  <si>
     <t>Android PIN</t>
   </si>
   <si>
@@ -186,9 +198,6 @@
   </si>
   <si>
     <t>$8$TnGX/fE4KGHOVU$pEhnEvxrvaynpi8j4f.EMHr6M.FzU8xnZnBr/tJdFWk</t>
-  </si>
-  <si>
-    <t>resource needed</t>
   </si>
   <si>
     <t>Cisco Type 9</t>
@@ -2338,10 +2347,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G202"/>
+  <dimension ref="A1:G203"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A107" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C138" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A208" activeCellId="0" sqref="A208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2521,21 +2530,20 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="9" t="s">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="8" t="n">
-        <v>5800</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8" t="s">
+      <c r="C9" s="2" t="n">
+        <v>8800</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="G9" s="3" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2547,7 +2555,7 @@
         <v>37</v>
       </c>
       <c r="C10" s="8" t="n">
-        <v>1600</v>
+        <v>5800</v>
       </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8" t="s">
@@ -2564,8 +2572,10 @@
       <c r="B11" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
+      <c r="C11" s="8" t="n">
+        <v>1600</v>
+      </c>
+      <c r="D11" s="8"/>
       <c r="E11" s="8" t="s">
         <v>42</v>
       </c>
@@ -2580,51 +2590,50 @@
       <c r="B12" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="8" t="n">
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="8" t="n">
         <v>3200</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="B13" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10" t="s">
+      <c r="E13" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="8" t="s">
+    </row>
+    <row r="14" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="11" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="14" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="10"/>
+      <c r="D14" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>9200</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="F14" s="8" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2636,65 +2645,64 @@
         <v>59</v>
       </c>
       <c r="C15" s="2" t="n">
-        <v>9300</v>
+        <v>9200</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>60</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="9" t="s">
+      <c r="A16" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
+      <c r="C16" s="2" t="n">
+        <v>9300</v>
+      </c>
       <c r="E16" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>64</v>
+      <c r="G16" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C17" s="8" t="n">
-        <v>2410</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8" t="s">
+      <c r="F17" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>70</v>
-      </c>
       <c r="C18" s="8" t="n">
-        <v>500</v>
+        <v>2410</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2705,14 +2713,14 @@
         <v>73</v>
       </c>
       <c r="C19" s="8" t="n">
-        <v>5700</v>
+        <v>500</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8" t="s">
         <v>74</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2723,57 +2731,59 @@
         <v>76</v>
       </c>
       <c r="C20" s="8" t="n">
-        <v>2400</v>
-      </c>
-      <c r="D20" s="8" t="s">
+        <v>5700</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>79</v>
+      <c r="G20" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="C21" s="8" t="n">
+        <v>2400</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="E21" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="8" t="n">
-        <v>8100</v>
-      </c>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8" t="s">
+      <c r="F21" s="8" t="s">
         <v>82</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="8" t="n">
+        <v>8100</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="8" t="s">
+      <c r="F22" s="8" t="s">
         <v>86</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="2" t="s">
         <v>88</v>
       </c>
       <c r="C23" s="10"/>
@@ -2781,16 +2791,16 @@
       <c r="E23" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>90</v>
+      <c r="G23" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="24" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>91</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>88</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
@@ -2802,35 +2812,35 @@
       </c>
     </row>
     <row r="25" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="9" t="s">
         <v>94</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F25" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="26" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="9" t="s">
+      <c r="A26" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>16</v>
+        <v>98</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="F26" s="8" t="s">
         <v>99</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2854,79 +2864,79 @@
         <v>103</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>104</v>
+        <v>16</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F28" s="8" t="s">
         <v>105</v>
-      </c>
-      <c r="F28" s="8" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B29" s="8" t="s">
         <v>107</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>108</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F29" s="8" t="s">
         <v>109</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B30" s="8" t="s">
         <v>111</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>112</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="F30" s="8" t="s">
         <v>113</v>
-      </c>
-      <c r="F30" s="8" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B31" s="8" t="s">
         <v>115</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>116</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
       <c r="E31" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F31" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="F31" s="8" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="32" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B32" s="8" t="s">
         <v>119</v>
-      </c>
-      <c r="B32" s="8" t="s">
-        <v>120</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
       <c r="E32" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" s="8" t="s">
         <v>121</v>
-      </c>
-      <c r="F32" s="8" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="33" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2934,233 +2944,231 @@
         <v>122</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C33" s="8" t="n">
+        <v>123</v>
+      </c>
+      <c r="C33" s="10"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C34" s="8" t="n">
         <v>3100</v>
       </c>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="F33" s="8" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="34" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="B34" s="8" t="s">
+      <c r="D34" s="8"/>
+      <c r="E34" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C34" s="8" t="n">
+      <c r="F34" s="8" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="35" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" s="8" t="n">
         <v>1500</v>
       </c>
-      <c r="D34" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="F34" s="8" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="35" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="s">
+      <c r="D35" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="E35" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="F35" s="8" t="s">
         <v>132</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="36" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B36" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="E36" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="F36" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B37" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="E37" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="E37" s="8" t="s">
+      <c r="F37" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="38" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="E38" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="E38" s="8" t="s">
+      <c r="F38" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="39" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="E39" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E39" s="8" t="s">
+      <c r="F39" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="40" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="E40" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="C40" s="8" t="n">
-        <v>800</v>
-      </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8" t="s">
+      <c r="F40" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="F40" s="8" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="41" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B41" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B41" s="8" t="s">
+      <c r="C41" s="8" t="n">
+        <v>800</v>
+      </c>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="C41" s="10"/>
-      <c r="D41" s="10"/>
-      <c r="E41" s="8" t="s">
+      <c r="F41" s="8" t="s">
         <v>156</v>
-      </c>
-      <c r="F41" s="8" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="42" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>158</v>
-      </c>
-      <c r="B42" s="8" t="s">
-        <v>159</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
       <c r="E42" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="F42" s="8" t="s">
         <v>160</v>
-      </c>
-      <c r="F42" s="8" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="43" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B43" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="C43" s="10" t="n">
-        <v>8300</v>
-      </c>
+      <c r="C43" s="10"/>
       <c r="D43" s="10"/>
       <c r="E43" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="F43" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="F43" s="8" t="s">
+    </row>
+    <row r="44" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="44" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="9" t="s">
+      <c r="B44" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="B44" s="8" t="s">
+      <c r="C44" s="10" t="n">
+        <v>8300</v>
+      </c>
+      <c r="D44" s="10"/>
+      <c r="E44" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="C44" s="8" t="n">
-        <v>1100</v>
-      </c>
-      <c r="D44" s="8" t="s">
+      <c r="F44" s="8" t="s">
         <v>168</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>169</v>
-      </c>
-      <c r="F44" s="8" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="45" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
+        <v>169</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="C45" s="8" t="n">
+        <v>1100</v>
+      </c>
+      <c r="D45" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="B45" s="8" t="s">
+      <c r="E45" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="C45" s="8" t="n">
+      <c r="F45" s="8" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="46" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="C46" s="8" t="n">
         <v>2100</v>
       </c>
-      <c r="D45" s="8" t="s">
-        <v>173</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="F45" s="8" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="46" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
+      <c r="D46" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="E46" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="C46" s="10" t="n">
-        <v>2600</v>
-      </c>
-      <c r="D46" s="10"/>
-      <c r="E46" s="8" t="s">
+      <c r="F46" s="8" t="s">
         <v>178</v>
-      </c>
-      <c r="G46" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="47" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3171,61 +3179,63 @@
         <v>180</v>
       </c>
       <c r="C47" s="10" t="n">
-        <v>4500</v>
+        <v>2600</v>
       </c>
       <c r="D47" s="10"/>
       <c r="E47" s="8" t="s">
         <v>181</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="48" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="9" t="s">
+      <c r="A48" s="1" t="s">
         <v>182</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="C48" s="8" t="n">
-        <v>7900</v>
-      </c>
-      <c r="D48" s="8"/>
+      <c r="C48" s="10" t="n">
+        <v>4500</v>
+      </c>
+      <c r="D48" s="10"/>
       <c r="E48" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="F48" s="8" t="s">
-        <v>185</v>
+      <c r="G48" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="49" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="C49" s="8" t="n">
+        <v>7900</v>
+      </c>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="C49" s="10"/>
-      <c r="D49" s="10" t="s">
+      <c r="F49" s="8" t="s">
         <v>188</v>
-      </c>
-      <c r="E49" s="8" t="s">
-        <v>189</v>
-      </c>
-      <c r="F49" s="8" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="C50" s="10"/>
+      <c r="D50" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="B50" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C50" s="10"/>
-      <c r="D50" s="10"/>
       <c r="E50" s="8" t="s">
         <v>192</v>
       </c>
@@ -3237,84 +3247,84 @@
       <c r="A51" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="10"/>
+      <c r="D51" s="10"/>
+      <c r="E51" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="C51" s="8" t="n">
-        <v>123</v>
-      </c>
-      <c r="D51" s="8"/>
-      <c r="E51" s="8" t="s">
+      <c r="F51" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="G51" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="52" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="B52" s="8" t="s">
+      <c r="B52" s="2" t="s">
         <v>198</v>
       </c>
       <c r="C52" s="8" t="n">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="D52" s="8"/>
       <c r="E52" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="F52" s="1" t="s">
-        <v>200</v>
-      </c>
       <c r="G52" s="3" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="B53" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="B53" s="8" t="s">
-        <v>202</v>
-      </c>
       <c r="C53" s="8" t="n">
-        <v>1441</v>
+        <v>141</v>
       </c>
       <c r="D53" s="8"/>
       <c r="E53" s="8" t="s">
+        <v>202</v>
+      </c>
+      <c r="F53" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="54" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="1" t="s">
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="9" t="s">
         <v>204</v>
       </c>
       <c r="B54" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="C54" s="10"/>
-      <c r="D54" s="10"/>
+      <c r="C54" s="8" t="n">
+        <v>1441</v>
+      </c>
+      <c r="D54" s="8"/>
       <c r="E54" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="F54" s="8" t="s">
+      <c r="F54" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="55" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="55" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="9" t="s">
+      <c r="B55" s="8" t="s">
         <v>208</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>88</v>
       </c>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
@@ -3330,7 +3340,7 @@
         <v>211</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>16</v>
+        <v>91</v>
       </c>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
@@ -3378,7 +3388,7 @@
         <v>220</v>
       </c>
       <c r="B59" s="8" t="s">
-        <v>104</v>
+        <v>16</v>
       </c>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
@@ -3394,17 +3404,15 @@
         <v>223</v>
       </c>
       <c r="B60" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C60" s="10"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="C60" s="8" t="n">
-        <v>7000</v>
-      </c>
-      <c r="D60" s="8"/>
-      <c r="E60" s="8" t="s">
+      <c r="F60" s="8" t="s">
         <v>225</v>
-      </c>
-      <c r="G60" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="61" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3412,35 +3420,37 @@
         <v>226</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>70</v>
+        <v>227</v>
       </c>
       <c r="C61" s="8" t="n">
-        <v>500</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>227</v>
-      </c>
+        <v>7000</v>
+      </c>
+      <c r="D61" s="8"/>
       <c r="E61" s="8" t="s">
-        <v>71</v>
+        <v>228</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C62" s="10"/>
-      <c r="D62" s="10"/>
+        <v>73</v>
+      </c>
+      <c r="C62" s="8" t="n">
+        <v>500</v>
+      </c>
+      <c r="D62" s="8" t="s">
+        <v>230</v>
+      </c>
       <c r="E62" s="8" t="s">
-        <v>229</v>
-      </c>
-      <c r="F62" s="8" t="s">
-        <v>230</v>
+        <v>74</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="63" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3464,46 +3474,44 @@
         <v>234</v>
       </c>
       <c r="B64" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C64" s="10"/>
+      <c r="D64" s="10"/>
+      <c r="E64" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="C64" s="8" t="n">
-        <v>6900</v>
-      </c>
-      <c r="D64" s="8"/>
-      <c r="E64" s="8" t="s">
+      <c r="F64" s="8" t="s">
         <v>236</v>
-      </c>
-      <c r="F64" s="8" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="65" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="B65" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="B65" s="8" t="s">
-        <v>239</v>
-      </c>
       <c r="C65" s="8" t="n">
-        <v>7200</v>
+        <v>6900</v>
       </c>
       <c r="D65" s="8"/>
       <c r="E65" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="F65" s="8" t="s">
         <v>240</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="66" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="B66" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="B66" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="C66" s="8" t="n">
-        <v>5100</v>
+        <v>7200</v>
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="8" t="s">
@@ -3518,14 +3526,16 @@
         <v>245</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="C67" s="10"/>
-      <c r="D67" s="10"/>
+        <v>107</v>
+      </c>
+      <c r="C67" s="8" t="n">
+        <v>5100</v>
+      </c>
+      <c r="D67" s="8"/>
       <c r="E67" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="F67" s="8" t="s">
+      <c r="F67" s="2" t="s">
         <v>247</v>
       </c>
     </row>
@@ -3534,7 +3544,7 @@
         <v>248</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C68" s="10"/>
       <c r="D68" s="10"/>
@@ -3558,15 +3568,15 @@
         <v>252</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="70" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="9" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>254</v>
+        <v>183</v>
       </c>
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
@@ -3574,7 +3584,7 @@
         <v>255</v>
       </c>
       <c r="F70" s="8" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="71" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3590,7 +3600,7 @@
         <v>258</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="72" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3598,289 +3608,287 @@
         <v>259</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>235</v>
+        <v>260</v>
       </c>
       <c r="C72" s="10"/>
       <c r="D72" s="10"/>
       <c r="E72" s="8" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
     </row>
     <row r="73" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="1" t="s">
-        <v>261</v>
+      <c r="A73" s="9" t="s">
+        <v>262</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>262</v>
-      </c>
-      <c r="C73" s="10" t="n">
+        <v>238</v>
+      </c>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="F73" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="74" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="C74" s="10" t="n">
         <v>1421</v>
       </c>
-      <c r="D73" s="10" t="s">
-        <v>263</v>
-      </c>
-      <c r="E73" s="8" t="s">
-        <v>264</v>
-      </c>
-      <c r="F73" s="8" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="13" t="s">
+      <c r="D74" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="E74" s="8" t="s">
         <v>267</v>
       </c>
-      <c r="C74" s="2" t="n">
-        <v>5300</v>
-      </c>
-      <c r="D74" s="7"/>
-      <c r="E74" s="8" t="s">
+      <c r="F74" s="8" t="s">
         <v>268</v>
-      </c>
-      <c r="F74" s="2" t="s">
-        <v>269</v>
-      </c>
-      <c r="G74" s="3" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="13" t="s">
+        <v>269</v>
+      </c>
+      <c r="B75" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>271</v>
-      </c>
       <c r="C75" s="2" t="n">
-        <v>5400</v>
+        <v>5300</v>
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="F75" s="2" t="s">
         <v>272</v>
-      </c>
-      <c r="F75" s="2" t="s">
-        <v>269</v>
       </c>
       <c r="G75" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="76" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="12" t="s">
+    <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="13" t="s">
         <v>273</v>
       </c>
-      <c r="B76" s="8" t="s">
+      <c r="B76" s="2" t="s">
         <v>274</v>
       </c>
-      <c r="C76" s="8" t="n">
-        <v>2811</v>
-      </c>
-      <c r="D76" s="8"/>
+      <c r="C76" s="2" t="n">
+        <v>5400</v>
+      </c>
+      <c r="D76" s="7"/>
       <c r="E76" s="8" t="s">
         <v>275</v>
       </c>
+      <c r="F76" s="2" t="s">
+        <v>272</v>
+      </c>
       <c r="G76" s="3" t="s">
-        <v>57</v>
+        <v>11</v>
       </c>
     </row>
     <row r="77" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="12" t="s">
         <v>276</v>
       </c>
-      <c r="B77" s="2" t="s">
+      <c r="B77" s="8" t="s">
         <v>277</v>
       </c>
-      <c r="C77" s="10" t="n">
-        <v>7300</v>
-      </c>
-      <c r="D77" s="10"/>
+      <c r="C77" s="8" t="n">
+        <v>2811</v>
+      </c>
+      <c r="D77" s="8"/>
       <c r="E77" s="8" t="s">
         <v>278</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="9" t="s">
+      <c r="A78" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B78" s="8" t="s">
+      <c r="B78" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="C78" s="8" t="n">
-        <v>4800</v>
-      </c>
-      <c r="D78" s="8"/>
+      <c r="C78" s="10" t="n">
+        <v>7300</v>
+      </c>
+      <c r="D78" s="10"/>
       <c r="E78" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="F78" s="8" t="s">
-        <v>282</v>
+      <c r="G78" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="79" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="B79" s="8" t="s">
         <v>283</v>
       </c>
-      <c r="B79" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C79" s="10"/>
-      <c r="D79" s="10"/>
+      <c r="C79" s="8" t="n">
+        <v>4800</v>
+      </c>
+      <c r="D79" s="8"/>
       <c r="E79" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="G79" s="3" t="s">
-        <v>57</v>
+      <c r="F79" s="8" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="80" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="9" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>286</v>
-      </c>
-      <c r="C80" s="8" t="n">
-        <v>11</v>
-      </c>
-      <c r="D80" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="C80" s="10"/>
+      <c r="D80" s="10"/>
       <c r="E80" s="8" t="s">
         <v>287</v>
       </c>
-      <c r="F80" s="8" t="s">
-        <v>288</v>
+      <c r="G80" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="81" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="9" t="s">
+        <v>288</v>
+      </c>
+      <c r="B81" s="8" t="s">
         <v>289</v>
       </c>
-      <c r="B81" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>291</v>
+      <c r="C81" s="8" t="n">
+        <v>11</v>
       </c>
       <c r="D81" s="8"/>
       <c r="E81" s="8" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F81" s="8" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="82" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C82" s="8" t="s">
         <v>294</v>
       </c>
-      <c r="B82" s="8" t="s">
+      <c r="D82" s="8"/>
+      <c r="E82" s="8" t="s">
         <v>295</v>
       </c>
-      <c r="C82" s="8" t="n">
+      <c r="F82" s="8" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="83" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="C83" s="8" t="n">
         <v>22</v>
       </c>
-      <c r="D82" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="E82" s="8" t="s">
-        <v>297</v>
-      </c>
-      <c r="F82" s="2" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="9" t="s">
+      <c r="D83" s="8" t="s">
         <v>299</v>
       </c>
-      <c r="B83" s="8" t="s">
+      <c r="E83" s="8" t="s">
         <v>300</v>
       </c>
-      <c r="C83" s="8" t="n">
+      <c r="F83" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="B84" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="C84" s="8" t="n">
         <v>7500</v>
-      </c>
-      <c r="D83" s="8"/>
-      <c r="E83" s="8" t="s">
-        <v>301</v>
-      </c>
-      <c r="F83" s="2" t="s">
-        <v>302</v>
-      </c>
-      <c r="G83" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="84" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="B84" s="2" t="s">
-        <v>304</v>
-      </c>
-      <c r="C84" s="8" t="n">
-        <v>6800</v>
       </c>
       <c r="D84" s="8"/>
       <c r="E84" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="F84" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="F84" s="8" t="s">
-        <v>306</v>
+      <c r="G84" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="85" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="B85" s="8" t="s">
-        <v>308</v>
-      </c>
       <c r="C85" s="8" t="n">
-        <v>1711</v>
+        <v>6800</v>
       </c>
       <c r="D85" s="8"/>
       <c r="E85" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="F85" s="8" t="s">
         <v>309</v>
-      </c>
-      <c r="F85" s="8" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="86" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="B86" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="B86" s="8" t="s">
+      <c r="C86" s="8" t="n">
+        <v>1711</v>
+      </c>
+      <c r="D86" s="8"/>
+      <c r="E86" s="8" t="s">
         <v>312</v>
       </c>
-      <c r="C86" s="10"/>
-      <c r="D86" s="10"/>
-      <c r="E86" s="8" t="s">
+      <c r="F86" s="8" t="s">
         <v>313</v>
-      </c>
-      <c r="F86" s="8" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="87" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="B87" s="8" t="s">
         <v>315</v>
       </c>
-      <c r="B87" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="C87" s="8" t="n">
-        <v>190</v>
-      </c>
-      <c r="D87" s="8"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="10"/>
       <c r="E87" s="8" t="s">
         <v>316</v>
       </c>
@@ -3893,91 +3901,93 @@
         <v>318</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C88" s="8" t="n">
+        <v>190</v>
+      </c>
+      <c r="D88" s="8"/>
+      <c r="E88" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="F88" s="8" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="89" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="B89" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C89" s="8" t="n">
         <v>3000</v>
       </c>
-      <c r="D88" s="8" t="s">
-        <v>319</v>
-      </c>
-      <c r="E88" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="F88" s="8" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="89" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="9" t="s">
+      <c r="D89" s="8" t="s">
         <v>322</v>
       </c>
-      <c r="B89" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C89" s="10" t="s">
+      <c r="E89" s="8" t="s">
         <v>323</v>
       </c>
-      <c r="D89" s="14" t="s">
+      <c r="F89" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="E89" s="8" t="s">
+    </row>
+    <row r="90" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="G89" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="90" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="9" t="s">
+      <c r="B90" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C90" s="10" t="s">
         <v>326</v>
       </c>
-      <c r="B90" s="8" t="s">
+      <c r="D90" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="C90" s="10" t="s">
+      <c r="E90" s="8" t="s">
         <v>328</v>
       </c>
-      <c r="D90" s="10" t="s">
+      <c r="G90" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="91" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="9" t="s">
         <v>329</v>
       </c>
-      <c r="E90" s="8" t="s">
+      <c r="B91" s="8" t="s">
         <v>330</v>
       </c>
-      <c r="G90" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="91" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="1" t="s">
+      <c r="C91" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="B91" s="2" t="s">
+      <c r="D91" s="10" t="s">
         <v>332</v>
-      </c>
-      <c r="C91" s="2" t="n">
-        <v>9100</v>
       </c>
       <c r="E91" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="F91" s="2" t="s">
+      <c r="G91" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="92" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="1" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="92" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="9" t="s">
+      <c r="B92" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="B92" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="C92" s="10"/>
-      <c r="D92" s="10"/>
+      <c r="C92" s="2" t="n">
+        <v>9100</v>
+      </c>
       <c r="E92" s="8" t="s">
         <v>336</v>
       </c>
-      <c r="F92" s="8" t="s">
+      <c r="F92" s="2" t="s">
         <v>337</v>
       </c>
     </row>
@@ -3986,7 +3996,7 @@
         <v>338</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="C93" s="10"/>
       <c r="D93" s="10"/>
@@ -4002,52 +4012,50 @@
         <v>341</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C94" s="8" t="n">
-        <v>900</v>
-      </c>
-      <c r="D94" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C94" s="10"/>
+      <c r="D94" s="10"/>
+      <c r="E94" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="E94" s="8" t="s">
+      <c r="F94" s="8" t="s">
         <v>343</v>
-      </c>
-      <c r="F94" s="8" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="95" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="B95" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C95" s="8" t="n">
+        <v>900</v>
+      </c>
+      <c r="D95" s="8" t="s">
         <v>345</v>
       </c>
-      <c r="B95" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C95" s="8" t="s">
+      <c r="E95" s="8" t="s">
         <v>346</v>
       </c>
-      <c r="D95" s="8" t="s">
+      <c r="F95" s="8" t="s">
         <v>347</v>
-      </c>
-      <c r="E95" s="8" t="s">
-        <v>348</v>
-      </c>
-      <c r="F95" s="8" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="96" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C96" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="D96" s="8" t="s">
         <v>350</v>
       </c>
-      <c r="B96" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C96" s="8" t="n">
-        <v>500</v>
-      </c>
-      <c r="D96" s="8"/>
       <c r="E96" s="8" t="s">
         <v>351</v>
       </c>
@@ -4060,268 +4068,266 @@
         <v>353</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>37</v>
+        <v>73</v>
       </c>
       <c r="C97" s="8" t="n">
-        <v>1600</v>
+        <v>500</v>
       </c>
       <c r="D97" s="8"/>
       <c r="E97" s="8" t="s">
-        <v>38</v>
+        <v>354</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>39</v>
+        <v>355</v>
       </c>
     </row>
     <row r="98" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="9" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B98" s="8" t="s">
-        <v>280</v>
+        <v>41</v>
       </c>
       <c r="C98" s="8" t="n">
-        <v>4800</v>
+        <v>1600</v>
       </c>
       <c r="D98" s="8"/>
       <c r="E98" s="8" t="s">
-        <v>281</v>
+        <v>42</v>
       </c>
       <c r="F98" s="8" t="s">
-        <v>282</v>
+        <v>43</v>
       </c>
     </row>
     <row r="99" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="9" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>356</v>
-      </c>
-      <c r="C99" s="10" t="s">
-        <v>357</v>
-      </c>
-      <c r="D99" s="10" t="s">
-        <v>358</v>
-      </c>
+        <v>283</v>
+      </c>
+      <c r="C99" s="8" t="n">
+        <v>4800</v>
+      </c>
+      <c r="D99" s="8"/>
       <c r="E99" s="8" t="s">
-        <v>359</v>
+        <v>284</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>360</v>
+        <v>285</v>
       </c>
     </row>
     <row r="100" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="B100" s="8" t="s">
+        <v>359</v>
+      </c>
+      <c r="C100" s="10" t="s">
+        <v>360</v>
+      </c>
+      <c r="D100" s="10" t="s">
         <v>361</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="E100" s="8" t="s">
         <v>362</v>
       </c>
-      <c r="C100" s="10"/>
-      <c r="D100" s="10"/>
-      <c r="E100" s="8" t="s">
+      <c r="F100" s="8" t="s">
         <v>363</v>
-      </c>
-      <c r="F100" s="2" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="101" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="9" t="s">
+        <v>364</v>
+      </c>
+      <c r="B101" s="2" t="s">
         <v>365</v>
-      </c>
-      <c r="B101" s="8" t="s">
-        <v>366</v>
       </c>
       <c r="C101" s="10"/>
       <c r="D101" s="10"/>
       <c r="E101" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="F101" s="2" t="s">
         <v>367</v>
-      </c>
-      <c r="F101" s="8" t="s">
-        <v>368</v>
       </c>
     </row>
     <row r="102" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="B102" s="8" t="s">
         <v>369</v>
-      </c>
-      <c r="B102" s="8" t="s">
-        <v>370</v>
       </c>
       <c r="C102" s="10"/>
       <c r="D102" s="10"/>
       <c r="E102" s="8" t="s">
+        <v>370</v>
+      </c>
+      <c r="F102" s="8" t="s">
         <v>371</v>
-      </c>
-      <c r="F102" s="8" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="103" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="9" t="s">
+        <v>372</v>
+      </c>
+      <c r="B103" s="8" t="s">
         <v>373</v>
       </c>
-      <c r="B103" s="8" t="s">
+      <c r="C103" s="10"/>
+      <c r="D103" s="10"/>
+      <c r="E103" s="8" t="s">
         <v>374</v>
       </c>
-      <c r="C103" s="8" t="n">
-        <v>131</v>
-      </c>
-      <c r="D103" s="8" t="s">
+      <c r="F103" s="8" t="s">
         <v>375</v>
-      </c>
-      <c r="E103" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="F103" s="8" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="104" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="9" t="s">
+        <v>376</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>377</v>
+      </c>
+      <c r="C104" s="8" t="n">
+        <v>131</v>
+      </c>
+      <c r="D104" s="8" t="s">
         <v>378</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="E104" s="8" t="s">
         <v>379</v>
       </c>
-      <c r="C104" s="8" t="n">
-        <v>132</v>
-      </c>
-      <c r="D104" s="8" t="s">
+      <c r="F104" s="8" t="s">
         <v>380</v>
-      </c>
-      <c r="E104" s="8" t="s">
-        <v>381</v>
-      </c>
-      <c r="F104" s="8" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="105" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="9" t="s">
+        <v>381</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>382</v>
+      </c>
+      <c r="C105" s="8" t="n">
+        <v>132</v>
+      </c>
+      <c r="D105" s="8" t="s">
         <v>383</v>
       </c>
-      <c r="B105" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="C105" s="10" t="n">
-        <v>132</v>
-      </c>
-      <c r="D105" s="10"/>
-      <c r="E105" s="8"/>
-      <c r="G105" s="3" t="s">
-        <v>57</v>
+      <c r="E105" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="F105" s="8" t="s">
+        <v>385</v>
       </c>
     </row>
     <row r="106" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="9" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="C106" s="8" t="n">
-        <v>1731</v>
-      </c>
-      <c r="D106" s="8"/>
-      <c r="E106" s="8" t="s">
-        <v>386</v>
-      </c>
+        <v>382</v>
+      </c>
+      <c r="C106" s="10" t="n">
+        <v>132</v>
+      </c>
+      <c r="D106" s="10"/>
+      <c r="E106" s="8"/>
       <c r="G106" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="107" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="9" t="s">
         <v>387</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="C107" s="8" t="n">
         <v>1731</v>
       </c>
       <c r="D107" s="8"/>
-      <c r="E107" s="8"/>
-      <c r="F107" s="8" t="s">
-        <v>388</v>
+      <c r="E107" s="8" t="s">
+        <v>389</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="108" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="9" t="s">
         <v>390</v>
       </c>
       <c r="B108" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="C108" s="8" t="n">
+        <v>1731</v>
+      </c>
+      <c r="D108" s="8"/>
+      <c r="E108" s="8"/>
+      <c r="F108" s="8" t="s">
         <v>391</v>
       </c>
-      <c r="C108" s="8" t="n">
-        <v>2811</v>
-      </c>
-      <c r="D108" s="8"/>
-      <c r="E108" s="8" t="s">
+      <c r="G108" s="3" t="s">
         <v>392</v>
-      </c>
-      <c r="F108" s="8" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="109" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="9" t="s">
+        <v>393</v>
+      </c>
+      <c r="B109" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="B109" s="8" t="s">
-        <v>104</v>
-      </c>
       <c r="C109" s="8" t="n">
+        <v>2811</v>
+      </c>
+      <c r="D109" s="8"/>
+      <c r="E109" s="8" t="s">
+        <v>395</v>
+      </c>
+      <c r="F109" s="8" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="110" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="9" t="s">
+        <v>397</v>
+      </c>
+      <c r="B110" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C110" s="8" t="n">
         <v>200</v>
       </c>
-      <c r="D109" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="E109" s="8" t="s">
-        <v>396</v>
-      </c>
-      <c r="F109" s="8" t="s">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="110" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="12" t="s">
+      <c r="D110" s="8" t="s">
         <v>398</v>
       </c>
-      <c r="B110" s="8" t="s">
+      <c r="E110" s="8" t="s">
         <v>399</v>
       </c>
-      <c r="C110" s="8" t="n">
-        <v>300</v>
-      </c>
-      <c r="D110" s="8" t="s">
+      <c r="F110" s="8" t="s">
         <v>400</v>
       </c>
-      <c r="E110" s="8" t="s">
+    </row>
+    <row r="111" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="12" t="s">
         <v>401</v>
       </c>
-      <c r="F110" s="8" t="s">
+      <c r="B111" s="8" t="s">
         <v>402</v>
-      </c>
-    </row>
-    <row r="111" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="9" t="s">
-        <v>403</v>
-      </c>
-      <c r="B111" s="8" t="s">
-        <v>399</v>
       </c>
       <c r="C111" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D111" s="8" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="E111" s="8" t="s">
         <v>404</v>
@@ -4335,17 +4341,19 @@
         <v>406</v>
       </c>
       <c r="B112" s="8" t="s">
+        <v>402</v>
+      </c>
+      <c r="C112" s="8" t="n">
+        <v>300</v>
+      </c>
+      <c r="D112" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="E112" s="8" t="s">
         <v>407</v>
       </c>
-      <c r="C112" s="8" t="n">
-        <v>5500</v>
-      </c>
-      <c r="D112" s="8"/>
-      <c r="E112" s="8" t="s">
+      <c r="F112" s="8" t="s">
         <v>408</v>
-      </c>
-      <c r="G112" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4356,14 +4364,14 @@
         <v>410</v>
       </c>
       <c r="C113" s="8" t="n">
-        <v>5600</v>
+        <v>5500</v>
       </c>
       <c r="D113" s="8"/>
       <c r="E113" s="8" t="s">
         <v>411</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="114" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4374,89 +4382,90 @@
         <v>413</v>
       </c>
       <c r="C114" s="8" t="n">
-        <v>101</v>
-      </c>
-      <c r="D114" s="8" t="s">
+        <v>5600</v>
+      </c>
+      <c r="D114" s="8"/>
+      <c r="E114" s="8" t="s">
         <v>414</v>
       </c>
-      <c r="E114" s="8" t="s">
-        <v>415</v>
-      </c>
       <c r="G114" s="3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="115" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="B115" s="8" t="s">
         <v>416</v>
       </c>
-      <c r="B115" s="8" t="s">
+      <c r="C115" s="8" t="n">
+        <v>101</v>
+      </c>
+      <c r="D115" s="8" t="s">
         <v>417</v>
       </c>
-      <c r="C115" s="8" t="n">
-        <v>111</v>
-      </c>
-      <c r="D115" s="8" t="s">
+      <c r="E115" s="8" t="s">
         <v>418</v>
       </c>
-      <c r="E115" s="8" t="s">
-        <v>419</v>
-      </c>
       <c r="G115" s="3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="116" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="9" t="s">
+        <v>419</v>
+      </c>
+      <c r="B116" s="8" t="s">
         <v>420</v>
       </c>
-      <c r="B116" s="8" t="s">
+      <c r="C116" s="8" t="n">
+        <v>111</v>
+      </c>
+      <c r="D116" s="8" t="s">
         <v>421</v>
       </c>
-      <c r="C116" s="10"/>
-      <c r="D116" s="10"/>
       <c r="E116" s="8" t="s">
         <v>422</v>
       </c>
-      <c r="F116" s="8" t="s">
-        <v>423</v>
+      <c r="G116" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="117" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="9" t="s">
+        <v>423</v>
+      </c>
+      <c r="B117" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="B117" s="8" t="s">
+      <c r="C117" s="10"/>
+      <c r="D117" s="10"/>
+      <c r="E117" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="C117" s="8" t="n">
+      <c r="F117" s="8" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="118" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="B118" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="C118" s="8" t="n">
         <v>1000</v>
       </c>
-      <c r="D117" s="8" t="s">
-        <v>426</v>
-      </c>
-      <c r="E117" s="8" t="s">
-        <v>343</v>
-      </c>
-      <c r="G117" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="118" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A118" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="C118" s="2" t="n">
-        <v>9400</v>
+      <c r="D118" s="8" t="s">
+        <v>429</v>
       </c>
       <c r="E118" s="8" t="s">
-        <v>429</v>
+        <v>346</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="119" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4467,13 +4476,13 @@
         <v>431</v>
       </c>
       <c r="C119" s="2" t="n">
-        <v>9500</v>
-      </c>
-      <c r="E119" s="15" t="s">
+        <v>9400</v>
+      </c>
+      <c r="E119" s="8" t="s">
         <v>432</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="120" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4484,46 +4493,45 @@
         <v>434</v>
       </c>
       <c r="C120" s="2" t="n">
+        <v>9500</v>
+      </c>
+      <c r="E120" s="15" t="s">
+        <v>435</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="121" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="C121" s="2" t="n">
         <v>9600</v>
       </c>
-      <c r="E120" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="G120" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="121" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="9" t="s">
-        <v>436</v>
-      </c>
-      <c r="B121" s="8" t="s">
-        <v>437</v>
-      </c>
-      <c r="C121" s="8" t="n">
-        <v>112</v>
-      </c>
-      <c r="D121" s="8" t="s">
+      <c r="E121" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="E121" s="8" t="s">
-        <v>439</v>
-      </c>
-      <c r="F121" s="8" t="s">
-        <v>440</v>
+      <c r="G121" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="122" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="B122" s="8" t="s">
+        <v>440</v>
+      </c>
+      <c r="C122" s="8" t="n">
+        <v>112</v>
+      </c>
+      <c r="D122" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="B122" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="C122" s="8" t="n">
-        <v>3100</v>
-      </c>
-      <c r="D122" s="8"/>
       <c r="E122" s="8" t="s">
         <v>442</v>
       </c>
@@ -4536,37 +4544,35 @@
         <v>444</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>445</v>
+        <v>107</v>
       </c>
       <c r="C123" s="8" t="n">
-        <v>21</v>
+        <v>3100</v>
       </c>
       <c r="D123" s="8"/>
       <c r="E123" s="8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F123" s="8" t="s">
         <v>446</v>
-      </c>
-      <c r="F123" s="8" t="s">
-        <v>447</v>
       </c>
     </row>
     <row r="124" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="9" t="s">
+        <v>447</v>
+      </c>
+      <c r="B124" s="8" t="s">
         <v>448</v>
       </c>
-      <c r="B124" s="8" t="s">
-        <v>254</v>
-      </c>
       <c r="C124" s="8" t="n">
-        <v>122</v>
-      </c>
-      <c r="D124" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D124" s="8"/>
+      <c r="E124" s="8" t="s">
         <v>449</v>
       </c>
-      <c r="E124" s="8" t="s">
+      <c r="F124" s="8" t="s">
         <v>450</v>
-      </c>
-      <c r="G124" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="125" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4574,17 +4580,19 @@
         <v>451</v>
       </c>
       <c r="B125" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C125" s="8" t="n">
+        <v>122</v>
+      </c>
+      <c r="D125" s="8" t="s">
         <v>452</v>
       </c>
-      <c r="C125" s="8" t="n">
-        <v>1722</v>
-      </c>
-      <c r="D125" s="8"/>
       <c r="E125" s="8" t="s">
         <v>453</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4595,14 +4603,14 @@
         <v>455</v>
       </c>
       <c r="C126" s="8" t="n">
-        <v>7100</v>
+        <v>1722</v>
       </c>
       <c r="D126" s="8"/>
       <c r="E126" s="8" t="s">
         <v>456</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4612,229 +4620,231 @@
       <c r="B127" s="8" t="s">
         <v>458</v>
       </c>
-      <c r="C127" s="10"/>
-      <c r="D127" s="10"/>
+      <c r="C127" s="8" t="n">
+        <v>7100</v>
+      </c>
+      <c r="D127" s="8"/>
       <c r="E127" s="8" t="s">
         <v>459</v>
       </c>
-      <c r="F127" s="8" t="s">
-        <v>460</v>
+      <c r="G127" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="128" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="B128" s="8" t="s">
         <v>461</v>
       </c>
-      <c r="B128" s="2" t="s">
+      <c r="C128" s="10"/>
+      <c r="D128" s="10"/>
+      <c r="E128" s="8" t="s">
         <v>462</v>
       </c>
-      <c r="E128" s="8" t="s">
+      <c r="F128" s="8" t="s">
         <v>463</v>
-      </c>
-      <c r="F128" s="2" t="s">
-        <v>464</v>
       </c>
     </row>
     <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="9" t="s">
+        <v>464</v>
+      </c>
+      <c r="B129" s="2" t="s">
         <v>465</v>
       </c>
-      <c r="B129" s="8" t="s">
+      <c r="E129" s="8" t="s">
         <v>466</v>
       </c>
-      <c r="C129" s="10"/>
-      <c r="D129" s="10"/>
-      <c r="E129" s="8" t="s">
+      <c r="F129" s="2" t="s">
         <v>467</v>
-      </c>
-      <c r="F129" s="8" t="s">
-        <v>468</v>
       </c>
     </row>
     <row r="130" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="9" t="s">
+        <v>468</v>
+      </c>
+      <c r="B130" s="8" t="s">
         <v>469</v>
-      </c>
-      <c r="B130" s="8" t="s">
-        <v>470</v>
       </c>
       <c r="C130" s="10"/>
       <c r="D130" s="10"/>
       <c r="E130" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="F130" s="8" t="s">
         <v>471</v>
       </c>
-      <c r="F130" s="8" t="s">
+    </row>
+    <row r="131" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="9" t="s">
         <v>472</v>
       </c>
-    </row>
-    <row r="131" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="1" t="s">
+      <c r="B131" s="8" t="s">
         <v>473</v>
-      </c>
-      <c r="B131" s="8" t="s">
-        <v>474</v>
       </c>
       <c r="C131" s="10"/>
       <c r="D131" s="10"/>
       <c r="E131" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="F131" s="8" t="s">
         <v>475</v>
-      </c>
-      <c r="F131" s="8" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="132" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="B132" s="8" t="s">
         <v>477</v>
       </c>
-      <c r="B132" s="2" t="s">
+      <c r="C132" s="10"/>
+      <c r="D132" s="10"/>
+      <c r="E132" s="8" t="s">
         <v>478</v>
       </c>
-      <c r="C132" s="2" t="n">
+      <c r="F132" s="8" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="133" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="1" t="s">
+        <v>480</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="C133" s="2" t="n">
         <v>133</v>
       </c>
-      <c r="E132" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="F132" s="2" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="133" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="9" t="s">
-        <v>481</v>
-      </c>
-      <c r="B133" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="C133" s="8" t="n">
-        <v>400</v>
-      </c>
-      <c r="D133" s="8" t="s">
+      <c r="E133" s="8" t="s">
         <v>482</v>
       </c>
-      <c r="E133" s="8" t="s">
+      <c r="F133" s="2" t="s">
         <v>483</v>
       </c>
-      <c r="F133" s="8" t="s">
+    </row>
+    <row r="134" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="9" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="134" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="1" t="s">
-        <v>485</v>
-      </c>
       <c r="B134" s="8" t="s">
-        <v>486</v>
+        <v>293</v>
       </c>
       <c r="C134" s="8" t="n">
         <v>400</v>
       </c>
-      <c r="D134" s="8"/>
+      <c r="D134" s="8" t="s">
+        <v>485</v>
+      </c>
       <c r="E134" s="8" t="s">
+        <v>486</v>
+      </c>
+      <c r="F134" s="8" t="s">
         <v>487</v>
-      </c>
-      <c r="F134" s="8" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="135" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
+        <v>488</v>
+      </c>
+      <c r="B135" s="8" t="s">
         <v>489</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="C135" s="8" t="n">
+        <v>400</v>
+      </c>
+      <c r="D135" s="8"/>
+      <c r="E135" s="8" t="s">
         <v>490</v>
       </c>
-      <c r="C135" s="2" t="n">
-        <v>2612</v>
-      </c>
-      <c r="D135" s="2" t="s">
+      <c r="F135" s="8" t="s">
         <v>491</v>
-      </c>
-      <c r="E135" s="8" t="s">
-        <v>492</v>
-      </c>
-      <c r="F135" s="8" t="s">
-        <v>493</v>
       </c>
     </row>
     <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B136" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="C136" s="2" t="n">
+        <v>2612</v>
+      </c>
+      <c r="D136" s="2" t="s">
         <v>494</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="E136" s="8" t="s">
         <v>495</v>
       </c>
-      <c r="E136" s="8" t="s">
+      <c r="F136" s="8" t="s">
         <v>496</v>
       </c>
-      <c r="F136" s="2" t="s">
+    </row>
+    <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="1" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A137" s="9" t="s">
+      <c r="B137" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="B137" s="8" t="s">
+      <c r="E137" s="8" t="s">
         <v>499</v>
       </c>
-      <c r="C137" s="8" t="s">
+      <c r="F137" s="2" t="s">
         <v>500</v>
-      </c>
-      <c r="D137" s="8"/>
-      <c r="E137" s="8" t="s">
-        <v>501</v>
-      </c>
-      <c r="F137" s="8" t="s">
-        <v>502</v>
       </c>
     </row>
     <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="9" t="s">
+        <v>501</v>
+      </c>
+      <c r="B138" s="8" t="s">
+        <v>502</v>
+      </c>
+      <c r="C138" s="8" t="s">
         <v>503</v>
       </c>
-      <c r="B138" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C138" s="10" t="s">
+      <c r="D138" s="8"/>
+      <c r="E138" s="8" t="s">
         <v>504</v>
       </c>
-      <c r="D138" s="10"/>
-      <c r="E138" s="8" t="s">
+      <c r="F138" s="8" t="s">
         <v>505</v>
-      </c>
-      <c r="F138" s="8" t="s">
-        <v>506</v>
       </c>
     </row>
     <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="9" t="s">
+        <v>506</v>
+      </c>
+      <c r="B139" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C139" s="10" t="s">
         <v>507</v>
       </c>
-      <c r="B139" s="8" t="s">
+      <c r="D139" s="10"/>
+      <c r="E139" s="8" t="s">
         <v>508</v>
       </c>
-      <c r="C139" s="8" t="n">
-        <v>7600</v>
-      </c>
-      <c r="D139" s="8"/>
-      <c r="E139" s="8" t="s">
+      <c r="F139" s="8" t="s">
         <v>509</v>
-      </c>
-      <c r="F139" s="8" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="B140" s="8" t="s">
         <v>511</v>
       </c>
-      <c r="B140" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C140" s="10"/>
-      <c r="D140" s="10"/>
+      <c r="C140" s="8" t="n">
+        <v>7600</v>
+      </c>
+      <c r="D140" s="8"/>
       <c r="E140" s="8" t="s">
         <v>512</v>
       </c>
@@ -4849,10 +4859,8 @@
       <c r="B141" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C141" s="8" t="n">
-        <v>6000</v>
-      </c>
-      <c r="D141" s="8"/>
+      <c r="C141" s="10"/>
+      <c r="D141" s="10"/>
       <c r="E141" s="8" t="s">
         <v>515</v>
       </c>
@@ -4865,10 +4873,12 @@
         <v>517</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="C142" s="10"/>
-      <c r="D142" s="10"/>
+        <v>183</v>
+      </c>
+      <c r="C142" s="8" t="n">
+        <v>6000</v>
+      </c>
+      <c r="D142" s="8"/>
       <c r="E142" s="8" t="s">
         <v>518</v>
       </c>
@@ -4881,39 +4891,39 @@
         <v>520</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>521</v>
+        <v>238</v>
       </c>
       <c r="C143" s="10"/>
       <c r="D143" s="10"/>
       <c r="E143" s="8" t="s">
+        <v>521</v>
+      </c>
+      <c r="F143" s="8" t="s">
         <v>522</v>
-      </c>
-      <c r="F143" s="8" t="s">
-        <v>523</v>
       </c>
     </row>
     <row r="144" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="9" t="s">
+        <v>523</v>
+      </c>
+      <c r="B144" s="8" t="s">
         <v>524</v>
-      </c>
-      <c r="B144" s="8" t="s">
-        <v>525</v>
       </c>
       <c r="C144" s="10"/>
       <c r="D144" s="10"/>
       <c r="E144" s="8" t="s">
+        <v>525</v>
+      </c>
+      <c r="F144" s="8" t="s">
         <v>526</v>
-      </c>
-      <c r="F144" s="8" t="s">
-        <v>527</v>
       </c>
     </row>
     <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="9" t="s">
+        <v>527</v>
+      </c>
+      <c r="B145" s="8" t="s">
         <v>528</v>
-      </c>
-      <c r="B145" s="8" t="s">
-        <v>525</v>
       </c>
       <c r="C145" s="10"/>
       <c r="D145" s="10"/>
@@ -4929,158 +4939,158 @@
         <v>531</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="C146" s="10"/>
       <c r="D146" s="10"/>
       <c r="E146" s="8" t="s">
+        <v>532</v>
+      </c>
+      <c r="F146" s="8" t="s">
         <v>533</v>
-      </c>
-      <c r="F146" s="8" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="9" t="s">
+        <v>534</v>
+      </c>
+      <c r="B147" s="8" t="s">
         <v>535</v>
       </c>
-      <c r="B147" s="8" t="s">
+      <c r="C147" s="10"/>
+      <c r="D147" s="10"/>
+      <c r="E147" s="8" t="s">
         <v>536</v>
       </c>
-      <c r="C147" s="8" t="n">
-        <v>7700</v>
-      </c>
-      <c r="D147" s="8" t="s">
+      <c r="F147" s="8" t="s">
         <v>537</v>
-      </c>
-      <c r="E147" s="8" t="s">
-        <v>538</v>
-      </c>
-      <c r="F147" s="8" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="9" t="s">
+        <v>538</v>
+      </c>
+      <c r="B148" s="8" t="s">
+        <v>539</v>
+      </c>
+      <c r="C148" s="8" t="n">
+        <v>7700</v>
+      </c>
+      <c r="D148" s="8" t="s">
         <v>540</v>
       </c>
-      <c r="B148" s="8" t="s">
+      <c r="E148" s="8" t="s">
         <v>541</v>
       </c>
-      <c r="C148" s="8" t="n">
-        <v>7800</v>
-      </c>
-      <c r="D148" s="8" t="s">
+      <c r="F148" s="8" t="s">
         <v>542</v>
-      </c>
-      <c r="E148" s="8" t="s">
-        <v>543</v>
-      </c>
-      <c r="F148" s="8" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="9" t="s">
+        <v>543</v>
+      </c>
+      <c r="B149" s="8" t="s">
         <v>544</v>
       </c>
-      <c r="B149" s="8" t="s">
+      <c r="C149" s="8" t="n">
+        <v>7800</v>
+      </c>
+      <c r="D149" s="8" t="s">
         <v>545</v>
       </c>
-      <c r="C149" s="10"/>
-      <c r="D149" s="10"/>
       <c r="E149" s="8" t="s">
         <v>546</v>
       </c>
       <c r="F149" s="8" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A150" s="9" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A150" s="1" t="s">
+      <c r="B150" s="8" t="s">
         <v>548</v>
       </c>
-      <c r="B150" s="2" t="s">
+      <c r="C150" s="10"/>
+      <c r="D150" s="10"/>
+      <c r="E150" s="8" t="s">
         <v>549</v>
       </c>
-      <c r="C150" s="2" t="n">
+      <c r="F150" s="8" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="1" t="s">
+        <v>551</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>552</v>
+      </c>
+      <c r="C151" s="2" t="n">
         <v>8900</v>
-      </c>
-      <c r="E150" s="8" t="s">
-        <v>550</v>
-      </c>
-      <c r="G150" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="9" t="s">
-        <v>551</v>
-      </c>
-      <c r="B151" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="C151" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="D151" s="10" t="s">
-        <v>552</v>
       </c>
       <c r="E151" s="8" t="s">
         <v>553</v>
       </c>
-      <c r="F151" s="8" t="s">
-        <v>554</v>
+      <c r="G151" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="B152" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C152" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="D152" s="10" t="s">
         <v>555</v>
       </c>
-      <c r="B152" s="8" t="s">
+      <c r="E152" s="8" t="s">
         <v>556</v>
       </c>
-      <c r="C152" s="10"/>
-      <c r="D152" s="10"/>
-      <c r="E152" s="8" t="s">
+      <c r="F152" s="8" t="s">
         <v>557</v>
-      </c>
-      <c r="F152" s="8" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="9" t="s">
+        <v>558</v>
+      </c>
+      <c r="B153" s="8" t="s">
         <v>559</v>
       </c>
-      <c r="B153" s="8" t="s">
-        <v>413</v>
-      </c>
-      <c r="C153" s="8" t="n">
-        <v>101</v>
-      </c>
-      <c r="D153" s="8"/>
+      <c r="C153" s="10"/>
+      <c r="D153" s="10"/>
       <c r="E153" s="8" t="s">
-        <v>415</v>
-      </c>
-      <c r="G153" s="3" t="s">
-        <v>57</v>
+        <v>560</v>
+      </c>
+      <c r="F153" s="8" t="s">
+        <v>561</v>
       </c>
     </row>
     <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="9" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="C154" s="10"/>
-      <c r="D154" s="10"/>
+        <v>416</v>
+      </c>
+      <c r="C154" s="8" t="n">
+        <v>101</v>
+      </c>
+      <c r="D154" s="8"/>
       <c r="E154" s="8" t="s">
-        <v>561</v>
-      </c>
-      <c r="F154" s="8" t="s">
-        <v>562</v>
+        <v>418</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5091,123 +5101,123 @@
         <v>257</v>
       </c>
       <c r="C155" s="10"/>
-      <c r="D155" s="10" t="s">
+      <c r="D155" s="10"/>
+      <c r="E155" s="8" t="s">
         <v>564</v>
       </c>
-      <c r="E155" s="8" t="s">
+      <c r="F155" s="8" t="s">
         <v>565</v>
-      </c>
-      <c r="F155" s="8" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="9" t="s">
+        <v>566</v>
+      </c>
+      <c r="B156" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C156" s="10"/>
+      <c r="D156" s="10" t="s">
         <v>567</v>
       </c>
-      <c r="B156" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="C156" s="8" t="n">
+      <c r="E156" s="8" t="s">
+        <v>568</v>
+      </c>
+      <c r="F156" s="8" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A157" s="9" t="s">
+        <v>570</v>
+      </c>
+      <c r="B157" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C157" s="8" t="n">
         <v>1400</v>
       </c>
-      <c r="D156" s="8" t="s">
-        <v>568</v>
-      </c>
-      <c r="E156" s="8" t="s">
-        <v>569</v>
-      </c>
-      <c r="F156" s="8" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="1" t="s">
+      <c r="D157" s="8" t="s">
         <v>571</v>
       </c>
-      <c r="B157" s="8" t="s">
+      <c r="E157" s="8" t="s">
         <v>572</v>
       </c>
-      <c r="C157" s="8" t="n">
+      <c r="F157" s="8" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="1" t="s">
+        <v>574</v>
+      </c>
+      <c r="B158" s="8" t="s">
+        <v>575</v>
+      </c>
+      <c r="C158" s="8" t="n">
         <v>7400</v>
       </c>
-      <c r="D157" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E157" s="8" t="s">
-        <v>573</v>
-      </c>
-      <c r="F157" s="8" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="9" t="s">
-        <v>575</v>
-      </c>
-      <c r="B158" s="8" t="s">
+      <c r="D158" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E158" s="8" t="s">
         <v>576</v>
       </c>
-      <c r="C158" s="10"/>
-      <c r="D158" s="10" t="s">
+      <c r="F158" s="8" t="s">
         <v>577</v>
-      </c>
-      <c r="E158" s="8" t="s">
-        <v>578</v>
-      </c>
-      <c r="F158" s="8" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="159" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="9" t="s">
+        <v>578</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>579</v>
+      </c>
+      <c r="C159" s="10"/>
+      <c r="D159" s="10" t="s">
         <v>580</v>
       </c>
-      <c r="B159" s="8" t="s">
-        <v>525</v>
-      </c>
-      <c r="C159" s="8" t="n">
-        <v>1700</v>
-      </c>
-      <c r="D159" s="8" t="s">
+      <c r="E159" s="8" t="s">
         <v>581</v>
       </c>
-      <c r="E159" s="8" t="s">
+      <c r="F159" s="8" t="s">
         <v>582</v>
-      </c>
-      <c r="F159" s="8" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="9" t="s">
+        <v>583</v>
+      </c>
+      <c r="B160" s="8" t="s">
+        <v>528</v>
+      </c>
+      <c r="C160" s="8" t="n">
+        <v>1700</v>
+      </c>
+      <c r="D160" s="8" t="s">
         <v>584</v>
       </c>
-      <c r="B160" s="8" t="s">
+      <c r="E160" s="8" t="s">
         <v>585</v>
       </c>
-      <c r="C160" s="8" t="n">
-        <v>1800</v>
-      </c>
-      <c r="D160" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="E160" s="8" t="s">
+      <c r="F160" s="8" t="s">
         <v>586</v>
-      </c>
-      <c r="F160" s="8" t="s">
-        <v>587</v>
       </c>
     </row>
     <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="9" t="s">
+        <v>587</v>
+      </c>
+      <c r="B161" s="8" t="s">
         <v>588</v>
       </c>
-      <c r="B161" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="C161" s="7"/>
-      <c r="D161" s="7"/>
+      <c r="C161" s="8" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D161" s="8" t="s">
+        <v>130</v>
+      </c>
       <c r="E161" s="8" t="s">
         <v>589</v>
       </c>
@@ -5220,17 +5230,15 @@
         <v>591</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="C162" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="C162" s="7"/>
+      <c r="D162" s="7"/>
+      <c r="E162" s="8" t="s">
         <v>592</v>
       </c>
-      <c r="D162" s="10"/>
-      <c r="E162" s="8" t="s">
+      <c r="F162" s="8" t="s">
         <v>593</v>
-      </c>
-      <c r="F162" s="8" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5238,39 +5246,41 @@
         <v>594</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="C163" s="10"/>
+        <v>238</v>
+      </c>
+      <c r="C163" s="10" t="s">
+        <v>595</v>
+      </c>
       <c r="D163" s="10"/>
       <c r="E163" s="8" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="F163" s="8" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
     </row>
     <row r="164" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="9" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>525</v>
+        <v>579</v>
       </c>
       <c r="C164" s="10"/>
       <c r="D164" s="10"/>
       <c r="E164" s="8" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="F164" s="8" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
     </row>
     <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="9" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>599</v>
+        <v>528</v>
       </c>
       <c r="C165" s="10"/>
       <c r="D165" s="10"/>
@@ -5278,15 +5288,15 @@
         <v>600</v>
       </c>
       <c r="F165" s="8" t="s">
-        <v>601</v>
+        <v>593</v>
       </c>
     </row>
     <row r="166" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="B166" s="8" t="s">
         <v>602</v>
-      </c>
-      <c r="B166" s="8" t="s">
-        <v>576</v>
       </c>
       <c r="C166" s="10"/>
       <c r="D166" s="10"/>
@@ -5302,7 +5312,7 @@
         <v>605</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>525</v>
+        <v>579</v>
       </c>
       <c r="C167" s="10"/>
       <c r="D167" s="10"/>
@@ -5318,7 +5328,7 @@
         <v>608</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>235</v>
+        <v>528</v>
       </c>
       <c r="C168" s="10"/>
       <c r="D168" s="10"/>
@@ -5334,7 +5344,7 @@
         <v>611</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>177</v>
+        <v>238</v>
       </c>
       <c r="C169" s="10"/>
       <c r="D169" s="10"/>
@@ -5366,7 +5376,7 @@
         <v>617</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>257</v>
+        <v>183</v>
       </c>
       <c r="C171" s="10"/>
       <c r="D171" s="10"/>
@@ -5382,7 +5392,7 @@
         <v>620</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>525</v>
+        <v>260</v>
       </c>
       <c r="C172" s="10"/>
       <c r="D172" s="10"/>
@@ -5398,7 +5408,7 @@
         <v>623</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>177</v>
+        <v>528</v>
       </c>
       <c r="C173" s="10"/>
       <c r="D173" s="10"/>
@@ -5430,7 +5440,7 @@
         <v>629</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>257</v>
+        <v>183</v>
       </c>
       <c r="C175" s="10"/>
       <c r="D175" s="10"/>
@@ -5446,7 +5456,7 @@
         <v>632</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>235</v>
+        <v>260</v>
       </c>
       <c r="C176" s="10"/>
       <c r="D176" s="10"/>
@@ -5462,7 +5472,7 @@
         <v>635</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>576</v>
+        <v>238</v>
       </c>
       <c r="C177" s="10"/>
       <c r="D177" s="10"/>
@@ -5474,38 +5484,36 @@
       </c>
     </row>
     <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A178" s="1" t="s">
+      <c r="A178" s="9" t="s">
         <v>638</v>
       </c>
-      <c r="B178" s="2" t="s">
+      <c r="B178" s="8" t="s">
+        <v>579</v>
+      </c>
+      <c r="C178" s="10"/>
+      <c r="D178" s="10"/>
+      <c r="E178" s="8" t="s">
         <v>639</v>
       </c>
-      <c r="C178" s="2" t="n">
+      <c r="F178" s="8" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A179" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>642</v>
+      </c>
+      <c r="C179" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="E178" s="8" t="s">
-        <v>640</v>
-      </c>
-      <c r="F178" s="2" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="9" t="s">
-        <v>642</v>
-      </c>
-      <c r="B179" s="8" t="s">
+      <c r="E179" s="8" t="s">
         <v>643</v>
       </c>
-      <c r="C179" s="8" t="n">
-        <v>121</v>
-      </c>
-      <c r="D179" s="8"/>
-      <c r="E179" s="8" t="s">
+      <c r="F179" s="2" t="s">
         <v>644</v>
-      </c>
-      <c r="G179" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5513,15 +5521,17 @@
         <v>645</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C180" s="10"/>
-      <c r="D180" s="10"/>
+        <v>646</v>
+      </c>
+      <c r="C180" s="8" t="n">
+        <v>121</v>
+      </c>
+      <c r="D180" s="8"/>
       <c r="E180" s="8" t="s">
-        <v>646</v>
-      </c>
-      <c r="F180" s="8" t="s">
         <v>647</v>
+      </c>
+      <c r="G180" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5529,7 +5539,7 @@
         <v>648</v>
       </c>
       <c r="B181" s="8" t="s">
-        <v>235</v>
+        <v>180</v>
       </c>
       <c r="C181" s="10"/>
       <c r="D181" s="10"/>
@@ -5545,84 +5555,84 @@
         <v>651</v>
       </c>
       <c r="B182" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C182" s="10"/>
+      <c r="D182" s="10"/>
+      <c r="E182" s="8" t="s">
         <v>652</v>
       </c>
-      <c r="C182" s="8" t="n">
-        <v>111</v>
-      </c>
-      <c r="D182" s="8"/>
-      <c r="E182" s="8" t="s">
-        <v>419</v>
-      </c>
-      <c r="G182" s="3" t="s">
-        <v>57</v>
+      <c r="F182" s="8" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="9" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>308</v>
+        <v>655</v>
       </c>
       <c r="C183" s="8" t="n">
-        <v>1711</v>
+        <v>111</v>
       </c>
       <c r="D183" s="8"/>
       <c r="E183" s="8" t="s">
-        <v>309</v>
-      </c>
-      <c r="F183" s="8" t="s">
-        <v>310</v>
+        <v>422</v>
+      </c>
+      <c r="G183" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A184" s="1" t="s">
-        <v>654</v>
+      <c r="A184" s="9" t="s">
+        <v>656</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>655</v>
+        <v>311</v>
       </c>
       <c r="C184" s="8" t="n">
-        <v>3300</v>
+        <v>1711</v>
       </c>
       <c r="D184" s="8"/>
       <c r="E184" s="8" t="s">
-        <v>656</v>
+        <v>312</v>
       </c>
       <c r="F184" s="8" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A185" s="1" t="s">
         <v>657</v>
       </c>
-    </row>
-    <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="9" t="s">
+      <c r="B185" s="8" t="s">
         <v>658</v>
       </c>
-      <c r="B185" s="8" t="s">
+      <c r="C185" s="8" t="n">
+        <v>3300</v>
+      </c>
+      <c r="D185" s="8"/>
+      <c r="E185" s="8" t="s">
         <v>659</v>
       </c>
-      <c r="C185" s="8" t="n">
-        <v>8000</v>
-      </c>
-      <c r="D185" s="8" t="s">
+      <c r="F185" s="8" t="s">
         <v>660</v>
-      </c>
-      <c r="E185" s="8" t="s">
-        <v>661</v>
-      </c>
-      <c r="F185" s="8" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="9" t="s">
+        <v>661</v>
+      </c>
+      <c r="B186" s="8" t="s">
+        <v>662</v>
+      </c>
+      <c r="C186" s="8" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D186" s="8" t="s">
         <v>663</v>
       </c>
-      <c r="B186" s="8" t="s">
-        <v>177</v>
-      </c>
-      <c r="C186" s="10"/>
-      <c r="D186" s="10"/>
       <c r="E186" s="8" t="s">
         <v>664</v>
       </c>
@@ -5651,7 +5661,7 @@
         <v>669</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>254</v>
+        <v>183</v>
       </c>
       <c r="C188" s="10"/>
       <c r="D188" s="10"/>
@@ -5667,55 +5677,53 @@
         <v>672</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="C189" s="8" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D189" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C189" s="10"/>
+      <c r="D189" s="10"/>
+      <c r="E189" s="8" t="s">
         <v>673</v>
       </c>
-      <c r="E189" s="8" t="s">
+      <c r="F189" s="8" t="s">
         <v>674</v>
-      </c>
-      <c r="F189" s="8" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="9" t="s">
         <v>675</v>
       </c>
-      <c r="B190" s="2" t="s">
+      <c r="B190" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C190" s="8" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D190" s="8" t="s">
         <v>676</v>
       </c>
-      <c r="C190" s="8" t="n">
-        <v>2611</v>
-      </c>
-      <c r="D190" s="8"/>
       <c r="E190" s="8" t="s">
         <v>677</v>
       </c>
-      <c r="G190" s="3" t="s">
-        <v>57</v>
+      <c r="F190" s="8" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="9" t="s">
         <v>678</v>
       </c>
-      <c r="B191" s="8" t="s">
+      <c r="B191" s="2" t="s">
         <v>679</v>
       </c>
       <c r="C191" s="8" t="n">
-        <v>2711</v>
+        <v>2611</v>
       </c>
       <c r="D191" s="8"/>
       <c r="E191" s="8" t="s">
         <v>680</v>
       </c>
       <c r="G191" s="3" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
     </row>
     <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5723,15 +5731,17 @@
         <v>681</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>235</v>
-      </c>
-      <c r="C192" s="10"/>
-      <c r="D192" s="10"/>
+        <v>682</v>
+      </c>
+      <c r="C192" s="8" t="n">
+        <v>2711</v>
+      </c>
+      <c r="D192" s="8"/>
       <c r="E192" s="8" t="s">
-        <v>682</v>
-      </c>
-      <c r="F192" s="8" t="s">
         <v>683</v>
+      </c>
+      <c r="G192" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5739,44 +5749,42 @@
         <v>684</v>
       </c>
       <c r="B193" s="8" t="s">
-        <v>685</v>
+        <v>238</v>
       </c>
       <c r="C193" s="10"/>
       <c r="D193" s="10"/>
       <c r="E193" s="8" t="s">
+        <v>685</v>
+      </c>
+      <c r="F193" s="8" t="s">
         <v>686</v>
-      </c>
-      <c r="F193" s="8" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="9" t="s">
+        <v>687</v>
+      </c>
+      <c r="B194" s="8" t="s">
         <v>688</v>
       </c>
-      <c r="B194" s="8" t="s">
+      <c r="C194" s="10"/>
+      <c r="D194" s="10"/>
+      <c r="E194" s="8" t="s">
         <v>689</v>
       </c>
-      <c r="C194" s="8" t="n">
-        <v>3721</v>
-      </c>
-      <c r="D194" s="8"/>
-      <c r="E194" s="8" t="s">
+      <c r="F194" s="8" t="s">
         <v>690</v>
-      </c>
-      <c r="F194" s="8" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="9" t="s">
+        <v>691</v>
+      </c>
+      <c r="B195" s="8" t="s">
         <v>692</v>
       </c>
-      <c r="B195" s="8" t="s">
-        <v>525</v>
-      </c>
       <c r="C195" s="8" t="n">
-        <v>6100</v>
+        <v>3721</v>
       </c>
       <c r="D195" s="8"/>
       <c r="E195" s="8" t="s">
@@ -5791,28 +5799,30 @@
         <v>695</v>
       </c>
       <c r="B196" s="8" t="s">
+        <v>528</v>
+      </c>
+      <c r="C196" s="8" t="n">
+        <v>6100</v>
+      </c>
+      <c r="D196" s="8"/>
+      <c r="E196" s="8" t="s">
         <v>696</v>
       </c>
-      <c r="C196" s="10" t="n">
-        <v>8400</v>
-      </c>
-      <c r="D196" s="10"/>
-      <c r="E196" s="8" t="s">
+      <c r="F196" s="8" t="s">
         <v>697</v>
-      </c>
-      <c r="F196" s="8" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="9" t="s">
+        <v>698</v>
+      </c>
+      <c r="B197" s="8" t="s">
         <v>699</v>
       </c>
-      <c r="B197" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C197" s="7"/>
-      <c r="D197" s="7"/>
+      <c r="C197" s="10" t="n">
+        <v>8400</v>
+      </c>
+      <c r="D197" s="10"/>
       <c r="E197" s="8" t="s">
         <v>700</v>
       </c>
@@ -5821,16 +5831,14 @@
       </c>
     </row>
     <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A198" s="1" t="s">
+      <c r="A198" s="9" t="s">
         <v>702</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>290</v>
-      </c>
-      <c r="C198" s="8" t="n">
-        <v>400</v>
-      </c>
-      <c r="D198" s="8"/>
+        <v>49</v>
+      </c>
+      <c r="C198" s="7"/>
+      <c r="D198" s="7"/>
       <c r="E198" s="8" t="s">
         <v>703</v>
       </c>
@@ -5843,7 +5851,7 @@
         <v>705</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>486</v>
+        <v>293</v>
       </c>
       <c r="C199" s="8" t="n">
         <v>400</v>
@@ -5853,23 +5861,25 @@
         <v>706</v>
       </c>
       <c r="F199" s="8" t="s">
-        <v>488</v>
+        <v>707</v>
       </c>
     </row>
     <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="9" t="s">
-        <v>707</v>
+      <c r="A200" s="1" t="s">
+        <v>708</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C200" s="10"/>
-      <c r="D200" s="10"/>
+        <v>489</v>
+      </c>
+      <c r="C200" s="8" t="n">
+        <v>400</v>
+      </c>
+      <c r="D200" s="8"/>
       <c r="E200" s="8" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="F200" s="8" t="s">
-        <v>709</v>
+        <v>491</v>
       </c>
     </row>
     <row r="201" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5877,31 +5887,47 @@
         <v>710</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="C201" s="8" t="n">
-        <v>21</v>
-      </c>
-      <c r="D201" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="C201" s="10"/>
+      <c r="D201" s="10"/>
       <c r="E201" s="8" t="s">
         <v>711</v>
       </c>
-      <c r="G201" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="1" t="s">
+      <c r="F201" s="8" t="s">
         <v>712</v>
       </c>
+    </row>
+    <row r="202" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A202" s="9" t="s">
+        <v>713</v>
+      </c>
       <c r="B202" s="8" t="s">
-        <v>177</v>
-      </c>
+        <v>448</v>
+      </c>
+      <c r="C202" s="8" t="n">
+        <v>21</v>
+      </c>
+      <c r="D202" s="8"/>
       <c r="E202" s="8" t="s">
-        <v>713</v>
-      </c>
-      <c r="F202" s="8" t="s">
         <v>714</v>
+      </c>
+      <c r="G202" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="B203" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E203" s="8" t="s">
+        <v>716</v>
+      </c>
+      <c r="F203" s="8" t="s">
+        <v>717</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Microsoft Office ≤ 2003
added Microsoft Office ≤ 2003 MD5&SHA1 supported in the latest beta of
oclHashcat
</commit_message>
<xml_diff>
--- a/hashinfo.xlsx
+++ b/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="724">
   <si>
     <t>Hash</t>
   </si>
@@ -116,7 +116,7 @@
     <t>Android FDE ≤ 4.3</t>
   </si>
   <si>
-    <t>^\$fde\$[0-9]{2}\$[a-f0-9]{32}\$[0-9]{2}\$[a-f0-9]{32}\$[a-f0-9]{3072}$</t>
+    <t>^\$fde\$[0-9]{2}\$[a-f0-9]{32}\$[0-9]{2}\$[a-f0-9]{32}\$[a-f0-9]{3072}$/i</t>
   </si>
   <si>
     <t>$fde$16$ca56e82e7b5a9c2fc1e3b5a7d671c2f9$16$7c124af19ac913be0fc137b75a34b20d$eac806ae7277c8d48243d52a8644fa57a817317bd3457f94dca727964cbc27c88296954f289597a9de3314a4e9d9f28dce70cf9ce3e1c3c0c6fc041687a0ad3cb333d4449bc9da8fcc7d5f85948a7ac3bc6d34f505e9d0d91da4396e35840bde3465ad11c5086c89ee6db68d65e47a2e5413f272caa01e02224e5ff3dc3bed3953a702e85e964e562e62f5c97a2df6c47547bfb5aeeb329ff8f9c9666724d399043fe970c8b282b45e93d008333f3b4edd5eb147bd023ed18ac1f9f75a6cd33444b507694c64e1e98a964b48c0a77276e9930250d01801813c235169a7b1952891c63ce0d462abc688bd96c0337174695a957858b4c9fd277d04abe8a0c2c5def4b352ba29410f8dbec91bcb2ca2b8faf26d44f02340b3373bc94e7487ce014e6adfbf7edfdd2057225f8aeb324c9d1be877c6ae4211ae387e07bf2a056984d2ed2815149b3e9cf9fbfae852f7dd5906c2b86e7910c0d7755ef5bcc39f0e135bf546c839693dc4af3e50b8382c7c8c754d4ee218fa85d70ee0a5707a9f827209a7ddb6c2fb9431a61c9775112cc88aa2a34f97c2f53dfce082aa0758917269a5fc30049ceab67d3efd721fee021ffca979f839b4f052e27f5c382c0dd5c02fd39fbc9b26e04bf9e051d1923eff9a7cde3244902bb8538b1b9f11631def5aad7c21d2113bcdc989b771ff6bf220f94354034dd417510117b55a669e969fc3bc6c5dcd4741b8313bf7d999dc94d4949f27eec0cd06f906c17a80d09f583a5dd601854832673b78d125a2c5ad0352932be7b93c611fee8c6049670442d8c532674f3d21d45d3d009211d2a9e6568252ac4682982172cb43e7c6b05e85851787ad90e25b77cce3f7968d455f92653a1d3790bc50e5f6e1f743ac47275ffa8e81bbe832a8d7d78d5d5a7c73f95703aebb355849ae566492093bd9cb51070f39c69bb4e22b99cc0e60e96d048385bb69f1c44a3b79547fbc19a873a632f43f05fa2d8a6f9155e59d153e2851b739c42444018b8c4e09a93be43570834667d0b5a5d2a53b1572dab3e750b3f9e641e303559bace06612fbd451a5e822201442828e79168c567a85d8c024cd8ce32bf650105b1af98cc5428675f4f4bbede37a0ef98d1533a8a6dcb27d87a2b799f18706f4677edaa0411becac4c591ede83993aedba660d1dd67f6c4a5c141ad3e6e0c77730cb0ecbf4f4bd8ef6067e05ca3bc563d9e1554a893fea0050bdd1733c883f533f87eac39cceee0ccf817fc1f19bcfdd13e9f241b89bfb149b509e9a0747658438536b6705514cc6d6bb3c64c903e4710435d8bebc35297d1ebbdff8074b203f37d1910d8b4637e4d3dab997f4aa378a7a67c79e698a11e83d0d7e759d0e7969c4f5408168b282fe28d3279ec1d4cc6f85a0f8e5d01f21c7508a69773c44167ff8d467d0801f9ec54f9ee2496d4e7e470214abc1ca11355bb18cd23273aac6b05b47f9e301b42b137a2455758c24e2716dcd2e55bbeb780f592e664e7392bf6eccb80959f24c8800816c84f2575e82e1f3559c33a5be7a3a0c843c2989f486b113d5eeada007caf6b5a0f6d71e2f5c09a4def57c7057168051868317a9ec790d570d76a0d21a45ad951c475db5a66101475871147c5a5907ec4e6b14128ed6695bb73c1c97952e96826eeb6003aa13462093e4afc209627241f03b0247e110fbab983640423b7cdf112e01579fed68c80ac7df7449d9d2114b9ae5539c03c2037be45c5f74e7357b25c6a24b7bd503864437147e50d7ac4ccc4bbd0cabecdc6bac60a362285fe450e2c2d0a446578c8880dc957e6e8061e691b83eb8062d1aad476e0c7b25e4d5454f1288686eb525f37fe649637b235b7828366b0219a9c63d6ddbb696dc3585a2ebfbd5f5e4c170d6784ab9993e15142535e194d2bee3dc9477ef8b8e1b07605e0c04f49edf6d42be3a9dabbc592dde78ce8b7dd9684bfcf4ca2f5a44b1872abe18fb6fa67a79390f273a9d12f9269389629456d71b9e7ed3447462269a849ce83e1893f253c832537f850b1acce5b11d2ba6b7c2f99e8e7c8085f390c21f69e1ce4bbf85b4e1ad86c0d6706432766978076f4cada9ca6f28d395d9cc5e74b2a6b46eb9d1de79eeecff7dc97ec2a8d8870e3894e1e4e26ccb98dd2f88c0229bbd3152fa149f0cc132561f</t>
@@ -1119,6 +1119,24 @@
   </si>
   <si>
     <t>http://www.remkoweijnen.nl/blog/2008/03/02/how-rdp-passwords-are-encrypted-2/</t>
+  </si>
+  <si>
+    <t>Microsoft Office ≤ 2003 (MD5+RC4)</t>
+  </si>
+  <si>
+    <t>^\$oldoffice\$[01]\*[0-9]{32}\*[a-f0-9]{32}\*[a-f0-9]{32}$/i</t>
+  </si>
+  <si>
+    <t>$oldoffice$1*04477077758555626246182730342136*b1b72ff351e41a7c68f6b45c4e938bd6*0d95331895e99f73ef8b6fbc4a78ac1a</t>
+  </si>
+  <si>
+    <t>Microsoft Office ≤ 2003 (SHA1+RC4)</t>
+  </si>
+  <si>
+    <t>^\$oldoffice\$[34]\*[0-9]{32}\*[a-f0-9]{32}\*[a-f0-9]{40}$/i</t>
+  </si>
+  <si>
+    <t>$oldoffice$3*83328705222323020515404251156288*2855956a165ff6511bc7f4cd77b9e101*941861655e73a09c40f7b1e9dfd0c256ed285acd</t>
   </si>
   <si>
     <t>Minecraft(AuthMe Reloaded)</t>
@@ -2264,7 +2282,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2325,6 +2343,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="true"/>
       <protection locked="true" hidden="false"/>
@@ -2347,10 +2369,10 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G203"/>
+  <dimension ref="A1:G205"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A208" activeCellId="0" sqref="A208"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A121" activeCellId="0" sqref="A121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2530,7 +2552,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -4153,92 +4175,90 @@
         <v>367</v>
       </c>
     </row>
-    <row r="102" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="9" t="s">
+    <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="13" t="s">
         <v>368</v>
       </c>
-      <c r="B102" s="8" t="s">
+      <c r="B102" s="2" t="s">
         <v>369</v>
       </c>
-      <c r="C102" s="10"/>
-      <c r="D102" s="10"/>
-      <c r="E102" s="8" t="s">
+      <c r="C102" s="2" t="n">
+        <v>9700</v>
+      </c>
+      <c r="E102" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="F102" s="8" t="s">
+      <c r="G102" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="13" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="103" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="9" t="s">
+      <c r="B103" s="2" t="s">
         <v>372</v>
       </c>
-      <c r="B103" s="8" t="s">
+      <c r="C103" s="2" t="n">
+        <v>9800</v>
+      </c>
+      <c r="E103" s="2" t="s">
         <v>373</v>
       </c>
-      <c r="C103" s="10"/>
-      <c r="D103" s="10"/>
-      <c r="E103" s="8" t="s">
-        <v>374</v>
-      </c>
-      <c r="F103" s="8" t="s">
-        <v>375</v>
+      <c r="G103" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="104" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="B104" s="8" t="s">
+        <v>375</v>
+      </c>
+      <c r="C104" s="10"/>
+      <c r="D104" s="10"/>
+      <c r="E104" s="8" t="s">
         <v>376</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="F104" s="8" t="s">
         <v>377</v>
-      </c>
-      <c r="C104" s="8" t="n">
-        <v>131</v>
-      </c>
-      <c r="D104" s="8" t="s">
-        <v>378</v>
-      </c>
-      <c r="E104" s="8" t="s">
-        <v>379</v>
-      </c>
-      <c r="F104" s="8" t="s">
-        <v>380</v>
       </c>
     </row>
     <row r="105" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="9" t="s">
+        <v>378</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>379</v>
+      </c>
+      <c r="C105" s="10"/>
+      <c r="D105" s="10"/>
+      <c r="E105" s="8" t="s">
+        <v>380</v>
+      </c>
+      <c r="F105" s="8" t="s">
         <v>381</v>
-      </c>
-      <c r="B105" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="C105" s="8" t="n">
-        <v>132</v>
-      </c>
-      <c r="D105" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="E105" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="F105" s="8" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="106" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="B106" s="8" t="s">
+        <v>383</v>
+      </c>
+      <c r="C106" s="8" t="n">
+        <v>131</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="E106" s="8" t="s">
+        <v>385</v>
+      </c>
+      <c r="F106" s="8" t="s">
         <v>386</v>
-      </c>
-      <c r="B106" s="8" t="s">
-        <v>382</v>
-      </c>
-      <c r="C106" s="10" t="n">
-        <v>132</v>
-      </c>
-      <c r="D106" s="10"/>
-      <c r="E106" s="8"/>
-      <c r="G106" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="107" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4249,33 +4269,32 @@
         <v>388</v>
       </c>
       <c r="C107" s="8" t="n">
-        <v>1731</v>
-      </c>
-      <c r="D107" s="8"/>
+        <v>132</v>
+      </c>
+      <c r="D107" s="8" t="s">
+        <v>389</v>
+      </c>
       <c r="E107" s="8" t="s">
-        <v>389</v>
-      </c>
-      <c r="G107" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>390</v>
+      </c>
+      <c r="F107" s="8" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="108" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="9" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="B108" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="C108" s="8" t="n">
-        <v>1731</v>
-      </c>
-      <c r="D108" s="8"/>
+      <c r="C108" s="10" t="n">
+        <v>132</v>
+      </c>
+      <c r="D108" s="10"/>
       <c r="E108" s="8"/>
-      <c r="F108" s="8" t="s">
-        <v>391</v>
-      </c>
       <c r="G108" s="3" t="s">
-        <v>392</v>
+        <v>35</v>
       </c>
     </row>
     <row r="109" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4286,92 +4305,91 @@
         <v>394</v>
       </c>
       <c r="C109" s="8" t="n">
-        <v>2811</v>
+        <v>1731</v>
       </c>
       <c r="D109" s="8"/>
       <c r="E109" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="F109" s="8" t="s">
+      <c r="G109" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A110" s="9" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="110" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="9" t="s">
+      <c r="B110" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="C110" s="8" t="n">
+        <v>1731</v>
+      </c>
+      <c r="D110" s="8"/>
+      <c r="E110" s="8"/>
+      <c r="F110" s="8" t="s">
         <v>397</v>
       </c>
-      <c r="B110" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C110" s="8" t="n">
-        <v>200</v>
-      </c>
-      <c r="D110" s="8" t="s">
+      <c r="G110" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="E110" s="8" t="s">
+    </row>
+    <row r="111" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="F110" s="8" t="s">
+      <c r="B111" s="8" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="111" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="12" t="s">
+      <c r="C111" s="8" t="n">
+        <v>2811</v>
+      </c>
+      <c r="D111" s="8"/>
+      <c r="E111" s="8" t="s">
         <v>401</v>
       </c>
-      <c r="B111" s="8" t="s">
+      <c r="F111" s="8" t="s">
         <v>402</v>
-      </c>
-      <c r="C111" s="8" t="n">
-        <v>300</v>
-      </c>
-      <c r="D111" s="8" t="s">
-        <v>403</v>
-      </c>
-      <c r="E111" s="8" t="s">
-        <v>404</v>
-      </c>
-      <c r="F111" s="8" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="112" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="B112" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C112" s="8" t="n">
+        <v>200</v>
+      </c>
+      <c r="D112" s="8" t="s">
+        <v>404</v>
+      </c>
+      <c r="E112" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="F112" s="8" t="s">
         <v>406</v>
       </c>
-      <c r="B112" s="8" t="s">
-        <v>402</v>
-      </c>
-      <c r="C112" s="8" t="n">
+    </row>
+    <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="12" t="s">
+        <v>407</v>
+      </c>
+      <c r="B113" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="C113" s="8" t="n">
         <v>300</v>
       </c>
-      <c r="D112" s="8" t="s">
-        <v>403</v>
-      </c>
-      <c r="E112" s="8" t="s">
-        <v>407</v>
-      </c>
-      <c r="F112" s="8" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="9" t="s">
+      <c r="D113" s="8" t="s">
         <v>409</v>
       </c>
-      <c r="B113" s="8" t="s">
+      <c r="E113" s="8" t="s">
         <v>410</v>
       </c>
-      <c r="C113" s="8" t="n">
-        <v>5500</v>
-      </c>
-      <c r="D113" s="8"/>
-      <c r="E113" s="8" t="s">
+      <c r="F113" s="8" t="s">
         <v>411</v>
-      </c>
-      <c r="G113" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="114" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4379,17 +4397,19 @@
         <v>412</v>
       </c>
       <c r="B114" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="C114" s="8" t="n">
+        <v>300</v>
+      </c>
+      <c r="D114" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="E114" s="8" t="s">
         <v>413</v>
       </c>
-      <c r="C114" s="8" t="n">
-        <v>5600</v>
-      </c>
-      <c r="D114" s="8"/>
-      <c r="E114" s="8" t="s">
+      <c r="F114" s="8" t="s">
         <v>414</v>
-      </c>
-      <c r="G114" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="115" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4400,13 +4420,11 @@
         <v>416</v>
       </c>
       <c r="C115" s="8" t="n">
-        <v>101</v>
-      </c>
-      <c r="D115" s="8" t="s">
+        <v>5500</v>
+      </c>
+      <c r="D115" s="8"/>
+      <c r="E115" s="8" t="s">
         <v>417</v>
-      </c>
-      <c r="E115" s="8" t="s">
-        <v>418</v>
       </c>
       <c r="G115" s="3" t="s">
         <v>35</v>
@@ -4414,19 +4432,17 @@
     </row>
     <row r="116" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="B116" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="B116" s="8" t="s">
+      <c r="C116" s="8" t="n">
+        <v>5600</v>
+      </c>
+      <c r="D116" s="8"/>
+      <c r="E116" s="8" t="s">
         <v>420</v>
-      </c>
-      <c r="C116" s="8" t="n">
-        <v>111</v>
-      </c>
-      <c r="D116" s="8" t="s">
-        <v>421</v>
-      </c>
-      <c r="E116" s="8" t="s">
-        <v>422</v>
       </c>
       <c r="G116" s="3" t="s">
         <v>35</v>
@@ -4434,69 +4450,75 @@
     </row>
     <row r="117" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="B117" s="8" t="s">
+        <v>422</v>
+      </c>
+      <c r="C117" s="8" t="n">
+        <v>101</v>
+      </c>
+      <c r="D117" s="8" t="s">
         <v>423</v>
       </c>
-      <c r="B117" s="8" t="s">
+      <c r="E117" s="8" t="s">
         <v>424</v>
       </c>
-      <c r="C117" s="10"/>
-      <c r="D117" s="10"/>
-      <c r="E117" s="8" t="s">
-        <v>425</v>
-      </c>
-      <c r="F117" s="8" t="s">
-        <v>426</v>
+      <c r="G117" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="118" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="B118" s="8" t="s">
+        <v>426</v>
+      </c>
+      <c r="C118" s="8" t="n">
+        <v>111</v>
+      </c>
+      <c r="D118" s="8" t="s">
         <v>427</v>
       </c>
-      <c r="B118" s="8" t="s">
+      <c r="E118" s="8" t="s">
         <v>428</v>
-      </c>
-      <c r="C118" s="8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D118" s="8" t="s">
-        <v>429</v>
-      </c>
-      <c r="E118" s="8" t="s">
-        <v>346</v>
       </c>
       <c r="G118" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="119" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A119" s="1" t="s">
+      <c r="A119" s="9" t="s">
+        <v>429</v>
+      </c>
+      <c r="B119" s="8" t="s">
         <v>430</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="C119" s="10"/>
+      <c r="D119" s="10"/>
+      <c r="E119" s="8" t="s">
         <v>431</v>
       </c>
-      <c r="C119" s="2" t="n">
-        <v>9400</v>
-      </c>
-      <c r="E119" s="8" t="s">
+      <c r="F119" s="8" t="s">
         <v>432</v>
       </c>
-      <c r="G119" s="3" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="120" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A120" s="1" t="s">
+      <c r="A120" s="9" t="s">
         <v>433</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B120" s="8" t="s">
         <v>434</v>
       </c>
-      <c r="C120" s="2" t="n">
-        <v>9500</v>
-      </c>
-      <c r="E120" s="15" t="s">
+      <c r="C120" s="8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D120" s="8" t="s">
         <v>435</v>
+      </c>
+      <c r="E120" s="8" t="s">
+        <v>346</v>
       </c>
       <c r="G120" s="3" t="s">
         <v>35</v>
@@ -4510,9 +4532,9 @@
         <v>437</v>
       </c>
       <c r="C121" s="2" t="n">
-        <v>9600</v>
-      </c>
-      <c r="E121" s="2" t="s">
+        <v>9400</v>
+      </c>
+      <c r="E121" s="8" t="s">
         <v>438</v>
       </c>
       <c r="G121" s="3" t="s">
@@ -4520,97 +4542,93 @@
       </c>
     </row>
     <row r="122" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="9" t="s">
+      <c r="A122" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="B122" s="8" t="s">
+      <c r="B122" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="C122" s="8" t="n">
-        <v>112</v>
-      </c>
-      <c r="D122" s="8" t="s">
+      <c r="C122" s="2" t="n">
+        <v>9500</v>
+      </c>
+      <c r="E122" s="16" t="s">
         <v>441</v>
       </c>
-      <c r="E122" s="8" t="s">
+      <c r="G122" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="123" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A123" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="F122" s="8" t="s">
+      <c r="B123" s="2" t="s">
         <v>443</v>
       </c>
-    </row>
-    <row r="123" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="9" t="s">
+      <c r="C123" s="2" t="n">
+        <v>9600</v>
+      </c>
+      <c r="E123" s="2" t="s">
         <v>444</v>
       </c>
-      <c r="B123" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C123" s="8" t="n">
-        <v>3100</v>
-      </c>
-      <c r="D123" s="8"/>
-      <c r="E123" s="8" t="s">
-        <v>445</v>
-      </c>
-      <c r="F123" s="8" t="s">
-        <v>446</v>
+      <c r="G123" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="124" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="9" t="s">
+        <v>445</v>
+      </c>
+      <c r="B124" s="8" t="s">
+        <v>446</v>
+      </c>
+      <c r="C124" s="8" t="n">
+        <v>112</v>
+      </c>
+      <c r="D124" s="8" t="s">
         <v>447</v>
       </c>
-      <c r="B124" s="8" t="s">
+      <c r="E124" s="8" t="s">
         <v>448</v>
       </c>
-      <c r="C124" s="8" t="n">
-        <v>21</v>
-      </c>
-      <c r="D124" s="8"/>
-      <c r="E124" s="8" t="s">
+      <c r="F124" s="8" t="s">
         <v>449</v>
-      </c>
-      <c r="F124" s="8" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="125" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="9" t="s">
+        <v>450</v>
+      </c>
+      <c r="B125" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C125" s="8" t="n">
+        <v>3100</v>
+      </c>
+      <c r="D125" s="8"/>
+      <c r="E125" s="8" t="s">
         <v>451</v>
       </c>
-      <c r="B125" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="C125" s="8" t="n">
-        <v>122</v>
-      </c>
-      <c r="D125" s="8" t="s">
+      <c r="F125" s="8" t="s">
         <v>452</v>
-      </c>
-      <c r="E125" s="8" t="s">
-        <v>453</v>
-      </c>
-      <c r="G125" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="9" t="s">
+        <v>453</v>
+      </c>
+      <c r="B126" s="8" t="s">
         <v>454</v>
       </c>
-      <c r="B126" s="8" t="s">
-        <v>455</v>
-      </c>
       <c r="C126" s="8" t="n">
-        <v>1722</v>
+        <v>21</v>
       </c>
       <c r="D126" s="8"/>
       <c r="E126" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="F126" s="8" t="s">
         <v>456</v>
-      </c>
-      <c r="G126" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4618,12 +4636,14 @@
         <v>457</v>
       </c>
       <c r="B127" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C127" s="8" t="n">
+        <v>122</v>
+      </c>
+      <c r="D127" s="8" t="s">
         <v>458</v>
       </c>
-      <c r="C127" s="8" t="n">
-        <v>7100</v>
-      </c>
-      <c r="D127" s="8"/>
       <c r="E127" s="8" t="s">
         <v>459</v>
       </c>
@@ -4638,245 +4658,247 @@
       <c r="B128" s="8" t="s">
         <v>461</v>
       </c>
-      <c r="C128" s="10"/>
-      <c r="D128" s="10"/>
+      <c r="C128" s="8" t="n">
+        <v>1722</v>
+      </c>
+      <c r="D128" s="8"/>
       <c r="E128" s="8" t="s">
         <v>462</v>
       </c>
-      <c r="F128" s="8" t="s">
-        <v>463</v>
+      <c r="G128" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="B129" s="8" t="s">
         <v>464</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="C129" s="8" t="n">
+        <v>7100</v>
+      </c>
+      <c r="D129" s="8"/>
+      <c r="E129" s="8" t="s">
         <v>465</v>
       </c>
-      <c r="E129" s="8" t="s">
-        <v>466</v>
-      </c>
-      <c r="F129" s="2" t="s">
-        <v>467</v>
+      <c r="G129" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="130" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="9" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C130" s="10"/>
       <c r="D130" s="10"/>
       <c r="E130" s="8" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F130" s="8" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="131" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="9" t="s">
+        <v>470</v>
+      </c>
+      <c r="B131" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="E131" s="8" t="s">
         <v>472</v>
       </c>
-      <c r="B131" s="8" t="s">
+      <c r="F131" s="2" t="s">
         <v>473</v>
       </c>
-      <c r="C131" s="10"/>
-      <c r="D131" s="10"/>
-      <c r="E131" s="8" t="s">
+    </row>
+    <row r="132" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A132" s="9" t="s">
         <v>474</v>
       </c>
-      <c r="F131" s="8" t="s">
+      <c r="B132" s="8" t="s">
         <v>475</v>
-      </c>
-    </row>
-    <row r="132" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A132" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="B132" s="8" t="s">
-        <v>477</v>
       </c>
       <c r="C132" s="10"/>
       <c r="D132" s="10"/>
       <c r="E132" s="8" t="s">
+        <v>476</v>
+      </c>
+      <c r="F132" s="8" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="133" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="9" t="s">
         <v>478</v>
       </c>
-      <c r="F132" s="8" t="s">
+      <c r="B133" s="8" t="s">
         <v>479</v>
       </c>
-    </row>
-    <row r="133" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="1" t="s">
+      <c r="C133" s="10"/>
+      <c r="D133" s="10"/>
+      <c r="E133" s="8" t="s">
         <v>480</v>
       </c>
-      <c r="B133" s="2" t="s">
+      <c r="F133" s="8" t="s">
         <v>481</v>
       </c>
-      <c r="C133" s="2" t="n">
-        <v>133</v>
-      </c>
-      <c r="E133" s="8" t="s">
+    </row>
+    <row r="134" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1" t="s">
         <v>482</v>
       </c>
-      <c r="F133" s="2" t="s">
+      <c r="B134" s="8" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="134" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="9" t="s">
+      <c r="C134" s="10"/>
+      <c r="D134" s="10"/>
+      <c r="E134" s="8" t="s">
         <v>484</v>
       </c>
-      <c r="B134" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="C134" s="8" t="n">
-        <v>400</v>
-      </c>
-      <c r="D134" s="8" t="s">
+      <c r="F134" s="8" t="s">
         <v>485</v>
-      </c>
-      <c r="E134" s="8" t="s">
-        <v>486</v>
-      </c>
-      <c r="F134" s="8" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="135" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
+        <v>486</v>
+      </c>
+      <c r="B135" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="C135" s="2" t="n">
+        <v>133</v>
+      </c>
+      <c r="E135" s="8" t="s">
         <v>488</v>
       </c>
-      <c r="B135" s="8" t="s">
+      <c r="F135" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="C135" s="8" t="n">
+    </row>
+    <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="9" t="s">
+        <v>490</v>
+      </c>
+      <c r="B136" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C136" s="8" t="n">
         <v>400</v>
       </c>
-      <c r="D135" s="8"/>
-      <c r="E135" s="8" t="s">
-        <v>490</v>
-      </c>
-      <c r="F135" s="8" t="s">
+      <c r="D136" s="8" t="s">
         <v>491</v>
       </c>
-    </row>
-    <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A136" s="1" t="s">
+      <c r="E136" s="8" t="s">
         <v>492</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="F136" s="8" t="s">
         <v>493</v>
-      </c>
-      <c r="C136" s="2" t="n">
-        <v>2612</v>
-      </c>
-      <c r="D136" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="E136" s="8" t="s">
-        <v>495</v>
-      </c>
-      <c r="F136" s="8" t="s">
-        <v>496</v>
       </c>
     </row>
     <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B137" s="8" t="s">
+        <v>495</v>
+      </c>
+      <c r="C137" s="8" t="n">
+        <v>400</v>
+      </c>
+      <c r="D137" s="8"/>
+      <c r="E137" s="8" t="s">
+        <v>496</v>
+      </c>
+      <c r="F137" s="8" t="s">
         <v>497</v>
       </c>
-      <c r="B137" s="2" t="s">
+    </row>
+    <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A138" s="1" t="s">
         <v>498</v>
       </c>
-      <c r="E137" s="8" t="s">
+      <c r="B138" s="2" t="s">
         <v>499</v>
       </c>
-      <c r="F137" s="2" t="s">
+      <c r="C138" s="2" t="n">
+        <v>2612</v>
+      </c>
+      <c r="D138" s="2" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="9" t="s">
+      <c r="E138" s="8" t="s">
         <v>501</v>
       </c>
-      <c r="B138" s="8" t="s">
+      <c r="F138" s="8" t="s">
         <v>502</v>
       </c>
-      <c r="C138" s="8" t="s">
+    </row>
+    <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A139" s="1" t="s">
         <v>503</v>
       </c>
-      <c r="D138" s="8"/>
-      <c r="E138" s="8" t="s">
+      <c r="B139" s="2" t="s">
         <v>504</v>
       </c>
-      <c r="F138" s="8" t="s">
+      <c r="E139" s="8" t="s">
         <v>505</v>
       </c>
-    </row>
-    <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="9" t="s">
+      <c r="F139" s="2" t="s">
         <v>506</v>
-      </c>
-      <c r="B139" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="C139" s="10" t="s">
-        <v>507</v>
-      </c>
-      <c r="D139" s="10"/>
-      <c r="E139" s="8" t="s">
-        <v>508</v>
-      </c>
-      <c r="F139" s="8" t="s">
-        <v>509</v>
       </c>
     </row>
     <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="9" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>511</v>
-      </c>
-      <c r="C140" s="8" t="n">
-        <v>7600</v>
+        <v>508</v>
+      </c>
+      <c r="C140" s="8" t="s">
+        <v>509</v>
       </c>
       <c r="D140" s="8"/>
       <c r="E140" s="8" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F140" s="8" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
     </row>
     <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="9" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="B141" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="C141" s="10"/>
+      <c r="C141" s="10" t="s">
+        <v>513</v>
+      </c>
       <c r="D141" s="10"/>
       <c r="E141" s="8" t="s">
+        <v>514</v>
+      </c>
+      <c r="F141" s="8" t="s">
         <v>515</v>
-      </c>
-      <c r="F141" s="8" t="s">
-        <v>516</v>
       </c>
     </row>
     <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="9" t="s">
+        <v>516</v>
+      </c>
+      <c r="B142" s="8" t="s">
         <v>517</v>
       </c>
-      <c r="B142" s="8" t="s">
-        <v>183</v>
-      </c>
       <c r="C142" s="8" t="n">
-        <v>6000</v>
+        <v>7600</v>
       </c>
       <c r="D142" s="8"/>
       <c r="E142" s="8" t="s">
@@ -4891,7 +4913,7 @@
         <v>520</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>238</v>
+        <v>180</v>
       </c>
       <c r="C143" s="10"/>
       <c r="D143" s="10"/>
@@ -4907,356 +4929,356 @@
         <v>523</v>
       </c>
       <c r="B144" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C144" s="8" t="n">
+        <v>6000</v>
+      </c>
+      <c r="D144" s="8"/>
+      <c r="E144" s="8" t="s">
         <v>524</v>
       </c>
-      <c r="C144" s="10"/>
-      <c r="D144" s="10"/>
-      <c r="E144" s="8" t="s">
+      <c r="F144" s="8" t="s">
         <v>525</v>
-      </c>
-      <c r="F144" s="8" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="9" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>528</v>
+        <v>238</v>
       </c>
       <c r="C145" s="10"/>
       <c r="D145" s="10"/>
       <c r="E145" s="8" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="F145" s="8" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="146" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="9" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="C146" s="10"/>
       <c r="D146" s="10"/>
       <c r="E146" s="8" t="s">
+        <v>531</v>
+      </c>
+      <c r="F146" s="8" t="s">
         <v>532</v>
-      </c>
-      <c r="F146" s="8" t="s">
-        <v>533</v>
       </c>
     </row>
     <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="9" t="s">
+        <v>533</v>
+      </c>
+      <c r="B147" s="8" t="s">
         <v>534</v>
-      </c>
-      <c r="B147" s="8" t="s">
-        <v>535</v>
       </c>
       <c r="C147" s="10"/>
       <c r="D147" s="10"/>
       <c r="E147" s="8" t="s">
+        <v>535</v>
+      </c>
+      <c r="F147" s="8" t="s">
         <v>536</v>
-      </c>
-      <c r="F147" s="8" t="s">
-        <v>537</v>
       </c>
     </row>
     <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="9" t="s">
+        <v>537</v>
+      </c>
+      <c r="B148" s="8" t="s">
+        <v>534</v>
+      </c>
+      <c r="C148" s="10"/>
+      <c r="D148" s="10"/>
+      <c r="E148" s="8" t="s">
         <v>538</v>
       </c>
-      <c r="B148" s="8" t="s">
+      <c r="F148" s="8" t="s">
         <v>539</v>
-      </c>
-      <c r="C148" s="8" t="n">
-        <v>7700</v>
-      </c>
-      <c r="D148" s="8" t="s">
-        <v>540</v>
-      </c>
-      <c r="E148" s="8" t="s">
-        <v>541</v>
-      </c>
-      <c r="F148" s="8" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="9" t="s">
+        <v>540</v>
+      </c>
+      <c r="B149" s="8" t="s">
+        <v>541</v>
+      </c>
+      <c r="C149" s="10"/>
+      <c r="D149" s="10"/>
+      <c r="E149" s="8" t="s">
+        <v>542</v>
+      </c>
+      <c r="F149" s="8" t="s">
         <v>543</v>
-      </c>
-      <c r="B149" s="8" t="s">
-        <v>544</v>
-      </c>
-      <c r="C149" s="8" t="n">
-        <v>7800</v>
-      </c>
-      <c r="D149" s="8" t="s">
-        <v>545</v>
-      </c>
-      <c r="E149" s="8" t="s">
-        <v>546</v>
-      </c>
-      <c r="F149" s="8" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="9" t="s">
+        <v>544</v>
+      </c>
+      <c r="B150" s="8" t="s">
+        <v>545</v>
+      </c>
+      <c r="C150" s="8" t="n">
+        <v>7700</v>
+      </c>
+      <c r="D150" s="8" t="s">
+        <v>546</v>
+      </c>
+      <c r="E150" s="8" t="s">
         <v>547</v>
       </c>
-      <c r="B150" s="8" t="s">
+      <c r="F150" s="8" t="s">
         <v>548</v>
       </c>
-      <c r="C150" s="10"/>
-      <c r="D150" s="10"/>
-      <c r="E150" s="8" t="s">
+    </row>
+    <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A151" s="9" t="s">
         <v>549</v>
       </c>
-      <c r="F150" s="8" t="s">
+      <c r="B151" s="8" t="s">
         <v>550</v>
       </c>
-    </row>
-    <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A151" s="1" t="s">
+      <c r="C151" s="8" t="n">
+        <v>7800</v>
+      </c>
+      <c r="D151" s="8" t="s">
         <v>551</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="E151" s="8" t="s">
         <v>552</v>
       </c>
-      <c r="C151" s="2" t="n">
-        <v>8900</v>
-      </c>
-      <c r="E151" s="8" t="s">
-        <v>553</v>
-      </c>
-      <c r="G151" s="3" t="s">
-        <v>11</v>
+      <c r="F151" s="8" t="s">
+        <v>548</v>
       </c>
     </row>
     <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="9" t="s">
+        <v>553</v>
+      </c>
+      <c r="B152" s="8" t="s">
         <v>554</v>
       </c>
-      <c r="B152" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="C152" s="10" t="n">
-        <v>100</v>
-      </c>
-      <c r="D152" s="10" t="s">
+      <c r="C152" s="10"/>
+      <c r="D152" s="10"/>
+      <c r="E152" s="8" t="s">
         <v>555</v>
       </c>
-      <c r="E152" s="8" t="s">
+      <c r="F152" s="8" t="s">
         <v>556</v>
       </c>
-      <c r="F152" s="8" t="s">
+    </row>
+    <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A153" s="1" t="s">
         <v>557</v>
       </c>
-    </row>
-    <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A153" s="9" t="s">
+      <c r="B153" s="2" t="s">
         <v>558</v>
       </c>
-      <c r="B153" s="8" t="s">
+      <c r="C153" s="2" t="n">
+        <v>8900</v>
+      </c>
+      <c r="E153" s="8" t="s">
         <v>559</v>
       </c>
-      <c r="C153" s="10"/>
-      <c r="D153" s="10"/>
-      <c r="E153" s="8" t="s">
-        <v>560</v>
-      </c>
-      <c r="F153" s="8" t="s">
-        <v>561</v>
+      <c r="G153" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="B154" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C154" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="D154" s="10" t="s">
+        <v>561</v>
+      </c>
+      <c r="E154" s="8" t="s">
         <v>562</v>
       </c>
-      <c r="B154" s="8" t="s">
-        <v>416</v>
-      </c>
-      <c r="C154" s="8" t="n">
-        <v>101</v>
-      </c>
-      <c r="D154" s="8"/>
-      <c r="E154" s="8" t="s">
-        <v>418</v>
-      </c>
-      <c r="G154" s="3" t="s">
-        <v>35</v>
+      <c r="F154" s="8" t="s">
+        <v>563</v>
       </c>
     </row>
     <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="9" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>257</v>
+        <v>565</v>
       </c>
       <c r="C155" s="10"/>
       <c r="D155" s="10"/>
       <c r="E155" s="8" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="F155" s="8" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
     </row>
     <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="9" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="C156" s="10"/>
-      <c r="D156" s="10" t="s">
-        <v>567</v>
-      </c>
+        <v>422</v>
+      </c>
+      <c r="C156" s="8" t="n">
+        <v>101</v>
+      </c>
+      <c r="D156" s="8"/>
       <c r="E156" s="8" t="s">
-        <v>568</v>
-      </c>
-      <c r="F156" s="8" t="s">
-        <v>569</v>
+        <v>424</v>
+      </c>
+      <c r="G156" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="9" t="s">
+        <v>569</v>
+      </c>
+      <c r="B157" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C157" s="10"/>
+      <c r="D157" s="10"/>
+      <c r="E157" s="8" t="s">
         <v>570</v>
       </c>
-      <c r="B157" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="C157" s="8" t="n">
-        <v>1400</v>
-      </c>
-      <c r="D157" s="8" t="s">
+      <c r="F157" s="8" t="s">
         <v>571</v>
       </c>
-      <c r="E157" s="8" t="s">
+    </row>
+    <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A158" s="9" t="s">
         <v>572</v>
       </c>
-      <c r="F157" s="8" t="s">
+      <c r="B158" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C158" s="10"/>
+      <c r="D158" s="10" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A158" s="1" t="s">
+      <c r="E158" s="8" t="s">
         <v>574</v>
       </c>
-      <c r="B158" s="8" t="s">
+      <c r="F158" s="8" t="s">
         <v>575</v>
-      </c>
-      <c r="C158" s="8" t="n">
-        <v>7400</v>
-      </c>
-      <c r="D158" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="E158" s="8" t="s">
-        <v>576</v>
-      </c>
-      <c r="F158" s="8" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="159" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="9" t="s">
+        <v>576</v>
+      </c>
+      <c r="B159" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C159" s="8" t="n">
+        <v>1400</v>
+      </c>
+      <c r="D159" s="8" t="s">
+        <v>577</v>
+      </c>
+      <c r="E159" s="8" t="s">
         <v>578</v>
       </c>
-      <c r="B159" s="8" t="s">
+      <c r="F159" s="8" t="s">
         <v>579</v>
       </c>
-      <c r="C159" s="10"/>
-      <c r="D159" s="10" t="s">
+    </row>
+    <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A160" s="1" t="s">
         <v>580</v>
       </c>
-      <c r="E159" s="8" t="s">
+      <c r="B160" s="8" t="s">
         <v>581</v>
       </c>
-      <c r="F159" s="8" t="s">
+      <c r="C160" s="8" t="n">
+        <v>7400</v>
+      </c>
+      <c r="D160" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E160" s="8" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A160" s="9" t="s">
+      <c r="F160" s="8" t="s">
         <v>583</v>
-      </c>
-      <c r="B160" s="8" t="s">
-        <v>528</v>
-      </c>
-      <c r="C160" s="8" t="n">
-        <v>1700</v>
-      </c>
-      <c r="D160" s="8" t="s">
-        <v>584</v>
-      </c>
-      <c r="E160" s="8" t="s">
-        <v>585</v>
-      </c>
-      <c r="F160" s="8" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="9" t="s">
+        <v>584</v>
+      </c>
+      <c r="B161" s="8" t="s">
+        <v>585</v>
+      </c>
+      <c r="C161" s="10"/>
+      <c r="D161" s="10" t="s">
+        <v>586</v>
+      </c>
+      <c r="E161" s="8" t="s">
         <v>587</v>
       </c>
-      <c r="B161" s="8" t="s">
+      <c r="F161" s="8" t="s">
         <v>588</v>
-      </c>
-      <c r="C161" s="8" t="n">
-        <v>1800</v>
-      </c>
-      <c r="D161" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="E161" s="8" t="s">
-        <v>589</v>
-      </c>
-      <c r="F161" s="8" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="9" t="s">
+        <v>589</v>
+      </c>
+      <c r="B162" s="8" t="s">
+        <v>534</v>
+      </c>
+      <c r="C162" s="8" t="n">
+        <v>1700</v>
+      </c>
+      <c r="D162" s="8" t="s">
+        <v>590</v>
+      </c>
+      <c r="E162" s="8" t="s">
         <v>591</v>
       </c>
-      <c r="B162" s="8" t="s">
-        <v>260</v>
-      </c>
-      <c r="C162" s="7"/>
-      <c r="D162" s="7"/>
-      <c r="E162" s="8" t="s">
+      <c r="F162" s="8" t="s">
         <v>592</v>
-      </c>
-      <c r="F162" s="8" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="B163" s="8" t="s">
         <v>594</v>
       </c>
-      <c r="B163" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="C163" s="10" t="s">
+      <c r="C163" s="8" t="n">
+        <v>1800</v>
+      </c>
+      <c r="D163" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="E163" s="8" t="s">
         <v>595</v>
       </c>
-      <c r="D163" s="10"/>
-      <c r="E163" s="8" t="s">
+      <c r="F163" s="8" t="s">
         <v>596</v>
-      </c>
-      <c r="F163" s="8" t="s">
-        <v>593</v>
       </c>
     </row>
     <row r="164" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5264,47 +5286,49 @@
         <v>597</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>579</v>
-      </c>
-      <c r="C164" s="10"/>
-      <c r="D164" s="10"/>
+        <v>260</v>
+      </c>
+      <c r="C164" s="7"/>
+      <c r="D164" s="7"/>
       <c r="E164" s="8" t="s">
         <v>598</v>
       </c>
       <c r="F164" s="8" t="s">
-        <v>593</v>
+        <v>599</v>
       </c>
     </row>
     <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="9" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>528</v>
-      </c>
-      <c r="C165" s="10"/>
+        <v>238</v>
+      </c>
+      <c r="C165" s="10" t="s">
+        <v>601</v>
+      </c>
       <c r="D165" s="10"/>
       <c r="E165" s="8" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="F165" s="8" t="s">
-        <v>593</v>
+        <v>599</v>
       </c>
     </row>
     <row r="166" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="9" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>602</v>
+        <v>585</v>
       </c>
       <c r="C166" s="10"/>
       <c r="D166" s="10"/>
       <c r="E166" s="8" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="F166" s="8" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
     </row>
     <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5312,7 +5336,7 @@
         <v>605</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>579</v>
+        <v>534</v>
       </c>
       <c r="C167" s="10"/>
       <c r="D167" s="10"/>
@@ -5320,15 +5344,15 @@
         <v>606</v>
       </c>
       <c r="F167" s="8" t="s">
-        <v>607</v>
+        <v>599</v>
       </c>
     </row>
     <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="9" t="s">
+        <v>607</v>
+      </c>
+      <c r="B168" s="8" t="s">
         <v>608</v>
-      </c>
-      <c r="B168" s="8" t="s">
-        <v>528</v>
       </c>
       <c r="C168" s="10"/>
       <c r="D168" s="10"/>
@@ -5344,7 +5368,7 @@
         <v>611</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>238</v>
+        <v>585</v>
       </c>
       <c r="C169" s="10"/>
       <c r="D169" s="10"/>
@@ -5360,7 +5384,7 @@
         <v>614</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>180</v>
+        <v>534</v>
       </c>
       <c r="C170" s="10"/>
       <c r="D170" s="10"/>
@@ -5376,7 +5400,7 @@
         <v>617</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>183</v>
+        <v>238</v>
       </c>
       <c r="C171" s="10"/>
       <c r="D171" s="10"/>
@@ -5392,7 +5416,7 @@
         <v>620</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>260</v>
+        <v>180</v>
       </c>
       <c r="C172" s="10"/>
       <c r="D172" s="10"/>
@@ -5408,7 +5432,7 @@
         <v>623</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>528</v>
+        <v>183</v>
       </c>
       <c r="C173" s="10"/>
       <c r="D173" s="10"/>
@@ -5424,7 +5448,7 @@
         <v>626</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>180</v>
+        <v>260</v>
       </c>
       <c r="C174" s="10"/>
       <c r="D174" s="10"/>
@@ -5440,7 +5464,7 @@
         <v>629</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>183</v>
+        <v>534</v>
       </c>
       <c r="C175" s="10"/>
       <c r="D175" s="10"/>
@@ -5456,7 +5480,7 @@
         <v>632</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>260</v>
+        <v>180</v>
       </c>
       <c r="C176" s="10"/>
       <c r="D176" s="10"/>
@@ -5472,7 +5496,7 @@
         <v>635</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>238</v>
+        <v>183</v>
       </c>
       <c r="C177" s="10"/>
       <c r="D177" s="10"/>
@@ -5488,7 +5512,7 @@
         <v>638</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>579</v>
+        <v>260</v>
       </c>
       <c r="C178" s="10"/>
       <c r="D178" s="10"/>
@@ -5500,53 +5524,51 @@
       </c>
     </row>
     <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A179" s="1" t="s">
+      <c r="A179" s="9" t="s">
         <v>641</v>
       </c>
-      <c r="B179" s="2" t="s">
+      <c r="B179" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C179" s="10"/>
+      <c r="D179" s="10"/>
+      <c r="E179" s="8" t="s">
         <v>642</v>
       </c>
-      <c r="C179" s="2" t="n">
-        <v>23</v>
-      </c>
-      <c r="E179" s="8" t="s">
+      <c r="F179" s="8" t="s">
         <v>643</v>
-      </c>
-      <c r="F179" s="2" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="9" t="s">
+        <v>644</v>
+      </c>
+      <c r="B180" s="8" t="s">
+        <v>585</v>
+      </c>
+      <c r="C180" s="10"/>
+      <c r="D180" s="10"/>
+      <c r="E180" s="8" t="s">
         <v>645</v>
       </c>
-      <c r="B180" s="8" t="s">
+      <c r="F180" s="8" t="s">
         <v>646</v>
       </c>
-      <c r="C180" s="8" t="n">
-        <v>121</v>
-      </c>
-      <c r="D180" s="8"/>
-      <c r="E180" s="8" t="s">
+    </row>
+    <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A181" s="1" t="s">
         <v>647</v>
       </c>
-      <c r="G180" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A181" s="9" t="s">
+      <c r="B181" s="2" t="s">
         <v>648</v>
       </c>
-      <c r="B181" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="C181" s="10"/>
-      <c r="D181" s="10"/>
+      <c r="C181" s="2" t="n">
+        <v>23</v>
+      </c>
       <c r="E181" s="8" t="s">
         <v>649</v>
       </c>
-      <c r="F181" s="8" t="s">
+      <c r="F181" s="2" t="s">
         <v>650</v>
       </c>
     </row>
@@ -5555,15 +5577,17 @@
         <v>651</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="C182" s="10"/>
-      <c r="D182" s="10"/>
+        <v>652</v>
+      </c>
+      <c r="C182" s="8" t="n">
+        <v>121</v>
+      </c>
+      <c r="D182" s="8"/>
       <c r="E182" s="8" t="s">
-        <v>652</v>
-      </c>
-      <c r="F182" s="8" t="s">
         <v>653</v>
+      </c>
+      <c r="G182" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5571,100 +5595,100 @@
         <v>654</v>
       </c>
       <c r="B183" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C183" s="10"/>
+      <c r="D183" s="10"/>
+      <c r="E183" s="8" t="s">
         <v>655</v>
       </c>
-      <c r="C183" s="8" t="n">
-        <v>111</v>
-      </c>
-      <c r="D183" s="8"/>
-      <c r="E183" s="8" t="s">
-        <v>422</v>
-      </c>
-      <c r="G183" s="3" t="s">
-        <v>35</v>
+      <c r="F183" s="8" t="s">
+        <v>656</v>
       </c>
     </row>
     <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="9" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>311</v>
-      </c>
-      <c r="C184" s="8" t="n">
-        <v>1711</v>
-      </c>
-      <c r="D184" s="8"/>
+        <v>238</v>
+      </c>
+      <c r="C184" s="10"/>
+      <c r="D184" s="10"/>
       <c r="E184" s="8" t="s">
-        <v>312</v>
+        <v>658</v>
       </c>
       <c r="F184" s="8" t="s">
-        <v>313</v>
+        <v>659</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A185" s="1" t="s">
-        <v>657</v>
+      <c r="A185" s="9" t="s">
+        <v>660</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="C185" s="8" t="n">
-        <v>3300</v>
+        <v>111</v>
       </c>
       <c r="D185" s="8"/>
       <c r="E185" s="8" t="s">
-        <v>659</v>
-      </c>
-      <c r="F185" s="8" t="s">
-        <v>660</v>
+        <v>428</v>
+      </c>
+      <c r="G185" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="9" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>662</v>
+        <v>311</v>
       </c>
       <c r="C186" s="8" t="n">
-        <v>8000</v>
-      </c>
-      <c r="D186" s="8" t="s">
+        <v>1711</v>
+      </c>
+      <c r="D186" s="8"/>
+      <c r="E186" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="F186" s="8" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A187" s="1" t="s">
         <v>663</v>
       </c>
-      <c r="E186" s="8" t="s">
+      <c r="B187" s="8" t="s">
         <v>664</v>
       </c>
-      <c r="F186" s="8" t="s">
+      <c r="C187" s="8" t="n">
+        <v>3300</v>
+      </c>
+      <c r="D187" s="8"/>
+      <c r="E187" s="8" t="s">
         <v>665</v>
       </c>
-    </row>
-    <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A187" s="9" t="s">
+      <c r="F187" s="8" t="s">
         <v>666</v>
-      </c>
-      <c r="B187" s="8" t="s">
-        <v>180</v>
-      </c>
-      <c r="C187" s="10"/>
-      <c r="D187" s="10"/>
-      <c r="E187" s="8" t="s">
-        <v>667</v>
-      </c>
-      <c r="F187" s="8" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="9" t="s">
+        <v>667</v>
+      </c>
+      <c r="B188" s="8" t="s">
+        <v>668</v>
+      </c>
+      <c r="C188" s="8" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D188" s="8" t="s">
         <v>669</v>
       </c>
-      <c r="B188" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="C188" s="10"/>
-      <c r="D188" s="10"/>
       <c r="E188" s="8" t="s">
         <v>670</v>
       </c>
@@ -5677,7 +5701,7 @@
         <v>672</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>257</v>
+        <v>180</v>
       </c>
       <c r="C189" s="10"/>
       <c r="D189" s="10"/>
@@ -5693,37 +5717,31 @@
         <v>675</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="C190" s="8" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D190" s="8" t="s">
+        <v>183</v>
+      </c>
+      <c r="C190" s="10"/>
+      <c r="D190" s="10"/>
+      <c r="E190" s="8" t="s">
         <v>676</v>
       </c>
-      <c r="E190" s="8" t="s">
+      <c r="F190" s="8" t="s">
         <v>677</v>
-      </c>
-      <c r="F190" s="8" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="9" t="s">
         <v>678</v>
       </c>
-      <c r="B191" s="2" t="s">
+      <c r="B191" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C191" s="10"/>
+      <c r="D191" s="10"/>
+      <c r="E191" s="8" t="s">
         <v>679</v>
       </c>
-      <c r="C191" s="8" t="n">
-        <v>2611</v>
-      </c>
-      <c r="D191" s="8"/>
-      <c r="E191" s="8" t="s">
+      <c r="F191" s="8" t="s">
         <v>680</v>
-      </c>
-      <c r="G191" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5731,33 +5749,37 @@
         <v>681</v>
       </c>
       <c r="B192" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C192" s="8" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D192" s="8" t="s">
         <v>682</v>
       </c>
-      <c r="C192" s="8" t="n">
-        <v>2711</v>
-      </c>
-      <c r="D192" s="8"/>
       <c r="E192" s="8" t="s">
         <v>683</v>
       </c>
-      <c r="G192" s="3" t="s">
-        <v>35</v>
+      <c r="F192" s="8" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="9" t="s">
         <v>684</v>
       </c>
-      <c r="B193" s="8" t="s">
-        <v>238</v>
-      </c>
-      <c r="C193" s="10"/>
-      <c r="D193" s="10"/>
+      <c r="B193" s="2" t="s">
+        <v>685</v>
+      </c>
+      <c r="C193" s="8" t="n">
+        <v>2611</v>
+      </c>
+      <c r="D193" s="8"/>
       <c r="E193" s="8" t="s">
-        <v>685</v>
-      </c>
-      <c r="F193" s="8" t="s">
         <v>686</v>
+      </c>
+      <c r="G193" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5767,96 +5789,96 @@
       <c r="B194" s="8" t="s">
         <v>688</v>
       </c>
-      <c r="C194" s="10"/>
-      <c r="D194" s="10"/>
+      <c r="C194" s="8" t="n">
+        <v>2711</v>
+      </c>
+      <c r="D194" s="8"/>
       <c r="E194" s="8" t="s">
         <v>689</v>
       </c>
-      <c r="F194" s="8" t="s">
-        <v>690</v>
+      <c r="G194" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="9" t="s">
+        <v>690</v>
+      </c>
+      <c r="B195" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="C195" s="10"/>
+      <c r="D195" s="10"/>
+      <c r="E195" s="8" t="s">
         <v>691</v>
       </c>
-      <c r="B195" s="8" t="s">
+      <c r="F195" s="8" t="s">
         <v>692</v>
-      </c>
-      <c r="C195" s="8" t="n">
-        <v>3721</v>
-      </c>
-      <c r="D195" s="8"/>
-      <c r="E195" s="8" t="s">
-        <v>693</v>
-      </c>
-      <c r="F195" s="8" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="9" t="s">
+        <v>693</v>
+      </c>
+      <c r="B196" s="8" t="s">
+        <v>694</v>
+      </c>
+      <c r="C196" s="10"/>
+      <c r="D196" s="10"/>
+      <c r="E196" s="8" t="s">
         <v>695</v>
       </c>
-      <c r="B196" s="8" t="s">
-        <v>528</v>
-      </c>
-      <c r="C196" s="8" t="n">
-        <v>6100</v>
-      </c>
-      <c r="D196" s="8"/>
-      <c r="E196" s="8" t="s">
+      <c r="F196" s="8" t="s">
         <v>696</v>
-      </c>
-      <c r="F196" s="8" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="9" t="s">
+        <v>697</v>
+      </c>
+      <c r="B197" s="8" t="s">
         <v>698</v>
       </c>
-      <c r="B197" s="8" t="s">
+      <c r="C197" s="8" t="n">
+        <v>3721</v>
+      </c>
+      <c r="D197" s="8"/>
+      <c r="E197" s="8" t="s">
         <v>699</v>
       </c>
-      <c r="C197" s="10" t="n">
-        <v>8400</v>
-      </c>
-      <c r="D197" s="10"/>
-      <c r="E197" s="8" t="s">
+      <c r="F197" s="8" t="s">
         <v>700</v>
-      </c>
-      <c r="F197" s="8" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="9" t="s">
+        <v>701</v>
+      </c>
+      <c r="B198" s="8" t="s">
+        <v>534</v>
+      </c>
+      <c r="C198" s="8" t="n">
+        <v>6100</v>
+      </c>
+      <c r="D198" s="8"/>
+      <c r="E198" s="8" t="s">
         <v>702</v>
       </c>
-      <c r="B198" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C198" s="7"/>
-      <c r="D198" s="7"/>
-      <c r="E198" s="8" t="s">
+      <c r="F198" s="8" t="s">
         <v>703</v>
       </c>
-      <c r="F198" s="8" t="s">
+    </row>
+    <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A199" s="9" t="s">
         <v>704</v>
       </c>
-    </row>
-    <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A199" s="1" t="s">
+      <c r="B199" s="8" t="s">
         <v>705</v>
       </c>
-      <c r="B199" s="8" t="s">
-        <v>293</v>
-      </c>
-      <c r="C199" s="8" t="n">
-        <v>400</v>
-      </c>
-      <c r="D199" s="8"/>
+      <c r="C199" s="10" t="n">
+        <v>8400</v>
+      </c>
+      <c r="D199" s="10"/>
       <c r="E199" s="8" t="s">
         <v>706</v>
       </c>
@@ -5865,69 +5887,103 @@
       </c>
     </row>
     <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A200" s="1" t="s">
+      <c r="A200" s="9" t="s">
         <v>708</v>
       </c>
       <c r="B200" s="8" t="s">
-        <v>489</v>
-      </c>
-      <c r="C200" s="8" t="n">
-        <v>400</v>
-      </c>
-      <c r="D200" s="8"/>
+        <v>49</v>
+      </c>
+      <c r="C200" s="7"/>
+      <c r="D200" s="7"/>
       <c r="E200" s="8" t="s">
         <v>709</v>
       </c>
       <c r="F200" s="8" t="s">
-        <v>491</v>
+        <v>710</v>
       </c>
     </row>
     <row r="201" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A201" s="9" t="s">
-        <v>710</v>
+      <c r="A201" s="1" t="s">
+        <v>711</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C201" s="10"/>
-      <c r="D201" s="10"/>
+        <v>293</v>
+      </c>
+      <c r="C201" s="8" t="n">
+        <v>400</v>
+      </c>
+      <c r="D201" s="8"/>
       <c r="E201" s="8" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="F201" s="8" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
     </row>
     <row r="202" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A202" s="9" t="s">
-        <v>713</v>
+      <c r="A202" s="1" t="s">
+        <v>714</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>448</v>
+        <v>495</v>
       </c>
       <c r="C202" s="8" t="n">
-        <v>21</v>
+        <v>400</v>
       </c>
       <c r="D202" s="8"/>
       <c r="E202" s="8" t="s">
-        <v>714</v>
-      </c>
-      <c r="G202" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="F202" s="8" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="203" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A203" s="9" t="s">
+        <v>716</v>
+      </c>
+      <c r="B203" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C203" s="10"/>
+      <c r="D203" s="10"/>
+      <c r="E203" s="8" t="s">
+        <v>717</v>
+      </c>
+      <c r="F203" s="8" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="204" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A204" s="9" t="s">
+        <v>719</v>
+      </c>
+      <c r="B204" s="8" t="s">
+        <v>454</v>
+      </c>
+      <c r="C204" s="8" t="n">
+        <v>21</v>
+      </c>
+      <c r="D204" s="8"/>
+      <c r="E204" s="8" t="s">
+        <v>720</v>
+      </c>
+      <c r="G204" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A203" s="1" t="s">
-        <v>715</v>
-      </c>
-      <c r="B203" s="8" t="s">
+    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A205" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="B205" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="E203" s="8" t="s">
-        <v>716</v>
-      </c>
-      <c r="F203" s="8" t="s">
-        <v>717</v>
+      <c r="E205" s="8" t="s">
+        <v>722</v>
+      </c>
+      <c r="F205" s="8" t="s">
+        <v>723</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renamed Office to Microsoft Office
small rename from Office to Microsoft Office
</commit_message>
<xml_diff>
--- a/hashinfo.xlsx
+++ b/hashinfo.xlsx
@@ -1139,6 +1139,33 @@
     <t>$oldoffice$3*83328705222323020515404251156288*2855956a165ff6511bc7f4cd77b9e101*941861655e73a09c40f7b1e9dfd0c256ed285acd</t>
   </si>
   <si>
+    <t>Microsoft Office 2007</t>
+  </si>
+  <si>
+    <t>^\$office\$\*2007\*[0-9]{2}\*[0-9]{3}\*[0-9]{2}\*[a-z0-9]{32}\*[a-z0-9]{32}\*[a-z0-9]{40}$/i</t>
+  </si>
+  <si>
+    <t>$office$*2007*20*128*16*411a51284e0d0200b131a8949aaaa5cc*117d532441c63968bee7647d9b7df7d6*df1d601ccf905b375575108f42ef838fb88e1cde</t>
+  </si>
+  <si>
+    <t>Microsoft Office 2010</t>
+  </si>
+  <si>
+    <t>^\$office\$\*2010\*[0-9]{6}\*[0-9]{3}\*[0-9]{2}\*[a-z0-9]{32}\*[a-z0-9]{32}\*[a-z0-9]{64}$/i</t>
+  </si>
+  <si>
+    <t>$office$*2010*100000*128*16*77233201017277788267221014757262*b2d0ca4854ba19cf95a2647d5eee906c*e30cbbb189575cafb6f142a90c2622fa9e78d293c5b0c001517b3f5b82993557</t>
+  </si>
+  <si>
+    <t>Microsoft Office 2013</t>
+  </si>
+  <si>
+    <t>^\$office\$\*2013\*[0-9]{6}\*[0-9]{3}\*[0-9]{2}\*[a-z0-9]{32}\*[a-z0-9]{32}\*[a-z0-9]{64}$/i</t>
+  </si>
+  <si>
+    <t>$office$*2013*100000*256*16*7dd611d7eb4c899f74816d1dec817b3b*948dc0b2c2c6c32f14b5995a543ad037*0b7ee0e48e935f937192a59de48a7d561ef2691d5c8a3ba87ec2d04402a94895</t>
+  </si>
+  <si>
     <t>Minecraft(AuthMe Reloaded)</t>
   </si>
   <si>
@@ -1323,33 +1350,6 @@
   </si>
   <si>
     <t>nt</t>
-  </si>
-  <si>
-    <t>Office 2007</t>
-  </si>
-  <si>
-    <t>^\$office\$\*2007\*[0-9]{2}\*[0-9]{3}\*[0-9]{2}\*[a-z0-9]{32}\*[a-z0-9]{32}\*[a-z0-9]{40}$/i</t>
-  </si>
-  <si>
-    <t>$office$*2007*20*128*16*411a51284e0d0200b131a8949aaaa5cc*117d532441c63968bee7647d9b7df7d6*df1d601ccf905b375575108f42ef838fb88e1cde</t>
-  </si>
-  <si>
-    <t>Office 2010</t>
-  </si>
-  <si>
-    <t>^\$office\$\*2010\*[0-9]{6}\*[0-9]{3}\*[0-9]{2}\*[a-z0-9]{32}\*[a-z0-9]{32}\*[a-z0-9]{64}$/i</t>
-  </si>
-  <si>
-    <t>$office$*2010*100000*128*16*77233201017277788267221014757262*b2d0ca4854ba19cf95a2647d5eee906c*e30cbbb189575cafb6f142a90c2622fa9e78d293c5b0c001517b3f5b82993557</t>
-  </si>
-  <si>
-    <t>Office 2013</t>
-  </si>
-  <si>
-    <t>^\$office\$\*2013\*[0-9]{6}\*[0-9]{3}\*[0-9]{2}\*[a-z0-9]{32}\*[a-z0-9]{32}\*[a-z0-9]{64}$/i</t>
-  </si>
-  <si>
-    <t>$office$*2013*100000*256*16*7dd611d7eb4c899f74816d1dec817b3b*948dc0b2c2c6c32f14b5995a543ad037*0b7ee0e48e935f937192a59de48a7d561ef2691d5c8a3ba87ec2d04402a94895</t>
   </si>
   <si>
     <t>Oracle 11g/12c</t>
@@ -2372,7 +2372,7 @@
   <dimension ref="A1:G205"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A82" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A121" activeCellId="0" sqref="A121"/>
+      <selection pane="topLeft" activeCell="A95" activeCellId="0" sqref="A95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4175,7 +4175,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="13" t="s">
         <v>368</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="13" t="s">
         <v>371</v>
       </c>
@@ -4210,242 +4210,237 @@
       </c>
     </row>
     <row r="104" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="9" t="s">
+      <c r="A104" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="B104" s="8" t="s">
+      <c r="B104" s="2" t="s">
         <v>375</v>
       </c>
-      <c r="C104" s="10"/>
-      <c r="D104" s="10"/>
+      <c r="C104" s="2" t="n">
+        <v>9400</v>
+      </c>
       <c r="E104" s="8" t="s">
         <v>376</v>
       </c>
-      <c r="F104" s="8" t="s">
+      <c r="G104" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="105" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="1" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="105" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="9" t="s">
+      <c r="B105" s="2" t="s">
         <v>378</v>
       </c>
-      <c r="B105" s="8" t="s">
+      <c r="C105" s="2" t="n">
+        <v>9500</v>
+      </c>
+      <c r="E105" s="16" t="s">
         <v>379</v>
       </c>
-      <c r="C105" s="10"/>
-      <c r="D105" s="10"/>
-      <c r="E105" s="8" t="s">
+      <c r="G105" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="106" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="F105" s="8" t="s">
+      <c r="B106" s="2" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="106" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="9" t="s">
+      <c r="C106" s="2" t="n">
+        <v>9600</v>
+      </c>
+      <c r="E106" s="2" t="s">
         <v>382</v>
       </c>
-      <c r="B106" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="C106" s="8" t="n">
-        <v>131</v>
-      </c>
-      <c r="D106" s="8" t="s">
-        <v>384</v>
-      </c>
-      <c r="E106" s="8" t="s">
-        <v>385</v>
-      </c>
-      <c r="F106" s="8" t="s">
-        <v>386</v>
+      <c r="G106" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="107" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="9" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>388</v>
-      </c>
-      <c r="C107" s="8" t="n">
-        <v>132</v>
-      </c>
-      <c r="D107" s="8" t="s">
-        <v>389</v>
-      </c>
+        <v>384</v>
+      </c>
+      <c r="C107" s="10"/>
+      <c r="D107" s="10"/>
       <c r="E107" s="8" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="F107" s="8" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
     </row>
     <row r="108" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="9" t="s">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="B108" s="8" t="s">
         <v>388</v>
       </c>
-      <c r="C108" s="10" t="n">
-        <v>132</v>
-      </c>
+      <c r="C108" s="10"/>
       <c r="D108" s="10"/>
-      <c r="E108" s="8"/>
-      <c r="G108" s="3" t="s">
-        <v>35</v>
+      <c r="E108" s="8" t="s">
+        <v>389</v>
+      </c>
+      <c r="F108" s="8" t="s">
+        <v>390</v>
       </c>
     </row>
     <row r="109" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="9" t="s">
+        <v>391</v>
+      </c>
+      <c r="B109" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="C109" s="8" t="n">
+        <v>131</v>
+      </c>
+      <c r="D109" s="8" t="s">
         <v>393</v>
       </c>
-      <c r="B109" s="8" t="s">
+      <c r="E109" s="8" t="s">
         <v>394</v>
       </c>
-      <c r="C109" s="8" t="n">
-        <v>1731</v>
-      </c>
-      <c r="D109" s="8"/>
-      <c r="E109" s="8" t="s">
+      <c r="F109" s="8" t="s">
         <v>395</v>
       </c>
-      <c r="G109" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="110" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="9" t="s">
         <v>396</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="C110" s="8" t="n">
-        <v>1731</v>
-      </c>
-      <c r="D110" s="8"/>
-      <c r="E110" s="8"/>
+        <v>132</v>
+      </c>
+      <c r="D110" s="8" t="s">
+        <v>398</v>
+      </c>
+      <c r="E110" s="8" t="s">
+        <v>399</v>
+      </c>
       <c r="F110" s="8" t="s">
-        <v>397</v>
-      </c>
-      <c r="G110" s="3" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="111" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="9" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>400</v>
-      </c>
-      <c r="C111" s="8" t="n">
-        <v>2811</v>
-      </c>
-      <c r="D111" s="8"/>
-      <c r="E111" s="8" t="s">
-        <v>401</v>
-      </c>
-      <c r="F111" s="8" t="s">
-        <v>402</v>
+        <v>397</v>
+      </c>
+      <c r="C111" s="10" t="n">
+        <v>132</v>
+      </c>
+      <c r="D111" s="10"/>
+      <c r="E111" s="8"/>
+      <c r="G111" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="112" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="B112" s="8" t="s">
         <v>403</v>
       </c>
-      <c r="B112" s="8" t="s">
-        <v>107</v>
-      </c>
       <c r="C112" s="8" t="n">
-        <v>200</v>
-      </c>
-      <c r="D112" s="8" t="s">
+        <v>1731</v>
+      </c>
+      <c r="D112" s="8"/>
+      <c r="E112" s="8" t="s">
         <v>404</v>
       </c>
-      <c r="E112" s="8" t="s">
+      <c r="G112" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="F112" s="8" t="s">
+      <c r="B113" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="C113" s="8" t="n">
+        <v>1731</v>
+      </c>
+      <c r="D113" s="8"/>
+      <c r="E113" s="8"/>
+      <c r="F113" s="8" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="113" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="12" t="s">
+      <c r="G113" s="3" t="s">
         <v>407</v>
-      </c>
-      <c r="B113" s="8" t="s">
-        <v>408</v>
-      </c>
-      <c r="C113" s="8" t="n">
-        <v>300</v>
-      </c>
-      <c r="D113" s="8" t="s">
-        <v>409</v>
-      </c>
-      <c r="E113" s="8" t="s">
-        <v>410</v>
-      </c>
-      <c r="F113" s="8" t="s">
-        <v>411</v>
       </c>
     </row>
     <row r="114" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="9" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="C114" s="8" t="n">
-        <v>300</v>
-      </c>
-      <c r="D114" s="8" t="s">
-        <v>409</v>
-      </c>
+        <v>2811</v>
+      </c>
+      <c r="D114" s="8"/>
       <c r="E114" s="8" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="F114" s="8" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
     </row>
     <row r="115" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="B115" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C115" s="8" t="n">
+        <v>200</v>
+      </c>
+      <c r="D115" s="8" t="s">
+        <v>413</v>
+      </c>
+      <c r="E115" s="8" t="s">
+        <v>414</v>
+      </c>
+      <c r="F115" s="8" t="s">
         <v>415</v>
       </c>
-      <c r="B115" s="8" t="s">
+    </row>
+    <row r="116" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A116" s="12" t="s">
         <v>416</v>
       </c>
-      <c r="C115" s="8" t="n">
-        <v>5500</v>
-      </c>
-      <c r="D115" s="8"/>
-      <c r="E115" s="8" t="s">
+      <c r="B116" s="8" t="s">
         <v>417</v>
       </c>
-      <c r="G115" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="116" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A116" s="9" t="s">
+      <c r="C116" s="8" t="n">
+        <v>300</v>
+      </c>
+      <c r="D116" s="8" t="s">
         <v>418</v>
       </c>
-      <c r="B116" s="8" t="s">
+      <c r="E116" s="8" t="s">
         <v>419</v>
       </c>
-      <c r="C116" s="8" t="n">
-        <v>5600</v>
-      </c>
-      <c r="D116" s="8"/>
-      <c r="E116" s="8" t="s">
+      <c r="F116" s="8" t="s">
         <v>420</v>
-      </c>
-      <c r="G116" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="117" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4453,36 +4448,34 @@
         <v>421</v>
       </c>
       <c r="B117" s="8" t="s">
+        <v>417</v>
+      </c>
+      <c r="C117" s="8" t="n">
+        <v>300</v>
+      </c>
+      <c r="D117" s="8" t="s">
+        <v>418</v>
+      </c>
+      <c r="E117" s="8" t="s">
         <v>422</v>
       </c>
-      <c r="C117" s="8" t="n">
-        <v>101</v>
-      </c>
-      <c r="D117" s="8" t="s">
+      <c r="F117" s="8" t="s">
         <v>423</v>
-      </c>
-      <c r="E117" s="8" t="s">
-        <v>424</v>
-      </c>
-      <c r="G117" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="118" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="B118" s="8" t="s">
         <v>425</v>
       </c>
-      <c r="B118" s="8" t="s">
+      <c r="C118" s="8" t="n">
+        <v>5500</v>
+      </c>
+      <c r="D118" s="8"/>
+      <c r="E118" s="8" t="s">
         <v>426</v>
-      </c>
-      <c r="C118" s="8" t="n">
-        <v>111</v>
-      </c>
-      <c r="D118" s="8" t="s">
-        <v>427</v>
-      </c>
-      <c r="E118" s="8" t="s">
-        <v>428</v>
       </c>
       <c r="G118" s="3" t="s">
         <v>35</v>
@@ -4490,86 +4483,93 @@
     </row>
     <row r="119" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="9" t="s">
+        <v>427</v>
+      </c>
+      <c r="B119" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="C119" s="8" t="n">
+        <v>5600</v>
+      </c>
+      <c r="D119" s="8"/>
+      <c r="E119" s="8" t="s">
         <v>429</v>
       </c>
-      <c r="B119" s="8" t="s">
-        <v>430</v>
-      </c>
-      <c r="C119" s="10"/>
-      <c r="D119" s="10"/>
-      <c r="E119" s="8" t="s">
-        <v>431</v>
-      </c>
-      <c r="F119" s="8" t="s">
-        <v>432</v>
+      <c r="G119" s="3" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="120" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="B120" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="C120" s="8" t="n">
+        <v>101</v>
+      </c>
+      <c r="D120" s="8" t="s">
+        <v>432</v>
+      </c>
+      <c r="E120" s="8" t="s">
         <v>433</v>
-      </c>
-      <c r="B120" s="8" t="s">
-        <v>434</v>
-      </c>
-      <c r="C120" s="8" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D120" s="8" t="s">
-        <v>435</v>
-      </c>
-      <c r="E120" s="8" t="s">
-        <v>346</v>
       </c>
       <c r="G120" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="121" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="1" t="s">
+      <c r="A121" s="9" t="s">
+        <v>434</v>
+      </c>
+      <c r="B121" s="8" t="s">
+        <v>435</v>
+      </c>
+      <c r="C121" s="8" t="n">
+        <v>111</v>
+      </c>
+      <c r="D121" s="8" t="s">
         <v>436</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="E121" s="8" t="s">
         <v>437</v>
-      </c>
-      <c r="C121" s="2" t="n">
-        <v>9400</v>
-      </c>
-      <c r="E121" s="8" t="s">
-        <v>438</v>
       </c>
       <c r="G121" s="3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="122" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A122" s="1" t="s">
+      <c r="A122" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="B122" s="8" t="s">
         <v>439</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="C122" s="10"/>
+      <c r="D122" s="10"/>
+      <c r="E122" s="8" t="s">
         <v>440</v>
       </c>
-      <c r="C122" s="2" t="n">
-        <v>9500</v>
-      </c>
-      <c r="E122" s="16" t="s">
+      <c r="F122" s="8" t="s">
         <v>441</v>
       </c>
-      <c r="G122" s="3" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="123" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="1" t="s">
+      <c r="A123" s="9" t="s">
         <v>442</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="B123" s="8" t="s">
         <v>443</v>
       </c>
-      <c r="C123" s="2" t="n">
-        <v>9600</v>
-      </c>
-      <c r="E123" s="2" t="s">
+      <c r="C123" s="8" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D123" s="8" t="s">
         <v>444</v>
+      </c>
+      <c r="E123" s="8" t="s">
+        <v>346</v>
       </c>
       <c r="G123" s="3" t="s">
         <v>35</v>
@@ -5136,14 +5136,14 @@
         <v>568</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
       <c r="C156" s="8" t="n">
         <v>101</v>
       </c>
       <c r="D156" s="8"/>
       <c r="E156" s="8" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
       <c r="G156" s="3" t="s">
         <v>35</v>
@@ -5634,7 +5634,7 @@
       </c>
       <c r="D185" s="8"/>
       <c r="E185" s="8" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
       <c r="G185" s="3" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
hashcat mode for Django(PBKDF2-HMAC-SHA256)
added hashcat mode for Django(PBKDF2-HMAC-SHA256) from the latest
hashcat wiki update
</commit_message>
<xml_diff>
--- a/hashinfo.xlsx
+++ b/hashinfo.xlsx
@@ -2371,8 +2371,8 @@
   </sheetPr>
   <dimension ref="A1:G205"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B187" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3022,6 +3022,7 @@
       <c r="B36" s="2" t="s">
         <v>134</v>
       </c>
+      <c r="C36" s="7"/>
       <c r="E36" s="8" t="s">
         <v>135</v>
       </c>
@@ -3036,6 +3037,7 @@
       <c r="B37" s="2" t="s">
         <v>138</v>
       </c>
+      <c r="C37" s="7"/>
       <c r="E37" s="8" t="s">
         <v>139</v>
       </c>
@@ -3050,6 +3052,7 @@
       <c r="B38" s="2" t="s">
         <v>142</v>
       </c>
+      <c r="C38" s="7"/>
       <c r="E38" s="8" t="s">
         <v>143</v>
       </c>
@@ -3064,6 +3067,7 @@
       <c r="B39" s="2" t="s">
         <v>146</v>
       </c>
+      <c r="C39" s="7"/>
       <c r="E39" s="8" t="s">
         <v>147</v>
       </c>
@@ -3077,6 +3081,9 @@
       </c>
       <c r="B40" s="2" t="s">
         <v>150</v>
+      </c>
+      <c r="C40" s="7" t="n">
+        <v>10000</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>151</v>
@@ -4710,6 +4717,7 @@
       <c r="B131" s="2" t="s">
         <v>471</v>
       </c>
+      <c r="C131" s="7"/>
       <c r="E131" s="8" t="s">
         <v>472</v>
       </c>
@@ -4847,6 +4855,7 @@
       <c r="B139" s="2" t="s">
         <v>504</v>
       </c>
+      <c r="C139" s="7"/>
       <c r="E139" s="8" t="s">
         <v>505</v>
       </c>

</xml_diff>

<commit_message>
Added some missing resource links
Added some missing resource links from hashcat forum
</commit_message>
<xml_diff>
--- a/hashinfo.xlsx
+++ b/hashinfo.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="724">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="880" uniqueCount="727">
   <si>
     <t>Hash</t>
   </si>
@@ -122,126 +122,132 @@
     <t>$fde$16$ca56e82e7b5a9c2fc1e3b5a7d671c2f9$16$7c124af19ac913be0fc137b75a34b20d$eac806ae7277c8d48243d52a8644fa57a817317bd3457f94dca727964cbc27c88296954f289597a9de3314a4e9d9f28dce70cf9ce3e1c3c0c6fc041687a0ad3cb333d4449bc9da8fcc7d5f85948a7ac3bc6d34f505e9d0d91da4396e35840bde3465ad11c5086c89ee6db68d65e47a2e5413f272caa01e02224e5ff3dc3bed3953a702e85e964e562e62f5c97a2df6c47547bfb5aeeb329ff8f9c9666724d399043fe970c8b282b45e93d008333f3b4edd5eb147bd023ed18ac1f9f75a6cd33444b507694c64e1e98a964b48c0a77276e9930250d01801813c235169a7b1952891c63ce0d462abc688bd96c0337174695a957858b4c9fd277d04abe8a0c2c5def4b352ba29410f8dbec91bcb2ca2b8faf26d44f02340b3373bc94e7487ce014e6adfbf7edfdd2057225f8aeb324c9d1be877c6ae4211ae387e07bf2a056984d2ed2815149b3e9cf9fbfae852f7dd5906c2b86e7910c0d7755ef5bcc39f0e135bf546c839693dc4af3e50b8382c7c8c754d4ee218fa85d70ee0a5707a9f827209a7ddb6c2fb9431a61c9775112cc88aa2a34f97c2f53dfce082aa0758917269a5fc30049ceab67d3efd721fee021ffca979f839b4f052e27f5c382c0dd5c02fd39fbc9b26e04bf9e051d1923eff9a7cde3244902bb8538b1b9f11631def5aad7c21d2113bcdc989b771ff6bf220f94354034dd417510117b55a669e969fc3bc6c5dcd4741b8313bf7d999dc94d4949f27eec0cd06f906c17a80d09f583a5dd601854832673b78d125a2c5ad0352932be7b93c611fee8c6049670442d8c532674f3d21d45d3d009211d2a9e6568252ac4682982172cb43e7c6b05e85851787ad90e25b77cce3f7968d455f92653a1d3790bc50e5f6e1f743ac47275ffa8e81bbe832a8d7d78d5d5a7c73f95703aebb355849ae566492093bd9cb51070f39c69bb4e22b99cc0e60e96d048385bb69f1c44a3b79547fbc19a873a632f43f05fa2d8a6f9155e59d153e2851b739c42444018b8c4e09a93be43570834667d0b5a5d2a53b1572dab3e750b3f9e641e303559bace06612fbd451a5e822201442828e79168c567a85d8c024cd8ce32bf650105b1af98cc5428675f4f4bbede37a0ef98d1533a8a6dcb27d87a2b799f18706f4677edaa0411becac4c591ede83993aedba660d1dd67f6c4a5c141ad3e6e0c77730cb0ecbf4f4bd8ef6067e05ca3bc563d9e1554a893fea0050bdd1733c883f533f87eac39cceee0ccf817fc1f19bcfdd13e9f241b89bfb149b509e9a0747658438536b6705514cc6d6bb3c64c903e4710435d8bebc35297d1ebbdff8074b203f37d1910d8b4637e4d3dab997f4aa378a7a67c79e698a11e83d0d7e759d0e7969c4f5408168b282fe28d3279ec1d4cc6f85a0f8e5d01f21c7508a69773c44167ff8d467d0801f9ec54f9ee2496d4e7e470214abc1ca11355bb18cd23273aac6b05b47f9e301b42b137a2455758c24e2716dcd2e55bbeb780f592e664e7392bf6eccb80959f24c8800816c84f2575e82e1f3559c33a5be7a3a0c843c2989f486b113d5eeada007caf6b5a0f6d71e2f5c09a4def57c7057168051868317a9ec790d570d76a0d21a45ad951c475db5a66101475871147c5a5907ec4e6b14128ed6695bb73c1c97952e96826eeb6003aa13462093e4afc209627241f03b0247e110fbab983640423b7cdf112e01579fed68c80ac7df7449d9d2114b9ae5539c03c2037be45c5f74e7357b25c6a24b7bd503864437147e50d7ac4ccc4bbd0cabecdc6bac60a362285fe450e2c2d0a446578c8880dc957e6e8061e691b83eb8062d1aad476e0c7b25e4d5454f1288686eb525f37fe649637b235b7828366b0219a9c63d6ddbb696dc3585a2ebfbd5f5e4c170d6784ab9993e15142535e194d2bee3dc9477ef8b8e1b07605e0c04f49edf6d42be3a9dabbc592dde78ce8b7dd9684bfcf4ca2f5a44b1872abe18fb6fa67a79390f273a9d12f9269389629456d71b9e7ed3447462269a849ce83e1893f253c832537f850b1acce5b11d2ba6b7c2f99e8e7c8085f390c21f69e1ce4bbf85b4e1ad86c0d6706432766978076f4cada9ca6f28d395d9cc5e74b2a6b46eb9d1de79eeecff7dc97ec2a8d8870e3894e1e4e26ccb98dd2f88c0229bbd3152fa149f0cc132561f</t>
   </si>
   <si>
+    <t>http://hashcat.net/forum/thread-2270.html</t>
+  </si>
+  <si>
+    <t>Android PIN</t>
+  </si>
+  <si>
+    <t>^[a-f0-9]{40}:[a-f0-9]{16}$/i</t>
+  </si>
+  <si>
+    <t>0223b799d526b596fe4ba5628b9e65068227e68e:f6d45822728ddb2c</t>
+  </si>
+  <si>
+    <t>http://hashcat.net/forum/thread-2202.html</t>
+  </si>
+  <si>
+    <t>Apache MD5</t>
+  </si>
+  <si>
+    <t>^\$apr1\$[a-z0-9\/.]{0,8}\$[a-z0-9\/.]{22}$/i</t>
+  </si>
+  <si>
+    <t>$apr1$2apDSb1n$VBnEoNgWg47PB5hZyt8kr/</t>
+  </si>
+  <si>
+    <t>http://pythonhosted.org/passlib/lib/passlib.hash.apr_md5_crypt.html</t>
+  </si>
+  <si>
+    <t>BCrypt(SHA-256)</t>
+  </si>
+  <si>
+    <t>^\$bcrypt-sha256\$(2[axy]|2)\,[0-9]+\$[a-z0-9\/.]{22}\$[a-z0-9\/.]{31}$/i</t>
+  </si>
+  <si>
+    <t>$bcrypt-sha256$2a,12$LrmaIX5x4TRtAwEfwJZa1.$2ehnw6LvuIUTM0iz4iz9hTxv21B6KFO</t>
+  </si>
+  <si>
+    <t>http://pythonhosted.org/passlib/lib/passlib.hash.bcrypt_sha256.html</t>
+  </si>
+  <si>
+    <t>Blowfish(OpenBSD)</t>
+  </si>
+  <si>
+    <t>^(\$2[axy]|\$2)\$[0-9]{0,2}?\$[a-z0-9\/.]{53}$/i</t>
+  </si>
+  <si>
+    <t>bf</t>
+  </si>
+  <si>
+    <t>$2a$12$GhvMmNVjRW29ulnudl.LbuAnUtN/LRfe1JsBm1Xu6LE3059z5Tr8m</t>
+  </si>
+  <si>
+    <t>http://pythonhosted.org/passlib/lib/passlib.hash.bcrypt.html</t>
+  </si>
+  <si>
+    <t>BSDi Crypt</t>
+  </si>
+  <si>
+    <t>^_[a-z0-9\/.]{19}$/i</t>
+  </si>
+  <si>
+    <t>bsdi</t>
+  </si>
+  <si>
+    <t>_EQ0.jzhSVeUyoSqLupI</t>
+  </si>
+  <si>
+    <t>http://pythonhosted.org/passlib/lib/passlib.hash.bsdi_crypt.html</t>
+  </si>
+  <si>
+    <t>Cisco Type 8</t>
+  </si>
+  <si>
+    <t>^\$8\$[a-z0-9\/.]{14}\$[a-z0-9\/.]{43}$/i</t>
+  </si>
+  <si>
+    <t>$8$TnGX/fE4KGHOVU$pEhnEvxrvaynpi8j4f.EMHr6M.FzU8xnZnBr/tJdFWk</t>
+  </si>
+  <si>
+    <t>http://hashcat.net/forum/thread-3803.html</t>
+  </si>
+  <si>
+    <t>Cisco Type 9</t>
+  </si>
+  <si>
+    <t>^\$9\$[a-z0-9\/.]{14}\$[a-z0-9\/.]{43}$/i</t>
+  </si>
+  <si>
+    <t>$9$2MJBozw/9R3UsU$2lFhcKvpghcyw8deP25GOfyZaagyUOGBymkryvOdfo6</t>
+  </si>
+  <si>
+    <t>Cisco VPN Client(PCF-File)</t>
+  </si>
+  <si>
+    <t>^[a-f0-9]{112}$/i</t>
+  </si>
+  <si>
+    <t>071B15CA6E98F1D339D9B25BE350DAAB9A1C5E0B6499850B610E631FCBFB79A91E4E8FDFF813E064DCECFE6A5233998DC58C9DB8099435DE</t>
+  </si>
+  <si>
+    <t>https://www.unix-ag.uni-kl.de/~massar/bin/cisco-decode/</t>
+  </si>
+  <si>
+    <t>Cisco-ASA(MD5)</t>
+  </si>
+  <si>
+    <t>^[a-z0-9\/.]{16}(:.{1,})?$/i</t>
+  </si>
+  <si>
+    <t>.ewJz0Du3XKnFk/d:hashid</t>
+  </si>
+  <si>
+    <t>https://github.com/stekershaw/asa-password-encrypt</t>
+  </si>
+  <si>
+    <t>Cisco-IOS(MD5)</t>
+  </si>
+  <si>
+    <t>^\$1\$[a-z0-9\/.]{0,8}\$[a-z0-9\/.]{22}(:.*)?$/i</t>
+  </si>
+  <si>
+    <t>$1$28772684$iEwNOgGugqO9.bIz5sk8k/</t>
+  </si>
+  <si>
     <t>resource needed</t>
   </si>
   <si>
-    <t>Android PIN</t>
-  </si>
-  <si>
-    <t>^[a-f0-9]{40}:[a-f0-9]{16}$/i</t>
-  </si>
-  <si>
-    <t>0223b799d526b596fe4ba5628b9e65068227e68e:f6d45822728ddb2c</t>
-  </si>
-  <si>
-    <t>http://hashcat.net/forum/thread-2202.html</t>
-  </si>
-  <si>
-    <t>Apache MD5</t>
-  </si>
-  <si>
-    <t>^\$apr1\$[a-z0-9\/.]{0,8}\$[a-z0-9\/.]{22}$/i</t>
-  </si>
-  <si>
-    <t>$apr1$2apDSb1n$VBnEoNgWg47PB5hZyt8kr/</t>
-  </si>
-  <si>
-    <t>http://pythonhosted.org/passlib/lib/passlib.hash.apr_md5_crypt.html</t>
-  </si>
-  <si>
-    <t>BCrypt(SHA-256)</t>
-  </si>
-  <si>
-    <t>^\$bcrypt-sha256\$(2[axy]|2)\,[0-9]+\$[a-z0-9\/.]{22}\$[a-z0-9\/.]{31}$/i</t>
-  </si>
-  <si>
-    <t>$bcrypt-sha256$2a,12$LrmaIX5x4TRtAwEfwJZa1.$2ehnw6LvuIUTM0iz4iz9hTxv21B6KFO</t>
-  </si>
-  <si>
-    <t>http://pythonhosted.org/passlib/lib/passlib.hash.bcrypt_sha256.html</t>
-  </si>
-  <si>
-    <t>Blowfish(OpenBSD)</t>
-  </si>
-  <si>
-    <t>^(\$2[axy]|\$2)\$[0-9]{0,2}?\$[a-z0-9\/.]{53}$/i</t>
-  </si>
-  <si>
-    <t>bf</t>
-  </si>
-  <si>
-    <t>$2a$12$GhvMmNVjRW29ulnudl.LbuAnUtN/LRfe1JsBm1Xu6LE3059z5Tr8m</t>
-  </si>
-  <si>
-    <t>http://pythonhosted.org/passlib/lib/passlib.hash.bcrypt.html</t>
-  </si>
-  <si>
-    <t>BSDi Crypt</t>
-  </si>
-  <si>
-    <t>^_[a-z0-9\/.]{19}$/i</t>
-  </si>
-  <si>
-    <t>bsdi</t>
-  </si>
-  <si>
-    <t>_EQ0.jzhSVeUyoSqLupI</t>
-  </si>
-  <si>
-    <t>http://pythonhosted.org/passlib/lib/passlib.hash.bsdi_crypt.html</t>
-  </si>
-  <si>
-    <t>Cisco Type 8</t>
-  </si>
-  <si>
-    <t>^\$8\$[a-z0-9\/.]{14}\$[a-z0-9\/.]{43}$/i</t>
-  </si>
-  <si>
-    <t>$8$TnGX/fE4KGHOVU$pEhnEvxrvaynpi8j4f.EMHr6M.FzU8xnZnBr/tJdFWk</t>
-  </si>
-  <si>
-    <t>Cisco Type 9</t>
-  </si>
-  <si>
-    <t>^\$9\$[a-z0-9\/.]{14}\$[a-z0-9\/.]{43}$/i</t>
-  </si>
-  <si>
-    <t>$9$2MJBozw/9R3UsU$2lFhcKvpghcyw8deP25GOfyZaagyUOGBymkryvOdfo6</t>
-  </si>
-  <si>
-    <t>Cisco VPN Client(PCF-File)</t>
-  </si>
-  <si>
-    <t>^[a-f0-9]{112}$/i</t>
-  </si>
-  <si>
-    <t>071B15CA6E98F1D339D9B25BE350DAAB9A1C5E0B6499850B610E631FCBFB79A91E4E8FDFF813E064DCECFE6A5233998DC58C9DB8099435DE</t>
-  </si>
-  <si>
-    <t>https://www.unix-ag.uni-kl.de/~massar/bin/cisco-decode/</t>
-  </si>
-  <si>
-    <t>Cisco-ASA(MD5)</t>
-  </si>
-  <si>
-    <t>^[a-z0-9\/.]{16}(:.{1,})?$/i</t>
-  </si>
-  <si>
-    <t>.ewJz0Du3XKnFk/d:hashid</t>
-  </si>
-  <si>
-    <t>https://github.com/stekershaw/asa-password-encrypt</t>
-  </si>
-  <si>
-    <t>Cisco-IOS(MD5)</t>
-  </si>
-  <si>
-    <t>^\$1\$[a-z0-9\/.]{0,8}\$[a-z0-9\/.]{22}(:.*)?$/i</t>
-  </si>
-  <si>
-    <t>$1$28772684$iEwNOgGugqO9.bIz5sk8k/</t>
-  </si>
-  <si>
     <t>Cisco-IOS(SHA-256)</t>
   </si>
   <si>
@@ -1128,6 +1134,9 @@
   </si>
   <si>
     <t>$oldoffice$1*04477077758555626246182730342136*b1b72ff351e41a7c68f6b45c4e938bd6*0d95331895e99f73ef8b6fbc4a78ac1a</t>
+  </si>
+  <si>
+    <t>http://hashcat.net/forum/thread-3665.html</t>
   </si>
   <si>
     <t>Microsoft Office ≤ 2003 (SHA1+RC4)</t>
@@ -2371,8 +2380,8 @@
   </sheetPr>
   <dimension ref="A1:G205"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B38" activeCellId="0" sqref="1:1048576"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A161" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A208" activeCellId="0" sqref="1:1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2552,7 +2561,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -2562,10 +2571,11 @@
       <c r="C9" s="2" t="n">
         <v>8800</v>
       </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="F9" s="1" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2659,7 +2669,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>58</v>
       </c>
@@ -2669,205 +2679,207 @@
       <c r="C15" s="2" t="n">
         <v>9200</v>
       </c>
+      <c r="D15" s="1"/>
       <c r="E15" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G15" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F15" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C16" s="2" t="n">
         <v>9300</v>
       </c>
+      <c r="D16" s="1"/>
       <c r="E16" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>35</v>
+        <v>64</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="17" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C18" s="8" t="n">
         <v>2410</v>
       </c>
       <c r="D18" s="8"/>
       <c r="E18" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C19" s="8" t="n">
         <v>500</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C20" s="8" t="n">
         <v>5700</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="8" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C21" s="8" t="n">
         <v>2400</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C22" s="8" t="n">
         <v>8100</v>
       </c>
       <c r="D22" s="8"/>
       <c r="E22" s="8" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10"/>
       <c r="E23" s="8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10"/>
       <c r="E24" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="9" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10"/>
       <c r="E25" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10"/>
       <c r="E26" s="8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B27" s="8" t="s">
         <v>16</v>
@@ -2875,15 +2887,15 @@
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="9" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>16</v>
@@ -2891,390 +2903,390 @@
       <c r="C28" s="10"/>
       <c r="D28" s="10"/>
       <c r="E28" s="8" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="F28" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="9" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10"/>
       <c r="E29" s="8" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="30" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="9" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10"/>
       <c r="E30" s="8" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="9" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10"/>
       <c r="E31" s="8" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="9" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
       <c r="E32" s="8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F32" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="33" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="9" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="C33" s="10"/>
       <c r="D33" s="10"/>
       <c r="E33" s="8" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F33" s="8" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="34" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="9" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C34" s="8" t="n">
         <v>3100</v>
       </c>
       <c r="D34" s="8"/>
       <c r="E34" s="8" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F34" s="8" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="12" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C35" s="8" t="n">
         <v>1500</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E35" s="8" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F35" s="8" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="36" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C36" s="7"/>
       <c r="E36" s="8" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row r="37" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C37" s="7"/>
       <c r="E37" s="8" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C38" s="7"/>
       <c r="E38" s="8" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C39" s="7"/>
       <c r="E39" s="8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C40" s="7" t="n">
         <v>10000</v>
       </c>
       <c r="E40" s="8" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="41" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="C41" s="8" t="n">
         <v>800</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="8" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="F41" s="8" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
     </row>
     <row r="42" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
       <c r="E42" s="8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="F42" s="8" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
       <c r="E43" s="8" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="F43" s="8" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="44" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C44" s="10" t="n">
         <v>8300</v>
       </c>
       <c r="D44" s="10"/>
       <c r="E44" s="8" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F44" s="8" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="9" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="C45" s="8" t="n">
         <v>1100</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="E45" s="8" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="9" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="C46" s="8" t="n">
         <v>2100</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E46" s="8" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="47" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C47" s="10" t="n">
         <v>2600</v>
       </c>
       <c r="D47" s="10"/>
       <c r="E47" s="8" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C48" s="10" t="n">
         <v>4500</v>
       </c>
       <c r="D48" s="10"/>
       <c r="E48" s="8" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="49" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C49" s="8" t="n">
         <v>7900</v>
       </c>
       <c r="D49" s="8"/>
       <c r="E49" s="8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="F49" s="8" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="50" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="E50" s="8" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="F50" s="8" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
     </row>
     <row r="51" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="9" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>16</v>
@@ -3282,46 +3294,46 @@
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
       <c r="E51" s="8" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="F51" s="8" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
     </row>
     <row r="52" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="9" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C52" s="8" t="n">
         <v>123</v>
       </c>
       <c r="D52" s="8"/>
       <c r="E52" s="8" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="9" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B53" s="8" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="C53" s="8" t="n">
         <v>141</v>
       </c>
       <c r="D53" s="8"/>
       <c r="E53" s="8" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>11</v>
@@ -3329,20 +3341,20 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="9" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="C54" s="8" t="n">
         <v>1441</v>
       </c>
       <c r="D54" s="8"/>
       <c r="E54" s="8" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>11</v>
@@ -3350,39 +3362,39 @@
     </row>
     <row r="55" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="B55" s="8" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
       <c r="E55" s="8" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="F55" s="8" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
     </row>
     <row r="56" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="9" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="B56" s="8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="C56" s="10"/>
       <c r="D56" s="10"/>
       <c r="E56" s="8" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="F56" s="8" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="57" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="9" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>16</v>
@@ -3390,15 +3402,15 @@
       <c r="C57" s="10"/>
       <c r="D57" s="10"/>
       <c r="E57" s="8" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F57" s="8" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="58" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="9" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>16</v>
@@ -3406,15 +3418,15 @@
       <c r="C58" s="10"/>
       <c r="D58" s="10"/>
       <c r="E58" s="8" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="9" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>16</v>
@@ -3422,69 +3434,69 @@
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
       <c r="E59" s="8" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="F59" s="8" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="60" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="9" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B60" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
       <c r="E60" s="8" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="F60" s="8" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
     </row>
     <row r="61" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="9" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="B61" s="8" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="C61" s="8" t="n">
         <v>7000</v>
       </c>
       <c r="D61" s="8"/>
       <c r="E61" s="8" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="62" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="9" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="B62" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C62" s="8" t="n">
         <v>500</v>
       </c>
       <c r="D62" s="8" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E62" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="63" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="9" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B63" s="8" t="s">
         <v>16</v>
@@ -3492,15 +3504,15 @@
       <c r="C63" s="10"/>
       <c r="D63" s="10"/>
       <c r="E63" s="8" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="F63" s="8" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
     </row>
     <row r="64" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="9" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="B64" s="8" t="s">
         <v>16</v>
@@ -3508,198 +3520,198 @@
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
       <c r="E64" s="8" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F64" s="8" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
     </row>
     <row r="65" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="9" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C65" s="8" t="n">
         <v>6900</v>
       </c>
       <c r="D65" s="8"/>
       <c r="E65" s="8" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="F65" s="8" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="66" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="9" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C66" s="8" t="n">
         <v>7200</v>
       </c>
       <c r="D66" s="8"/>
       <c r="E66" s="8" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
     </row>
     <row r="67" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="9" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C67" s="8" t="n">
         <v>5100</v>
       </c>
       <c r="D67" s="8"/>
       <c r="E67" s="8" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="68" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="9" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C68" s="10"/>
       <c r="D68" s="10"/>
       <c r="E68" s="8" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="F68" s="8" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
     </row>
     <row r="69" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="9" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C69" s="10"/>
       <c r="D69" s="10"/>
       <c r="E69" s="8" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="F69" s="8" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="70" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="9" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C70" s="10"/>
       <c r="D70" s="10"/>
       <c r="E70" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="F70" s="8" t="s">
         <v>255</v>
-      </c>
-      <c r="F70" s="8" t="s">
-        <v>253</v>
       </c>
     </row>
     <row r="71" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="9" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C71" s="10"/>
       <c r="D71" s="10"/>
       <c r="E71" s="8" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="F71" s="8" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="72" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="9" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C72" s="10"/>
       <c r="D72" s="10"/>
       <c r="E72" s="8" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="F72" s="8" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="73" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="9" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C73" s="10"/>
       <c r="D73" s="10"/>
       <c r="E73" s="8" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="F73" s="8" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
     </row>
     <row r="74" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B74" s="8" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="C74" s="10" t="n">
         <v>1421</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E74" s="8" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="F74" s="8" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="13" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="C75" s="2" t="n">
         <v>5300</v>
       </c>
       <c r="D75" s="7"/>
       <c r="E75" s="8" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="G75" s="3" t="s">
         <v>11</v>
@@ -3707,20 +3719,20 @@
     </row>
     <row r="76" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="13" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="C76" s="2" t="n">
         <v>5400</v>
       </c>
       <c r="D76" s="7"/>
       <c r="E76" s="8" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="G76" s="3" t="s">
         <v>11</v>
@@ -3728,61 +3740,61 @@
     </row>
     <row r="77" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="12" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C77" s="8" t="n">
         <v>2811</v>
       </c>
       <c r="D77" s="8"/>
       <c r="E77" s="8" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="C78" s="10" t="n">
         <v>7300</v>
       </c>
       <c r="D78" s="10"/>
       <c r="E78" s="8" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="79" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="9" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C79" s="8" t="n">
         <v>4800</v>
       </c>
       <c r="D79" s="8"/>
       <c r="E79" s="8" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="F79" s="8" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="80" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="9" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="B80" s="8" t="s">
         <v>16</v>
@@ -3790,84 +3802,84 @@
       <c r="C80" s="10"/>
       <c r="D80" s="10"/>
       <c r="E80" s="8" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="81" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="9" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="C81" s="8" t="n">
         <v>11</v>
       </c>
       <c r="D81" s="8"/>
       <c r="E81" s="8" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="F81" s="8" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
     </row>
     <row r="82" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="9" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C82" s="8" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D82" s="8"/>
       <c r="E82" s="8" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="F82" s="8" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
     </row>
     <row r="83" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="9" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="C83" s="8" t="n">
         <v>22</v>
       </c>
       <c r="D83" s="8" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="E83" s="8" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="9" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C84" s="8" t="n">
         <v>7500</v>
       </c>
       <c r="D84" s="8"/>
       <c r="E84" s="8" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="G84" s="3" t="s">
         <v>11</v>
@@ -3875,244 +3887,244 @@
     </row>
     <row r="85" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A85" s="9" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C85" s="8" t="n">
         <v>6800</v>
       </c>
       <c r="D85" s="8"/>
       <c r="E85" s="8" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="F85" s="8" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
     </row>
     <row r="86" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="9" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C86" s="8" t="n">
         <v>1711</v>
       </c>
       <c r="D86" s="8"/>
       <c r="E86" s="8" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="F86" s="8" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="87" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="9" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="C87" s="10"/>
       <c r="D87" s="10"/>
       <c r="E87" s="8" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="F87" s="8" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
     </row>
     <row r="88" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="9" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="B88" s="8" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C88" s="8" t="n">
         <v>190</v>
       </c>
       <c r="D88" s="8"/>
       <c r="E88" s="8" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
     </row>
     <row r="89" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A89" s="9" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="B89" s="8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C89" s="8" t="n">
         <v>3000</v>
       </c>
       <c r="D89" s="8" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="E89" s="8" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="F89" s="8" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="90" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="9" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C90" s="10" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D90" s="14" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="E90" s="8" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="91" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="9" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="C91" s="10" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D91" s="10" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="E91" s="8" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="92" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="1" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C92" s="2" t="n">
         <v>9100</v>
       </c>
       <c r="E92" s="8" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
     </row>
     <row r="93" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="9" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C93" s="10"/>
       <c r="D93" s="10"/>
       <c r="E93" s="8" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="F93" s="8" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="94" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="9" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C94" s="10"/>
       <c r="D94" s="10"/>
       <c r="E94" s="8" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="F94" s="8" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
     </row>
     <row r="95" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="9" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C95" s="8" t="n">
         <v>900</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="E95" s="8" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="F95" s="8" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
     </row>
     <row r="96" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="9" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C96" s="8" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E96" s="8" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="F96" s="8" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="97" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="9" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B97" s="8" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C97" s="8" t="n">
         <v>500</v>
       </c>
       <c r="D97" s="8"/>
       <c r="E97" s="8" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="F97" s="8" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="98" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="9" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B98" s="8" t="s">
         <v>41</v>
@@ -4130,221 +4142,226 @@
     </row>
     <row r="99" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="9" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B99" s="8" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="C99" s="8" t="n">
         <v>4800</v>
       </c>
       <c r="D99" s="8"/>
       <c r="E99" s="8" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="F99" s="8" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
     </row>
     <row r="100" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="9" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B100" s="8" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="C100" s="10" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="D100" s="10" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E100" s="8" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="F100" s="8" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="101" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="9" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C101" s="10"/>
       <c r="D101" s="10"/>
       <c r="E101" s="8" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>367</v>
-      </c>
-    </row>
-    <row r="102" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="102" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="13" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="C102" s="2" t="n">
         <v>9700</v>
       </c>
+      <c r="D102" s="1"/>
       <c r="E102" s="15" t="s">
-        <v>370</v>
-      </c>
-      <c r="G102" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="103" s="1" customFormat="true" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>372</v>
+      </c>
+      <c r="F102" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="13" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="C103" s="2" t="n">
         <v>9800</v>
       </c>
+      <c r="D103" s="1"/>
       <c r="E103" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="F103" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="G103" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="104" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="1" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="C104" s="2" t="n">
         <v>9400</v>
       </c>
+      <c r="D104" s="1"/>
       <c r="E104" s="8" t="s">
-        <v>376</v>
-      </c>
-      <c r="G104" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="105" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>379</v>
+      </c>
+      <c r="F104" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="C105" s="2" t="n">
         <v>9500</v>
       </c>
+      <c r="D105" s="1"/>
       <c r="E105" s="16" t="s">
-        <v>379</v>
-      </c>
-      <c r="G105" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="106" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>382</v>
+      </c>
+      <c r="F105" s="1" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="1" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="C106" s="2" t="n">
         <v>9600</v>
       </c>
+      <c r="D106" s="1"/>
       <c r="E106" s="2" t="s">
-        <v>382</v>
-      </c>
-      <c r="G106" s="3" t="s">
-        <v>35</v>
+        <v>385</v>
+      </c>
+      <c r="F106" s="1" t="s">
+        <v>373</v>
       </c>
     </row>
     <row r="107" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="9" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="C107" s="10"/>
       <c r="D107" s="10"/>
       <c r="E107" s="8" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="F107" s="8" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="108" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A108" s="9" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="C108" s="10"/>
       <c r="D108" s="10"/>
       <c r="E108" s="8" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="F108" s="8" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
     </row>
     <row r="109" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="9" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="C109" s="8" t="n">
         <v>131</v>
       </c>
       <c r="D109" s="8" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="E109" s="8" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="F109" s="8" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
     </row>
     <row r="110" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="9" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="C110" s="8" t="n">
         <v>132</v>
       </c>
       <c r="D110" s="8" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="E110" s="8" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="F110" s="8" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
     </row>
     <row r="111" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="9" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="C111" s="10" t="n">
         <v>132</v>
@@ -4352,33 +4369,33 @@
       <c r="D111" s="10"/>
       <c r="E111" s="8"/>
       <c r="G111" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="112" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="9" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="B112" s="8" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="C112" s="8" t="n">
         <v>1731</v>
       </c>
       <c r="D112" s="8"/>
       <c r="E112" s="8" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="9" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="B113" s="8" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="C113" s="8" t="n">
         <v>1731</v>
@@ -4386,719 +4403,719 @@
       <c r="D113" s="8"/>
       <c r="E113" s="8"/>
       <c r="F113" s="8" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
     </row>
     <row r="114" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="9" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="C114" s="8" t="n">
         <v>2811</v>
       </c>
       <c r="D114" s="8"/>
       <c r="E114" s="8" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="F114" s="8" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
     </row>
     <row r="115" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="9" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="B115" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C115" s="8" t="n">
         <v>200</v>
       </c>
       <c r="D115" s="8" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="E115" s="8" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="F115" s="8" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
     </row>
     <row r="116" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="12" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="B116" s="8" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="C116" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D116" s="8" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="E116" s="8" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="F116" s="8" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
     </row>
     <row r="117" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="9" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="B117" s="8" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="C117" s="8" t="n">
         <v>300</v>
       </c>
       <c r="D117" s="8" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="E117" s="8" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="F117" s="8" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
     </row>
     <row r="118" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="9" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="B118" s="8" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="C118" s="8" t="n">
         <v>5500</v>
       </c>
       <c r="D118" s="8"/>
       <c r="E118" s="8" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="119" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="9" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="C119" s="8" t="n">
         <v>5600</v>
       </c>
       <c r="D119" s="8"/>
       <c r="E119" s="8" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="120" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="9" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="B120" s="8" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="C120" s="8" t="n">
         <v>101</v>
       </c>
       <c r="D120" s="8" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="E120" s="8" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="121" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="9" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="B121" s="8" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="C121" s="8" t="n">
         <v>111</v>
       </c>
       <c r="D121" s="8" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="E121" s="8" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="122" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="9" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="C122" s="10"/>
       <c r="D122" s="10"/>
       <c r="E122" s="8" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="F122" s="8" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
     </row>
     <row r="123" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="9" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="B123" s="8" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="C123" s="8" t="n">
         <v>1000</v>
       </c>
       <c r="D123" s="8" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="E123" s="8" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="124" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="9" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="C124" s="8" t="n">
         <v>112</v>
       </c>
       <c r="D124" s="8" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="E124" s="8" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="F124" s="8" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
     </row>
     <row r="125" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="9" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="B125" s="8" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C125" s="8" t="n">
         <v>3100</v>
       </c>
       <c r="D125" s="8"/>
       <c r="E125" s="8" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="F125" s="8" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
     </row>
     <row r="126" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="9" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="B126" s="8" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="C126" s="8" t="n">
         <v>21</v>
       </c>
       <c r="D126" s="8"/>
       <c r="E126" s="8" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="F126" s="8" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
     <row r="127" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="9" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C127" s="8" t="n">
         <v>122</v>
       </c>
       <c r="D127" s="8" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="E127" s="8" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="128" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="9" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="B128" s="8" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="C128" s="8" t="n">
         <v>1722</v>
       </c>
       <c r="D128" s="8"/>
       <c r="E128" s="8" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="129" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="9" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="B129" s="8" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="C129" s="8" t="n">
         <v>7100</v>
       </c>
       <c r="D129" s="8"/>
       <c r="E129" s="8" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="130" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="9" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="C130" s="10"/>
       <c r="D130" s="10"/>
       <c r="E130" s="8" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="F130" s="8" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
     <row r="131" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="9" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="C131" s="7"/>
       <c r="E131" s="8" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
     </row>
     <row r="132" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="9" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="C132" s="10"/>
       <c r="D132" s="10"/>
       <c r="E132" s="8" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="F132" s="8" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
     </row>
     <row r="133" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="9" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="B133" s="8" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="C133" s="10"/>
       <c r="D133" s="10"/>
       <c r="E133" s="8" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="F133" s="8" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
     </row>
     <row r="134" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="C134" s="10"/>
       <c r="D134" s="10"/>
       <c r="E134" s="8" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="F134" s="8" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="135" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="C135" s="2" t="n">
         <v>133</v>
       </c>
       <c r="E135" s="8" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
     </row>
     <row r="136" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A136" s="9" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="B136" s="8" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C136" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D136" s="8" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="E136" s="8" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="F136" s="8" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
     </row>
     <row r="137" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A137" s="1" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="C137" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D137" s="8"/>
       <c r="E137" s="8" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="F137" s="8" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
     </row>
     <row r="138" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A138" s="1" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="C138" s="2" t="n">
         <v>2612</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="E138" s="8" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="F138" s="8" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
     </row>
     <row r="139" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A139" s="1" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="C139" s="7"/>
       <c r="E139" s="8" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
     </row>
     <row r="140" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="9" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="B140" s="8" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="C140" s="8" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="D140" s="8"/>
       <c r="E140" s="8" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="F140" s="8" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
     </row>
     <row r="141" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="9" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C141" s="10" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="D141" s="10"/>
       <c r="E141" s="8" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="F141" s="8" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
     </row>
     <row r="142" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="9" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="B142" s="8" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="C142" s="8" t="n">
         <v>7600</v>
       </c>
       <c r="D142" s="8"/>
       <c r="E142" s="8" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="F142" s="8" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
     </row>
     <row r="143" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="9" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="B143" s="8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C143" s="10"/>
       <c r="D143" s="10"/>
       <c r="E143" s="8" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="F143" s="8" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
     </row>
     <row r="144" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="9" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="B144" s="8" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C144" s="8" t="n">
         <v>6000</v>
       </c>
       <c r="D144" s="8"/>
       <c r="E144" s="8" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="F144" s="8" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
     </row>
     <row r="145" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A145" s="9" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="B145" s="8" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C145" s="10"/>
       <c r="D145" s="10"/>
       <c r="E145" s="8" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="F145" s="8" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
     </row>
     <row r="146" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="9" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="B146" s="8" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="C146" s="10"/>
       <c r="D146" s="10"/>
       <c r="E146" s="8" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="F146" s="8" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
     </row>
     <row r="147" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="9" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="B147" s="8" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="C147" s="10"/>
       <c r="D147" s="10"/>
       <c r="E147" s="8" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="F147" s="8" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
     </row>
     <row r="148" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="9" t="s">
+        <v>540</v>
+      </c>
+      <c r="B148" s="8" t="s">
         <v>537</v>
-      </c>
-      <c r="B148" s="8" t="s">
-        <v>534</v>
       </c>
       <c r="C148" s="10"/>
       <c r="D148" s="10"/>
       <c r="E148" s="8" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="F148" s="8" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
     </row>
     <row r="149" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="9" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="B149" s="8" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="C149" s="10"/>
       <c r="D149" s="10"/>
       <c r="E149" s="8" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="F149" s="8" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
     </row>
     <row r="150" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="9" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="B150" s="8" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="C150" s="8" t="n">
         <v>7700</v>
       </c>
       <c r="D150" s="8" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="E150" s="8" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="F150" s="8" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="151" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A151" s="9" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="B151" s="8" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="C151" s="8" t="n">
         <v>7800</v>
       </c>
       <c r="D151" s="8" t="s">
+        <v>554</v>
+      </c>
+      <c r="E151" s="8" t="s">
+        <v>555</v>
+      </c>
+      <c r="F151" s="8" t="s">
         <v>551</v>
-      </c>
-      <c r="E151" s="8" t="s">
-        <v>552</v>
-      </c>
-      <c r="F151" s="8" t="s">
-        <v>548</v>
       </c>
     </row>
     <row r="152" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="9" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="B152" s="8" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="C152" s="10"/>
       <c r="D152" s="10"/>
       <c r="E152" s="8" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="F152" s="8" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
     </row>
     <row r="153" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="1" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="C153" s="2" t="n">
         <v>8900</v>
       </c>
       <c r="E153" s="8" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="G153" s="3" t="s">
         <v>11</v>
@@ -5106,798 +5123,798 @@
     </row>
     <row r="154" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="9" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="B154" s="8" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C154" s="10" t="n">
         <v>100</v>
       </c>
       <c r="D154" s="10" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="E154" s="8" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="F154" s="8" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
     </row>
     <row r="155" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="9" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="C155" s="10"/>
       <c r="D155" s="10"/>
       <c r="E155" s="8" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="F155" s="8" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
     </row>
     <row r="156" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="9" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="B156" s="8" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="C156" s="8" t="n">
         <v>101</v>
       </c>
       <c r="D156" s="8"/>
       <c r="E156" s="8" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="G156" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="157" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="9" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="B157" s="8" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C157" s="10"/>
       <c r="D157" s="10"/>
       <c r="E157" s="8" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="F157" s="8" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
     </row>
     <row r="158" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="9" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="B158" s="8" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C158" s="10"/>
       <c r="D158" s="10" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="E158" s="8" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="F158" s="8" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
     </row>
     <row r="159" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="9" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="B159" s="8" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C159" s="8" t="n">
         <v>1400</v>
       </c>
       <c r="D159" s="8" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="E159" s="8" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="F159" s="8" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
     </row>
     <row r="160" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="1" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="B160" s="8" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="C160" s="8" t="n">
         <v>7400</v>
       </c>
       <c r="D160" s="8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E160" s="8" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="F160" s="8" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
     </row>
     <row r="161" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A161" s="9" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="B161" s="8" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="C161" s="10"/>
       <c r="D161" s="10" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="E161" s="8" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="F161" s="8" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
     </row>
     <row r="162" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A162" s="9" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="B162" s="8" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="C162" s="8" t="n">
         <v>1700</v>
       </c>
       <c r="D162" s="8" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="E162" s="8" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="F162" s="8" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
     </row>
     <row r="163" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A163" s="9" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="B163" s="8" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="C163" s="8" t="n">
         <v>1800</v>
       </c>
       <c r="D163" s="8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E163" s="8" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="F163" s="8" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
     </row>
     <row r="164" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A164" s="9" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="B164" s="8" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C164" s="7"/>
       <c r="D164" s="7"/>
       <c r="E164" s="8" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="F164" s="8" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
     </row>
     <row r="165" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A165" s="9" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C165" s="10" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="D165" s="10"/>
       <c r="E165" s="8" t="s">
+        <v>605</v>
+      </c>
+      <c r="F165" s="8" t="s">
         <v>602</v>
-      </c>
-      <c r="F165" s="8" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="166" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A166" s="9" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="B166" s="8" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="C166" s="10"/>
       <c r="D166" s="10"/>
       <c r="E166" s="8" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="F166" s="8" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
     </row>
     <row r="167" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A167" s="9" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="C167" s="10"/>
       <c r="D167" s="10"/>
       <c r="E167" s="8" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="F167" s="8" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
     </row>
     <row r="168" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A168" s="9" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="C168" s="10"/>
       <c r="D168" s="10"/>
       <c r="E168" s="8" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="F168" s="8" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
     </row>
     <row r="169" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A169" s="9" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="C169" s="10"/>
       <c r="D169" s="10"/>
       <c r="E169" s="8" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="F169" s="8" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
     </row>
     <row r="170" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A170" s="9" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="B170" s="8" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="C170" s="10"/>
       <c r="D170" s="10"/>
       <c r="E170" s="8" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="F170" s="8" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
     </row>
     <row r="171" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A171" s="9" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C171" s="10"/>
       <c r="D171" s="10"/>
       <c r="E171" s="8" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="F171" s="8" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
     </row>
     <row r="172" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A172" s="9" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="B172" s="8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C172" s="10"/>
       <c r="D172" s="10"/>
       <c r="E172" s="8" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="F172" s="8" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
     </row>
     <row r="173" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A173" s="9" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="B173" s="8" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C173" s="10"/>
       <c r="D173" s="10"/>
       <c r="E173" s="8" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="F173" s="8" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
     </row>
     <row r="174" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A174" s="9" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="B174" s="8" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C174" s="10"/>
       <c r="D174" s="10"/>
       <c r="E174" s="8" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="F174" s="8" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
     </row>
     <row r="175" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A175" s="9" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="B175" s="8" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="C175" s="10"/>
       <c r="D175" s="10"/>
       <c r="E175" s="8" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="F175" s="8" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
     </row>
     <row r="176" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A176" s="9" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="B176" s="8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C176" s="10"/>
       <c r="D176" s="10"/>
       <c r="E176" s="8" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="F176" s="8" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
     </row>
     <row r="177" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A177" s="9" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="B177" s="8" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C177" s="10"/>
       <c r="D177" s="10"/>
       <c r="E177" s="8" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="F177" s="8" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
     </row>
     <row r="178" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A178" s="9" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="B178" s="8" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C178" s="10"/>
       <c r="D178" s="10"/>
       <c r="E178" s="8" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="F178" s="8" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
     </row>
     <row r="179" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A179" s="9" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="B179" s="8" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C179" s="10"/>
       <c r="D179" s="10"/>
       <c r="E179" s="8" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="F179" s="8" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
     </row>
     <row r="180" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A180" s="9" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="C180" s="10"/>
       <c r="D180" s="10"/>
       <c r="E180" s="8" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="F180" s="8" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
     </row>
     <row r="181" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A181" s="1" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>648</v>
+        <v>651</v>
       </c>
       <c r="C181" s="2" t="n">
         <v>23</v>
       </c>
       <c r="E181" s="8" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="F181" s="2" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
     </row>
     <row r="182" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A182" s="9" t="s">
-        <v>651</v>
+        <v>654</v>
       </c>
       <c r="B182" s="8" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="C182" s="8" t="n">
         <v>121</v>
       </c>
       <c r="D182" s="8"/>
       <c r="E182" s="8" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="G182" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="183" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A183" s="9" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C183" s="10"/>
       <c r="D183" s="10"/>
       <c r="E183" s="8" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="F183" s="8" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
     </row>
     <row r="184" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A184" s="9" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C184" s="10"/>
       <c r="D184" s="10"/>
       <c r="E184" s="8" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="F184" s="8" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
     </row>
     <row r="185" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A185" s="9" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="C185" s="8" t="n">
         <v>111</v>
       </c>
       <c r="D185" s="8"/>
       <c r="E185" s="8" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="G185" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="186" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A186" s="9" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="B186" s="8" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="C186" s="8" t="n">
         <v>1711</v>
       </c>
       <c r="D186" s="8"/>
       <c r="E186" s="8" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="F186" s="8" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
     </row>
     <row r="187" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A187" s="1" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="B187" s="8" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="C187" s="8" t="n">
         <v>3300</v>
       </c>
       <c r="D187" s="8"/>
       <c r="E187" s="8" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="F187" s="8" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
     </row>
     <row r="188" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A188" s="9" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="B188" s="8" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="C188" s="8" t="n">
         <v>8000</v>
       </c>
       <c r="D188" s="8" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="E188" s="8" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="F188" s="8" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
     </row>
     <row r="189" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A189" s="9" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="C189" s="10"/>
       <c r="D189" s="10"/>
       <c r="E189" s="8" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="F189" s="8" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
     </row>
     <row r="190" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A190" s="9" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="B190" s="8" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="C190" s="10"/>
       <c r="D190" s="10"/>
       <c r="E190" s="8" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="F190" s="8" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
     </row>
     <row r="191" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A191" s="9" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="B191" s="8" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C191" s="10"/>
       <c r="D191" s="10"/>
       <c r="E191" s="8" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="F191" s="8" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
     </row>
     <row r="192" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A192" s="9" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="B192" s="8" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="C192" s="8" t="n">
         <v>1500</v>
       </c>
       <c r="D192" s="8" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="E192" s="8" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="F192" s="8" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="193" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A193" s="9" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="C193" s="8" t="n">
         <v>2611</v>
       </c>
       <c r="D193" s="8"/>
       <c r="E193" s="8" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="G193" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="194" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A194" s="9" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="B194" s="8" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="C194" s="8" t="n">
         <v>2711</v>
       </c>
       <c r="D194" s="8"/>
       <c r="E194" s="8" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
       <c r="G194" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="195" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A195" s="9" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="C195" s="10"/>
       <c r="D195" s="10"/>
       <c r="E195" s="8" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
       <c r="F195" s="8" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
     </row>
     <row r="196" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A196" s="9" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
       <c r="B196" s="8" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="C196" s="10"/>
       <c r="D196" s="10"/>
       <c r="E196" s="8" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
       <c r="F196" s="8" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
     </row>
     <row r="197" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A197" s="9" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
       <c r="C197" s="8" t="n">
         <v>3721</v>
       </c>
       <c r="D197" s="8"/>
       <c r="E197" s="8" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
       <c r="F197" s="8" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
     </row>
     <row r="198" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A198" s="9" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="C198" s="8" t="n">
         <v>6100</v>
       </c>
       <c r="D198" s="8"/>
       <c r="E198" s="8" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
       <c r="F198" s="8" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
     </row>
     <row r="199" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A199" s="9" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
       <c r="C199" s="10" t="n">
         <v>8400</v>
       </c>
       <c r="D199" s="10"/>
       <c r="E199" s="8" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="F199" s="8" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
     </row>
     <row r="200" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A200" s="9" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="B200" s="8" t="s">
         <v>49</v>
@@ -5905,51 +5922,51 @@
       <c r="C200" s="7"/>
       <c r="D200" s="7"/>
       <c r="E200" s="8" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
       <c r="F200" s="8" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
     </row>
     <row r="201" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A201" s="1" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="C201" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D201" s="8"/>
       <c r="E201" s="8" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="F201" s="8" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
     </row>
     <row r="202" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A202" s="1" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="B202" s="8" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="C202" s="8" t="n">
         <v>400</v>
       </c>
       <c r="D202" s="8"/>
       <c r="E202" s="8" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
       <c r="F202" s="8" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
     </row>
     <row r="203" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A203" s="9" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="B203" s="8" t="s">
         <v>16</v>
@@ -5957,42 +5974,42 @@
       <c r="C203" s="10"/>
       <c r="D203" s="10"/>
       <c r="E203" s="8" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
       <c r="F203" s="8" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
     </row>
     <row r="204" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A204" s="9" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
       <c r="B204" s="8" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="C204" s="8" t="n">
         <v>21</v>
       </c>
       <c r="D204" s="8"/>
       <c r="E204" s="8" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="G204" s="3" t="s">
-        <v>35</v>
+        <v>76</v>
       </c>
     </row>
     <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A205" s="1" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
       <c r="B205" s="8" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E205" s="8" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="F205" s="8" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
     </row>
   </sheetData>

</xml_diff>